<commit_message>
updating data and analysis
</commit_message>
<xml_diff>
--- a/data/observation_datasheet.xlsx
+++ b/data/observation_datasheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/catchamberlain/Documents/git/chillfreeze/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{2103F9AE-8D70-DB49-BDE6-35AA4C3DC354}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{368483CA-8E4D-DC40-AB80-2AAF8495ECF9}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11540" yWindow="5480" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21500" yWindow="3660" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="observation_datasheet" sheetId="1" r:id="rId1"/>
@@ -4824,10 +4824,10 @@
   <dimension ref="A1:G481"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B432" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E354" sqref="E354"/>
+      <selection pane="bottomRight" activeCell="F445" sqref="F445"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4973,7 +4973,9 @@
       <c r="A11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="4"/>
+      <c r="B11" s="4">
+        <v>43500</v>
+      </c>
       <c r="C11" s="4"/>
       <c r="D11" s="13"/>
       <c r="E11" s="4">
@@ -5035,7 +5037,9 @@
       <c r="A16" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="4"/>
+      <c r="B16" s="4">
+        <v>43500</v>
+      </c>
       <c r="C16" s="4"/>
       <c r="D16" s="13"/>
       <c r="E16" s="4">
@@ -5046,7 +5050,9 @@
       <c r="A17" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="4"/>
+      <c r="B17" s="4">
+        <v>43500</v>
+      </c>
       <c r="C17" s="4"/>
       <c r="D17" s="13"/>
       <c r="E17" s="4">
@@ -5219,7 +5225,9 @@
       <c r="A32" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B32" s="6"/>
+      <c r="B32" s="6">
+        <v>43500</v>
+      </c>
       <c r="C32" s="6"/>
       <c r="D32" s="14"/>
       <c r="E32" s="6">
@@ -5555,7 +5563,9 @@
       <c r="A59" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B59" s="4"/>
+      <c r="B59" s="4">
+        <v>43500</v>
+      </c>
       <c r="C59" s="4"/>
       <c r="D59" s="13"/>
       <c r="E59" s="4">
@@ -5792,7 +5802,9 @@
       <c r="A77" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="B77" s="6"/>
+      <c r="B77" s="6">
+        <v>43500</v>
+      </c>
       <c r="C77" s="6"/>
       <c r="D77" s="14"/>
       <c r="E77" s="6">
@@ -5825,7 +5837,9 @@
       <c r="E79" s="6">
         <v>43472</v>
       </c>
-      <c r="F79" s="10"/>
+      <c r="F79" s="10">
+        <v>43500</v>
+      </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" s="5" t="s">
@@ -5852,7 +5866,9 @@
       <c r="E81" s="6">
         <v>43472</v>
       </c>
-      <c r="F81" s="10"/>
+      <c r="F81" s="10">
+        <v>43500</v>
+      </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" s="7" t="s">
@@ -6383,7 +6399,9 @@
       <c r="E117" s="6">
         <v>43472</v>
       </c>
-      <c r="F117" s="10"/>
+      <c r="F117" s="10">
+        <v>43500</v>
+      </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A118" s="5" t="s">
@@ -6450,8 +6468,12 @@
       <c r="B122" s="6">
         <v>43481</v>
       </c>
-      <c r="C122" s="6"/>
-      <c r="D122" s="14"/>
+      <c r="C122" s="6">
+        <v>43500</v>
+      </c>
+      <c r="D122" s="14">
+        <v>45.8</v>
+      </c>
       <c r="E122" s="6">
         <v>43472</v>
       </c>
@@ -6534,7 +6556,9 @@
       <c r="E127" s="6">
         <v>43472</v>
       </c>
-      <c r="F127" s="10"/>
+      <c r="F127" s="10">
+        <v>43500</v>
+      </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A128" s="5" t="s">
@@ -6569,7 +6593,9 @@
       <c r="A130" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="B130" s="11"/>
+      <c r="B130" s="11">
+        <v>43500</v>
+      </c>
       <c r="C130" s="11"/>
       <c r="D130" s="15"/>
       <c r="E130" s="11">
@@ -6580,7 +6606,9 @@
       <c r="A131" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="B131" s="11"/>
+      <c r="B131" s="11">
+        <v>43500</v>
+      </c>
       <c r="C131" s="11"/>
       <c r="D131" s="15"/>
       <c r="E131" s="11">
@@ -6661,7 +6689,9 @@
       <c r="E137" s="11">
         <v>43486</v>
       </c>
-      <c r="F137" s="10"/>
+      <c r="F137" s="10">
+        <v>43500</v>
+      </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A138" s="7" t="s">
@@ -6711,13 +6741,17 @@
       <c r="E141" s="11">
         <v>43486</v>
       </c>
-      <c r="F141" s="10"/>
+      <c r="F141" s="10">
+        <v>43500</v>
+      </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A142" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="B142" s="11"/>
+      <c r="B142" s="11">
+        <v>43500</v>
+      </c>
       <c r="C142" s="11"/>
       <c r="D142" s="15"/>
       <c r="E142" s="11">
@@ -6728,7 +6762,9 @@
       <c r="A143" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="B143" s="11"/>
+      <c r="B143" s="11">
+        <v>43500</v>
+      </c>
       <c r="C143" s="11"/>
       <c r="D143" s="15"/>
       <c r="E143" s="11">
@@ -6785,7 +6821,9 @@
       <c r="B147" s="4">
         <v>43481</v>
       </c>
-      <c r="C147" s="4"/>
+      <c r="C147" s="4">
+        <v>43500</v>
+      </c>
       <c r="D147" s="13"/>
       <c r="E147" s="4">
         <v>43458</v>
@@ -6895,7 +6933,9 @@
       <c r="B153" s="4">
         <v>43486</v>
       </c>
-      <c r="C153" s="4"/>
+      <c r="C153" s="4">
+        <v>43500</v>
+      </c>
       <c r="D153" s="13"/>
       <c r="E153" s="4">
         <v>43458</v>
@@ -6911,7 +6951,9 @@
       <c r="B154" s="4">
         <v>43476</v>
       </c>
-      <c r="C154" s="4"/>
+      <c r="C154" s="4">
+        <v>43500</v>
+      </c>
       <c r="D154" s="13"/>
       <c r="E154" s="4">
         <v>43458</v>
@@ -6924,7 +6966,9 @@
       <c r="B155" s="4">
         <v>43483</v>
       </c>
-      <c r="C155" s="4"/>
+      <c r="C155" s="4">
+        <v>43500</v>
+      </c>
       <c r="D155" s="13"/>
       <c r="E155" s="4">
         <v>43458</v>
@@ -7031,7 +7075,9 @@
       <c r="B161" s="4">
         <v>43483</v>
       </c>
-      <c r="C161" s="4"/>
+      <c r="C161" s="4">
+        <v>43500</v>
+      </c>
       <c r="D161" s="13"/>
       <c r="E161" s="4">
         <v>43458</v>
@@ -7065,7 +7111,9 @@
       <c r="E163" s="6">
         <v>43472</v>
       </c>
-      <c r="F163" s="10"/>
+      <c r="F163" s="10">
+        <v>43500</v>
+      </c>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A164" s="5" t="s">
@@ -7092,7 +7140,9 @@
       <c r="E165" s="6">
         <v>43472</v>
       </c>
-      <c r="F165" s="10"/>
+      <c r="F165" s="10">
+        <v>43500</v>
+      </c>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A166" s="5" t="s">
@@ -7119,7 +7169,9 @@
       <c r="E167" s="6">
         <v>43472</v>
       </c>
-      <c r="F167" s="10"/>
+      <c r="F167" s="10">
+        <v>43500</v>
+      </c>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A168" s="5" t="s">
@@ -7260,7 +7312,9 @@
       <c r="E177" s="6">
         <v>43472</v>
       </c>
-      <c r="F177" s="10"/>
+      <c r="F177" s="10">
+        <v>43500</v>
+      </c>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A178" s="7" t="s">
@@ -7335,7 +7389,9 @@
       <c r="A184" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="B184" s="11"/>
+      <c r="B184" s="11">
+        <v>43500</v>
+      </c>
       <c r="C184" s="11"/>
       <c r="D184" s="15"/>
       <c r="E184" s="11">
@@ -7346,7 +7402,9 @@
       <c r="A185" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="B185" s="11"/>
+      <c r="B185" s="11">
+        <v>43500</v>
+      </c>
       <c r="C185" s="11"/>
       <c r="D185" s="15"/>
       <c r="E185" s="11">
@@ -7381,7 +7439,9 @@
       <c r="A188" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="B188" s="11"/>
+      <c r="B188" s="11">
+        <v>43500</v>
+      </c>
       <c r="C188" s="11"/>
       <c r="D188" s="15"/>
       <c r="E188" s="11">
@@ -7427,7 +7487,9 @@
       <c r="A192" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="B192" s="11"/>
+      <c r="B192" s="11">
+        <v>43500</v>
+      </c>
       <c r="C192" s="11"/>
       <c r="D192" s="15"/>
       <c r="E192" s="11">
@@ -7540,8 +7602,12 @@
       <c r="B199" s="4">
         <v>43476</v>
       </c>
-      <c r="C199" s="4"/>
-      <c r="D199" s="13"/>
+      <c r="C199" s="4">
+        <v>43500</v>
+      </c>
+      <c r="D199" s="13">
+        <v>54.4</v>
+      </c>
       <c r="E199" s="4">
         <v>43458</v>
       </c>
@@ -7622,8 +7688,12 @@
       <c r="B204" s="4">
         <v>43479</v>
       </c>
-      <c r="C204" s="4"/>
-      <c r="D204" s="13"/>
+      <c r="C204" s="4">
+        <v>43500</v>
+      </c>
+      <c r="D204" s="13">
+        <v>51.3</v>
+      </c>
       <c r="E204" s="4">
         <v>43458</v>
       </c>
@@ -7777,7 +7847,9 @@
       <c r="E213" s="6">
         <v>43472</v>
       </c>
-      <c r="F213" s="10"/>
+      <c r="F213" s="10">
+        <v>43500</v>
+      </c>
     </row>
     <row r="214" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A214" s="5" t="s">
@@ -7844,8 +7916,12 @@
       <c r="B218" s="6">
         <v>43486</v>
       </c>
-      <c r="C218" s="6"/>
-      <c r="D218" s="14"/>
+      <c r="C218" s="6">
+        <v>43500</v>
+      </c>
+      <c r="D218" s="14">
+        <v>48.2</v>
+      </c>
       <c r="E218" s="6">
         <v>43472</v>
       </c>
@@ -7862,7 +7938,9 @@
       <c r="E219" s="6">
         <v>43472</v>
       </c>
-      <c r="F219" s="10"/>
+      <c r="F219" s="10">
+        <v>43500</v>
+      </c>
     </row>
     <row r="220" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A220" s="5" t="s">
@@ -7884,8 +7962,12 @@
       <c r="B221" s="6">
         <v>43483</v>
       </c>
-      <c r="C221" s="6"/>
-      <c r="D221" s="14"/>
+      <c r="C221" s="6">
+        <v>43500</v>
+      </c>
+      <c r="D221" s="14">
+        <v>50.2</v>
+      </c>
       <c r="E221" s="6">
         <v>43472</v>
       </c>
@@ -7946,8 +8028,12 @@
       <c r="B225" s="6">
         <v>43483</v>
       </c>
-      <c r="C225" s="6"/>
-      <c r="D225" s="14"/>
+      <c r="C225" s="6">
+        <v>43500</v>
+      </c>
+      <c r="D225" s="14">
+        <v>34.200000000000003</v>
+      </c>
       <c r="E225" s="6">
         <v>43472</v>
       </c>
@@ -7959,7 +8045,9 @@
       <c r="A226" s="7" t="s">
         <v>227</v>
       </c>
-      <c r="B226" s="11"/>
+      <c r="B226" s="11">
+        <v>43500</v>
+      </c>
       <c r="C226" s="11"/>
       <c r="D226" s="15"/>
       <c r="E226" s="11">
@@ -8076,7 +8164,9 @@
       <c r="E235" s="11">
         <v>43486</v>
       </c>
-      <c r="F235" s="10"/>
+      <c r="F235" s="10">
+        <v>43500</v>
+      </c>
     </row>
     <row r="236" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A236" s="7" t="s">
@@ -8095,7 +8185,9 @@
       <c r="A237" s="7" t="s">
         <v>238</v>
       </c>
-      <c r="B237" s="11"/>
+      <c r="B237" s="11">
+        <v>43500</v>
+      </c>
       <c r="C237" s="11"/>
       <c r="D237" s="15"/>
       <c r="E237" s="11">
@@ -8120,7 +8212,9 @@
       <c r="A239" s="7" t="s">
         <v>240</v>
       </c>
-      <c r="B239" s="11"/>
+      <c r="B239" s="11">
+        <v>43500</v>
+      </c>
       <c r="C239" s="11"/>
       <c r="D239" s="15"/>
       <c r="E239" s="11">
@@ -8132,7 +8226,9 @@
       <c r="A240" s="7" t="s">
         <v>241</v>
       </c>
-      <c r="B240" s="11"/>
+      <c r="B240" s="11">
+        <v>43500</v>
+      </c>
       <c r="C240" s="11"/>
       <c r="D240" s="15"/>
       <c r="E240" s="11">
@@ -8151,7 +8247,9 @@
       <c r="E241" s="11">
         <v>43486</v>
       </c>
-      <c r="F241" s="10"/>
+      <c r="F241" s="10">
+        <v>43500</v>
+      </c>
     </row>
     <row r="242" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A242" s="3" t="s">
@@ -9643,8 +9741,12 @@
       <c r="B358" s="6">
         <v>43483</v>
       </c>
-      <c r="C358" s="6"/>
-      <c r="D358" s="14"/>
+      <c r="C358" s="6">
+        <v>43500</v>
+      </c>
+      <c r="D358" s="14">
+        <v>29.4</v>
+      </c>
       <c r="E358" s="6">
         <v>43472</v>
       </c>
@@ -9738,8 +9840,12 @@
       <c r="B364" s="6">
         <v>43486</v>
       </c>
-      <c r="C364" s="6"/>
-      <c r="D364" s="14"/>
+      <c r="C364" s="6">
+        <v>43500</v>
+      </c>
+      <c r="D364" s="14">
+        <v>27.8</v>
+      </c>
       <c r="E364" s="6">
         <v>43472</v>
       </c>
@@ -9751,8 +9857,12 @@
       <c r="B365" s="6">
         <v>43483</v>
       </c>
-      <c r="C365" s="6"/>
-      <c r="D365" s="14"/>
+      <c r="C365" s="6">
+        <v>43500</v>
+      </c>
+      <c r="D365" s="14">
+        <v>29.6</v>
+      </c>
       <c r="E365" s="6">
         <v>43472</v>
       </c>
@@ -9767,8 +9877,12 @@
       <c r="B366" s="6">
         <v>43481</v>
       </c>
-      <c r="C366" s="6"/>
-      <c r="D366" s="14"/>
+      <c r="C366" s="6">
+        <v>43493</v>
+      </c>
+      <c r="D366" s="14">
+        <v>28.6</v>
+      </c>
       <c r="E366" s="6">
         <v>43472</v>
       </c>
@@ -9780,8 +9894,12 @@
       <c r="B367" s="6">
         <v>43481</v>
       </c>
-      <c r="C367" s="6"/>
-      <c r="D367" s="14"/>
+      <c r="C367" s="6">
+        <v>43500</v>
+      </c>
+      <c r="D367" s="14">
+        <v>25.6</v>
+      </c>
       <c r="E367" s="6">
         <v>43472</v>
       </c>
@@ -9874,7 +9992,9 @@
       <c r="E373" s="11">
         <v>43486</v>
       </c>
-      <c r="F373" s="10"/>
+      <c r="F373" s="10">
+        <v>43500</v>
+      </c>
     </row>
     <row r="374" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A374" s="7" t="s">
@@ -9901,7 +10021,9 @@
       <c r="E375" s="11">
         <v>43486</v>
       </c>
-      <c r="F375" s="10"/>
+      <c r="F375" s="10">
+        <v>43500</v>
+      </c>
     </row>
     <row r="376" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A376" s="7" t="s">
@@ -9928,7 +10050,9 @@
       <c r="E377" s="11">
         <v>43486</v>
       </c>
-      <c r="F377" s="10"/>
+      <c r="F377" s="10">
+        <v>43500</v>
+      </c>
     </row>
     <row r="378" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A378" s="7" t="s">
@@ -9982,7 +10106,9 @@
       <c r="E381" s="11">
         <v>43486</v>
       </c>
-      <c r="F381" s="10"/>
+      <c r="F381" s="10">
+        <v>43500</v>
+      </c>
     </row>
     <row r="382" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A382" s="7" t="s">
@@ -10001,7 +10127,9 @@
       <c r="A383" s="7" t="s">
         <v>384</v>
       </c>
-      <c r="B383" s="11"/>
+      <c r="B383" s="11">
+        <v>43500</v>
+      </c>
       <c r="C383" s="11"/>
       <c r="D383" s="15"/>
       <c r="E383" s="11">
@@ -10169,7 +10297,7 @@
         <v>397</v>
       </c>
       <c r="B396" s="4">
-        <v>43495</v>
+        <v>43500</v>
       </c>
       <c r="C396" s="4"/>
       <c r="D396" s="13"/>
@@ -10181,7 +10309,9 @@
       <c r="A397" s="3" t="s">
         <v>398</v>
       </c>
-      <c r="B397" s="4"/>
+      <c r="B397" s="4">
+        <v>43500</v>
+      </c>
       <c r="C397" s="4"/>
       <c r="D397" s="13"/>
       <c r="E397" s="4">
@@ -10354,7 +10484,9 @@
       <c r="A411" s="5" t="s">
         <v>412</v>
       </c>
-      <c r="B411" s="6"/>
+      <c r="B411" s="6">
+        <v>43500</v>
+      </c>
       <c r="C411" s="6"/>
       <c r="D411" s="14"/>
       <c r="E411" s="6">
@@ -10772,14 +10904,14 @@
       <c r="B445" s="4">
         <v>43488</v>
       </c>
-      <c r="C445" s="4">
-        <v>43497</v>
-      </c>
+      <c r="C445" s="4"/>
       <c r="D445" s="13"/>
       <c r="E445" s="4">
         <v>43458</v>
       </c>
-      <c r="F445" s="10"/>
+      <c r="F445" s="10">
+        <v>43497</v>
+      </c>
     </row>
     <row r="446" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A446" s="3" t="s">
@@ -10804,13 +10936,17 @@
       <c r="E447" s="4">
         <v>43458</v>
       </c>
-      <c r="F447" s="10"/>
+      <c r="F447" s="10">
+        <v>43500</v>
+      </c>
     </row>
     <row r="448" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A448" s="3" t="s">
         <v>449</v>
       </c>
-      <c r="B448" s="4"/>
+      <c r="B448" s="4">
+        <v>43500</v>
+      </c>
       <c r="C448" s="4"/>
       <c r="D448" s="13"/>
       <c r="E448" s="4">
@@ -10933,7 +11069,9 @@
       <c r="A458" s="5" t="s">
         <v>459</v>
       </c>
-      <c r="B458" s="6"/>
+      <c r="B458" s="6">
+        <v>43500</v>
+      </c>
       <c r="C458" s="6"/>
       <c r="D458" s="14"/>
       <c r="E458" s="6">
@@ -10952,7 +11090,9 @@
       <c r="E459" s="6">
         <v>43472</v>
       </c>
-      <c r="F459" s="10"/>
+      <c r="F459" s="10">
+        <v>43500</v>
+      </c>
     </row>
     <row r="460" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A460" s="5" t="s">

</xml_diff>

<commit_message>
more data to work with
</commit_message>
<xml_diff>
--- a/data/observation_datasheet.xlsx
+++ b/data/observation_datasheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/catchamberlain/Documents/git/chillfreeze/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{9442D32D-1751-FF4F-B16A-A7D8623D0FCC}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{988C57D9-9262-EA4E-A554-E132BDA4BE2F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13260" yWindow="1320" windowWidth="29720" windowHeight="20980" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10760" yWindow="3720" windowWidth="29720" windowHeight="20980" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="observation_datasheet" sheetId="1" r:id="rId1"/>
@@ -5053,10 +5053,10 @@
   <dimension ref="A1:M481"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B442" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B432" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D474" sqref="D474"/>
+      <selection pane="bottomRight" activeCell="H464" sqref="H464"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5204,8 +5204,12 @@
       <c r="B7" s="4">
         <v>43512</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="13"/>
+      <c r="C7" s="4">
+        <v>43528</v>
+      </c>
+      <c r="D7" s="13">
+        <v>22.1</v>
+      </c>
       <c r="E7" s="4">
         <v>43458</v>
       </c>
@@ -5220,8 +5224,12 @@
       <c r="B8" s="4">
         <v>43512</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="13"/>
+      <c r="C8" s="4">
+        <v>43528</v>
+      </c>
+      <c r="D8" s="13">
+        <v>22.5</v>
+      </c>
       <c r="E8" s="4">
         <v>43458</v>
       </c>
@@ -5400,7 +5408,9 @@
       <c r="B18" s="6">
         <v>43512</v>
       </c>
-      <c r="C18" s="6"/>
+      <c r="C18" s="6">
+        <v>43528</v>
+      </c>
       <c r="D18" s="14"/>
       <c r="E18" s="6">
         <v>43472</v>
@@ -5410,7 +5420,9 @@
       <c r="A19" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="6"/>
+      <c r="B19" s="6">
+        <v>43528</v>
+      </c>
       <c r="C19" s="6"/>
       <c r="D19" s="14"/>
       <c r="E19" s="6">
@@ -5462,8 +5474,12 @@
       <c r="B22" s="6">
         <v>43515</v>
       </c>
-      <c r="C22" s="6"/>
-      <c r="D22" s="14"/>
+      <c r="C22" s="6">
+        <v>43528</v>
+      </c>
+      <c r="D22" s="14">
+        <v>30.9</v>
+      </c>
       <c r="E22" s="6">
         <v>43472</v>
       </c>
@@ -5509,13 +5525,17 @@
       <c r="A25" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B25" s="6"/>
+      <c r="B25" s="6">
+        <v>43521</v>
+      </c>
       <c r="C25" s="6"/>
       <c r="D25" s="14"/>
       <c r="E25" s="6">
         <v>43472</v>
       </c>
-      <c r="F25" s="10"/>
+      <c r="F25" s="10">
+        <v>43528</v>
+      </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
@@ -5557,8 +5577,12 @@
       <c r="B28" s="6">
         <v>43512</v>
       </c>
-      <c r="C28" s="6"/>
-      <c r="D28" s="14"/>
+      <c r="C28" s="6">
+        <v>43528</v>
+      </c>
+      <c r="D28" s="14">
+        <v>27.7</v>
+      </c>
       <c r="E28" s="6">
         <v>43472</v>
       </c>
@@ -5575,7 +5599,9 @@
       <c r="E29" s="6">
         <v>43472</v>
       </c>
-      <c r="F29" s="10"/>
+      <c r="F29" s="10">
+        <v>43528</v>
+      </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
@@ -5595,8 +5621,12 @@
       <c r="B31" s="6">
         <v>43515</v>
       </c>
-      <c r="C31" s="6"/>
-      <c r="D31" s="14"/>
+      <c r="C31" s="6">
+        <v>43528</v>
+      </c>
+      <c r="D31" s="14">
+        <v>35.200000000000003</v>
+      </c>
       <c r="E31" s="6">
         <v>43472</v>
       </c>
@@ -5666,7 +5696,9 @@
       <c r="E35" s="11">
         <v>43486</v>
       </c>
-      <c r="F35" s="10"/>
+      <c r="F35" s="10">
+        <v>43528</v>
+      </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="7" t="s">
@@ -5675,8 +5707,12 @@
       <c r="B36" s="11">
         <v>43515</v>
       </c>
-      <c r="C36" s="11"/>
-      <c r="D36" s="15"/>
+      <c r="C36" s="11">
+        <v>43528</v>
+      </c>
+      <c r="D36" s="15">
+        <v>28.8</v>
+      </c>
       <c r="E36" s="11">
         <v>43486</v>
       </c>
@@ -5693,7 +5729,9 @@
       <c r="E37" s="11">
         <v>43486</v>
       </c>
-      <c r="F37" s="10"/>
+      <c r="F37" s="10">
+        <v>43528</v>
+      </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="7" t="s">
@@ -5772,7 +5810,9 @@
       <c r="E43" s="11">
         <v>43486</v>
       </c>
-      <c r="F43" s="10"/>
+      <c r="F43" s="10">
+        <v>43528</v>
+      </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="7" t="s">
@@ -5791,7 +5831,9 @@
       <c r="A45" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B45" s="11"/>
+      <c r="B45" s="11">
+        <v>43528</v>
+      </c>
       <c r="C45" s="11"/>
       <c r="D45" s="15"/>
       <c r="E45" s="11">
@@ -5806,8 +5848,12 @@
       <c r="B46" s="11">
         <v>43518</v>
       </c>
-      <c r="C46" s="11"/>
-      <c r="D46" s="15"/>
+      <c r="C46" s="11">
+        <v>43528</v>
+      </c>
+      <c r="D46" s="15">
+        <v>33</v>
+      </c>
       <c r="E46" s="11">
         <v>43486</v>
       </c>
@@ -6150,8 +6196,12 @@
       <c r="B66" s="6">
         <v>43507</v>
       </c>
-      <c r="C66" s="6"/>
-      <c r="D66" s="14"/>
+      <c r="C66" s="6">
+        <v>43528</v>
+      </c>
+      <c r="D66" s="14">
+        <v>46.5</v>
+      </c>
       <c r="E66" s="6">
         <v>43472</v>
       </c>
@@ -6613,8 +6663,12 @@
       <c r="B93" s="11">
         <v>43507</v>
       </c>
-      <c r="C93" s="11"/>
-      <c r="D93" s="15"/>
+      <c r="C93" s="11">
+        <v>43528</v>
+      </c>
+      <c r="D93" s="15">
+        <v>25.5</v>
+      </c>
       <c r="E93" s="11">
         <v>43486</v>
       </c>
@@ -6646,8 +6700,12 @@
       <c r="B95" s="11">
         <v>43504</v>
       </c>
-      <c r="C95" s="11"/>
-      <c r="D95" s="15"/>
+      <c r="C95" s="11">
+        <v>43528</v>
+      </c>
+      <c r="D95" s="15">
+        <v>28.3</v>
+      </c>
       <c r="E95" s="11">
         <v>43486</v>
       </c>
@@ -6679,8 +6737,12 @@
       <c r="B97" s="11">
         <v>43512</v>
       </c>
-      <c r="C97" s="11"/>
-      <c r="D97" s="15"/>
+      <c r="C97" s="11">
+        <v>43528</v>
+      </c>
+      <c r="D97" s="15">
+        <v>23.4</v>
+      </c>
       <c r="E97" s="11">
         <v>43486</v>
       </c>
@@ -9585,7 +9647,9 @@
       <c r="E243" s="4">
         <v>43458</v>
       </c>
-      <c r="F243" s="10"/>
+      <c r="F243" s="10">
+        <v>43528</v>
+      </c>
     </row>
     <row r="244" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A244" s="3" t="s">
@@ -9612,7 +9676,9 @@
       <c r="E245" s="4">
         <v>43458</v>
       </c>
-      <c r="F245" s="10"/>
+      <c r="F245" s="10">
+        <v>43528</v>
+      </c>
     </row>
     <row r="246" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A246" s="3" t="s">
@@ -9675,7 +9741,9 @@
       <c r="A251" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="B251" s="4"/>
+      <c r="B251" s="4">
+        <v>43528</v>
+      </c>
       <c r="C251" s="4"/>
       <c r="D251" s="13"/>
       <c r="E251" s="4">
@@ -10250,8 +10318,12 @@
       <c r="B300" s="4">
         <v>43495</v>
       </c>
-      <c r="C300" s="4"/>
-      <c r="D300" s="13"/>
+      <c r="C300" s="4">
+        <v>43528</v>
+      </c>
+      <c r="D300" s="13">
+        <v>21.8</v>
+      </c>
       <c r="E300" s="4">
         <v>43458</v>
       </c>
@@ -10558,7 +10630,9 @@
       <c r="E325" s="11">
         <v>43486</v>
       </c>
-      <c r="F325" s="10"/>
+      <c r="F325" s="10">
+        <v>43528</v>
+      </c>
     </row>
     <row r="326" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A326" s="7" t="s">
@@ -10675,7 +10749,9 @@
       <c r="E335" s="11">
         <v>43486</v>
       </c>
-      <c r="F335" s="10"/>
+      <c r="F335" s="10">
+        <v>43528</v>
+      </c>
     </row>
     <row r="336" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A336" s="7" t="s">
@@ -11969,8 +12045,12 @@
       <c r="B391" s="4">
         <v>43512</v>
       </c>
-      <c r="C391" s="4"/>
-      <c r="D391" s="13"/>
+      <c r="C391" s="4">
+        <v>43528</v>
+      </c>
+      <c r="D391" s="13">
+        <v>48.6</v>
+      </c>
       <c r="E391" s="4">
         <v>43458</v>
       </c>
@@ -12076,8 +12156,12 @@
       <c r="B397" s="4">
         <v>43500</v>
       </c>
-      <c r="C397" s="4"/>
-      <c r="D397" s="13"/>
+      <c r="C397" s="4">
+        <v>43528</v>
+      </c>
+      <c r="D397" s="13">
+        <v>56.6</v>
+      </c>
       <c r="E397" s="4">
         <v>43458</v>
       </c>
@@ -12226,7 +12310,9 @@
       <c r="C405" s="6">
         <v>43518</v>
       </c>
-      <c r="D405" s="14"/>
+      <c r="D405" s="14">
+        <v>45.4</v>
+      </c>
       <c r="E405" s="6">
         <v>43472</v>
       </c>
@@ -12258,8 +12344,12 @@
       <c r="B407" s="6">
         <v>43518</v>
       </c>
-      <c r="C407" s="6"/>
-      <c r="D407" s="14"/>
+      <c r="C407" s="6">
+        <v>43528</v>
+      </c>
+      <c r="D407" s="14">
+        <v>58.3</v>
+      </c>
       <c r="E407" s="6">
         <v>43472</v>
       </c>
@@ -12469,13 +12559,17 @@
       <c r="A419" s="7" t="s">
         <v>420</v>
       </c>
-      <c r="B419" s="11"/>
+      <c r="B419" s="11">
+        <v>43528</v>
+      </c>
       <c r="C419" s="11"/>
       <c r="D419" s="15"/>
       <c r="E419" s="11">
         <v>43486</v>
       </c>
-      <c r="F419" s="10"/>
+      <c r="F419" s="10">
+        <v>43528</v>
+      </c>
     </row>
     <row r="420" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A420" s="7" t="s">
@@ -12497,8 +12591,12 @@
       <c r="B421" s="11">
         <v>43515</v>
       </c>
-      <c r="C421" s="11"/>
-      <c r="D421" s="15"/>
+      <c r="C421" s="11">
+        <v>43528</v>
+      </c>
+      <c r="D421" s="15">
+        <v>46.8</v>
+      </c>
       <c r="E421" s="11">
         <v>43486</v>
       </c>
@@ -12556,7 +12654,9 @@
       <c r="A425" s="7" t="s">
         <v>426</v>
       </c>
-      <c r="B425" s="11"/>
+      <c r="B425" s="11">
+        <v>43521</v>
+      </c>
       <c r="C425" s="11"/>
       <c r="D425" s="15"/>
       <c r="E425" s="11">
@@ -12583,13 +12683,17 @@
       <c r="A427" s="7" t="s">
         <v>428</v>
       </c>
-      <c r="B427" s="11"/>
+      <c r="B427" s="11">
+        <v>43528</v>
+      </c>
       <c r="C427" s="11"/>
       <c r="D427" s="15"/>
       <c r="E427" s="11">
         <v>43486</v>
       </c>
-      <c r="F427" s="10"/>
+      <c r="F427" s="10">
+        <v>43528</v>
+      </c>
     </row>
     <row r="428" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A428" s="7" t="s">
@@ -12598,8 +12702,12 @@
       <c r="B428" s="11">
         <v>43518</v>
       </c>
-      <c r="C428" s="11"/>
-      <c r="D428" s="15"/>
+      <c r="C428" s="11">
+        <v>43528</v>
+      </c>
+      <c r="D428" s="15">
+        <v>40.5</v>
+      </c>
       <c r="E428" s="11">
         <v>43486</v>
       </c>
@@ -12651,9 +12759,15 @@
       <c r="A432" s="7" t="s">
         <v>433</v>
       </c>
-      <c r="B432" s="11"/>
-      <c r="C432" s="11"/>
-      <c r="D432" s="15"/>
+      <c r="B432" s="11">
+        <v>43515</v>
+      </c>
+      <c r="C432" s="11">
+        <v>43528</v>
+      </c>
+      <c r="D432" s="15">
+        <v>42.9</v>
+      </c>
       <c r="E432" s="11">
         <v>43486</v>
       </c>
@@ -12773,7 +12887,9 @@
       <c r="B439" s="4">
         <v>43502</v>
       </c>
-      <c r="C439" s="4"/>
+      <c r="C439" s="4">
+        <v>43528</v>
+      </c>
       <c r="D439" s="13"/>
       <c r="E439" s="4">
         <v>43458</v>
@@ -12858,8 +12974,12 @@
       <c r="B444" s="4">
         <v>43497</v>
       </c>
-      <c r="C444" s="4"/>
-      <c r="D444" s="13"/>
+      <c r="C444" s="4">
+        <v>43528</v>
+      </c>
+      <c r="D444" s="13">
+        <v>22.2</v>
+      </c>
       <c r="E444" s="4">
         <v>43458</v>
       </c>
@@ -12871,8 +12991,12 @@
       <c r="B445" s="4">
         <v>43488</v>
       </c>
-      <c r="C445" s="4"/>
-      <c r="D445" s="13"/>
+      <c r="C445" s="4">
+        <v>43528</v>
+      </c>
+      <c r="D445" s="13">
+        <v>18</v>
+      </c>
       <c r="E445" s="4">
         <v>43458</v>
       </c>
@@ -12887,8 +13011,12 @@
       <c r="B446" s="4">
         <v>43512</v>
       </c>
-      <c r="C446" s="4"/>
-      <c r="D446" s="13"/>
+      <c r="C446" s="4">
+        <v>43528</v>
+      </c>
+      <c r="D446" s="13">
+        <v>27.6</v>
+      </c>
       <c r="E446" s="4">
         <v>43458</v>
       </c>
@@ -12930,7 +13058,7 @@
         <v>43458</v>
       </c>
     </row>
-    <row r="449" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="449" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A449" s="3" t="s">
         <v>450</v>
       </c>
@@ -12946,7 +13074,7 @@
         <v>43523</v>
       </c>
     </row>
-    <row r="450" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="450" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A450" s="5" t="s">
         <v>451</v>
       </c>
@@ -12963,7 +13091,7 @@
         <v>43472</v>
       </c>
     </row>
-    <row r="451" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="451" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A451" s="5" t="s">
         <v>452</v>
       </c>
@@ -12983,7 +13111,7 @@
         <v>43507</v>
       </c>
     </row>
-    <row r="452" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="452" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A452" s="5" t="s">
         <v>453</v>
       </c>
@@ -13000,7 +13128,7 @@
         <v>43472</v>
       </c>
     </row>
-    <row r="453" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="453" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A453" s="5" t="s">
         <v>454</v>
       </c>
@@ -13020,7 +13148,7 @@
         <v>43509</v>
       </c>
     </row>
-    <row r="454" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="454" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A454" s="5" t="s">
         <v>455</v>
       </c>
@@ -13037,7 +13165,7 @@
         <v>43472</v>
       </c>
     </row>
-    <row r="455" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="455" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A455" s="5" t="s">
         <v>456</v>
       </c>
@@ -13057,7 +13185,7 @@
         <v>43509</v>
       </c>
     </row>
-    <row r="456" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="456" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A456" s="5" t="s">
         <v>457</v>
       </c>
@@ -13074,7 +13202,7 @@
         <v>43472</v>
       </c>
     </row>
-    <row r="457" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="457" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A457" s="5" t="s">
         <v>458</v>
       </c>
@@ -13082,10 +13210,10 @@
         <v>43512</v>
       </c>
       <c r="C457" s="6">
-        <v>43515</v>
+        <v>43528</v>
       </c>
       <c r="D457" s="14">
-        <v>20.399999999999999</v>
+        <v>27</v>
       </c>
       <c r="E457" s="6">
         <v>43472</v>
@@ -13093,29 +13221,38 @@
       <c r="F457" s="10">
         <v>43515</v>
       </c>
-    </row>
-    <row r="458" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G457" s="1"/>
+    </row>
+    <row r="458" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A458" s="5" t="s">
         <v>459</v>
       </c>
       <c r="B458" s="6">
         <v>43500</v>
       </c>
-      <c r="C458" s="6"/>
-      <c r="D458" s="14"/>
+      <c r="C458" s="6">
+        <v>43515</v>
+      </c>
+      <c r="D458" s="14">
+        <v>20.399999999999999</v>
+      </c>
       <c r="E458" s="6">
         <v>43472</v>
       </c>
     </row>
-    <row r="459" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="459" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A459" s="5" t="s">
         <v>460</v>
       </c>
       <c r="B459" s="6">
         <v>43493</v>
       </c>
-      <c r="C459" s="6"/>
-      <c r="D459" s="14"/>
+      <c r="C459" s="6">
+        <v>43515</v>
+      </c>
+      <c r="D459" s="14">
+        <v>25.9</v>
+      </c>
       <c r="E459" s="6">
         <v>43472</v>
       </c>
@@ -13123,20 +13260,24 @@
         <v>43500</v>
       </c>
     </row>
-    <row r="460" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="460" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A460" s="5" t="s">
         <v>461</v>
       </c>
       <c r="B460" s="6">
         <v>43507</v>
       </c>
-      <c r="C460" s="6"/>
-      <c r="D460" s="14"/>
+      <c r="C460" s="6">
+        <v>43528</v>
+      </c>
+      <c r="D460" s="14">
+        <v>34.299999999999997</v>
+      </c>
       <c r="E460" s="6">
         <v>43472</v>
       </c>
     </row>
-    <row r="461" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="461" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A461" s="5" t="s">
         <v>462</v>
       </c>
@@ -13156,7 +13297,7 @@
         <v>43509</v>
       </c>
     </row>
-    <row r="462" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="462" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A462" s="5" t="s">
         <v>463</v>
       </c>
@@ -13173,7 +13314,7 @@
         <v>43472</v>
       </c>
     </row>
-    <row r="463" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="463" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A463" s="5" t="s">
         <v>464</v>
       </c>
@@ -13193,7 +13334,7 @@
         <v>43507</v>
       </c>
     </row>
-    <row r="464" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="464" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A464" s="5" t="s">
         <v>465</v>
       </c>
@@ -13217,8 +13358,12 @@
       <c r="B465" s="6">
         <v>43507</v>
       </c>
-      <c r="C465" s="6"/>
-      <c r="D465" s="14"/>
+      <c r="C465" s="6">
+        <v>43528</v>
+      </c>
+      <c r="D465" s="14">
+        <v>30.7</v>
+      </c>
       <c r="E465" s="6">
         <v>43472</v>
       </c>
@@ -13369,8 +13514,12 @@
       <c r="B474" s="11">
         <v>43515</v>
       </c>
-      <c r="C474" s="11"/>
-      <c r="D474" s="15"/>
+      <c r="C474" s="11">
+        <v>43528</v>
+      </c>
+      <c r="D474" s="15">
+        <v>23</v>
+      </c>
       <c r="E474" s="11">
         <v>43486</v>
       </c>
@@ -13382,8 +13531,12 @@
       <c r="B475" s="11">
         <v>43512</v>
       </c>
-      <c r="C475" s="11"/>
-      <c r="D475" s="15"/>
+      <c r="C475" s="11">
+        <v>43528</v>
+      </c>
+      <c r="D475" s="15">
+        <v>28.3</v>
+      </c>
       <c r="E475" s="11">
         <v>43486</v>
       </c>
@@ -13485,8 +13638,12 @@
       <c r="B481" s="11">
         <v>43509</v>
       </c>
-      <c r="C481" s="11"/>
-      <c r="D481" s="15"/>
+      <c r="C481" s="11">
+        <v>43528</v>
+      </c>
+      <c r="D481" s="15">
+        <v>29.1</v>
+      </c>
       <c r="E481" s="11">
         <v>43486</v>
       </c>

</xml_diff>

<commit_message>
updates to breakdown pre drought conditions
</commit_message>
<xml_diff>
--- a/data/observation_datasheet.xlsx
+++ b/data/observation_datasheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/catchamberlain/Documents/git/chillfreeze/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{988C57D9-9262-EA4E-A554-E132BDA4BE2F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{2220AB96-8819-2942-B12D-214AF01D4EFB}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10760" yWindow="3720" windowWidth="29720" windowHeight="20980" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10020" yWindow="2160" windowWidth="29720" windowHeight="20980" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="observation_datasheet" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="988" uniqueCount="499">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1051" uniqueCount="542">
   <si>
     <t>ID</t>
   </si>
@@ -1523,6 +1523,135 @@
   </si>
   <si>
     <t>BBCH</t>
+  </si>
+  <si>
+    <t>7= full leafout; 5 cont, 2 frz</t>
+  </si>
+  <si>
+    <t>15=budburst</t>
+  </si>
+  <si>
+    <t>5=budburst and frz</t>
+  </si>
+  <si>
+    <t>9=budburst; 5 cont, 4 frz</t>
+  </si>
+  <si>
+    <t>1= in growth chamber during heat</t>
+  </si>
+  <si>
+    <t>none bursted before heat</t>
+  </si>
+  <si>
+    <t>4 bursted day of; 1 cont, 3 frz</t>
+  </si>
+  <si>
+    <t>14 full leaf out before heat</t>
+  </si>
+  <si>
+    <t>1 budburst and frz</t>
+  </si>
+  <si>
+    <t>1 never going to burst</t>
+  </si>
+  <si>
+    <t>9 full leafed out</t>
+  </si>
+  <si>
+    <t>6 budburst; 1 cont and 5 tx; all tx frz</t>
+  </si>
+  <si>
+    <t>13 budburst; 6 cont, 7 tx</t>
+  </si>
+  <si>
+    <t>3 in growth chamber during</t>
+  </si>
+  <si>
+    <t>3 frz before, 1 after</t>
+  </si>
+  <si>
+    <t>all done before</t>
+  </si>
+  <si>
+    <t>8 fully leafed out</t>
+  </si>
+  <si>
+    <t>8 budburst; 5 tx, 3 cont</t>
+  </si>
+  <si>
+    <t>all frz before</t>
+  </si>
+  <si>
+    <t>all before</t>
+  </si>
+  <si>
+    <t>8 budburst; 3 cont, 5 tx</t>
+  </si>
+  <si>
+    <t>On or Before 2/19</t>
+  </si>
+  <si>
+    <t>8 budbursted; 5 tx, 3 cont</t>
+  </si>
+  <si>
+    <t>no budburst</t>
+  </si>
+  <si>
+    <t>1 full leafout</t>
+  </si>
+  <si>
+    <t>one in growth chamber during</t>
+  </si>
+  <si>
+    <t>2 frz before</t>
+  </si>
+  <si>
+    <t>6 budburst; 3 cont, 3 frz</t>
+  </si>
+  <si>
+    <t>10 full leaf out</t>
+  </si>
+  <si>
+    <t>1 no budburst</t>
+  </si>
+  <si>
+    <t>5 budburst; 1 cont, 4 frz</t>
+  </si>
+  <si>
+    <t>1 in growth chamber</t>
+  </si>
+  <si>
+    <t>12 budburst; 5 cont, 7 frz</t>
+  </si>
+  <si>
+    <t>2 in growth chamber</t>
+  </si>
+  <si>
+    <t>1 frz after</t>
+  </si>
+  <si>
+    <t>10 budburst after</t>
+  </si>
+  <si>
+    <t>all frz after</t>
+  </si>
+  <si>
+    <t>5 full leaf out</t>
+  </si>
+  <si>
+    <t>10 budburst; 6 cont, 4 frz</t>
+  </si>
+  <si>
+    <t>6 frz before, 1 after, 1 no bb</t>
+  </si>
+  <si>
+    <t>10 budburst; 7 frz, 3 cont</t>
+  </si>
+  <si>
+    <t>rest frz before</t>
+  </si>
+  <si>
+    <t>15 budburst; 8 frz, 7 cont</t>
   </si>
 </sst>
 </file>
@@ -5050,13 +5179,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:M481"/>
+  <dimension ref="A1:N481"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B432" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B444" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H464" sqref="H464"/>
+      <selection pane="bottomRight" activeCell="N469" sqref="N469"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5068,7 +5197,7 @@
     <col min="5" max="6" width="10.7109375" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>487</v>
       </c>
@@ -5105,8 +5234,11 @@
       <c r="M1" s="18" t="s">
         <v>497</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N1" s="18" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -5122,8 +5254,11 @@
       <c r="E2" s="4">
         <v>43458</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N2" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -5142,8 +5277,11 @@
       <c r="F3" s="10">
         <v>43511</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N3" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -5159,8 +5297,11 @@
       <c r="E4" s="4">
         <v>43458</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N4" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
@@ -5180,7 +5321,7 @@
         <v>43511</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -5197,7 +5338,7 @@
         <v>43458</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
@@ -5217,7 +5358,7 @@
         <v>43521</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
@@ -5234,7 +5375,7 @@
         <v>43458</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>10</v>
       </c>
@@ -5254,7 +5395,7 @@
         <v>43511</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>11</v>
       </c>
@@ -5271,7 +5412,7 @@
         <v>43458</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>12</v>
       </c>
@@ -5294,7 +5435,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>13</v>
       </c>
@@ -5307,7 +5448,7 @@
         <v>43458</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>14</v>
       </c>
@@ -5327,7 +5468,7 @@
         <v>43504</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>15</v>
       </c>
@@ -5344,7 +5485,7 @@
         <v>43458</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>16</v>
       </c>
@@ -5364,7 +5505,7 @@
         <v>43502</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>17</v>
       </c>
@@ -5381,7 +5522,7 @@
         <v>43458</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>18</v>
       </c>
@@ -5401,7 +5542,7 @@
         <v>43509</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>19</v>
       </c>
@@ -5415,8 +5556,11 @@
       <c r="E18" s="6">
         <v>43472</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="N18" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>20</v>
       </c>
@@ -5429,8 +5573,11 @@
         <v>43472</v>
       </c>
       <c r="F19" s="10"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="N19" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
         <v>21</v>
       </c>
@@ -5447,7 +5594,7 @@
         <v>43472</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
         <v>22</v>
       </c>
@@ -5467,7 +5614,7 @@
         <v>43518</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
         <v>23</v>
       </c>
@@ -5484,7 +5631,7 @@
         <v>43472</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
         <v>24</v>
       </c>
@@ -5504,7 +5651,7 @@
         <v>43518</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
         <v>25</v>
       </c>
@@ -5521,7 +5668,7 @@
         <v>43472</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
         <v>26</v>
       </c>
@@ -5537,7 +5684,7 @@
         <v>43528</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
         <v>27</v>
       </c>
@@ -5550,7 +5697,7 @@
         <v>43472</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
         <v>28</v>
       </c>
@@ -5570,7 +5717,7 @@
         <v>43518</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
         <v>29</v>
       </c>
@@ -5587,7 +5734,7 @@
         <v>43472</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
         <v>30</v>
       </c>
@@ -5603,7 +5750,7 @@
         <v>43528</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
         <v>31</v>
       </c>
@@ -5614,7 +5761,7 @@
         <v>43472</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
         <v>32</v>
       </c>
@@ -5634,7 +5781,7 @@
         <v>43521</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
         <v>33</v>
       </c>
@@ -5651,7 +5798,7 @@
         <v>43472</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
         <v>34</v>
       </c>
@@ -5671,7 +5818,7 @@
         <v>43515</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" s="7" t="s">
         <v>35</v>
       </c>
@@ -5683,8 +5830,11 @@
       <c r="E34" s="11">
         <v>43486</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="N34" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" s="7" t="s">
         <v>36</v>
       </c>
@@ -5699,8 +5849,11 @@
       <c r="F35" s="10">
         <v>43528</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="N35" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" s="7" t="s">
         <v>37</v>
       </c>
@@ -5717,7 +5870,7 @@
         <v>43486</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" s="7" t="s">
         <v>38</v>
       </c>
@@ -5733,7 +5886,7 @@
         <v>43528</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" s="7" t="s">
         <v>39</v>
       </c>
@@ -5744,7 +5897,7 @@
         <v>43486</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" s="7" t="s">
         <v>40</v>
       </c>
@@ -5760,7 +5913,7 @@
         <v>43521</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="s">
         <v>41</v>
       </c>
@@ -5771,7 +5924,7 @@
         <v>43486</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" s="7" t="s">
         <v>42</v>
       </c>
@@ -5787,7 +5940,7 @@
         <v>43523</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42" s="7" t="s">
         <v>43</v>
       </c>
@@ -5798,7 +5951,7 @@
         <v>43486</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" s="7" t="s">
         <v>44</v>
       </c>
@@ -5814,7 +5967,7 @@
         <v>43528</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44" s="7" t="s">
         <v>45</v>
       </c>
@@ -5827,7 +5980,7 @@
         <v>43486</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45" s="7" t="s">
         <v>46</v>
       </c>
@@ -5841,7 +5994,7 @@
       </c>
       <c r="F45" s="10"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A46" s="7" t="s">
         <v>47</v>
       </c>
@@ -5858,7 +6011,7 @@
         <v>43486</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47" s="7" t="s">
         <v>48</v>
       </c>
@@ -5874,7 +6027,7 @@
         <v>43523</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48" s="7" t="s">
         <v>49</v>
       </c>
@@ -5887,7 +6040,7 @@
         <v>43486</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A49" s="7" t="s">
         <v>50</v>
       </c>
@@ -5901,7 +6054,7 @@
       </c>
       <c r="F49" s="10"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>51</v>
       </c>
@@ -5917,8 +6070,11 @@
       <c r="E50" s="4">
         <v>43458</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="N50" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>52</v>
       </c>
@@ -5937,8 +6093,11 @@
       <c r="F51" s="10">
         <v>43493</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="N51" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
         <v>53</v>
       </c>
@@ -5954,8 +6113,11 @@
       <c r="E52" s="4">
         <v>43458</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="N52" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
         <v>54</v>
       </c>
@@ -5975,7 +6137,7 @@
         <v>43488</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
         <v>55</v>
       </c>
@@ -5992,7 +6154,7 @@
         <v>43458</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
         <v>56</v>
       </c>
@@ -6012,7 +6174,7 @@
         <v>43490</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
         <v>57</v>
       </c>
@@ -6029,7 +6191,7 @@
         <v>43458</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
         <v>58</v>
       </c>
@@ -6049,7 +6211,7 @@
         <v>43493</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
         <v>59</v>
       </c>
@@ -6066,7 +6228,7 @@
         <v>43458</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
         <v>60</v>
       </c>
@@ -6086,7 +6248,7 @@
         <v>43504</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
         <v>61</v>
       </c>
@@ -6103,7 +6265,7 @@
         <v>43458</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
         <v>62</v>
       </c>
@@ -6115,7 +6277,7 @@
       </c>
       <c r="F61" s="10"/>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
         <v>63</v>
       </c>
@@ -6132,7 +6294,7 @@
         <v>43458</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
         <v>64</v>
       </c>
@@ -6152,7 +6314,7 @@
         <v>43488</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
         <v>65</v>
       </c>
@@ -6169,7 +6331,7 @@
         <v>43458</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
         <v>66</v>
       </c>
@@ -6189,7 +6351,7 @@
         <v>43479</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A66" s="5" t="s">
         <v>67</v>
       </c>
@@ -6205,8 +6367,11 @@
       <c r="E66" s="6">
         <v>43472</v>
       </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="N66" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A67" s="5" t="s">
         <v>68</v>
       </c>
@@ -6225,8 +6390,11 @@
       <c r="F67" s="10">
         <v>43507</v>
       </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="N67" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A68" s="5" t="s">
         <v>69</v>
       </c>
@@ -6243,7 +6411,7 @@
         <v>43472</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A69" s="5" t="s">
         <v>70</v>
       </c>
@@ -6263,7 +6431,7 @@
         <v>43504</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A70" s="5" t="s">
         <v>71</v>
       </c>
@@ -6280,7 +6448,7 @@
         <v>43472</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A71" s="5" t="s">
         <v>72</v>
       </c>
@@ -6300,7 +6468,7 @@
         <v>43497</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A72" s="5" t="s">
         <v>73</v>
       </c>
@@ -6311,7 +6479,7 @@
         <v>43472</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A73" s="5" t="s">
         <v>74</v>
       </c>
@@ -6331,7 +6499,7 @@
         <v>43502</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A74" s="5" t="s">
         <v>75</v>
       </c>
@@ -6348,7 +6516,7 @@
         <v>43472</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A75" s="5" t="s">
         <v>76</v>
       </c>
@@ -6364,7 +6532,7 @@
         <v>43518</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A76" s="5" t="s">
         <v>77</v>
       </c>
@@ -6381,7 +6549,7 @@
         <v>43472</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A77" s="5" t="s">
         <v>78</v>
       </c>
@@ -6404,7 +6572,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A78" s="5" t="s">
         <v>79</v>
       </c>
@@ -6421,7 +6589,7 @@
         <v>43472</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A79" s="5" t="s">
         <v>80</v>
       </c>
@@ -6441,7 +6609,7 @@
         <v>43500</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A80" s="5" t="s">
         <v>81</v>
       </c>
@@ -6458,7 +6626,7 @@
         <v>43472</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A81" s="5" t="s">
         <v>82</v>
       </c>
@@ -6478,7 +6646,7 @@
         <v>43500</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A82" s="7" t="s">
         <v>83</v>
       </c>
@@ -6488,8 +6656,11 @@
       <c r="E82" s="11">
         <v>43486</v>
       </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="N82" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="83" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A83" s="7" t="s">
         <v>84</v>
       </c>
@@ -6508,8 +6679,11 @@
       <c r="F83" s="10">
         <v>43511</v>
       </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="N83" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="84" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A84" s="7" t="s">
         <v>85</v>
       </c>
@@ -6525,8 +6699,11 @@
       <c r="E84" s="11">
         <v>43486</v>
       </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="N84" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="85" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A85" s="7" t="s">
         <v>86</v>
       </c>
@@ -6542,7 +6719,7 @@
         <v>43509</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A86" s="7" t="s">
         <v>87</v>
       </c>
@@ -6559,7 +6736,7 @@
         <v>43486</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A87" s="7" t="s">
         <v>88</v>
       </c>
@@ -6571,7 +6748,7 @@
       </c>
       <c r="F87" s="10"/>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A88" s="7" t="s">
         <v>89</v>
       </c>
@@ -6582,7 +6759,7 @@
         <v>43486</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A89" s="7" t="s">
         <v>90</v>
       </c>
@@ -6602,7 +6779,7 @@
         <v>43518</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A90" s="7" t="s">
         <v>91</v>
       </c>
@@ -6619,7 +6796,7 @@
         <v>43486</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A91" s="7" t="s">
         <v>92</v>
       </c>
@@ -6639,7 +6816,7 @@
         <v>43511</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A92" s="7" t="s">
         <v>93</v>
       </c>
@@ -6656,7 +6833,7 @@
         <v>43486</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A93" s="7" t="s">
         <v>94</v>
       </c>
@@ -6676,7 +6853,7 @@
         <v>43515</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A94" s="7" t="s">
         <v>95</v>
       </c>
@@ -6693,7 +6870,7 @@
         <v>43486</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A95" s="7" t="s">
         <v>96</v>
       </c>
@@ -6713,7 +6890,7 @@
         <v>43515</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A96" s="7" t="s">
         <v>97</v>
       </c>
@@ -6730,7 +6907,7 @@
         <v>43486</v>
       </c>
     </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A97" s="7" t="s">
         <v>98</v>
       </c>
@@ -6750,7 +6927,7 @@
         <v>43515</v>
       </c>
     </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A98" s="3" t="s">
         <v>99</v>
       </c>
@@ -6766,8 +6943,11 @@
       <c r="E98" s="4">
         <v>43458</v>
       </c>
-    </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N98" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="99" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A99" s="3" t="s">
         <v>100</v>
       </c>
@@ -6787,7 +6967,7 @@
         <v>43476</v>
       </c>
     </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A100" s="3" t="s">
         <v>101</v>
       </c>
@@ -6823,7 +7003,7 @@
         <v>30.5</v>
       </c>
     </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A101" s="3" t="s">
         <v>102</v>
       </c>
@@ -6843,7 +7023,7 @@
         <v>43473</v>
       </c>
     </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A102" s="3" t="s">
         <v>103</v>
       </c>
@@ -6879,7 +7059,7 @@
         <v>35.375</v>
       </c>
     </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A103" s="3" t="s">
         <v>104</v>
       </c>
@@ -6899,7 +7079,7 @@
         <v>43476</v>
       </c>
     </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A104" s="3" t="s">
         <v>105</v>
       </c>
@@ -6935,7 +7115,7 @@
         <v>37.1</v>
       </c>
     </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A105" s="3" t="s">
         <v>106</v>
       </c>
@@ -6974,7 +7154,7 @@
         <v>33.475000000000001</v>
       </c>
     </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A106" s="3" t="s">
         <v>107</v>
       </c>
@@ -6991,7 +7171,7 @@
         <v>43458</v>
       </c>
     </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A107" s="3" t="s">
         <v>108</v>
       </c>
@@ -7011,7 +7191,7 @@
         <v>43476</v>
       </c>
     </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A108" s="3" t="s">
         <v>109</v>
       </c>
@@ -7047,7 +7227,7 @@
         <v>38.375</v>
       </c>
     </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A109" s="3" t="s">
         <v>110</v>
       </c>
@@ -7067,7 +7247,7 @@
         <v>43488</v>
       </c>
     </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A110" s="3" t="s">
         <v>111</v>
       </c>
@@ -7084,7 +7264,7 @@
         <v>43458</v>
       </c>
     </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A111" s="3" t="s">
         <v>112</v>
       </c>
@@ -7104,7 +7284,7 @@
         <v>43473</v>
       </c>
     </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A112" s="3" t="s">
         <v>113</v>
       </c>
@@ -7121,7 +7301,7 @@
         <v>43458</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A113" s="3" t="s">
         <v>114</v>
       </c>
@@ -7144,7 +7324,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A114" s="5" t="s">
         <v>115</v>
       </c>
@@ -7160,8 +7340,11 @@
       <c r="E114" s="6">
         <v>43472</v>
       </c>
-    </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="N114" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="115" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A115" s="5" t="s">
         <v>116</v>
       </c>
@@ -7181,7 +7364,7 @@
         <v>43493</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A116" s="5" t="s">
         <v>117</v>
       </c>
@@ -7198,7 +7381,7 @@
         <v>43472</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A117" s="5" t="s">
         <v>118</v>
       </c>
@@ -7218,7 +7401,7 @@
         <v>43500</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A118" s="5" t="s">
         <v>119</v>
       </c>
@@ -7235,7 +7418,7 @@
         <v>43472</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A119" s="5" t="s">
         <v>120</v>
       </c>
@@ -7258,7 +7441,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A120" s="5" t="s">
         <v>121</v>
       </c>
@@ -7275,7 +7458,7 @@
         <v>43472</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A121" s="5" t="s">
         <v>122</v>
       </c>
@@ -7295,7 +7478,7 @@
         <v>43497</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A122" s="5" t="s">
         <v>123</v>
       </c>
@@ -7312,7 +7495,7 @@
         <v>43472</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A123" s="5" t="s">
         <v>124</v>
       </c>
@@ -7335,7 +7518,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A124" s="5" t="s">
         <v>125</v>
       </c>
@@ -7352,7 +7535,7 @@
         <v>43472</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A125" s="5" t="s">
         <v>126</v>
       </c>
@@ -7372,7 +7555,7 @@
         <v>43490</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A126" s="5" t="s">
         <v>127</v>
       </c>
@@ -7389,7 +7572,7 @@
         <v>43472</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A127" s="5" t="s">
         <v>128</v>
       </c>
@@ -7409,7 +7592,7 @@
         <v>43500</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A128" s="5" t="s">
         <v>129</v>
       </c>
@@ -7426,7 +7609,7 @@
         <v>43472</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A129" s="5" t="s">
         <v>130</v>
       </c>
@@ -7446,7 +7629,7 @@
         <v>43490</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A130" s="7" t="s">
         <v>131</v>
       </c>
@@ -7462,8 +7645,11 @@
       <c r="E130" s="11">
         <v>43486</v>
       </c>
-    </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="N130" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="131" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A131" s="7" t="s">
         <v>132</v>
       </c>
@@ -7482,8 +7668,11 @@
       <c r="F131" s="10">
         <v>43504</v>
       </c>
-    </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="N131" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="132" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A132" s="7" t="s">
         <v>133</v>
       </c>
@@ -7499,8 +7688,11 @@
       <c r="E132" s="11">
         <v>43486</v>
       </c>
-    </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="N132" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="133" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A133" s="7" t="s">
         <v>134</v>
       </c>
@@ -7520,7 +7712,7 @@
         <v>43507</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A134" s="7" t="s">
         <v>135</v>
       </c>
@@ -7537,7 +7729,7 @@
         <v>43486</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A135" s="7" t="s">
         <v>136</v>
       </c>
@@ -7557,7 +7749,7 @@
         <v>43511</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A136" s="7" t="s">
         <v>137</v>
       </c>
@@ -7574,7 +7766,7 @@
         <v>43486</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A137" s="7" t="s">
         <v>138</v>
       </c>
@@ -7594,7 +7786,7 @@
         <v>43500</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A138" s="7" t="s">
         <v>139</v>
       </c>
@@ -7611,7 +7803,7 @@
         <v>43486</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A139" s="7" t="s">
         <v>140</v>
       </c>
@@ -7631,7 +7823,7 @@
         <v>43507</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A140" s="7" t="s">
         <v>141</v>
       </c>
@@ -7648,7 +7840,7 @@
         <v>43486</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A141" s="7" t="s">
         <v>142</v>
       </c>
@@ -7668,7 +7860,7 @@
         <v>43500</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A142" s="7" t="s">
         <v>143</v>
       </c>
@@ -7685,7 +7877,7 @@
         <v>43486</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A143" s="7" t="s">
         <v>144</v>
       </c>
@@ -7701,7 +7893,7 @@
         <v>43504</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A144" s="7" t="s">
         <v>145</v>
       </c>
@@ -7718,7 +7910,7 @@
         <v>43486</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A145" s="7" t="s">
         <v>146</v>
       </c>
@@ -7738,7 +7930,7 @@
         <v>43507</v>
       </c>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A146" s="3" t="s">
         <v>147</v>
       </c>
@@ -7754,8 +7946,11 @@
       <c r="E146" s="4">
         <v>43458</v>
       </c>
-    </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="N146" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="147" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A147" s="3" t="s">
         <v>148</v>
       </c>
@@ -7775,7 +7970,7 @@
         <v>43488</v>
       </c>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A148" s="3" t="s">
         <v>149</v>
       </c>
@@ -7792,7 +7987,7 @@
         <v>43458</v>
       </c>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A149" s="3" t="s">
         <v>150</v>
       </c>
@@ -7815,7 +8010,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A150" s="3" t="s">
         <v>151</v>
       </c>
@@ -7832,7 +8027,7 @@
         <v>43458</v>
       </c>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A151" s="3" t="s">
         <v>152</v>
       </c>
@@ -7852,7 +8047,7 @@
         <v>43483</v>
       </c>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A152" s="3" t="s">
         <v>153</v>
       </c>
@@ -7869,7 +8064,7 @@
         <v>43458</v>
       </c>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A153" s="3" t="s">
         <v>154</v>
       </c>
@@ -7889,7 +8084,7 @@
         <v>43490</v>
       </c>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A154" s="3" t="s">
         <v>155</v>
       </c>
@@ -7906,7 +8101,7 @@
         <v>43458</v>
       </c>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A155" s="3" t="s">
         <v>156</v>
       </c>
@@ -7926,7 +8121,7 @@
         <v>43488</v>
       </c>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A156" s="3" t="s">
         <v>157</v>
       </c>
@@ -7943,7 +8138,7 @@
         <v>43458</v>
       </c>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A157" s="3" t="s">
         <v>158</v>
       </c>
@@ -7963,7 +8158,7 @@
         <v>43488</v>
       </c>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A158" s="3" t="s">
         <v>159</v>
       </c>
@@ -7980,7 +8175,7 @@
         <v>43458</v>
       </c>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A159" s="3" t="s">
         <v>160</v>
       </c>
@@ -8000,7 +8195,7 @@
         <v>43483</v>
       </c>
     </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A160" s="3" t="s">
         <v>161</v>
       </c>
@@ -8017,7 +8212,7 @@
         <v>43458</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A161" s="3" t="s">
         <v>162</v>
       </c>
@@ -8037,7 +8232,7 @@
         <v>43490</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A162" s="5" t="s">
         <v>163</v>
       </c>
@@ -8053,8 +8248,11 @@
       <c r="E162" s="6">
         <v>43472</v>
       </c>
-    </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="N162" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="163" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A163" s="5" t="s">
         <v>164</v>
       </c>
@@ -8074,7 +8272,7 @@
         <v>43500</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A164" s="5" t="s">
         <v>165</v>
       </c>
@@ -8091,7 +8289,7 @@
         <v>43472</v>
       </c>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A165" s="5" t="s">
         <v>166</v>
       </c>
@@ -8111,7 +8309,7 @@
         <v>43500</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A166" s="5" t="s">
         <v>167</v>
       </c>
@@ -8128,7 +8326,7 @@
         <v>43472</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A167" s="5" t="s">
         <v>168</v>
       </c>
@@ -8148,7 +8346,7 @@
         <v>43500</v>
       </c>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A168" s="5" t="s">
         <v>169</v>
       </c>
@@ -8165,7 +8363,7 @@
         <v>43472</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A169" s="5" t="s">
         <v>170</v>
       </c>
@@ -8185,7 +8383,7 @@
         <v>43493</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A170" s="5" t="s">
         <v>171</v>
       </c>
@@ -8202,7 +8400,7 @@
         <v>43472</v>
       </c>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A171" s="5" t="s">
         <v>172</v>
       </c>
@@ -8222,7 +8420,7 @@
         <v>43497</v>
       </c>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A172" s="5" t="s">
         <v>173</v>
       </c>
@@ -8239,7 +8437,7 @@
         <v>43472</v>
       </c>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A173" s="5" t="s">
         <v>174</v>
       </c>
@@ -8259,7 +8457,7 @@
         <v>43502</v>
       </c>
     </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A174" s="5" t="s">
         <v>175</v>
       </c>
@@ -8276,7 +8474,7 @@
         <v>43472</v>
       </c>
     </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A175" s="5" t="s">
         <v>176</v>
       </c>
@@ -8296,7 +8494,7 @@
         <v>43497</v>
       </c>
     </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A176" s="5" t="s">
         <v>177</v>
       </c>
@@ -8313,7 +8511,7 @@
         <v>43472</v>
       </c>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A177" s="5" t="s">
         <v>178</v>
       </c>
@@ -8333,7 +8531,7 @@
         <v>43500</v>
       </c>
     </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A178" s="7" t="s">
         <v>179</v>
       </c>
@@ -8349,8 +8547,11 @@
       <c r="E178" s="11">
         <v>43486</v>
       </c>
-    </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="N178" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="179" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A179" s="7" t="s">
         <v>180</v>
       </c>
@@ -8369,8 +8570,11 @@
       <c r="F179" s="10">
         <v>43507</v>
       </c>
-    </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="N179" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="180" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A180" s="7" t="s">
         <v>181</v>
       </c>
@@ -8387,7 +8591,7 @@
         <v>43486</v>
       </c>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A181" s="7" t="s">
         <v>182</v>
       </c>
@@ -8407,7 +8611,7 @@
         <v>43509</v>
       </c>
     </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A182" s="7" t="s">
         <v>183</v>
       </c>
@@ -8424,7 +8628,7 @@
         <v>43486</v>
       </c>
     </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A183" s="7" t="s">
         <v>184</v>
       </c>
@@ -8444,7 +8648,7 @@
         <v>43509</v>
       </c>
     </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A184" s="7" t="s">
         <v>185</v>
       </c>
@@ -8461,7 +8665,7 @@
         <v>43486</v>
       </c>
     </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A185" s="7" t="s">
         <v>186</v>
       </c>
@@ -8481,7 +8685,7 @@
         <v>43504</v>
       </c>
     </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A186" s="7" t="s">
         <v>187</v>
       </c>
@@ -8498,7 +8702,7 @@
         <v>43486</v>
       </c>
     </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A187" s="7" t="s">
         <v>188</v>
       </c>
@@ -8518,7 +8722,7 @@
         <v>43507</v>
       </c>
     </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A188" s="7" t="s">
         <v>189</v>
       </c>
@@ -8535,7 +8739,7 @@
         <v>43486</v>
       </c>
     </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A189" s="7" t="s">
         <v>190</v>
       </c>
@@ -8555,7 +8759,7 @@
         <v>43507</v>
       </c>
     </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A190" s="7" t="s">
         <v>191</v>
       </c>
@@ -8572,7 +8776,7 @@
         <v>43486</v>
       </c>
     </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A191" s="7" t="s">
         <v>192</v>
       </c>
@@ -8592,7 +8796,7 @@
         <v>43507</v>
       </c>
     </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A192" s="7" t="s">
         <v>193</v>
       </c>
@@ -8609,7 +8813,7 @@
         <v>43486</v>
       </c>
     </row>
-    <row r="193" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A193" s="7" t="s">
         <v>194</v>
       </c>
@@ -8629,7 +8833,7 @@
         <v>43507</v>
       </c>
     </row>
-    <row r="194" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A194" s="3" t="s">
         <v>195</v>
       </c>
@@ -8664,8 +8868,11 @@
         <f>AVERAGE(I194:L194)</f>
         <v>33.75</v>
       </c>
-    </row>
-    <row r="195" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N194" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="195" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A195" s="3" t="s">
         <v>196</v>
       </c>
@@ -8685,7 +8892,7 @@
         <v>43479</v>
       </c>
     </row>
-    <row r="196" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A196" s="3" t="s">
         <v>197</v>
       </c>
@@ -8702,7 +8909,7 @@
         <v>43458</v>
       </c>
     </row>
-    <row r="197" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A197" s="3" t="s">
         <v>198</v>
       </c>
@@ -8722,7 +8929,7 @@
         <v>43493</v>
       </c>
     </row>
-    <row r="198" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A198" s="3" t="s">
         <v>199</v>
       </c>
@@ -8758,7 +8965,7 @@
         <v>34.375</v>
       </c>
     </row>
-    <row r="199" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A199" s="3" t="s">
         <v>200</v>
       </c>
@@ -8778,7 +8985,7 @@
         <v>43488</v>
       </c>
     </row>
-    <row r="200" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A200" s="3" t="s">
         <v>201</v>
       </c>
@@ -8795,7 +9002,7 @@
         <v>43458</v>
       </c>
     </row>
-    <row r="201" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A201" s="3" t="s">
         <v>202</v>
       </c>
@@ -8815,7 +9022,7 @@
         <v>43493</v>
       </c>
     </row>
-    <row r="202" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A202" s="3" t="s">
         <v>203</v>
       </c>
@@ -8832,7 +9039,7 @@
         <v>43458</v>
       </c>
     </row>
-    <row r="203" spans="1:13" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A203" s="3" t="s">
         <v>204</v>
       </c>
@@ -8852,7 +9059,7 @@
         <v>43488</v>
       </c>
     </row>
-    <row r="204" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A204" s="3" t="s">
         <v>205</v>
       </c>
@@ -8869,7 +9076,7 @@
         <v>43458</v>
       </c>
     </row>
-    <row r="205" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A205" s="3" t="s">
         <v>206</v>
       </c>
@@ -8908,7 +9115,7 @@
         <v>32.799999999999997</v>
       </c>
     </row>
-    <row r="206" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A206" s="3" t="s">
         <v>207</v>
       </c>
@@ -8944,7 +9151,7 @@
         <v>28.674999999999997</v>
       </c>
     </row>
-    <row r="207" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A207" s="3" t="s">
         <v>208</v>
       </c>
@@ -8967,7 +9174,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="208" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A208" s="3" t="s">
         <v>209</v>
       </c>
@@ -9003,7 +9210,7 @@
         <v>27.574999999999999</v>
       </c>
     </row>
-    <row r="209" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A209" s="3" t="s">
         <v>210</v>
       </c>
@@ -9023,7 +9230,7 @@
         <v>43473</v>
       </c>
     </row>
-    <row r="210" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A210" s="5" t="s">
         <v>211</v>
       </c>
@@ -9039,8 +9246,11 @@
       <c r="E210" s="6">
         <v>43472</v>
       </c>
-    </row>
-    <row r="211" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="N210" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="211" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A211" s="5" t="s">
         <v>212</v>
       </c>
@@ -9060,7 +9270,7 @@
         <v>43502</v>
       </c>
     </row>
-    <row r="212" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A212" s="5" t="s">
         <v>213</v>
       </c>
@@ -9077,7 +9287,7 @@
         <v>43472</v>
       </c>
     </row>
-    <row r="213" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A213" s="5" t="s">
         <v>214</v>
       </c>
@@ -9100,7 +9310,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="214" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A214" s="5" t="s">
         <v>215</v>
       </c>
@@ -9117,7 +9327,7 @@
         <v>43472</v>
       </c>
     </row>
-    <row r="215" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A215" s="5" t="s">
         <v>216</v>
       </c>
@@ -9137,7 +9347,7 @@
         <v>43493</v>
       </c>
     </row>
-    <row r="216" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A216" s="5" t="s">
         <v>217</v>
       </c>
@@ -9154,7 +9364,7 @@
         <v>43472</v>
       </c>
     </row>
-    <row r="217" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A217" s="5" t="s">
         <v>218</v>
       </c>
@@ -9174,7 +9384,7 @@
         <v>43497</v>
       </c>
     </row>
-    <row r="218" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A218" s="5" t="s">
         <v>219</v>
       </c>
@@ -9191,7 +9401,7 @@
         <v>43472</v>
       </c>
     </row>
-    <row r="219" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A219" s="5" t="s">
         <v>220</v>
       </c>
@@ -9211,7 +9421,7 @@
         <v>43500</v>
       </c>
     </row>
-    <row r="220" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A220" s="5" t="s">
         <v>221</v>
       </c>
@@ -9228,7 +9438,7 @@
         <v>43472</v>
       </c>
     </row>
-    <row r="221" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A221" s="5" t="s">
         <v>222</v>
       </c>
@@ -9248,7 +9458,7 @@
         <v>43490</v>
       </c>
     </row>
-    <row r="222" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A222" s="5" t="s">
         <v>223</v>
       </c>
@@ -9265,7 +9475,7 @@
         <v>43472</v>
       </c>
     </row>
-    <row r="223" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A223" s="5" t="s">
         <v>224</v>
       </c>
@@ -9285,7 +9495,7 @@
         <v>43490</v>
       </c>
     </row>
-    <row r="224" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A224" s="5" t="s">
         <v>225</v>
       </c>
@@ -9302,7 +9512,7 @@
         <v>43472</v>
       </c>
     </row>
-    <row r="225" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A225" s="5" t="s">
         <v>226</v>
       </c>
@@ -9322,7 +9532,7 @@
         <v>43490</v>
       </c>
     </row>
-    <row r="226" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A226" s="7" t="s">
         <v>227</v>
       </c>
@@ -9338,8 +9548,11 @@
       <c r="E226" s="11">
         <v>43486</v>
       </c>
-    </row>
-    <row r="227" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="N226" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="227" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A227" s="7" t="s">
         <v>228</v>
       </c>
@@ -9358,8 +9571,11 @@
       <c r="F227" s="10">
         <v>43504</v>
       </c>
-    </row>
-    <row r="228" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="N227" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="228" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A228" s="7" t="s">
         <v>229</v>
       </c>
@@ -9376,7 +9592,7 @@
         <v>43486</v>
       </c>
     </row>
-    <row r="229" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A229" s="7" t="s">
         <v>230</v>
       </c>
@@ -9396,7 +9612,7 @@
         <v>43511</v>
       </c>
     </row>
-    <row r="230" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A230" s="7" t="s">
         <v>231</v>
       </c>
@@ -9413,7 +9629,7 @@
         <v>43486</v>
       </c>
     </row>
-    <row r="231" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A231" s="7" t="s">
         <v>232</v>
       </c>
@@ -9433,7 +9649,7 @@
         <v>43502</v>
       </c>
     </row>
-    <row r="232" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A232" s="7" t="s">
         <v>233</v>
       </c>
@@ -9450,7 +9666,7 @@
         <v>43486</v>
       </c>
     </row>
-    <row r="233" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A233" s="7" t="s">
         <v>234</v>
       </c>
@@ -9470,7 +9686,7 @@
         <v>43507</v>
       </c>
     </row>
-    <row r="234" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A234" s="7" t="s">
         <v>235</v>
       </c>
@@ -9487,7 +9703,7 @@
         <v>43486</v>
       </c>
     </row>
-    <row r="235" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A235" s="7" t="s">
         <v>236</v>
       </c>
@@ -9507,7 +9723,7 @@
         <v>43500</v>
       </c>
     </row>
-    <row r="236" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A236" s="7" t="s">
         <v>237</v>
       </c>
@@ -9524,7 +9740,7 @@
         <v>43486</v>
       </c>
     </row>
-    <row r="237" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A237" s="7" t="s">
         <v>238</v>
       </c>
@@ -9547,7 +9763,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="238" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A238" s="7" t="s">
         <v>239</v>
       </c>
@@ -9564,7 +9780,7 @@
         <v>43486</v>
       </c>
     </row>
-    <row r="239" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A239" s="7" t="s">
         <v>240</v>
       </c>
@@ -9584,7 +9800,7 @@
         <v>43507</v>
       </c>
     </row>
-    <row r="240" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A240" s="7" t="s">
         <v>241</v>
       </c>
@@ -9601,7 +9817,7 @@
         <v>43486</v>
       </c>
     </row>
-    <row r="241" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A241" s="7" t="s">
         <v>242</v>
       </c>
@@ -9624,7 +9840,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="242" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A242" s="3" t="s">
         <v>243</v>
       </c>
@@ -9634,8 +9850,11 @@
       <c r="E242" s="4">
         <v>43458</v>
       </c>
-    </row>
-    <row r="243" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="N242" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="243" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A243" s="3" t="s">
         <v>244</v>
       </c>
@@ -9651,7 +9870,7 @@
         <v>43528</v>
       </c>
     </row>
-    <row r="244" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A244" s="3" t="s">
         <v>245</v>
       </c>
@@ -9664,7 +9883,7 @@
         <v>43458</v>
       </c>
     </row>
-    <row r="245" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A245" s="3" t="s">
         <v>246</v>
       </c>
@@ -9680,7 +9899,7 @@
         <v>43528</v>
       </c>
     </row>
-    <row r="246" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A246" s="3" t="s">
         <v>247</v>
       </c>
@@ -9691,7 +9910,7 @@
         <v>43458</v>
       </c>
     </row>
-    <row r="247" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A247" s="3" t="s">
         <v>248</v>
       </c>
@@ -9703,7 +9922,7 @@
       </c>
       <c r="F247" s="10"/>
     </row>
-    <row r="248" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A248" s="3" t="s">
         <v>249</v>
       </c>
@@ -9714,7 +9933,7 @@
         <v>43458</v>
       </c>
     </row>
-    <row r="249" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A249" s="3" t="s">
         <v>250</v>
       </c>
@@ -9726,7 +9945,7 @@
       </c>
       <c r="F249" s="10"/>
     </row>
-    <row r="250" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A250" s="3" t="s">
         <v>251</v>
       </c>
@@ -9737,7 +9956,7 @@
         <v>43458</v>
       </c>
     </row>
-    <row r="251" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A251" s="3" t="s">
         <v>252</v>
       </c>
@@ -9751,7 +9970,7 @@
       </c>
       <c r="F251" s="10"/>
     </row>
-    <row r="252" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A252" s="3" t="s">
         <v>253</v>
       </c>
@@ -9762,7 +9981,7 @@
         <v>43458</v>
       </c>
     </row>
-    <row r="253" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A253" s="3" t="s">
         <v>254</v>
       </c>
@@ -9774,7 +9993,7 @@
       </c>
       <c r="F253" s="10"/>
     </row>
-    <row r="254" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A254" s="3" t="s">
         <v>255</v>
       </c>
@@ -9785,7 +10004,7 @@
         <v>43458</v>
       </c>
     </row>
-    <row r="255" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A255" s="3" t="s">
         <v>256</v>
       </c>
@@ -9797,7 +10016,7 @@
       </c>
       <c r="F255" s="10"/>
     </row>
-    <row r="256" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A256" s="3" t="s">
         <v>257</v>
       </c>
@@ -9808,7 +10027,7 @@
         <v>43458</v>
       </c>
     </row>
-    <row r="257" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A257" s="3" t="s">
         <v>258</v>
       </c>
@@ -9820,7 +10039,7 @@
       </c>
       <c r="F257" s="10"/>
     </row>
-    <row r="258" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A258" s="5" t="s">
         <v>259</v>
       </c>
@@ -9830,8 +10049,11 @@
       <c r="E258" s="6">
         <v>43472</v>
       </c>
-    </row>
-    <row r="259" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="N258" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="259" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A259" s="5" t="s">
         <v>260</v>
       </c>
@@ -9843,7 +10065,7 @@
       </c>
       <c r="F259" s="10"/>
     </row>
-    <row r="260" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A260" s="5" t="s">
         <v>261</v>
       </c>
@@ -9854,7 +10076,7 @@
         <v>43472</v>
       </c>
     </row>
-    <row r="261" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A261" s="5" t="s">
         <v>262</v>
       </c>
@@ -9866,7 +10088,7 @@
       </c>
       <c r="F261" s="10"/>
     </row>
-    <row r="262" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A262" s="5" t="s">
         <v>263</v>
       </c>
@@ -9877,7 +10099,7 @@
         <v>43472</v>
       </c>
     </row>
-    <row r="263" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A263" s="5" t="s">
         <v>264</v>
       </c>
@@ -9889,7 +10111,7 @@
       </c>
       <c r="F263" s="10"/>
     </row>
-    <row r="264" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A264" s="5" t="s">
         <v>265</v>
       </c>
@@ -9900,7 +10122,7 @@
         <v>43472</v>
       </c>
     </row>
-    <row r="265" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A265" s="5" t="s">
         <v>266</v>
       </c>
@@ -9912,7 +10134,7 @@
       </c>
       <c r="F265" s="10"/>
     </row>
-    <row r="266" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A266" s="5" t="s">
         <v>267</v>
       </c>
@@ -9923,7 +10145,7 @@
         <v>43472</v>
       </c>
     </row>
-    <row r="267" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A267" s="5" t="s">
         <v>268</v>
       </c>
@@ -9935,7 +10157,7 @@
       </c>
       <c r="F267" s="10"/>
     </row>
-    <row r="268" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A268" s="5" t="s">
         <v>269</v>
       </c>
@@ -9946,7 +10168,7 @@
         <v>43472</v>
       </c>
     </row>
-    <row r="269" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A269" s="5" t="s">
         <v>270</v>
       </c>
@@ -9958,7 +10180,7 @@
       </c>
       <c r="F269" s="10"/>
     </row>
-    <row r="270" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A270" s="5" t="s">
         <v>271</v>
       </c>
@@ -9971,7 +10193,7 @@
         <v>43472</v>
       </c>
     </row>
-    <row r="271" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A271" s="5" t="s">
         <v>272</v>
       </c>
@@ -9983,7 +10205,7 @@
       </c>
       <c r="F271" s="10"/>
     </row>
-    <row r="272" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A272" s="5" t="s">
         <v>273</v>
       </c>
@@ -9994,7 +10216,7 @@
         <v>43472</v>
       </c>
     </row>
-    <row r="273" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A273" s="5" t="s">
         <v>274</v>
       </c>
@@ -10006,7 +10228,7 @@
       </c>
       <c r="F273" s="10"/>
     </row>
-    <row r="274" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A274" s="7" t="s">
         <v>275</v>
       </c>
@@ -10016,8 +10238,11 @@
       <c r="E274" s="11">
         <v>43486</v>
       </c>
-    </row>
-    <row r="275" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="N274" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="275" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A275" s="7" t="s">
         <v>276</v>
       </c>
@@ -10029,7 +10254,7 @@
       </c>
       <c r="F275" s="10"/>
     </row>
-    <row r="276" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A276" s="7" t="s">
         <v>277</v>
       </c>
@@ -10040,7 +10265,7 @@
         <v>43486</v>
       </c>
     </row>
-    <row r="277" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A277" s="7" t="s">
         <v>278</v>
       </c>
@@ -10052,7 +10277,7 @@
       </c>
       <c r="F277" s="10"/>
     </row>
-    <row r="278" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A278" s="7" t="s">
         <v>279</v>
       </c>
@@ -10063,7 +10288,7 @@
         <v>43486</v>
       </c>
     </row>
-    <row r="279" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A279" s="7" t="s">
         <v>280</v>
       </c>
@@ -10075,7 +10300,7 @@
       </c>
       <c r="F279" s="10"/>
     </row>
-    <row r="280" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A280" s="7" t="s">
         <v>281</v>
       </c>
@@ -10086,7 +10311,7 @@
         <v>43486</v>
       </c>
     </row>
-    <row r="281" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A281" s="7" t="s">
         <v>282</v>
       </c>
@@ -10098,7 +10323,7 @@
       </c>
       <c r="F281" s="10"/>
     </row>
-    <row r="282" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A282" s="7" t="s">
         <v>283</v>
       </c>
@@ -10109,7 +10334,7 @@
         <v>43486</v>
       </c>
     </row>
-    <row r="283" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A283" s="7" t="s">
         <v>284</v>
       </c>
@@ -10121,7 +10346,7 @@
       </c>
       <c r="F283" s="10"/>
     </row>
-    <row r="284" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A284" s="7" t="s">
         <v>285</v>
       </c>
@@ -10132,7 +10357,7 @@
         <v>43486</v>
       </c>
     </row>
-    <row r="285" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A285" s="7" t="s">
         <v>286</v>
       </c>
@@ -10144,7 +10369,7 @@
       </c>
       <c r="F285" s="10"/>
     </row>
-    <row r="286" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A286" s="7" t="s">
         <v>287</v>
       </c>
@@ -10155,7 +10380,7 @@
         <v>43486</v>
       </c>
     </row>
-    <row r="287" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A287" s="7" t="s">
         <v>288</v>
       </c>
@@ -10167,7 +10392,7 @@
       </c>
       <c r="F287" s="10"/>
     </row>
-    <row r="288" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A288" s="7" t="s">
         <v>289</v>
       </c>
@@ -10178,7 +10403,7 @@
         <v>43486</v>
       </c>
     </row>
-    <row r="289" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A289" s="7" t="s">
         <v>290</v>
       </c>
@@ -10190,7 +10415,7 @@
       </c>
       <c r="F289" s="10"/>
     </row>
-    <row r="290" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A290" s="3" t="s">
         <v>291</v>
       </c>
@@ -10200,8 +10425,11 @@
       <c r="E290" s="4">
         <v>43458</v>
       </c>
-    </row>
-    <row r="291" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="N290" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="291" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A291" s="3" t="s">
         <v>292</v>
       </c>
@@ -10212,8 +10440,11 @@
         <v>43458</v>
       </c>
       <c r="F291" s="10"/>
-    </row>
-    <row r="292" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="N291" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="292" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A292" s="3" t="s">
         <v>293</v>
       </c>
@@ -10223,8 +10454,11 @@
       <c r="E292" s="4">
         <v>43458</v>
       </c>
-    </row>
-    <row r="293" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="N292" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="293" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A293" s="3" t="s">
         <v>294</v>
       </c>
@@ -10235,8 +10469,11 @@
         <v>43458</v>
       </c>
       <c r="F293" s="10"/>
-    </row>
-    <row r="294" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="N293" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="294" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A294" s="3" t="s">
         <v>295</v>
       </c>
@@ -10247,7 +10484,7 @@
         <v>43458</v>
       </c>
     </row>
-    <row r="295" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A295" s="3" t="s">
         <v>296</v>
       </c>
@@ -10259,7 +10496,7 @@
       </c>
       <c r="F295" s="10"/>
     </row>
-    <row r="296" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A296" s="3" t="s">
         <v>297</v>
       </c>
@@ -10272,7 +10509,7 @@
         <v>43458</v>
       </c>
     </row>
-    <row r="297" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A297" s="3" t="s">
         <v>298</v>
       </c>
@@ -10284,7 +10521,7 @@
       </c>
       <c r="F297" s="10"/>
     </row>
-    <row r="298" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A298" s="3" t="s">
         <v>299</v>
       </c>
@@ -10295,7 +10532,7 @@
         <v>43458</v>
       </c>
     </row>
-    <row r="299" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A299" s="3" t="s">
         <v>300</v>
       </c>
@@ -10311,7 +10548,7 @@
         <v>43509</v>
       </c>
     </row>
-    <row r="300" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A300" s="3" t="s">
         <v>301</v>
       </c>
@@ -10328,7 +10565,7 @@
         <v>43458</v>
       </c>
     </row>
-    <row r="301" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A301" s="3" t="s">
         <v>302</v>
       </c>
@@ -10344,7 +10581,7 @@
         <v>43515</v>
       </c>
     </row>
-    <row r="302" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A302" s="3" t="s">
         <v>303</v>
       </c>
@@ -10355,7 +10592,7 @@
         <v>43458</v>
       </c>
     </row>
-    <row r="303" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A303" s="3" t="s">
         <v>304</v>
       </c>
@@ -10371,7 +10608,7 @@
         <v>43509</v>
       </c>
     </row>
-    <row r="304" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A304" s="3" t="s">
         <v>305</v>
       </c>
@@ -10388,7 +10625,7 @@
         <v>43458</v>
       </c>
     </row>
-    <row r="305" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A305" s="3" t="s">
         <v>306</v>
       </c>
@@ -10400,7 +10637,7 @@
       </c>
       <c r="F305" s="10"/>
     </row>
-    <row r="306" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A306" s="5" t="s">
         <v>307</v>
       </c>
@@ -10410,8 +10647,11 @@
       <c r="E306" s="6">
         <v>43472</v>
       </c>
-    </row>
-    <row r="307" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="N306" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="307" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A307" s="5" t="s">
         <v>308</v>
       </c>
@@ -10423,7 +10663,7 @@
       </c>
       <c r="F307" s="10"/>
     </row>
-    <row r="308" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A308" s="5" t="s">
         <v>309</v>
       </c>
@@ -10434,7 +10674,7 @@
         <v>43472</v>
       </c>
     </row>
-    <row r="309" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A309" s="5" t="s">
         <v>310</v>
       </c>
@@ -10446,7 +10686,7 @@
       </c>
       <c r="F309" s="10"/>
     </row>
-    <row r="310" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A310" s="5" t="s">
         <v>311</v>
       </c>
@@ -10457,7 +10697,7 @@
         <v>43472</v>
       </c>
     </row>
-    <row r="311" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A311" s="5" t="s">
         <v>312</v>
       </c>
@@ -10469,7 +10709,7 @@
       </c>
       <c r="F311" s="10"/>
     </row>
-    <row r="312" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A312" s="5" t="s">
         <v>313</v>
       </c>
@@ -10480,7 +10720,7 @@
         <v>43472</v>
       </c>
     </row>
-    <row r="313" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A313" s="5" t="s">
         <v>314</v>
       </c>
@@ -10492,7 +10732,7 @@
       </c>
       <c r="F313" s="10"/>
     </row>
-    <row r="314" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A314" s="5" t="s">
         <v>315</v>
       </c>
@@ -10503,7 +10743,7 @@
         <v>43472</v>
       </c>
     </row>
-    <row r="315" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A315" s="5" t="s">
         <v>316</v>
       </c>
@@ -10515,7 +10755,7 @@
       </c>
       <c r="F315" s="10"/>
     </row>
-    <row r="316" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A316" s="5" t="s">
         <v>317</v>
       </c>
@@ -10526,7 +10766,7 @@
         <v>43472</v>
       </c>
     </row>
-    <row r="317" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A317" s="5" t="s">
         <v>318</v>
       </c>
@@ -10538,7 +10778,7 @@
       </c>
       <c r="F317" s="10"/>
     </row>
-    <row r="318" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A318" s="5" t="s">
         <v>319</v>
       </c>
@@ -10549,7 +10789,7 @@
         <v>43472</v>
       </c>
     </row>
-    <row r="319" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A319" s="5" t="s">
         <v>320</v>
       </c>
@@ -10561,7 +10801,7 @@
       </c>
       <c r="F319" s="10"/>
     </row>
-    <row r="320" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A320" s="5" t="s">
         <v>321</v>
       </c>
@@ -10572,7 +10812,7 @@
         <v>43472</v>
       </c>
     </row>
-    <row r="321" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A321" s="5" t="s">
         <v>322</v>
       </c>
@@ -10584,7 +10824,7 @@
       </c>
       <c r="F321" s="10"/>
     </row>
-    <row r="322" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A322" s="7" t="s">
         <v>323</v>
       </c>
@@ -10594,8 +10834,11 @@
       <c r="E322" s="11">
         <v>43486</v>
       </c>
-    </row>
-    <row r="323" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="N322" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="323" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A323" s="7" t="s">
         <v>324</v>
       </c>
@@ -10607,7 +10850,7 @@
       </c>
       <c r="F323" s="10"/>
     </row>
-    <row r="324" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A324" s="7" t="s">
         <v>325</v>
       </c>
@@ -10618,7 +10861,7 @@
         <v>43486</v>
       </c>
     </row>
-    <row r="325" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A325" s="7" t="s">
         <v>326</v>
       </c>
@@ -10634,7 +10877,7 @@
         <v>43528</v>
       </c>
     </row>
-    <row r="326" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A326" s="7" t="s">
         <v>327</v>
       </c>
@@ -10645,7 +10888,7 @@
         <v>43486</v>
       </c>
     </row>
-    <row r="327" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A327" s="7" t="s">
         <v>328</v>
       </c>
@@ -10657,7 +10900,7 @@
       </c>
       <c r="F327" s="10"/>
     </row>
-    <row r="328" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A328" s="7" t="s">
         <v>329</v>
       </c>
@@ -10668,7 +10911,7 @@
         <v>43486</v>
       </c>
     </row>
-    <row r="329" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A329" s="7" t="s">
         <v>330</v>
       </c>
@@ -10680,7 +10923,7 @@
       </c>
       <c r="F329" s="10"/>
     </row>
-    <row r="330" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A330" s="7" t="s">
         <v>331</v>
       </c>
@@ -10691,7 +10934,7 @@
         <v>43486</v>
       </c>
     </row>
-    <row r="331" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A331" s="7" t="s">
         <v>332</v>
       </c>
@@ -10703,7 +10946,7 @@
       </c>
       <c r="F331" s="10"/>
     </row>
-    <row r="332" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A332" s="7" t="s">
         <v>333</v>
       </c>
@@ -10714,7 +10957,7 @@
         <v>43486</v>
       </c>
     </row>
-    <row r="333" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A333" s="7" t="s">
         <v>334</v>
       </c>
@@ -10726,7 +10969,7 @@
       </c>
       <c r="F333" s="10"/>
     </row>
-    <row r="334" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A334" s="7" t="s">
         <v>335</v>
       </c>
@@ -10737,7 +10980,7 @@
         <v>43486</v>
       </c>
     </row>
-    <row r="335" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A335" s="7" t="s">
         <v>336</v>
       </c>
@@ -10753,7 +10996,7 @@
         <v>43528</v>
       </c>
     </row>
-    <row r="336" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="336" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A336" s="7" t="s">
         <v>337</v>
       </c>
@@ -10764,7 +11007,7 @@
         <v>43486</v>
       </c>
     </row>
-    <row r="337" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A337" s="7" t="s">
         <v>338</v>
       </c>
@@ -10776,7 +11019,7 @@
       </c>
       <c r="F337" s="10"/>
     </row>
-    <row r="338" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A338" s="3" t="s">
         <v>339</v>
       </c>
@@ -10811,8 +11054,11 @@
         <f>AVERAGE(I338:L338)</f>
         <v>42.125</v>
       </c>
-    </row>
-    <row r="339" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N338" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="339" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A339" s="3" t="s">
         <v>340</v>
       </c>
@@ -10851,7 +11097,7 @@
         <v>42.3</v>
       </c>
     </row>
-    <row r="340" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A340" s="3" t="s">
         <v>341</v>
       </c>
@@ -10887,7 +11133,7 @@
         <v>48.449999999999996</v>
       </c>
     </row>
-    <row r="341" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="341" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A341" s="3" t="s">
         <v>342</v>
       </c>
@@ -10926,7 +11172,7 @@
         <v>45.824999999999996</v>
       </c>
     </row>
-    <row r="342" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A342" s="3" t="s">
         <v>343</v>
       </c>
@@ -10962,7 +11208,7 @@
         <v>45.05</v>
       </c>
     </row>
-    <row r="343" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="343" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A343" s="3" t="s">
         <v>344</v>
       </c>
@@ -11001,7 +11247,7 @@
         <v>40.825000000000003</v>
       </c>
     </row>
-    <row r="344" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="344" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A344" s="3" t="s">
         <v>345</v>
       </c>
@@ -11037,7 +11283,7 @@
         <v>37.875</v>
       </c>
     </row>
-    <row r="345" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="345" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A345" s="3" t="s">
         <v>346</v>
       </c>
@@ -11076,7 +11322,7 @@
         <v>37.650000000000006</v>
       </c>
     </row>
-    <row r="346" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="346" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A346" s="3" t="s">
         <v>347</v>
       </c>
@@ -11112,7 +11358,7 @@
         <v>44.024999999999999</v>
       </c>
     </row>
-    <row r="347" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="347" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A347" s="3" t="s">
         <v>348</v>
       </c>
@@ -11151,7 +11397,7 @@
         <v>44.024999999999999</v>
       </c>
     </row>
-    <row r="348" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="348" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A348" s="3" t="s">
         <v>349</v>
       </c>
@@ -11187,7 +11433,7 @@
         <v>42.05</v>
       </c>
     </row>
-    <row r="349" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="349" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A349" s="3" t="s">
         <v>350</v>
       </c>
@@ -11226,7 +11472,7 @@
         <v>39.950000000000003</v>
       </c>
     </row>
-    <row r="350" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="350" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A350" s="3" t="s">
         <v>351</v>
       </c>
@@ -11262,7 +11508,7 @@
         <v>47.775000000000006</v>
       </c>
     </row>
-    <row r="351" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="351" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A351" s="3" t="s">
         <v>352</v>
       </c>
@@ -11304,7 +11550,7 @@
         <v>45.275000000000006</v>
       </c>
     </row>
-    <row r="352" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="352" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A352" s="3" t="s">
         <v>353</v>
       </c>
@@ -11340,7 +11586,7 @@
         <v>47.625</v>
       </c>
     </row>
-    <row r="353" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="353" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A353" s="3" t="s">
         <v>354</v>
       </c>
@@ -11360,7 +11606,7 @@
         <v>43472</v>
       </c>
     </row>
-    <row r="354" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="354" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A354" s="5" t="s">
         <v>355</v>
       </c>
@@ -11376,8 +11622,11 @@
       <c r="E354" s="6">
         <v>43472</v>
       </c>
-    </row>
-    <row r="355" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="N354" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="355" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A355" s="5" t="s">
         <v>356</v>
       </c>
@@ -11397,7 +11646,7 @@
         <v>43493</v>
       </c>
     </row>
-    <row r="356" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="356" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A356" s="5" t="s">
         <v>357</v>
       </c>
@@ -11414,7 +11663,7 @@
         <v>43472</v>
       </c>
     </row>
-    <row r="357" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="357" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A357" s="5" t="s">
         <v>358</v>
       </c>
@@ -11434,7 +11683,7 @@
         <v>43488</v>
       </c>
     </row>
-    <row r="358" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="358" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A358" s="5" t="s">
         <v>359</v>
       </c>
@@ -11451,7 +11700,7 @@
         <v>43472</v>
       </c>
     </row>
-    <row r="359" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="359" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A359" s="5" t="s">
         <v>360</v>
       </c>
@@ -11471,7 +11720,7 @@
         <v>43490</v>
       </c>
     </row>
-    <row r="360" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="360" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A360" s="5" t="s">
         <v>361</v>
       </c>
@@ -11488,7 +11737,7 @@
         <v>43472</v>
       </c>
     </row>
-    <row r="361" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="361" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A361" s="5" t="s">
         <v>362</v>
       </c>
@@ -11508,7 +11757,7 @@
         <v>43488</v>
       </c>
     </row>
-    <row r="362" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="362" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A362" s="5" t="s">
         <v>363</v>
       </c>
@@ -11525,7 +11774,7 @@
         <v>43472</v>
       </c>
     </row>
-    <row r="363" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="363" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A363" s="5" t="s">
         <v>364</v>
       </c>
@@ -11545,7 +11794,7 @@
         <v>43488</v>
       </c>
     </row>
-    <row r="364" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="364" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A364" s="5" t="s">
         <v>365</v>
       </c>
@@ -11562,7 +11811,7 @@
         <v>43472</v>
       </c>
     </row>
-    <row r="365" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="365" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A365" s="5" t="s">
         <v>366</v>
       </c>
@@ -11582,7 +11831,7 @@
         <v>43490</v>
       </c>
     </row>
-    <row r="366" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="366" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A366" s="5" t="s">
         <v>367</v>
       </c>
@@ -11599,7 +11848,7 @@
         <v>43472</v>
       </c>
     </row>
-    <row r="367" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="367" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A367" s="5" t="s">
         <v>368</v>
       </c>
@@ -11619,7 +11868,7 @@
         <v>43488</v>
       </c>
     </row>
-    <row r="368" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="368" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A368" s="5" t="s">
         <v>369</v>
       </c>
@@ -11636,7 +11885,7 @@
         <v>43472</v>
       </c>
     </row>
-    <row r="369" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="369" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A369" s="5" t="s">
         <v>370</v>
       </c>
@@ -11659,7 +11908,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="370" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="370" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A370" s="7" t="s">
         <v>371</v>
       </c>
@@ -11675,8 +11924,11 @@
       <c r="E370" s="11">
         <v>43486</v>
       </c>
-    </row>
-    <row r="371" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="N370" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="371" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A371" s="7" t="s">
         <v>372</v>
       </c>
@@ -11696,7 +11948,7 @@
         <v>43502</v>
       </c>
     </row>
-    <row r="372" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="372" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A372" s="7" t="s">
         <v>373</v>
       </c>
@@ -11713,7 +11965,7 @@
         <v>43486</v>
       </c>
     </row>
-    <row r="373" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="373" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A373" s="7" t="s">
         <v>374</v>
       </c>
@@ -11733,7 +11985,7 @@
         <v>43500</v>
       </c>
     </row>
-    <row r="374" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="374" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A374" s="7" t="s">
         <v>375</v>
       </c>
@@ -11750,7 +12002,7 @@
         <v>43486</v>
       </c>
     </row>
-    <row r="375" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="375" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A375" s="7" t="s">
         <v>376</v>
       </c>
@@ -11770,7 +12022,7 @@
         <v>43500</v>
       </c>
     </row>
-    <row r="376" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="376" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A376" s="7" t="s">
         <v>377</v>
       </c>
@@ -11787,7 +12039,7 @@
         <v>43486</v>
       </c>
     </row>
-    <row r="377" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="377" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A377" s="7" t="s">
         <v>378</v>
       </c>
@@ -11807,7 +12059,7 @@
         <v>43500</v>
       </c>
     </row>
-    <row r="378" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="378" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A378" s="7" t="s">
         <v>379</v>
       </c>
@@ -11824,7 +12076,7 @@
         <v>43486</v>
       </c>
     </row>
-    <row r="379" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="379" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A379" s="7" t="s">
         <v>380</v>
       </c>
@@ -11844,7 +12096,7 @@
         <v>43502</v>
       </c>
     </row>
-    <row r="380" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="380" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A380" s="7" t="s">
         <v>381</v>
       </c>
@@ -11861,7 +12113,7 @@
         <v>43486</v>
       </c>
     </row>
-    <row r="381" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="381" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A381" s="7" t="s">
         <v>382</v>
       </c>
@@ -11881,7 +12133,7 @@
         <v>43500</v>
       </c>
     </row>
-    <row r="382" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="382" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A382" s="7" t="s">
         <v>383</v>
       </c>
@@ -11898,7 +12150,7 @@
         <v>43486</v>
       </c>
     </row>
-    <row r="383" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="383" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A383" s="7" t="s">
         <v>384</v>
       </c>
@@ -11921,7 +12173,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="384" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="384" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A384" s="7" t="s">
         <v>385</v>
       </c>
@@ -11938,7 +12190,7 @@
         <v>43486</v>
       </c>
     </row>
-    <row r="385" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="385" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A385" s="20" t="s">
         <v>386</v>
       </c>
@@ -11951,7 +12203,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="386" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="386" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A386" s="3" t="s">
         <v>387</v>
       </c>
@@ -11967,8 +12219,11 @@
       <c r="E386" s="4">
         <v>43458</v>
       </c>
-    </row>
-    <row r="387" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="N386" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="387" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A387" s="3" t="s">
         <v>388</v>
       </c>
@@ -11987,8 +12242,11 @@
       <c r="F387" s="10">
         <v>43507</v>
       </c>
-    </row>
-    <row r="388" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="N387" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="388" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A388" s="3" t="s">
         <v>389</v>
       </c>
@@ -12000,8 +12258,11 @@
       <c r="E388" s="4">
         <v>43458</v>
       </c>
-    </row>
-    <row r="389" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="N388" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="389" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A389" s="3" t="s">
         <v>390</v>
       </c>
@@ -12020,8 +12281,11 @@
       <c r="F389" s="10">
         <v>43493</v>
       </c>
-    </row>
-    <row r="390" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="N389" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="390" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A390" s="3" t="s">
         <v>391</v>
       </c>
@@ -12037,8 +12301,11 @@
       <c r="E390" s="4">
         <v>43458</v>
       </c>
-    </row>
-    <row r="391" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="N390" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="391" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A391" s="3" t="s">
         <v>392</v>
       </c>
@@ -12058,7 +12325,7 @@
         <v>43515</v>
       </c>
     </row>
-    <row r="392" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="392" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A392" s="3" t="s">
         <v>393</v>
       </c>
@@ -12075,7 +12342,7 @@
         <v>43458</v>
       </c>
     </row>
-    <row r="393" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="393" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A393" s="3" t="s">
         <v>394</v>
       </c>
@@ -12095,7 +12362,7 @@
         <v>43493</v>
       </c>
     </row>
-    <row r="394" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="394" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A394" s="3" t="s">
         <v>395</v>
       </c>
@@ -12112,7 +12379,7 @@
         <v>43458</v>
       </c>
     </row>
-    <row r="395" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="395" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A395" s="3" t="s">
         <v>396</v>
       </c>
@@ -12132,7 +12399,7 @@
         <v>43507</v>
       </c>
     </row>
-    <row r="396" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="396" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A396" s="3" t="s">
         <v>397</v>
       </c>
@@ -12149,7 +12416,7 @@
         <v>43458</v>
       </c>
     </row>
-    <row r="397" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="397" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A397" s="3" t="s">
         <v>398</v>
       </c>
@@ -12169,7 +12436,7 @@
         <v>43504</v>
       </c>
     </row>
-    <row r="398" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="398" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A398" s="3" t="s">
         <v>399</v>
       </c>
@@ -12186,7 +12453,7 @@
         <v>43458</v>
       </c>
     </row>
-    <row r="399" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="399" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A399" s="3" t="s">
         <v>400</v>
       </c>
@@ -12209,7 +12476,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="400" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="400" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A400" s="3" t="s">
         <v>401</v>
       </c>
@@ -12226,7 +12493,7 @@
         <v>43458</v>
       </c>
     </row>
-    <row r="401" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="401" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A401" s="3" t="s">
         <v>402</v>
       </c>
@@ -12246,7 +12513,7 @@
         <v>43493</v>
       </c>
     </row>
-    <row r="402" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="402" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A402" s="5" t="s">
         <v>403</v>
       </c>
@@ -12262,8 +12529,11 @@
       <c r="E402" s="6">
         <v>43472</v>
       </c>
-    </row>
-    <row r="403" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="N402" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="403" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A403" s="5" t="s">
         <v>404</v>
       </c>
@@ -12282,8 +12552,11 @@
       <c r="F403" s="10">
         <v>43515</v>
       </c>
-    </row>
-    <row r="404" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="N403" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="404" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A404" s="5" t="s">
         <v>405</v>
       </c>
@@ -12299,8 +12572,11 @@
       <c r="E404" s="6">
         <v>43472</v>
       </c>
-    </row>
-    <row r="405" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="N404" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="405" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A405" s="5" t="s">
         <v>406</v>
       </c>
@@ -12319,8 +12595,11 @@
       <c r="F405" s="10">
         <v>43507</v>
       </c>
-    </row>
-    <row r="406" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="N405" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="406" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A406" s="5" t="s">
         <v>407</v>
       </c>
@@ -12337,7 +12616,7 @@
         <v>43472</v>
       </c>
     </row>
-    <row r="407" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="407" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A407" s="5" t="s">
         <v>408</v>
       </c>
@@ -12357,7 +12636,7 @@
         <v>43518</v>
       </c>
     </row>
-    <row r="408" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="408" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A408" s="5" t="s">
         <v>409</v>
       </c>
@@ -12374,7 +12653,7 @@
         <v>43472</v>
       </c>
     </row>
-    <row r="409" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="409" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A409" s="5" t="s">
         <v>410</v>
       </c>
@@ -12394,7 +12673,7 @@
         <v>43511</v>
       </c>
     </row>
-    <row r="410" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="410" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A410" s="5" t="s">
         <v>411</v>
       </c>
@@ -12411,7 +12690,7 @@
         <v>43472</v>
       </c>
     </row>
-    <row r="411" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="411" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A411" s="5" t="s">
         <v>412</v>
       </c>
@@ -12431,7 +12710,7 @@
         <v>43502</v>
       </c>
     </row>
-    <row r="412" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="412" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A412" s="5" t="s">
         <v>413</v>
       </c>
@@ -12448,7 +12727,7 @@
         <v>43472</v>
       </c>
     </row>
-    <row r="413" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="413" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A413" s="5" t="s">
         <v>414</v>
       </c>
@@ -12468,7 +12747,7 @@
         <v>43515</v>
       </c>
     </row>
-    <row r="414" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="414" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A414" s="5" t="s">
         <v>415</v>
       </c>
@@ -12485,7 +12764,7 @@
         <v>43472</v>
       </c>
     </row>
-    <row r="415" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="415" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A415" s="5" t="s">
         <v>416</v>
       </c>
@@ -12505,7 +12784,7 @@
         <v>43511</v>
       </c>
     </row>
-    <row r="416" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="416" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A416" s="5" t="s">
         <v>417</v>
       </c>
@@ -12522,7 +12801,7 @@
         <v>43472</v>
       </c>
     </row>
-    <row r="417" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="417" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A417" s="5" t="s">
         <v>418</v>
       </c>
@@ -12542,7 +12821,7 @@
         <v>43509</v>
       </c>
     </row>
-    <row r="418" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="418" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A418" s="7" t="s">
         <v>419</v>
       </c>
@@ -12554,8 +12833,11 @@
       <c r="E418" s="11">
         <v>43486</v>
       </c>
-    </row>
-    <row r="419" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="N418" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="419" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A419" s="7" t="s">
         <v>420</v>
       </c>
@@ -12570,8 +12852,11 @@
       <c r="F419" s="10">
         <v>43528</v>
       </c>
-    </row>
-    <row r="420" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="N419" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="420" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A420" s="7" t="s">
         <v>421</v>
       </c>
@@ -12583,8 +12868,11 @@
       <c r="E420" s="11">
         <v>43486</v>
       </c>
-    </row>
-    <row r="421" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="N420" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="421" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A421" s="7" t="s">
         <v>422</v>
       </c>
@@ -12604,7 +12892,7 @@
         <v>43518</v>
       </c>
     </row>
-    <row r="422" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="422" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A422" s="7" t="s">
         <v>423</v>
       </c>
@@ -12617,7 +12905,7 @@
         <v>43486</v>
       </c>
     </row>
-    <row r="423" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="423" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A423" s="7" t="s">
         <v>424</v>
       </c>
@@ -12633,7 +12921,7 @@
         <v>43518</v>
       </c>
     </row>
-    <row r="424" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="424" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A424" s="7" t="s">
         <v>425</v>
       </c>
@@ -12650,7 +12938,7 @@
         <v>43486</v>
       </c>
     </row>
-    <row r="425" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="425" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A425" s="7" t="s">
         <v>426</v>
       </c>
@@ -12666,7 +12954,7 @@
         <v>43521</v>
       </c>
     </row>
-    <row r="426" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="426" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A426" s="7" t="s">
         <v>427</v>
       </c>
@@ -12679,7 +12967,7 @@
         <v>43486</v>
       </c>
     </row>
-    <row r="427" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="427" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A427" s="7" t="s">
         <v>428</v>
       </c>
@@ -12695,7 +12983,7 @@
         <v>43528</v>
       </c>
     </row>
-    <row r="428" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="428" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A428" s="7" t="s">
         <v>429</v>
       </c>
@@ -12712,7 +13000,7 @@
         <v>43486</v>
       </c>
     </row>
-    <row r="429" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="429" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A429" s="7" t="s">
         <v>430</v>
       </c>
@@ -12728,7 +13016,7 @@
         <v>43518</v>
       </c>
     </row>
-    <row r="430" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="430" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A430" s="7" t="s">
         <v>431</v>
       </c>
@@ -12741,7 +13029,7 @@
         <v>43486</v>
       </c>
     </row>
-    <row r="431" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="431" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A431" s="7" t="s">
         <v>432</v>
       </c>
@@ -12755,7 +13043,7 @@
       </c>
       <c r="F431" s="10"/>
     </row>
-    <row r="432" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="432" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A432" s="7" t="s">
         <v>433</v>
       </c>
@@ -12773,7 +13061,7 @@
       </c>
       <c r="F432" s="8"/>
     </row>
-    <row r="433" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="433" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A433" s="7" t="s">
         <v>434</v>
       </c>
@@ -12789,7 +13077,7 @@
         <v>43521</v>
       </c>
     </row>
-    <row r="434" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="434" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A434" s="3" t="s">
         <v>435</v>
       </c>
@@ -12805,8 +13093,11 @@
       <c r="E434" s="4">
         <v>43458</v>
       </c>
-    </row>
-    <row r="435" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="N434" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="435" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A435" s="3" t="s">
         <v>436</v>
       </c>
@@ -12825,8 +13116,11 @@
       <c r="F435" s="10">
         <v>43497</v>
       </c>
-    </row>
-    <row r="436" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="N435" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="436" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A436" s="3" t="s">
         <v>437</v>
       </c>
@@ -12842,8 +13136,11 @@
       <c r="E436" s="4">
         <v>43458</v>
       </c>
-    </row>
-    <row r="437" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="N436" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="437" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A437" s="3" t="s">
         <v>438</v>
       </c>
@@ -12862,8 +13159,11 @@
       <c r="F437" s="10">
         <v>43502</v>
       </c>
-    </row>
-    <row r="438" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="N437" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="438" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A438" s="3" t="s">
         <v>439</v>
       </c>
@@ -12880,7 +13180,7 @@
         <v>43458</v>
       </c>
     </row>
-    <row r="439" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="439" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A439" s="3" t="s">
         <v>440</v>
       </c>
@@ -12898,7 +13198,7 @@
         <v>43507</v>
       </c>
     </row>
-    <row r="440" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="440" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A440" s="3" t="s">
         <v>441</v>
       </c>
@@ -12915,7 +13215,7 @@
         <v>43458</v>
       </c>
     </row>
-    <row r="441" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="441" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A441" s="3" t="s">
         <v>442</v>
       </c>
@@ -12927,7 +13227,7 @@
       </c>
       <c r="F441" s="10"/>
     </row>
-    <row r="442" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="442" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A442" s="3" t="s">
         <v>443</v>
       </c>
@@ -12944,7 +13244,7 @@
         <v>43458</v>
       </c>
     </row>
-    <row r="443" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="443" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A443" s="3" t="s">
         <v>444</v>
       </c>
@@ -12967,7 +13267,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="444" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="444" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A444" s="3" t="s">
         <v>445</v>
       </c>
@@ -12984,7 +13284,7 @@
         <v>43458</v>
       </c>
     </row>
-    <row r="445" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="445" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A445" s="3" t="s">
         <v>446</v>
       </c>
@@ -13004,7 +13304,7 @@
         <v>43497</v>
       </c>
     </row>
-    <row r="446" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="446" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A446" s="3" t="s">
         <v>447</v>
       </c>
@@ -13021,7 +13321,7 @@
         <v>43458</v>
       </c>
     </row>
-    <row r="447" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="447" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A447" s="3" t="s">
         <v>448</v>
       </c>
@@ -13041,7 +13341,7 @@
         <v>43500</v>
       </c>
     </row>
-    <row r="448" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="448" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A448" s="3" t="s">
         <v>449</v>
       </c>
@@ -13058,7 +13358,7 @@
         <v>43458</v>
       </c>
     </row>
-    <row r="449" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="449" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A449" s="3" t="s">
         <v>450</v>
       </c>
@@ -13074,7 +13374,7 @@
         <v>43523</v>
       </c>
     </row>
-    <row r="450" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="450" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A450" s="5" t="s">
         <v>451</v>
       </c>
@@ -13090,8 +13390,11 @@
       <c r="E450" s="6">
         <v>43472</v>
       </c>
-    </row>
-    <row r="451" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="N450" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="451" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A451" s="5" t="s">
         <v>452</v>
       </c>
@@ -13110,8 +13413,11 @@
       <c r="F451" s="10">
         <v>43507</v>
       </c>
-    </row>
-    <row r="452" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="N451" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="452" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A452" s="5" t="s">
         <v>453</v>
       </c>
@@ -13127,8 +13433,11 @@
       <c r="E452" s="6">
         <v>43472</v>
       </c>
-    </row>
-    <row r="453" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="N452" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="453" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A453" s="5" t="s">
         <v>454</v>
       </c>
@@ -13148,7 +13457,7 @@
         <v>43509</v>
       </c>
     </row>
-    <row r="454" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="454" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A454" s="5" t="s">
         <v>455</v>
       </c>
@@ -13165,7 +13474,7 @@
         <v>43472</v>
       </c>
     </row>
-    <row r="455" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="455" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A455" s="5" t="s">
         <v>456</v>
       </c>
@@ -13185,7 +13494,7 @@
         <v>43509</v>
       </c>
     </row>
-    <row r="456" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="456" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A456" s="5" t="s">
         <v>457</v>
       </c>
@@ -13202,7 +13511,7 @@
         <v>43472</v>
       </c>
     </row>
-    <row r="457" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="457" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A457" s="5" t="s">
         <v>458</v>
       </c>
@@ -13223,7 +13532,7 @@
       </c>
       <c r="G457" s="1"/>
     </row>
-    <row r="458" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="458" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A458" s="5" t="s">
         <v>459</v>
       </c>
@@ -13240,7 +13549,7 @@
         <v>43472</v>
       </c>
     </row>
-    <row r="459" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="459" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A459" s="5" t="s">
         <v>460</v>
       </c>
@@ -13260,7 +13569,7 @@
         <v>43500</v>
       </c>
     </row>
-    <row r="460" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="460" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A460" s="5" t="s">
         <v>461</v>
       </c>
@@ -13277,7 +13586,7 @@
         <v>43472</v>
       </c>
     </row>
-    <row r="461" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="461" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A461" s="5" t="s">
         <v>462</v>
       </c>
@@ -13297,7 +13606,7 @@
         <v>43509</v>
       </c>
     </row>
-    <row r="462" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="462" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A462" s="5" t="s">
         <v>463</v>
       </c>
@@ -13314,7 +13623,7 @@
         <v>43472</v>
       </c>
     </row>
-    <row r="463" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="463" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A463" s="5" t="s">
         <v>464</v>
       </c>
@@ -13334,7 +13643,7 @@
         <v>43507</v>
       </c>
     </row>
-    <row r="464" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="464" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A464" s="5" t="s">
         <v>465</v>
       </c>
@@ -13351,7 +13660,7 @@
         <v>43472</v>
       </c>
     </row>
-    <row r="465" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="465" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A465" s="5" t="s">
         <v>466</v>
       </c>
@@ -13371,7 +13680,7 @@
         <v>43515</v>
       </c>
     </row>
-    <row r="466" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="466" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A466" s="7" t="s">
         <v>467</v>
       </c>
@@ -13387,8 +13696,11 @@
       <c r="E466" s="11">
         <v>43486</v>
       </c>
-    </row>
-    <row r="467" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="N466" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="467" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A467" s="7" t="s">
         <v>468</v>
       </c>
@@ -13407,8 +13719,11 @@
       <c r="F467" s="10">
         <v>43507</v>
       </c>
-    </row>
-    <row r="468" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="N467" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="468" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A468" s="7" t="s">
         <v>469</v>
       </c>
@@ -13424,8 +13739,11 @@
       <c r="E468" s="11">
         <v>43486</v>
       </c>
-    </row>
-    <row r="469" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="N468" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="469" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A469" s="7" t="s">
         <v>470</v>
       </c>
@@ -13441,7 +13759,7 @@
         <v>43518</v>
       </c>
     </row>
-    <row r="470" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="470" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A470" s="7" t="s">
         <v>471</v>
       </c>
@@ -13458,7 +13776,7 @@
         <v>43486</v>
       </c>
     </row>
-    <row r="471" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="471" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A471" s="7" t="s">
         <v>472</v>
       </c>
@@ -13474,7 +13792,7 @@
         <v>43518</v>
       </c>
     </row>
-    <row r="472" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="472" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A472" s="7" t="s">
         <v>473</v>
       </c>
@@ -13487,7 +13805,7 @@
         <v>43486</v>
       </c>
     </row>
-    <row r="473" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="473" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A473" s="7" t="s">
         <v>474</v>
       </c>
@@ -13507,7 +13825,7 @@
         <v>43515</v>
       </c>
     </row>
-    <row r="474" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="474" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A474" s="7" t="s">
         <v>475</v>
       </c>
@@ -13524,7 +13842,7 @@
         <v>43486</v>
       </c>
     </row>
-    <row r="475" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="475" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A475" s="7" t="s">
         <v>476</v>
       </c>
@@ -13544,7 +13862,7 @@
         <v>43518</v>
       </c>
     </row>
-    <row r="476" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="476" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A476" s="7" t="s">
         <v>477</v>
       </c>
@@ -13561,7 +13879,7 @@
         <v>43486</v>
       </c>
     </row>
-    <row r="477" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="477" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A477" s="7" t="s">
         <v>478</v>
       </c>
@@ -13581,7 +13899,7 @@
         <v>43518</v>
       </c>
     </row>
-    <row r="478" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="478" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A478" s="7" t="s">
         <v>479</v>
       </c>
@@ -13598,7 +13916,7 @@
         <v>43486</v>
       </c>
     </row>
-    <row r="479" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="479" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A479" s="7" t="s">
         <v>480</v>
       </c>
@@ -13618,7 +13936,7 @@
         <v>43507</v>
       </c>
     </row>
-    <row r="480" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="480" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A480" s="7" t="s">
         <v>481</v>
       </c>

</xml_diff>

<commit_message>
checking on drought effect
</commit_message>
<xml_diff>
--- a/data/observation_datasheet.xlsx
+++ b/data/observation_datasheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="28125"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1000" yWindow="0" windowWidth="24580" windowHeight="13200" activeTab="2"/>
+    <workbookView xWindow="1000" yWindow="0" windowWidth="17940" windowHeight="13100" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="observation_datasheet" sheetId="1" r:id="rId1"/>
@@ -2826,7 +2826,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Atlas" id="{5156B0E4-0EB1-49FE-A26B-15F6F698AEC6}" vid="{508F7963-D0B5-43F7-BB2C-FCE3009C08EC}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Atlas" id="{5156B0E4-0EB1-49FE-A26B-15F6F698AEC6}" vid="{508F7963-D0B5-43F7-BB2C-FCE3009C08EC}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -18092,10 +18092,10 @@
   <dimension ref="A1:J61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B37" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomRight" activeCell="F62" sqref="F62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -18158,7 +18158,7 @@
         <v>0</v>
       </c>
       <c r="F2" s="33">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G2" s="33" t="s">
         <v>561</v>
@@ -18187,7 +18187,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="36">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G3" s="36" t="s">
         <v>561</v>
@@ -18216,7 +18216,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="38">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G4" s="38" t="s">
         <v>561</v>
@@ -18245,7 +18245,7 @@
         <v>1</v>
       </c>
       <c r="F5" s="41">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G5" s="41">
         <v>7</v>
@@ -18274,7 +18274,7 @@
         <v>1</v>
       </c>
       <c r="F6" s="41">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G6" s="41">
         <v>0</v>
@@ -18303,7 +18303,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="43">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G7" s="43">
         <v>0</v>
@@ -18332,7 +18332,7 @@
         <v>0</v>
       </c>
       <c r="F8" s="33">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G8" s="33" t="s">
         <v>561</v>
@@ -18361,7 +18361,7 @@
         <v>0</v>
       </c>
       <c r="F9" s="36">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G9" s="36" t="s">
         <v>561</v>
@@ -18390,7 +18390,7 @@
         <v>0</v>
       </c>
       <c r="F10" s="38">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G10" s="38" t="s">
         <v>561</v>
@@ -18419,7 +18419,7 @@
         <v>1</v>
       </c>
       <c r="F11" s="41">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G11" s="41">
         <v>7</v>
@@ -18448,7 +18448,7 @@
         <v>1</v>
       </c>
       <c r="F12" s="41">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G12" s="41">
         <v>7</v>
@@ -18477,7 +18477,7 @@
         <v>1</v>
       </c>
       <c r="F13" s="43">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G13" s="43">
         <v>3</v>
@@ -18506,7 +18506,7 @@
         <v>0</v>
       </c>
       <c r="F14" s="33">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G14" s="33" t="s">
         <v>561</v>
@@ -18535,7 +18535,7 @@
         <v>0</v>
       </c>
       <c r="F15" s="36">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G15" s="36" t="s">
         <v>561</v>
@@ -18564,7 +18564,7 @@
         <v>0</v>
       </c>
       <c r="F16" s="38">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G16" s="38" t="s">
         <v>561</v>
@@ -18593,7 +18593,7 @@
         <v>1</v>
       </c>
       <c r="F17" s="41">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G17" s="41">
         <v>8</v>
@@ -18622,7 +18622,7 @@
         <v>1</v>
       </c>
       <c r="F18" s="41">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G18" s="41">
         <v>8</v>
@@ -18651,7 +18651,7 @@
         <v>1</v>
       </c>
       <c r="F19" s="43">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G19" s="43">
         <v>8</v>
@@ -18680,7 +18680,7 @@
         <v>0</v>
       </c>
       <c r="F20" s="33">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G20" s="33" t="s">
         <v>561</v>
@@ -18709,7 +18709,7 @@
         <v>0</v>
       </c>
       <c r="F21" s="36">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G21" s="36" t="s">
         <v>561</v>
@@ -18738,7 +18738,7 @@
         <v>0</v>
       </c>
       <c r="F22" s="38">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G22" s="38" t="s">
         <v>561</v>
@@ -18767,7 +18767,7 @@
         <v>1</v>
       </c>
       <c r="F23" s="41">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G23" s="41">
         <v>8</v>
@@ -18796,7 +18796,7 @@
         <v>1</v>
       </c>
       <c r="F24" s="41">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G24" s="41">
         <v>8</v>
@@ -18825,7 +18825,7 @@
         <v>1</v>
       </c>
       <c r="F25" s="43">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G25" s="43">
         <v>8</v>
@@ -18854,7 +18854,7 @@
         <v>0</v>
       </c>
       <c r="F26" s="33">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G26" s="33" t="s">
         <v>561</v>
@@ -18883,7 +18883,7 @@
         <v>0</v>
       </c>
       <c r="F27" s="36">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G27" s="36" t="s">
         <v>561</v>
@@ -18912,7 +18912,7 @@
         <v>0</v>
       </c>
       <c r="F28" s="38">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G28" s="38" t="s">
         <v>561</v>
@@ -18941,7 +18941,7 @@
         <v>1</v>
       </c>
       <c r="F29" s="41">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G29" s="41">
         <v>8</v>
@@ -18970,7 +18970,7 @@
         <v>1</v>
       </c>
       <c r="F30" s="41">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G30" s="41">
         <v>8</v>
@@ -18999,7 +18999,7 @@
         <v>1</v>
       </c>
       <c r="F31" s="43">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G31" s="43">
         <v>8</v>
@@ -19028,7 +19028,7 @@
         <v>0</v>
       </c>
       <c r="F32" s="33">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G32" s="33" t="s">
         <v>561</v>
@@ -19057,7 +19057,7 @@
         <v>0</v>
       </c>
       <c r="F33" s="36">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G33" s="36" t="s">
         <v>561</v>
@@ -19086,7 +19086,7 @@
         <v>0</v>
       </c>
       <c r="F34" s="38">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G34" s="38" t="s">
         <v>561</v>
@@ -19115,7 +19115,7 @@
         <v>1</v>
       </c>
       <c r="F35" s="41">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G35" s="41">
         <v>0</v>
@@ -19144,7 +19144,7 @@
         <v>1</v>
       </c>
       <c r="F36" s="41">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G36" s="41">
         <v>0</v>
@@ -19173,7 +19173,7 @@
         <v>1</v>
       </c>
       <c r="F37" s="43">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G37" s="43">
         <v>0</v>
@@ -19202,7 +19202,7 @@
         <v>0</v>
       </c>
       <c r="F38" s="33">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G38" s="33" t="s">
         <v>561</v>
@@ -19231,7 +19231,7 @@
         <v>0</v>
       </c>
       <c r="F39" s="36">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G39" s="36" t="s">
         <v>561</v>
@@ -19260,7 +19260,7 @@
         <v>0</v>
       </c>
       <c r="F40" s="38">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G40" s="38" t="s">
         <v>561</v>
@@ -19289,7 +19289,7 @@
         <v>1</v>
       </c>
       <c r="F41" s="41">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G41" s="41">
         <v>2</v>
@@ -19318,7 +19318,7 @@
         <v>1</v>
       </c>
       <c r="F42" s="41">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G42" s="41">
         <v>0</v>
@@ -19347,7 +19347,7 @@
         <v>1</v>
       </c>
       <c r="F43" s="43">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G43" s="43">
         <v>0</v>
@@ -19376,7 +19376,7 @@
         <v>0</v>
       </c>
       <c r="F44" s="33">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G44" s="33" t="s">
         <v>561</v>
@@ -19405,7 +19405,7 @@
         <v>0</v>
       </c>
       <c r="F45" s="36">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G45" s="36" t="s">
         <v>561</v>
@@ -19434,7 +19434,7 @@
         <v>0</v>
       </c>
       <c r="F46" s="38">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G46" s="38" t="s">
         <v>561</v>
@@ -19463,7 +19463,7 @@
         <v>1</v>
       </c>
       <c r="F47" s="41">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G47" s="41">
         <v>8</v>
@@ -19492,7 +19492,7 @@
         <v>1</v>
       </c>
       <c r="F48" s="41">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G48" s="41">
         <v>8</v>
@@ -19521,7 +19521,7 @@
         <v>1</v>
       </c>
       <c r="F49" s="43">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G49" s="43">
         <v>7</v>
@@ -19553,7 +19553,7 @@
         <v>0</v>
       </c>
       <c r="F50" s="33">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G50" s="33" t="s">
         <v>561</v>
@@ -19582,7 +19582,7 @@
         <v>0</v>
       </c>
       <c r="F51" s="36">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G51" s="36" t="s">
         <v>561</v>
@@ -19611,7 +19611,7 @@
         <v>0</v>
       </c>
       <c r="F52" s="38">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G52" s="38" t="s">
         <v>561</v>
@@ -19640,7 +19640,7 @@
         <v>1</v>
       </c>
       <c r="F53" s="41">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G53" s="41">
         <v>7</v>
@@ -19669,7 +19669,7 @@
         <v>1</v>
       </c>
       <c r="F54" s="41">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G54" s="41">
         <v>5</v>
@@ -19698,7 +19698,7 @@
         <v>1</v>
       </c>
       <c r="F55" s="43">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G55" s="43">
         <v>0</v>
@@ -19727,7 +19727,7 @@
         <v>0</v>
       </c>
       <c r="F56" s="33">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G56" s="33" t="s">
         <v>561</v>
@@ -19756,7 +19756,7 @@
         <v>0</v>
       </c>
       <c r="F57" s="36">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G57" s="36" t="s">
         <v>561</v>
@@ -19785,7 +19785,7 @@
         <v>0</v>
       </c>
       <c r="F58" s="38">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G58" s="38" t="s">
         <v>561</v>
@@ -19814,7 +19814,7 @@
         <v>1</v>
       </c>
       <c r="F59" s="41">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G59" s="41">
         <v>6</v>
@@ -19843,7 +19843,7 @@
         <v>1</v>
       </c>
       <c r="F60" s="41">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G60" s="41">
         <v>6</v>
@@ -19872,7 +19872,7 @@
         <v>1</v>
       </c>
       <c r="F61" s="43">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G61" s="43">
         <v>2</v>

</xml_diff>

<commit_message>
working on analyses a bit
</commit_message>
<xml_diff>
--- a/data/observation_datasheet.xlsx
+++ b/data/observation_datasheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/catchamberlain/Documents/git/chillfreeze/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E20FFDA5-127E-EF42-842F-11BD018B8B98}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09847A0C-4A1D-2141-9849-7B7A56D3F770}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30980" windowHeight="20960" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5486,10 +5486,10 @@
   <dimension ref="A1:AA481"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B369" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B450" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P402" sqref="P402"/>
+      <selection pane="bottomRight" activeCell="P480" sqref="P480"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -24108,13 +24108,31 @@
       <c r="N402" s="12" t="s">
         <v>528</v>
       </c>
-      <c r="W402" t="e">
+      <c r="P402">
+        <v>66.5</v>
+      </c>
+      <c r="Q402">
+        <v>24.2</v>
+      </c>
+      <c r="R402">
+        <v>23.7</v>
+      </c>
+      <c r="S402">
+        <v>22.5</v>
+      </c>
+      <c r="T402">
+        <v>23.1</v>
+      </c>
+      <c r="W402">
         <f t="shared" si="16"/>
-        <v>#DIV/0!</v>
+        <v>23.375</v>
       </c>
       <c r="X402">
         <f t="shared" si="17"/>
-        <v>-57.6</v>
+        <v>8.8999999999999986</v>
+      </c>
+      <c r="AA402">
+        <v>6.3E-3</v>
       </c>
     </row>
     <row r="403" spans="1:27" x14ac:dyDescent="0.2">
@@ -24182,13 +24200,31 @@
       <c r="N404" s="12" t="s">
         <v>532</v>
       </c>
-      <c r="W404" t="e">
+      <c r="P404">
+        <v>55.2</v>
+      </c>
+      <c r="Q404">
+        <v>21.9</v>
+      </c>
+      <c r="R404">
+        <v>21.3</v>
+      </c>
+      <c r="S404">
+        <v>20.8</v>
+      </c>
+      <c r="T404">
+        <v>22.2</v>
+      </c>
+      <c r="W404">
         <f t="shared" si="16"/>
-        <v>#DIV/0!</v>
+        <v>21.55</v>
       </c>
       <c r="X404">
         <f t="shared" si="17"/>
-        <v>-50.4</v>
+        <v>4.8000000000000043</v>
+      </c>
+      <c r="AA404">
+        <v>4.5999999999999999E-3</v>
       </c>
     </row>
     <row r="405" spans="1:27" x14ac:dyDescent="0.2">
@@ -24220,13 +24256,31 @@
       <c r="N405" s="12" t="s">
         <v>533</v>
       </c>
-      <c r="W405" t="e">
+      <c r="P405">
+        <v>51.6</v>
+      </c>
+      <c r="Q405">
+        <v>27.2</v>
+      </c>
+      <c r="R405">
+        <v>25.5</v>
+      </c>
+      <c r="S405">
+        <v>23.6</v>
+      </c>
+      <c r="T405">
+        <v>25.1</v>
+      </c>
+      <c r="W405">
         <f t="shared" si="16"/>
-        <v>#DIV/0!</v>
+        <v>25.35</v>
       </c>
       <c r="X405">
         <f t="shared" si="17"/>
-        <v>-45.4</v>
+        <v>6.2000000000000028</v>
+      </c>
+      <c r="AA405">
+        <v>4.5999999999999999E-3</v>
       </c>
     </row>
     <row r="406" spans="1:27" x14ac:dyDescent="0.2">
@@ -24254,13 +24308,31 @@
       <c r="L406" s="12"/>
       <c r="M406" s="12"/>
       <c r="N406" s="12"/>
-      <c r="W406" t="e">
+      <c r="P406">
+        <v>62.1</v>
+      </c>
+      <c r="Q406">
+        <v>22.1</v>
+      </c>
+      <c r="R406">
+        <v>21.3</v>
+      </c>
+      <c r="S406">
+        <v>21.7</v>
+      </c>
+      <c r="T406">
+        <v>14.3</v>
+      </c>
+      <c r="W406">
         <f t="shared" si="16"/>
-        <v>#DIV/0!</v>
+        <v>19.850000000000001</v>
       </c>
       <c r="X406">
         <f t="shared" si="17"/>
-        <v>-50.6</v>
+        <v>11.5</v>
+      </c>
+      <c r="AA406">
+        <v>0</v>
       </c>
     </row>
     <row r="407" spans="1:27" x14ac:dyDescent="0.2">
@@ -24324,13 +24396,31 @@
       <c r="L408" s="12"/>
       <c r="M408" s="12"/>
       <c r="N408" s="12"/>
-      <c r="W408" t="e">
+      <c r="P408">
+        <v>65.400000000000006</v>
+      </c>
+      <c r="Q408">
+        <v>22.6</v>
+      </c>
+      <c r="R408">
+        <v>21.7</v>
+      </c>
+      <c r="S408">
+        <v>20.5</v>
+      </c>
+      <c r="T408">
+        <v>20.6</v>
+      </c>
+      <c r="W408">
         <f t="shared" si="16"/>
-        <v>#DIV/0!</v>
+        <v>21.35</v>
       </c>
       <c r="X408">
         <f t="shared" si="17"/>
-        <v>-58.3</v>
+        <v>7.1000000000000085</v>
+      </c>
+      <c r="AA408">
+        <v>4.4000000000000003E-3</v>
       </c>
     </row>
     <row r="409" spans="1:27" x14ac:dyDescent="0.2">
@@ -24360,13 +24450,31 @@
       <c r="L409" s="12"/>
       <c r="M409" s="12"/>
       <c r="N409" s="12"/>
-      <c r="W409" t="e">
+      <c r="P409">
+        <v>52.3</v>
+      </c>
+      <c r="Q409">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="R409">
+        <v>23</v>
+      </c>
+      <c r="S409">
+        <v>24.4</v>
+      </c>
+      <c r="T409">
+        <v>24.3</v>
+      </c>
+      <c r="W409">
         <f t="shared" si="16"/>
-        <v>#DIV/0!</v>
+        <v>22.824999999999999</v>
       </c>
       <c r="X409">
         <f t="shared" si="17"/>
-        <v>-50.4</v>
+        <v>1.8999999999999986</v>
+      </c>
+      <c r="AA409">
+        <v>5.7999999999999996E-3</v>
       </c>
     </row>
     <row r="410" spans="1:27" x14ac:dyDescent="0.2">
@@ -24394,13 +24502,31 @@
       <c r="L410" s="12"/>
       <c r="M410" s="12"/>
       <c r="N410" s="12"/>
-      <c r="W410" t="e">
+      <c r="P410">
+        <v>46.4</v>
+      </c>
+      <c r="Q410">
+        <v>24.2</v>
+      </c>
+      <c r="R410">
+        <v>22.7</v>
+      </c>
+      <c r="S410">
+        <v>25</v>
+      </c>
+      <c r="T410">
+        <v>25</v>
+      </c>
+      <c r="W410">
         <f t="shared" si="16"/>
-        <v>#DIV/0!</v>
+        <v>24.225000000000001</v>
       </c>
       <c r="X410">
         <f t="shared" si="17"/>
-        <v>-43.7</v>
+        <v>2.6999999999999957</v>
+      </c>
+      <c r="AA410">
+        <v>7.1000000000000004E-3</v>
       </c>
     </row>
     <row r="411" spans="1:27" x14ac:dyDescent="0.2">
@@ -24430,13 +24556,31 @@
       <c r="L411" s="12"/>
       <c r="M411" s="12"/>
       <c r="N411" s="12"/>
-      <c r="W411" t="e">
+      <c r="P411">
+        <v>49.4</v>
+      </c>
+      <c r="Q411">
+        <v>23.6</v>
+      </c>
+      <c r="R411">
+        <v>24.4</v>
+      </c>
+      <c r="S411">
+        <v>25.5</v>
+      </c>
+      <c r="T411">
+        <v>24</v>
+      </c>
+      <c r="W411">
         <f t="shared" si="16"/>
-        <v>#DIV/0!</v>
+        <v>24.375</v>
       </c>
       <c r="X411">
         <f t="shared" si="17"/>
-        <v>-44.8</v>
+        <v>4.6000000000000014</v>
+      </c>
+      <c r="AA411">
+        <v>7.1999999999999998E-3</v>
       </c>
     </row>
     <row r="412" spans="1:27" x14ac:dyDescent="0.2">
@@ -24464,13 +24608,31 @@
       <c r="L412" s="12"/>
       <c r="M412" s="12"/>
       <c r="N412" s="12"/>
-      <c r="W412" t="e">
+      <c r="P412">
+        <v>64.8</v>
+      </c>
+      <c r="Q412">
+        <v>22.3</v>
+      </c>
+      <c r="R412">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="S412">
+        <v>20.9</v>
+      </c>
+      <c r="T412">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="W412">
         <f t="shared" si="16"/>
-        <v>#DIV/0!</v>
+        <v>20.55</v>
       </c>
       <c r="X412">
         <f t="shared" si="17"/>
-        <v>-57.2</v>
+        <v>7.5999999999999943</v>
+      </c>
+      <c r="AA412">
+        <v>3.7000000000000002E-3</v>
       </c>
     </row>
     <row r="413" spans="1:27" x14ac:dyDescent="0.2">
@@ -24534,13 +24696,31 @@
       <c r="L414" s="12"/>
       <c r="M414" s="12"/>
       <c r="N414" s="12"/>
-      <c r="W414" t="e">
+      <c r="P414">
+        <v>58.7</v>
+      </c>
+      <c r="Q414">
+        <v>23.2</v>
+      </c>
+      <c r="R414">
+        <v>21</v>
+      </c>
+      <c r="S414">
+        <v>21.4</v>
+      </c>
+      <c r="T414">
+        <v>22.8</v>
+      </c>
+      <c r="W414">
         <f t="shared" si="16"/>
-        <v>#DIV/0!</v>
+        <v>22.099999999999998</v>
       </c>
       <c r="X414">
         <f t="shared" si="17"/>
-        <v>-51.1</v>
+        <v>7.6000000000000014</v>
+      </c>
+      <c r="AA414">
+        <v>5.1000000000000004E-3</v>
       </c>
     </row>
     <row r="415" spans="1:27" x14ac:dyDescent="0.2">
@@ -24570,13 +24750,31 @@
       <c r="L415" s="12"/>
       <c r="M415" s="12"/>
       <c r="N415" s="12"/>
-      <c r="W415" t="e">
+      <c r="P415">
+        <v>63.4</v>
+      </c>
+      <c r="Q415">
+        <v>23.6</v>
+      </c>
+      <c r="R415">
+        <v>22.6</v>
+      </c>
+      <c r="S415">
+        <v>22.6</v>
+      </c>
+      <c r="T415">
+        <v>26.7</v>
+      </c>
+      <c r="W415">
         <f t="shared" si="16"/>
-        <v>#DIV/0!</v>
+        <v>23.875000000000004</v>
       </c>
       <c r="X415">
         <f t="shared" si="17"/>
-        <v>-58.5</v>
+        <v>4.8999999999999986</v>
+      </c>
+      <c r="AA415">
+        <v>6.7000000000000002E-3</v>
       </c>
     </row>
     <row r="416" spans="1:27" x14ac:dyDescent="0.2">
@@ -24658,13 +24856,31 @@
       <c r="L417" s="12"/>
       <c r="M417" s="12"/>
       <c r="N417" s="12"/>
-      <c r="W417" t="e">
+      <c r="P417">
+        <v>57.9</v>
+      </c>
+      <c r="Q417">
+        <v>24.1</v>
+      </c>
+      <c r="R417">
+        <v>30</v>
+      </c>
+      <c r="S417">
+        <v>29.3</v>
+      </c>
+      <c r="T417">
+        <v>27</v>
+      </c>
+      <c r="W417">
         <f t="shared" si="16"/>
-        <v>#DIV/0!</v>
+        <v>27.6</v>
       </c>
       <c r="X417">
         <f t="shared" si="17"/>
-        <v>-44.1</v>
+        <v>13.799999999999997</v>
+      </c>
+      <c r="AA417">
+        <v>1.03E-2</v>
       </c>
     </row>
     <row r="418" spans="1:27" x14ac:dyDescent="0.2">
@@ -25259,15 +25475,32 @@
       <c r="N434" s="12" t="s">
         <v>536</v>
       </c>
-      <c r="W434" t="e">
+      <c r="P434">
+        <v>23.2</v>
+      </c>
+      <c r="Q434">
+        <v>29.9</v>
+      </c>
+      <c r="R434">
+        <v>29.8</v>
+      </c>
+      <c r="S434">
+        <v>36.299999999999997</v>
+      </c>
+      <c r="T434">
+        <v>32.200000000000003</v>
+      </c>
+      <c r="W434">
         <f t="shared" si="16"/>
-        <v>#DIV/0!</v>
+        <v>32.049999999999997</v>
       </c>
       <c r="X434">
         <f t="shared" si="17"/>
-        <v>-21.1</v>
-      </c>
-      <c r="AA434" s="5"/>
+        <v>2.0999999999999979</v>
+      </c>
+      <c r="AA434">
+        <v>1.49E-2</v>
+      </c>
     </row>
     <row r="435" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A435" s="14" t="s">
@@ -25352,13 +25585,31 @@
       <c r="N436" s="12" t="s">
         <v>537</v>
       </c>
-      <c r="W436" t="e">
+      <c r="P436">
+        <v>33.4</v>
+      </c>
+      <c r="Q436">
+        <v>37.799999999999997</v>
+      </c>
+      <c r="R436">
+        <v>32.299999999999997</v>
+      </c>
+      <c r="S436">
+        <v>33.799999999999997</v>
+      </c>
+      <c r="T436">
+        <v>39.6</v>
+      </c>
+      <c r="W436">
         <f t="shared" si="16"/>
-        <v>#DIV/0!</v>
+        <v>35.875</v>
       </c>
       <c r="X436">
         <f t="shared" si="17"/>
-        <v>-33.6</v>
+        <v>-0.20000000000000284</v>
+      </c>
+      <c r="AA436">
+        <v>1.9199999999999998E-2</v>
       </c>
     </row>
     <row r="437" spans="1:27" x14ac:dyDescent="0.2">
@@ -25390,13 +25641,31 @@
       <c r="N437" s="12" t="s">
         <v>538</v>
       </c>
-      <c r="W437" t="e">
+      <c r="P437">
+        <v>30.8</v>
+      </c>
+      <c r="Q437">
+        <v>28.9</v>
+      </c>
+      <c r="R437">
+        <v>29.7</v>
+      </c>
+      <c r="S437">
+        <v>41.5</v>
+      </c>
+      <c r="T437">
+        <v>38.299999999999997</v>
+      </c>
+      <c r="W437">
         <f t="shared" si="16"/>
-        <v>#DIV/0!</v>
+        <v>34.599999999999994</v>
       </c>
       <c r="X437">
         <f t="shared" si="17"/>
-        <v>-29.5</v>
+        <v>1.3000000000000007</v>
+      </c>
+      <c r="AA437">
+        <v>1.77E-2</v>
       </c>
     </row>
     <row r="438" spans="1:27" x14ac:dyDescent="0.2">
@@ -25510,13 +25779,31 @@
       <c r="L440" s="12"/>
       <c r="M440" s="12"/>
       <c r="N440" s="12"/>
-      <c r="W440" t="e">
+      <c r="P440">
+        <v>32.200000000000003</v>
+      </c>
+      <c r="Q440">
+        <v>23.2</v>
+      </c>
+      <c r="R440">
+        <v>25</v>
+      </c>
+      <c r="S440">
+        <v>14.4</v>
+      </c>
+      <c r="T440">
+        <v>22.5</v>
+      </c>
+      <c r="W440">
         <f t="shared" si="16"/>
-        <v>#DIV/0!</v>
+        <v>21.274999999999999</v>
       </c>
       <c r="X440">
         <f t="shared" si="17"/>
-        <v>-32.200000000000003</v>
+        <v>0</v>
+      </c>
+      <c r="AA440">
+        <v>4.4000000000000003E-3</v>
       </c>
     </row>
     <row r="441" spans="1:27" x14ac:dyDescent="0.2">
@@ -25786,13 +26073,31 @@
       <c r="L447" s="12"/>
       <c r="M447" s="12"/>
       <c r="N447" s="12"/>
-      <c r="W447" t="e">
+      <c r="P447">
+        <v>21.6</v>
+      </c>
+      <c r="Q447">
+        <v>24.6</v>
+      </c>
+      <c r="R447">
+        <v>28</v>
+      </c>
+      <c r="S447">
+        <v>25.4</v>
+      </c>
+      <c r="T447">
+        <v>25.9</v>
+      </c>
+      <c r="W447">
         <f t="shared" si="16"/>
-        <v>#DIV/0!</v>
+        <v>25.975000000000001</v>
       </c>
       <c r="X447">
         <f t="shared" si="17"/>
-        <v>-24.7</v>
+        <v>-3.0999999999999979</v>
+      </c>
+      <c r="AA447">
+        <v>8.6999999999999994E-3</v>
       </c>
     </row>
     <row r="448" spans="1:27" x14ac:dyDescent="0.2">
@@ -25820,13 +26125,31 @@
       <c r="L448" s="12"/>
       <c r="M448" s="12"/>
       <c r="N448" s="12"/>
-      <c r="W448" t="e">
+      <c r="P448">
+        <v>33.700000000000003</v>
+      </c>
+      <c r="Q448">
+        <v>29.4</v>
+      </c>
+      <c r="R448">
+        <v>30.2</v>
+      </c>
+      <c r="S448">
+        <v>27</v>
+      </c>
+      <c r="T448">
+        <v>27.7</v>
+      </c>
+      <c r="W448">
         <f t="shared" si="16"/>
-        <v>#DIV/0!</v>
+        <v>28.574999999999999</v>
       </c>
       <c r="X448">
         <f t="shared" si="17"/>
-        <v>-33</v>
+        <v>0.70000000000000284</v>
+      </c>
+      <c r="AA448">
+        <v>1.1299999999999999E-2</v>
       </c>
     </row>
     <row r="449" spans="1:27" x14ac:dyDescent="0.2">
@@ -25948,13 +26271,31 @@
       <c r="N451" s="12" t="s">
         <v>532</v>
       </c>
-      <c r="W451" t="e">
+      <c r="P451">
+        <v>28.6</v>
+      </c>
+      <c r="Q451">
+        <v>30.9</v>
+      </c>
+      <c r="R451">
+        <v>27</v>
+      </c>
+      <c r="S451">
+        <v>28.7</v>
+      </c>
+      <c r="T451">
+        <v>30.4</v>
+      </c>
+      <c r="W451">
         <f t="shared" ref="W451:W481" si="18">AVERAGE(Q451:T451)</f>
-        <v>#DIV/0!</v>
+        <v>29.25</v>
       </c>
       <c r="X451">
         <f t="shared" ref="X451:X481" si="19">P451-D451</f>
-        <v>-27.9</v>
+        <v>0.70000000000000284</v>
+      </c>
+      <c r="AA451">
+        <v>1.2E-2</v>
       </c>
     </row>
     <row r="452" spans="1:27" x14ac:dyDescent="0.2">
@@ -25984,13 +26325,31 @@
       <c r="N452" s="12" t="s">
         <v>540</v>
       </c>
-      <c r="W452" t="e">
+      <c r="P452">
+        <v>29.2</v>
+      </c>
+      <c r="Q452">
+        <v>26.7</v>
+      </c>
+      <c r="R452">
+        <v>24.3</v>
+      </c>
+      <c r="S452">
+        <v>27.8</v>
+      </c>
+      <c r="T452">
+        <v>26.3</v>
+      </c>
+      <c r="W452">
         <f t="shared" si="18"/>
-        <v>#DIV/0!</v>
+        <v>26.274999999999999</v>
       </c>
       <c r="X452">
         <f t="shared" si="19"/>
-        <v>-28.4</v>
+        <v>0.80000000000000071</v>
+      </c>
+      <c r="AA452">
+        <v>8.9999999999999993E-3</v>
       </c>
     </row>
     <row r="453" spans="1:27" x14ac:dyDescent="0.2">
@@ -26020,13 +26379,31 @@
       <c r="L453" s="12"/>
       <c r="M453" s="12"/>
       <c r="N453" s="12"/>
-      <c r="W453" t="e">
+      <c r="P453">
+        <v>34.299999999999997</v>
+      </c>
+      <c r="Q453">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="R453">
+        <v>30.1</v>
+      </c>
+      <c r="S453">
+        <v>23.5</v>
+      </c>
+      <c r="T453">
+        <v>29.7</v>
+      </c>
+      <c r="W453">
         <f t="shared" si="18"/>
-        <v>#DIV/0!</v>
+        <v>25.475000000000001</v>
       </c>
       <c r="X453">
         <f t="shared" si="19"/>
-        <v>-34.799999999999997</v>
+        <v>-0.5</v>
+      </c>
+      <c r="AA453">
+        <v>8.3000000000000001E-3</v>
       </c>
     </row>
     <row r="454" spans="1:27" x14ac:dyDescent="0.2">
@@ -26108,13 +26485,31 @@
       <c r="L455" s="12"/>
       <c r="M455" s="12"/>
       <c r="N455" s="12"/>
-      <c r="W455" t="e">
+      <c r="P455">
+        <v>26.4</v>
+      </c>
+      <c r="Q455">
+        <v>26.1</v>
+      </c>
+      <c r="R455">
+        <v>27.4</v>
+      </c>
+      <c r="S455">
+        <v>25.2</v>
+      </c>
+      <c r="T455">
+        <v>24</v>
+      </c>
+      <c r="W455">
         <f t="shared" si="18"/>
-        <v>#DIV/0!</v>
+        <v>25.675000000000001</v>
       </c>
       <c r="X455">
         <f t="shared" si="19"/>
-        <v>-26.4</v>
+        <v>0</v>
+      </c>
+      <c r="AA455">
+        <v>8.3999999999999995E-3</v>
       </c>
     </row>
     <row r="456" spans="1:27" x14ac:dyDescent="0.2">
@@ -26142,13 +26537,31 @@
       <c r="L456" s="12"/>
       <c r="M456" s="12"/>
       <c r="N456" s="12"/>
-      <c r="W456" t="e">
+      <c r="P456">
+        <v>22.1</v>
+      </c>
+      <c r="Q456">
+        <v>22</v>
+      </c>
+      <c r="R456">
+        <v>20.2</v>
+      </c>
+      <c r="S456">
+        <v>20.6</v>
+      </c>
+      <c r="T456">
+        <v>21.9</v>
+      </c>
+      <c r="W456">
         <f t="shared" si="18"/>
-        <v>#DIV/0!</v>
+        <v>21.175000000000001</v>
       </c>
       <c r="X456">
         <f t="shared" si="19"/>
-        <v>-22.7</v>
+        <v>-0.59999999999999787</v>
+      </c>
+      <c r="AA456">
+        <v>4.3E-3</v>
       </c>
     </row>
     <row r="457" spans="1:27" x14ac:dyDescent="0.2">
@@ -26212,13 +26625,31 @@
       <c r="L458" s="12"/>
       <c r="M458" s="12"/>
       <c r="N458" s="12"/>
-      <c r="W458" t="e">
+      <c r="P458">
+        <v>26.3</v>
+      </c>
+      <c r="Q458">
+        <v>30</v>
+      </c>
+      <c r="R458">
+        <v>30.3</v>
+      </c>
+      <c r="S458">
+        <v>25.6</v>
+      </c>
+      <c r="T458">
+        <v>24.6</v>
+      </c>
+      <c r="W458">
         <f t="shared" si="18"/>
-        <v>#DIV/0!</v>
+        <v>27.625</v>
       </c>
       <c r="X458">
         <f t="shared" si="19"/>
-        <v>-20.399999999999999</v>
+        <v>5.9000000000000021</v>
+      </c>
+      <c r="AA458">
+        <v>1.04E-2</v>
       </c>
     </row>
     <row r="459" spans="1:27" x14ac:dyDescent="0.2">
@@ -26248,13 +26679,31 @@
       <c r="L459" s="12"/>
       <c r="M459" s="12"/>
       <c r="N459" s="12"/>
-      <c r="W459" t="e">
+      <c r="P459">
+        <v>21</v>
+      </c>
+      <c r="Q459">
+        <v>28.4</v>
+      </c>
+      <c r="R459">
+        <v>30.2</v>
+      </c>
+      <c r="S459">
+        <v>27.3</v>
+      </c>
+      <c r="T459">
+        <v>28.5</v>
+      </c>
+      <c r="W459">
         <f t="shared" si="18"/>
-        <v>#DIV/0!</v>
+        <v>28.599999999999998</v>
       </c>
       <c r="X459">
         <f t="shared" si="19"/>
-        <v>-25.9</v>
+        <v>-4.8999999999999986</v>
+      </c>
+      <c r="AA459">
+        <v>1.1299999999999999E-2</v>
       </c>
     </row>
     <row r="460" spans="1:27" x14ac:dyDescent="0.2">
@@ -26318,13 +26767,31 @@
       <c r="L461" s="12"/>
       <c r="M461" s="12"/>
       <c r="N461" s="12"/>
-      <c r="W461" t="e">
+      <c r="P461">
+        <v>33.799999999999997</v>
+      </c>
+      <c r="Q461">
+        <v>26</v>
+      </c>
+      <c r="R461">
+        <v>25.5</v>
+      </c>
+      <c r="S461">
+        <v>29</v>
+      </c>
+      <c r="T461">
+        <v>26.6</v>
+      </c>
+      <c r="W461">
         <f t="shared" si="18"/>
-        <v>#DIV/0!</v>
+        <v>26.774999999999999</v>
       </c>
       <c r="X461">
         <f t="shared" si="19"/>
-        <v>-32.700000000000003</v>
+        <v>1.0999999999999943</v>
+      </c>
+      <c r="AA461">
+        <v>9.4999999999999998E-3</v>
       </c>
     </row>
     <row r="462" spans="1:27" x14ac:dyDescent="0.2">
@@ -26352,13 +26819,31 @@
       <c r="L462" s="12"/>
       <c r="M462" s="12"/>
       <c r="N462" s="12"/>
-      <c r="W462" t="e">
+      <c r="P462">
+        <v>23.4</v>
+      </c>
+      <c r="Q462">
+        <v>23.1</v>
+      </c>
+      <c r="R462">
+        <v>28.4</v>
+      </c>
+      <c r="S462">
+        <v>24</v>
+      </c>
+      <c r="T462">
+        <v>28.6</v>
+      </c>
+      <c r="W462">
         <f t="shared" si="18"/>
-        <v>#DIV/0!</v>
+        <v>26.024999999999999</v>
       </c>
       <c r="X462">
         <f t="shared" si="19"/>
-        <v>-22.5</v>
+        <v>0.89999999999999858</v>
+      </c>
+      <c r="AA462">
+        <v>8.8000000000000005E-3</v>
       </c>
     </row>
     <row r="463" spans="1:27" x14ac:dyDescent="0.2">
@@ -26388,13 +26873,31 @@
       <c r="L463" s="12"/>
       <c r="M463" s="12"/>
       <c r="N463" s="12"/>
-      <c r="W463" t="e">
+      <c r="P463">
+        <v>30.6</v>
+      </c>
+      <c r="Q463">
+        <v>22.6</v>
+      </c>
+      <c r="R463">
+        <v>20.6</v>
+      </c>
+      <c r="S463">
+        <v>24.3</v>
+      </c>
+      <c r="T463">
+        <v>22.4</v>
+      </c>
+      <c r="W463">
         <f t="shared" si="18"/>
-        <v>#DIV/0!</v>
+        <v>22.475000000000001</v>
       </c>
       <c r="X463">
         <f t="shared" si="19"/>
-        <v>-31.6</v>
+        <v>-1</v>
+      </c>
+      <c r="AA463">
+        <v>5.4999999999999997E-3</v>
       </c>
     </row>
     <row r="464" spans="1:27" x14ac:dyDescent="0.2">
@@ -26422,16 +26925,34 @@
       <c r="L464" s="12"/>
       <c r="M464" s="12"/>
       <c r="N464" s="12"/>
-      <c r="W464" t="e">
+      <c r="P464">
+        <v>24.8</v>
+      </c>
+      <c r="Q464">
+        <v>27.3</v>
+      </c>
+      <c r="R464">
+        <v>27</v>
+      </c>
+      <c r="S464">
+        <v>29.8</v>
+      </c>
+      <c r="T464">
+        <v>25.6</v>
+      </c>
+      <c r="W464">
         <f t="shared" si="18"/>
-        <v>#DIV/0!</v>
+        <v>27.424999999999997</v>
       </c>
       <c r="X464">
         <f t="shared" si="19"/>
-        <v>-25</v>
-      </c>
-    </row>
-    <row r="465" spans="1:24" x14ac:dyDescent="0.2">
+        <v>-0.19999999999999929</v>
+      </c>
+      <c r="AA464">
+        <v>1.0200000000000001E-2</v>
+      </c>
+    </row>
+    <row r="465" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A465" s="19" t="s">
         <v>466</v>
       </c>
@@ -26467,7 +26988,7 @@
         <v>-30.7</v>
       </c>
     </row>
-    <row r="466" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="466" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A466" s="22" t="s">
         <v>467</v>
       </c>
@@ -26494,16 +27015,34 @@
       <c r="N466" s="12" t="s">
         <v>541</v>
       </c>
-      <c r="W466" t="e">
+      <c r="P466">
+        <v>21.4</v>
+      </c>
+      <c r="Q466">
+        <v>29.2</v>
+      </c>
+      <c r="R466">
+        <v>23.2</v>
+      </c>
+      <c r="S466">
+        <v>25.5</v>
+      </c>
+      <c r="T466">
+        <v>25.4</v>
+      </c>
+      <c r="W466">
         <f t="shared" si="18"/>
-        <v>#DIV/0!</v>
+        <v>25.825000000000003</v>
       </c>
       <c r="X466">
         <f t="shared" si="19"/>
-        <v>-20.3</v>
-      </c>
-    </row>
-    <row r="467" spans="1:24" x14ac:dyDescent="0.2">
+        <v>1.0999999999999979</v>
+      </c>
+      <c r="AA466">
+        <v>8.6E-3</v>
+      </c>
+    </row>
+    <row r="467" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A467" s="22" t="s">
         <v>468</v>
       </c>
@@ -26532,16 +27071,34 @@
       <c r="N467" s="12" t="s">
         <v>532</v>
       </c>
-      <c r="W467" t="e">
+      <c r="P467">
+        <v>26.8</v>
+      </c>
+      <c r="Q467">
+        <v>34.4</v>
+      </c>
+      <c r="R467">
+        <v>32.4</v>
+      </c>
+      <c r="S467">
+        <v>36.200000000000003</v>
+      </c>
+      <c r="T467">
+        <v>33</v>
+      </c>
+      <c r="W467">
         <f t="shared" si="18"/>
-        <v>#DIV/0!</v>
+        <v>34</v>
       </c>
       <c r="X467">
         <f t="shared" si="19"/>
-        <v>-23.6</v>
-      </c>
-    </row>
-    <row r="468" spans="1:24" x14ac:dyDescent="0.2">
+        <v>3.1999999999999993</v>
+      </c>
+      <c r="AA467">
+        <v>1.7100000000000001E-2</v>
+      </c>
+    </row>
+    <row r="468" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A468" s="22" t="s">
         <v>469</v>
       </c>
@@ -26568,16 +27125,34 @@
       <c r="N468" s="12" t="s">
         <v>525</v>
       </c>
-      <c r="W468" t="e">
+      <c r="P468">
+        <v>33.700000000000003</v>
+      </c>
+      <c r="Q468">
+        <v>30.8</v>
+      </c>
+      <c r="R468">
+        <v>28.3</v>
+      </c>
+      <c r="S468">
+        <v>23</v>
+      </c>
+      <c r="T468">
+        <v>28.6</v>
+      </c>
+      <c r="W468">
         <f t="shared" si="18"/>
-        <v>#DIV/0!</v>
+        <v>27.674999999999997</v>
       </c>
       <c r="X468">
         <f t="shared" si="19"/>
-        <v>-32.4</v>
-      </c>
-    </row>
-    <row r="469" spans="1:24" x14ac:dyDescent="0.2">
+        <v>1.3000000000000043</v>
+      </c>
+      <c r="AA468">
+        <v>1.04E-2</v>
+      </c>
+    </row>
+    <row r="469" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A469" s="22" t="s">
         <v>470</v>
       </c>
@@ -26613,7 +27188,7 @@
         <v>-29.4</v>
       </c>
     </row>
-    <row r="470" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="470" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A470" s="22" t="s">
         <v>471</v>
       </c>
@@ -26638,16 +27213,34 @@
       <c r="L470" s="12"/>
       <c r="M470" s="12"/>
       <c r="N470" s="12"/>
-      <c r="W470" t="e">
+      <c r="P470">
+        <v>30.6</v>
+      </c>
+      <c r="Q470">
+        <v>27.9</v>
+      </c>
+      <c r="R470">
+        <v>23.6</v>
+      </c>
+      <c r="S470">
+        <v>25.4</v>
+      </c>
+      <c r="T470">
+        <v>26.6</v>
+      </c>
+      <c r="W470">
         <f t="shared" si="18"/>
-        <v>#DIV/0!</v>
+        <v>25.875</v>
       </c>
       <c r="X470">
         <f t="shared" si="19"/>
-        <v>-26.4</v>
-      </c>
-    </row>
-    <row r="471" spans="1:24" x14ac:dyDescent="0.2">
+        <v>4.2000000000000028</v>
+      </c>
+      <c r="AA470">
+        <v>8.6E-3</v>
+      </c>
+    </row>
+    <row r="471" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A471" s="22" t="s">
         <v>472</v>
       </c>
@@ -26683,7 +27276,7 @@
         <v>-32.4</v>
       </c>
     </row>
-    <row r="472" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="472" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A472" s="22" t="s">
         <v>473</v>
       </c>
@@ -26708,16 +27301,34 @@
       <c r="L472" s="12"/>
       <c r="M472" s="12"/>
       <c r="N472" s="12"/>
-      <c r="W472" t="e">
+      <c r="P472">
+        <v>35.5</v>
+      </c>
+      <c r="Q472">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="R472">
+        <v>22.5</v>
+      </c>
+      <c r="S472">
+        <v>24.9</v>
+      </c>
+      <c r="T472">
+        <v>28.5</v>
+      </c>
+      <c r="W472">
         <f t="shared" si="18"/>
-        <v>#DIV/0!</v>
+        <v>24</v>
       </c>
       <c r="X472">
         <f t="shared" si="19"/>
-        <v>-35.4</v>
-      </c>
-    </row>
-    <row r="473" spans="1:24" x14ac:dyDescent="0.2">
+        <v>0.10000000000000142</v>
+      </c>
+      <c r="AA472">
+        <v>6.8999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="473" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A473" s="22" t="s">
         <v>474</v>
       </c>
@@ -26753,7 +27364,7 @@
         <v>-35.4</v>
       </c>
     </row>
-    <row r="474" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="474" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A474" s="22" t="s">
         <v>475</v>
       </c>
@@ -26787,7 +27398,7 @@
         <v>-23</v>
       </c>
     </row>
-    <row r="475" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="475" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A475" s="22" t="s">
         <v>476</v>
       </c>
@@ -26823,7 +27434,7 @@
         <v>-28.3</v>
       </c>
     </row>
-    <row r="476" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="476" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A476" s="22" t="s">
         <v>477</v>
       </c>
@@ -26848,16 +27459,34 @@
       <c r="L476" s="12"/>
       <c r="M476" s="12"/>
       <c r="N476" s="12"/>
-      <c r="W476" t="e">
+      <c r="P476">
+        <v>23.9</v>
+      </c>
+      <c r="Q476">
+        <v>21.1</v>
+      </c>
+      <c r="R476">
+        <v>17.7</v>
+      </c>
+      <c r="S476">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="T476">
+        <v>17</v>
+      </c>
+      <c r="W476">
         <f t="shared" si="18"/>
-        <v>#DIV/0!</v>
+        <v>18.975000000000001</v>
       </c>
       <c r="X476">
         <f t="shared" si="19"/>
-        <v>-23.4</v>
-      </c>
-    </row>
-    <row r="477" spans="1:24" x14ac:dyDescent="0.2">
+        <v>0.5</v>
+      </c>
+      <c r="AA476">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="477" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A477" s="22" t="s">
         <v>478</v>
       </c>
@@ -26884,16 +27513,34 @@
       <c r="L477" s="12"/>
       <c r="M477" s="12"/>
       <c r="N477" s="12"/>
-      <c r="W477" t="e">
+      <c r="P477">
+        <v>25.9</v>
+      </c>
+      <c r="Q477">
+        <v>20.8</v>
+      </c>
+      <c r="R477">
+        <v>20.7</v>
+      </c>
+      <c r="S477">
+        <v>28.3</v>
+      </c>
+      <c r="T477">
+        <v>25.3</v>
+      </c>
+      <c r="W477">
         <f t="shared" si="18"/>
-        <v>#DIV/0!</v>
+        <v>23.774999999999999</v>
       </c>
       <c r="X477">
         <f t="shared" si="19"/>
-        <v>-25.4</v>
-      </c>
-    </row>
-    <row r="478" spans="1:24" x14ac:dyDescent="0.2">
+        <v>0.5</v>
+      </c>
+      <c r="AA477">
+        <v>6.6E-3</v>
+      </c>
+    </row>
+    <row r="478" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A478" s="22" t="s">
         <v>479</v>
       </c>
@@ -26918,16 +27565,34 @@
       <c r="L478" s="12"/>
       <c r="M478" s="12"/>
       <c r="N478" s="12"/>
-      <c r="W478" t="e">
+      <c r="P478">
+        <v>29.6</v>
+      </c>
+      <c r="Q478">
+        <v>21.1</v>
+      </c>
+      <c r="R478">
+        <v>25.3</v>
+      </c>
+      <c r="S478">
+        <v>28.7</v>
+      </c>
+      <c r="T478">
+        <v>18.8</v>
+      </c>
+      <c r="W478">
         <f t="shared" si="18"/>
-        <v>#DIV/0!</v>
+        <v>23.475000000000001</v>
       </c>
       <c r="X478">
         <f t="shared" si="19"/>
-        <v>-27.9</v>
-      </c>
-    </row>
-    <row r="479" spans="1:24" x14ac:dyDescent="0.2">
+        <v>1.7000000000000028</v>
+      </c>
+      <c r="AA478">
+        <v>6.4000000000000003E-3</v>
+      </c>
+    </row>
+    <row r="479" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A479" s="22" t="s">
         <v>480</v>
       </c>
@@ -26954,16 +27619,34 @@
       <c r="L479" s="12"/>
       <c r="M479" s="12"/>
       <c r="N479" s="12"/>
-      <c r="W479" t="e">
+      <c r="P479">
+        <v>30</v>
+      </c>
+      <c r="Q479">
+        <v>24.2</v>
+      </c>
+      <c r="R479">
+        <v>26.8</v>
+      </c>
+      <c r="S479">
+        <v>27.7</v>
+      </c>
+      <c r="T479">
+        <v>22.3</v>
+      </c>
+      <c r="W479">
         <f t="shared" si="18"/>
-        <v>#DIV/0!</v>
+        <v>25.25</v>
       </c>
       <c r="X479">
         <f t="shared" si="19"/>
-        <v>-30</v>
-      </c>
-    </row>
-    <row r="480" spans="1:24" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="AA479">
+        <v>8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="480" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A480" s="22" t="s">
         <v>481</v>
       </c>

</xml_diff>

<commit_message>
more data and analyses
</commit_message>
<xml_diff>
--- a/data/observation_datasheet.xlsx
+++ b/data/observation_datasheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/catchamberlain/Documents/git/chillfreeze/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09847A0C-4A1D-2141-9849-7B7A56D3F770}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{336FFD1E-3A16-064E-88A6-CD8167AD586C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30980" windowHeight="20960" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5486,10 +5486,10 @@
   <dimension ref="A1:AA481"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B450" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B447" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P480" sqref="P480"/>
+      <selection pane="bottomRight" activeCell="U481" sqref="U481"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5876,13 +5876,28 @@
       <c r="L7" s="12"/>
       <c r="M7" s="12"/>
       <c r="N7" s="12"/>
-      <c r="W7" t="e">
+      <c r="P7">
+        <v>23.2</v>
+      </c>
+      <c r="Q7">
+        <v>19.7</v>
+      </c>
+      <c r="R7">
+        <v>28</v>
+      </c>
+      <c r="S7">
+        <v>21.4</v>
+      </c>
+      <c r="T7">
+        <v>21.6</v>
+      </c>
+      <c r="W7">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>22.674999999999997</v>
       </c>
       <c r="X7">
         <f t="shared" si="3"/>
-        <v>-22.1</v>
+        <v>1.0999999999999979</v>
       </c>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.2">
@@ -5910,13 +5925,28 @@
       <c r="L8" s="12"/>
       <c r="M8" s="12"/>
       <c r="N8" s="12"/>
-      <c r="W8" t="e">
+      <c r="P8">
+        <v>23.8</v>
+      </c>
+      <c r="Q8">
+        <v>24.9</v>
+      </c>
+      <c r="R8">
+        <v>29.5</v>
+      </c>
+      <c r="S8">
+        <v>24.2</v>
+      </c>
+      <c r="T8">
+        <v>22.6</v>
+      </c>
+      <c r="W8">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>25.299999999999997</v>
       </c>
       <c r="X8">
         <f t="shared" si="3"/>
-        <v>-22.5</v>
+        <v>1.3000000000000007</v>
       </c>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.2">
@@ -6408,13 +6438,28 @@
       <c r="N18" s="12" t="s">
         <v>502</v>
       </c>
-      <c r="W18" t="e">
+      <c r="P18">
+        <v>25.8</v>
+      </c>
+      <c r="Q18">
+        <v>29.4</v>
+      </c>
+      <c r="R18">
+        <v>28.7</v>
+      </c>
+      <c r="S18">
+        <v>32.200000000000003</v>
+      </c>
+      <c r="T18">
+        <v>29.4</v>
+      </c>
+      <c r="W18">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>29.924999999999997</v>
       </c>
       <c r="X18">
         <f t="shared" si="3"/>
-        <v>-22.1</v>
+        <v>3.6999999999999993</v>
       </c>
     </row>
     <row r="19" spans="1:27" x14ac:dyDescent="0.2">
@@ -6534,13 +6579,28 @@
       <c r="L21" s="12"/>
       <c r="M21" s="12"/>
       <c r="N21" s="12"/>
-      <c r="W21" t="e">
+      <c r="P21">
+        <v>33.1</v>
+      </c>
+      <c r="Q21">
+        <v>26.1</v>
+      </c>
+      <c r="R21">
+        <v>24.4</v>
+      </c>
+      <c r="S21">
+        <v>22.5</v>
+      </c>
+      <c r="T21">
+        <v>25.5</v>
+      </c>
+      <c r="W21">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>24.625</v>
       </c>
       <c r="X21">
         <f t="shared" si="3"/>
-        <v>-30.9</v>
+        <v>2.2000000000000028</v>
       </c>
     </row>
     <row r="22" spans="1:27" x14ac:dyDescent="0.2">
@@ -6568,13 +6628,28 @@
       <c r="L22" s="12"/>
       <c r="M22" s="12"/>
       <c r="N22" s="12"/>
-      <c r="W22" t="e">
+      <c r="P22">
+        <v>32.9</v>
+      </c>
+      <c r="Q22">
+        <v>28.3</v>
+      </c>
+      <c r="R22">
+        <v>25.7</v>
+      </c>
+      <c r="S22">
+        <v>24.4</v>
+      </c>
+      <c r="T22">
+        <v>25.5</v>
+      </c>
+      <c r="W22">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>25.975000000000001</v>
       </c>
       <c r="X22">
         <f t="shared" si="3"/>
-        <v>-30.9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:27" x14ac:dyDescent="0.2">
@@ -6604,13 +6679,28 @@
       <c r="L23" s="12"/>
       <c r="M23" s="12"/>
       <c r="N23" s="12"/>
-      <c r="W23" t="e">
+      <c r="P23">
+        <v>24.2</v>
+      </c>
+      <c r="Q23">
+        <v>26.7</v>
+      </c>
+      <c r="R23">
+        <v>26.2</v>
+      </c>
+      <c r="S23">
+        <v>28.8</v>
+      </c>
+      <c r="T23">
+        <v>22.4</v>
+      </c>
+      <c r="W23">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>26.024999999999999</v>
       </c>
       <c r="X23">
         <f t="shared" si="3"/>
-        <v>-21</v>
+        <v>3.1999999999999993</v>
       </c>
     </row>
     <row r="24" spans="1:27" x14ac:dyDescent="0.2">
@@ -6652,7 +6742,7 @@
       </c>
       <c r="W24">
         <f>AVERAGE(Q23:T24)</f>
-        <v>30.033333333333331</v>
+        <v>27.74285714285714</v>
       </c>
       <c r="X24">
         <f t="shared" si="3"/>
@@ -6805,13 +6895,28 @@
       <c r="L28" s="12"/>
       <c r="M28" s="12"/>
       <c r="N28" s="12"/>
-      <c r="W28" t="e">
+      <c r="P28">
+        <v>28.7</v>
+      </c>
+      <c r="Q28">
+        <v>23.3</v>
+      </c>
+      <c r="R28">
+        <v>23.2</v>
+      </c>
+      <c r="S28">
+        <v>25.2</v>
+      </c>
+      <c r="T28">
+        <v>41</v>
+      </c>
+      <c r="W28">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>28.175000000000001</v>
       </c>
       <c r="X28">
         <f t="shared" si="3"/>
-        <v>-27.7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:27" x14ac:dyDescent="0.2">
@@ -6911,13 +7016,28 @@
       <c r="L31" s="12"/>
       <c r="M31" s="12"/>
       <c r="N31" s="12"/>
-      <c r="W31" t="e">
+      <c r="P31">
+        <v>37.1</v>
+      </c>
+      <c r="Q31">
+        <v>24.3</v>
+      </c>
+      <c r="R31">
+        <v>25.7</v>
+      </c>
+      <c r="S31">
+        <v>23.3</v>
+      </c>
+      <c r="T31">
+        <v>22</v>
+      </c>
+      <c r="W31">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>23.824999999999999</v>
       </c>
       <c r="X31">
         <f t="shared" si="3"/>
-        <v>-35.200000000000003</v>
+        <v>1.8999999999999986</v>
       </c>
     </row>
     <row r="32" spans="1:27" x14ac:dyDescent="0.2">
@@ -7113,13 +7233,28 @@
       <c r="L36" s="12"/>
       <c r="M36" s="12"/>
       <c r="N36" s="12"/>
-      <c r="W36" t="e">
+      <c r="P36">
+        <v>31</v>
+      </c>
+      <c r="Q36">
+        <v>28.9</v>
+      </c>
+      <c r="R36">
+        <v>27.3</v>
+      </c>
+      <c r="S36">
+        <v>27.9</v>
+      </c>
+      <c r="T36">
+        <v>25.6</v>
+      </c>
+      <c r="W36">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>27.424999999999997</v>
       </c>
       <c r="X36">
         <f t="shared" si="3"/>
-        <v>-28.8</v>
+        <v>2.1999999999999993</v>
       </c>
     </row>
     <row r="37" spans="1:27" x14ac:dyDescent="0.2">
@@ -7463,13 +7598,28 @@
       <c r="L46" s="12"/>
       <c r="M46" s="12"/>
       <c r="N46" s="12"/>
-      <c r="W46" t="e">
+      <c r="P46">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="Q46">
+        <v>22.1</v>
+      </c>
+      <c r="R46">
+        <v>20.3</v>
+      </c>
+      <c r="S46">
+        <v>20.9</v>
+      </c>
+      <c r="T46">
+        <v>20.3</v>
+      </c>
+      <c r="W46">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>20.900000000000002</v>
       </c>
       <c r="X46">
         <f t="shared" si="3"/>
-        <v>-33</v>
+        <v>2.2000000000000028</v>
       </c>
     </row>
     <row r="47" spans="1:27" x14ac:dyDescent="0.2">
@@ -8433,13 +8583,28 @@
       <c r="N66" s="12" t="s">
         <v>509</v>
       </c>
-      <c r="W66" t="e">
+      <c r="P66">
+        <v>59.2</v>
+      </c>
+      <c r="Q66">
+        <v>33.9</v>
+      </c>
+      <c r="R66">
+        <v>35.9</v>
+      </c>
+      <c r="S66">
+        <v>50.6</v>
+      </c>
+      <c r="T66">
+        <v>40.6</v>
+      </c>
+      <c r="W66">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>40.25</v>
       </c>
       <c r="X66">
         <f t="shared" si="3"/>
-        <v>-46.5</v>
+        <v>12.700000000000003</v>
       </c>
     </row>
     <row r="67" spans="1:27" x14ac:dyDescent="0.2">
@@ -8471,13 +8636,28 @@
       <c r="N67" s="12" t="s">
         <v>510</v>
       </c>
-      <c r="W67" t="e">
+      <c r="P67">
+        <v>24.6</v>
+      </c>
+      <c r="Q67">
+        <v>21.4</v>
+      </c>
+      <c r="R67">
+        <v>34.5</v>
+      </c>
+      <c r="S67">
+        <v>32.299999999999997</v>
+      </c>
+      <c r="T67">
+        <v>25</v>
+      </c>
+      <c r="W67">
         <f t="shared" ref="W67:W130" si="4">AVERAGE(Q67:T67)</f>
-        <v>#DIV/0!</v>
+        <v>28.299999999999997</v>
       </c>
       <c r="X67">
         <f t="shared" ref="X67:X130" si="5">P67-D67</f>
-        <v>-17.100000000000001</v>
+        <v>7.5</v>
       </c>
     </row>
     <row r="68" spans="1:27" x14ac:dyDescent="0.2">
@@ -9245,13 +9425,28 @@
       <c r="N83" s="12" t="s">
         <v>512</v>
       </c>
-      <c r="W83" t="e">
+      <c r="P83">
+        <v>30.2</v>
+      </c>
+      <c r="Q83">
+        <v>40.799999999999997</v>
+      </c>
+      <c r="R83">
+        <v>37.4</v>
+      </c>
+      <c r="S83">
+        <v>35.9</v>
+      </c>
+      <c r="T83">
+        <v>33.200000000000003</v>
+      </c>
+      <c r="W83">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>36.825000000000003</v>
       </c>
       <c r="X83">
         <f t="shared" si="5"/>
-        <v>-29</v>
+        <v>1.1999999999999993</v>
       </c>
     </row>
     <row r="84" spans="1:27" x14ac:dyDescent="0.2">
@@ -9673,13 +9868,28 @@
       <c r="L93" s="12"/>
       <c r="M93" s="12"/>
       <c r="N93" s="12"/>
-      <c r="W93" t="e">
+      <c r="P93">
+        <v>30.8</v>
+      </c>
+      <c r="Q93">
+        <v>33.5</v>
+      </c>
+      <c r="R93">
+        <v>34.9</v>
+      </c>
+      <c r="S93">
+        <v>34.4</v>
+      </c>
+      <c r="T93">
+        <v>33.5</v>
+      </c>
+      <c r="W93">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>34.075000000000003</v>
       </c>
       <c r="X93">
         <f t="shared" si="5"/>
-        <v>-25.5</v>
+        <v>5.3000000000000007</v>
       </c>
     </row>
     <row r="94" spans="1:27" x14ac:dyDescent="0.2">
@@ -9761,13 +9971,28 @@
       <c r="L95" s="12"/>
       <c r="M95" s="12"/>
       <c r="N95" s="12"/>
-      <c r="W95" t="e">
+      <c r="P95">
+        <v>41.4</v>
+      </c>
+      <c r="Q95">
+        <v>29.5</v>
+      </c>
+      <c r="R95">
+        <v>36</v>
+      </c>
+      <c r="S95">
+        <v>33</v>
+      </c>
+      <c r="T95">
+        <v>29.6</v>
+      </c>
+      <c r="W95">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>32.024999999999999</v>
       </c>
       <c r="X95">
         <f t="shared" si="5"/>
-        <v>-28.3</v>
+        <v>13.099999999999998</v>
       </c>
     </row>
     <row r="96" spans="1:27" x14ac:dyDescent="0.2">
@@ -9795,13 +10020,28 @@
       <c r="L96" s="12"/>
       <c r="M96" s="12"/>
       <c r="N96" s="12"/>
-      <c r="W96" t="e">
+      <c r="P96">
+        <v>37.9</v>
+      </c>
+      <c r="Q96">
+        <v>39.9</v>
+      </c>
+      <c r="R96">
+        <v>42.6</v>
+      </c>
+      <c r="S96">
+        <v>41.8</v>
+      </c>
+      <c r="T96">
+        <v>37.799999999999997</v>
+      </c>
+      <c r="W96">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>40.524999999999999</v>
       </c>
       <c r="X96">
         <f t="shared" si="5"/>
-        <v>-33.1</v>
+        <v>4.7999999999999972</v>
       </c>
     </row>
     <row r="97" spans="1:27" x14ac:dyDescent="0.2">
@@ -9831,13 +10071,28 @@
       <c r="L97" s="12"/>
       <c r="M97" s="12"/>
       <c r="N97" s="12"/>
-      <c r="W97" t="e">
+      <c r="P97">
+        <v>36.799999999999997</v>
+      </c>
+      <c r="Q97">
+        <v>37.299999999999997</v>
+      </c>
+      <c r="R97">
+        <v>37.9</v>
+      </c>
+      <c r="S97">
+        <v>36.6</v>
+      </c>
+      <c r="T97">
+        <v>32.6</v>
+      </c>
+      <c r="W97">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>36.099999999999994</v>
       </c>
       <c r="X97">
         <f t="shared" si="5"/>
-        <v>-23.4</v>
+        <v>13.399999999999999</v>
       </c>
     </row>
     <row r="98" spans="1:27" x14ac:dyDescent="0.2">
@@ -19430,13 +19685,28 @@
       <c r="L300" s="12"/>
       <c r="M300" s="12"/>
       <c r="N300" s="12"/>
-      <c r="W300" t="e">
+      <c r="P300">
+        <v>21.4</v>
+      </c>
+      <c r="Q300">
+        <v>22.4</v>
+      </c>
+      <c r="R300">
+        <v>34.6</v>
+      </c>
+      <c r="S300">
+        <v>21.9</v>
+      </c>
+      <c r="T300">
+        <v>26.6</v>
+      </c>
+      <c r="W300">
         <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
+        <v>26.375</v>
       </c>
       <c r="X300">
         <f t="shared" si="12"/>
-        <v>-21.8</v>
+        <v>-0.40000000000000213</v>
       </c>
     </row>
     <row r="301" spans="1:27" x14ac:dyDescent="0.2">
@@ -23858,13 +24128,28 @@
       <c r="L397" s="12"/>
       <c r="M397" s="12"/>
       <c r="N397" s="12"/>
-      <c r="W397" t="e">
+      <c r="P397">
+        <v>61.4</v>
+      </c>
+      <c r="Q397">
+        <v>29.9</v>
+      </c>
+      <c r="R397">
+        <v>27.8</v>
+      </c>
+      <c r="S397">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="T397">
+        <v>28.5</v>
+      </c>
+      <c r="W397">
         <f t="shared" si="16"/>
-        <v>#DIV/0!</v>
+        <v>25.65</v>
       </c>
       <c r="X397">
         <f t="shared" si="17"/>
-        <v>-56.6</v>
+        <v>4.7999999999999972</v>
       </c>
     </row>
     <row r="398" spans="1:27" x14ac:dyDescent="0.2">
@@ -24164,13 +24449,28 @@
       <c r="N403" s="12" t="s">
         <v>531</v>
       </c>
-      <c r="W403" t="e">
+      <c r="P403">
+        <v>56.6</v>
+      </c>
+      <c r="Q403">
+        <v>21.6</v>
+      </c>
+      <c r="R403">
+        <v>9.5</v>
+      </c>
+      <c r="S403">
+        <v>21.2</v>
+      </c>
+      <c r="T403">
+        <v>18.7</v>
+      </c>
+      <c r="W403">
         <f t="shared" si="16"/>
-        <v>#DIV/0!</v>
+        <v>17.75</v>
       </c>
       <c r="X403">
         <f t="shared" si="17"/>
-        <v>-50.9</v>
+        <v>5.7000000000000028</v>
       </c>
     </row>
     <row r="404" spans="1:27" x14ac:dyDescent="0.2">
@@ -24362,13 +24662,28 @@
       <c r="L407" s="12"/>
       <c r="M407" s="12"/>
       <c r="N407" s="12"/>
-      <c r="W407" t="e">
+      <c r="P407">
+        <v>53.6</v>
+      </c>
+      <c r="Q407">
+        <v>24.3</v>
+      </c>
+      <c r="R407">
+        <v>21.8</v>
+      </c>
+      <c r="S407">
+        <v>25</v>
+      </c>
+      <c r="T407">
+        <v>20.8</v>
+      </c>
+      <c r="W407">
         <f t="shared" si="16"/>
-        <v>#DIV/0!</v>
+        <v>22.974999999999998</v>
       </c>
       <c r="X407">
         <f t="shared" si="17"/>
-        <v>-58.3</v>
+        <v>-4.6999999999999957</v>
       </c>
     </row>
     <row r="408" spans="1:27" x14ac:dyDescent="0.2">
@@ -24662,13 +24977,28 @@
       <c r="L413" s="12"/>
       <c r="M413" s="12"/>
       <c r="N413" s="12"/>
-      <c r="W413" t="e">
+      <c r="P413">
+        <v>49.9</v>
+      </c>
+      <c r="Q413">
+        <v>32.6</v>
+      </c>
+      <c r="R413">
+        <v>33.200000000000003</v>
+      </c>
+      <c r="S413">
+        <v>31.8</v>
+      </c>
+      <c r="T413">
+        <v>33.700000000000003</v>
+      </c>
+      <c r="W413">
         <f t="shared" si="16"/>
-        <v>#DIV/0!</v>
+        <v>32.825000000000003</v>
       </c>
       <c r="X413">
         <f t="shared" si="17"/>
-        <v>-44.1</v>
+        <v>5.7999999999999972</v>
       </c>
     </row>
     <row r="414" spans="1:27" x14ac:dyDescent="0.2">
@@ -25020,13 +25350,28 @@
       <c r="L421" s="12"/>
       <c r="M421" s="12"/>
       <c r="N421" s="12"/>
-      <c r="W421" t="e">
+      <c r="P421">
+        <v>50.6</v>
+      </c>
+      <c r="Q421">
+        <v>19.7</v>
+      </c>
+      <c r="R421">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="S421">
+        <v>21.6</v>
+      </c>
+      <c r="T421">
+        <v>22.9</v>
+      </c>
+      <c r="W421">
         <f t="shared" si="16"/>
-        <v>#DIV/0!</v>
+        <v>21.074999999999999</v>
       </c>
       <c r="X421">
         <f t="shared" si="17"/>
-        <v>-46.8</v>
+        <v>3.8000000000000043</v>
       </c>
     </row>
     <row r="422" spans="1:27" x14ac:dyDescent="0.2">
@@ -25264,13 +25609,28 @@
       <c r="L428" s="12"/>
       <c r="M428" s="12"/>
       <c r="N428" s="12"/>
-      <c r="W428" t="e">
+      <c r="P428">
+        <v>46.8</v>
+      </c>
+      <c r="Q428">
+        <v>21.2</v>
+      </c>
+      <c r="R428">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="S428">
+        <v>22.2</v>
+      </c>
+      <c r="T428">
+        <v>19.100000000000001</v>
+      </c>
+      <c r="W428">
         <f t="shared" si="16"/>
-        <v>#DIV/0!</v>
+        <v>19.850000000000001</v>
       </c>
       <c r="X428">
         <f t="shared" si="17"/>
-        <v>-40.5</v>
+        <v>6.2999999999999972</v>
       </c>
     </row>
     <row r="429" spans="1:27" x14ac:dyDescent="0.2">
@@ -25402,13 +25762,28 @@
       <c r="L432" s="29"/>
       <c r="M432" s="29"/>
       <c r="N432" s="29"/>
-      <c r="W432" t="e">
+      <c r="P432" s="5">
+        <v>48</v>
+      </c>
+      <c r="Q432" s="5">
+        <v>25.7</v>
+      </c>
+      <c r="R432" s="5">
+        <v>27.4</v>
+      </c>
+      <c r="S432" s="5">
+        <v>24</v>
+      </c>
+      <c r="T432" s="5">
+        <v>22.8</v>
+      </c>
+      <c r="W432">
         <f t="shared" si="16"/>
-        <v>#DIV/0!</v>
+        <v>24.974999999999998</v>
       </c>
       <c r="X432">
         <f t="shared" si="17"/>
-        <v>-42.9</v>
+        <v>5.1000000000000014</v>
       </c>
       <c r="AA432"/>
     </row>
@@ -25745,13 +26120,28 @@
       <c r="L439" s="12"/>
       <c r="M439" s="12"/>
       <c r="N439" s="12"/>
-      <c r="W439" t="e">
+      <c r="P439">
+        <v>30.6</v>
+      </c>
+      <c r="Q439">
+        <v>21.9</v>
+      </c>
+      <c r="R439">
+        <v>22</v>
+      </c>
+      <c r="S439">
+        <v>26.2</v>
+      </c>
+      <c r="T439">
+        <v>21.8</v>
+      </c>
+      <c r="W439">
         <f t="shared" si="16"/>
-        <v>#DIV/0!</v>
+        <v>22.974999999999998</v>
       </c>
       <c r="X439">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>30.6</v>
       </c>
     </row>
     <row r="440" spans="1:27" x14ac:dyDescent="0.2">
@@ -25967,13 +26357,28 @@
       <c r="L444" s="12"/>
       <c r="M444" s="12"/>
       <c r="N444" s="12"/>
-      <c r="W444" t="e">
+      <c r="P444">
+        <v>16.8</v>
+      </c>
+      <c r="Q444">
+        <v>22.5</v>
+      </c>
+      <c r="R444">
+        <v>17.8</v>
+      </c>
+      <c r="S444">
+        <v>20.9</v>
+      </c>
+      <c r="T444">
+        <v>19.3</v>
+      </c>
+      <c r="W444">
         <f t="shared" si="16"/>
-        <v>#DIV/0!</v>
+        <v>20.125</v>
       </c>
       <c r="X444">
         <f t="shared" si="17"/>
-        <v>-22.2</v>
+        <v>-5.3999999999999986</v>
       </c>
     </row>
     <row r="445" spans="1:27" x14ac:dyDescent="0.2">
@@ -26003,13 +26408,28 @@
       <c r="L445" s="12"/>
       <c r="M445" s="12"/>
       <c r="N445" s="12"/>
-      <c r="W445" t="e">
+      <c r="P445">
+        <v>21.3</v>
+      </c>
+      <c r="Q445">
+        <v>23.4</v>
+      </c>
+      <c r="R445">
+        <v>21.2</v>
+      </c>
+      <c r="S445">
+        <v>27.6</v>
+      </c>
+      <c r="T445">
+        <v>20.9</v>
+      </c>
+      <c r="W445">
         <f t="shared" si="16"/>
-        <v>#DIV/0!</v>
+        <v>23.274999999999999</v>
       </c>
       <c r="X445">
         <f t="shared" si="17"/>
-        <v>-18</v>
+        <v>3.3000000000000007</v>
       </c>
     </row>
     <row r="446" spans="1:27" x14ac:dyDescent="0.2">
@@ -26037,13 +26457,28 @@
       <c r="L446" s="12"/>
       <c r="M446" s="12"/>
       <c r="N446" s="12"/>
-      <c r="W446" t="e">
+      <c r="P446">
+        <v>28.2</v>
+      </c>
+      <c r="Q446">
+        <v>21.5</v>
+      </c>
+      <c r="R446">
+        <v>22.8</v>
+      </c>
+      <c r="S446">
+        <v>26.5</v>
+      </c>
+      <c r="T446">
+        <v>26.1</v>
+      </c>
+      <c r="W446">
         <f t="shared" si="16"/>
-        <v>#DIV/0!</v>
+        <v>24.225000000000001</v>
       </c>
       <c r="X446">
         <f t="shared" si="17"/>
-        <v>-27.6</v>
+        <v>0.59999999999999787</v>
       </c>
     </row>
     <row r="447" spans="1:27" x14ac:dyDescent="0.2">
@@ -26591,13 +27026,28 @@
       <c r="L457" s="12"/>
       <c r="M457" s="12"/>
       <c r="N457" s="12"/>
-      <c r="W457" t="e">
+      <c r="P457">
+        <v>27.3</v>
+      </c>
+      <c r="Q457">
+        <v>29.8</v>
+      </c>
+      <c r="R457">
+        <v>32.6</v>
+      </c>
+      <c r="S457">
+        <v>26.2</v>
+      </c>
+      <c r="T457">
+        <v>18.7</v>
+      </c>
+      <c r="W457">
         <f t="shared" si="18"/>
-        <v>#DIV/0!</v>
+        <v>26.825000000000003</v>
       </c>
       <c r="X457">
         <f t="shared" si="19"/>
-        <v>-27</v>
+        <v>0.30000000000000071</v>
       </c>
     </row>
     <row r="458" spans="1:27" x14ac:dyDescent="0.2">
@@ -26731,13 +27181,28 @@
       <c r="L460" s="12"/>
       <c r="M460" s="12"/>
       <c r="N460" s="12"/>
-      <c r="W460" t="e">
+      <c r="P460">
+        <v>35.1</v>
+      </c>
+      <c r="Q460">
+        <v>26</v>
+      </c>
+      <c r="R460">
+        <v>23.2</v>
+      </c>
+      <c r="S460">
+        <v>26.5</v>
+      </c>
+      <c r="T460">
+        <v>23</v>
+      </c>
+      <c r="W460">
         <f t="shared" si="18"/>
-        <v>#DIV/0!</v>
+        <v>24.675000000000001</v>
       </c>
       <c r="X460">
         <f t="shared" si="19"/>
-        <v>-34.299999999999997</v>
+        <v>0.80000000000000426</v>
       </c>
     </row>
     <row r="461" spans="1:27" x14ac:dyDescent="0.2">
@@ -26979,13 +27444,28 @@
       <c r="L465" s="12"/>
       <c r="M465" s="12"/>
       <c r="N465" s="12"/>
-      <c r="W465" t="e">
+      <c r="P465">
+        <v>31</v>
+      </c>
+      <c r="Q465">
+        <v>24.7</v>
+      </c>
+      <c r="R465">
+        <v>22.5</v>
+      </c>
+      <c r="S465">
+        <v>25.8</v>
+      </c>
+      <c r="T465">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="W465">
         <f t="shared" si="18"/>
-        <v>#DIV/0!</v>
+        <v>22.725000000000001</v>
       </c>
       <c r="X465">
         <f t="shared" si="19"/>
-        <v>-30.7</v>
+        <v>0.30000000000000071</v>
       </c>
     </row>
     <row r="466" spans="1:27" x14ac:dyDescent="0.2">
@@ -27389,13 +27869,28 @@
       <c r="L474" s="12"/>
       <c r="M474" s="12"/>
       <c r="N474" s="12"/>
-      <c r="W474" t="e">
+      <c r="P474">
+        <v>27.3</v>
+      </c>
+      <c r="Q474">
+        <v>19.7</v>
+      </c>
+      <c r="R474">
+        <v>20.8</v>
+      </c>
+      <c r="S474">
+        <v>27.4</v>
+      </c>
+      <c r="T474">
+        <v>21.5</v>
+      </c>
+      <c r="W474">
         <f t="shared" si="18"/>
-        <v>#DIV/0!</v>
+        <v>22.35</v>
       </c>
       <c r="X474">
         <f t="shared" si="19"/>
-        <v>-23</v>
+        <v>4.3000000000000007</v>
       </c>
     </row>
     <row r="475" spans="1:27" x14ac:dyDescent="0.2">
@@ -27425,13 +27920,28 @@
       <c r="L475" s="12"/>
       <c r="M475" s="12"/>
       <c r="N475" s="12"/>
-      <c r="W475" t="e">
+      <c r="P475">
+        <v>21.4</v>
+      </c>
+      <c r="Q475">
+        <v>20.7</v>
+      </c>
+      <c r="R475">
+        <v>26</v>
+      </c>
+      <c r="S475">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="T475">
+        <v>19.2</v>
+      </c>
+      <c r="W475">
         <f t="shared" si="18"/>
-        <v>#DIV/0!</v>
+        <v>21.45</v>
       </c>
       <c r="X475">
         <f t="shared" si="19"/>
-        <v>-28.3</v>
+        <v>-6.9000000000000021</v>
       </c>
     </row>
     <row r="476" spans="1:27" x14ac:dyDescent="0.2">
@@ -27709,13 +28219,28 @@
       <c r="L481" s="12"/>
       <c r="M481" s="12"/>
       <c r="N481" s="12"/>
-      <c r="W481" t="e">
+      <c r="P481">
+        <v>30.5</v>
+      </c>
+      <c r="Q481">
+        <v>24.4</v>
+      </c>
+      <c r="R481">
+        <v>25.7</v>
+      </c>
+      <c r="S481">
+        <v>26</v>
+      </c>
+      <c r="T481">
+        <v>24.4</v>
+      </c>
+      <c r="W481">
         <f t="shared" si="18"/>
-        <v>#DIV/0!</v>
+        <v>25.125</v>
       </c>
       <c r="X481">
         <f t="shared" si="19"/>
-        <v>-29.1</v>
+        <v>1.3999999999999986</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
lots of fruitless work
</commit_message>
<xml_diff>
--- a/data/observation_datasheet.xlsx
+++ b/data/observation_datasheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/catchamberlain/Documents/git/chillfreeze/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCD554A7-FF96-184B-9A53-34B4312DFA0D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49BA412C-B069-9B4C-AB72-AE66F2F88E53}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4800" yWindow="460" windowWidth="30980" windowHeight="20960" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5492,10 +5492,10 @@
   <dimension ref="A1:AD481"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="P411" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="P422" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AD450" sqref="AD450"/>
+      <selection pane="bottomRight" activeCell="AD466" sqref="AD466"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6468,7 +6468,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A17" s="14" t="s">
         <v>18</v>
       </c>
@@ -6522,7 +6522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A18" s="19" t="s">
         <v>19</v>
       </c>
@@ -6572,8 +6572,14 @@
         <f t="shared" si="3"/>
         <v>3.6999999999999993</v>
       </c>
-    </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AC18">
+        <v>0.09</v>
+      </c>
+      <c r="AD18">
+        <v>8.2000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A19" s="19" t="s">
         <v>20</v>
       </c>
@@ -6610,8 +6616,14 @@
         <f t="shared" si="3"/>
         <v>-27.9</v>
       </c>
-    </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AC19">
+        <v>0.114</v>
+      </c>
+      <c r="AD19">
+        <v>0.10199999999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A20" s="19" t="s">
         <v>21</v>
       </c>
@@ -6662,8 +6674,14 @@
       <c r="AA20">
         <v>9.1000000000000004E-3</v>
       </c>
-    </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AC20">
+        <v>0.106</v>
+      </c>
+      <c r="AD20">
+        <v>0.105</v>
+      </c>
+    </row>
+    <row r="21" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A21" s="19" t="s">
         <v>22</v>
       </c>
@@ -6713,8 +6731,14 @@
         <f t="shared" si="3"/>
         <v>2.2000000000000028</v>
       </c>
-    </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AC21">
+        <v>0.114</v>
+      </c>
+      <c r="AD21">
+        <v>0.107</v>
+      </c>
+    </row>
+    <row r="22" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A22" s="19" t="s">
         <v>23</v>
       </c>
@@ -6762,8 +6786,14 @@
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AC22">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="AD22">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="23" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A23" s="19" t="s">
         <v>24</v>
       </c>
@@ -6813,8 +6843,14 @@
         <f t="shared" si="3"/>
         <v>3.1999999999999993</v>
       </c>
-    </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AC23">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="AD23">
+        <v>0.105</v>
+      </c>
+    </row>
+    <row r="24" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A24" s="19" t="s">
         <v>25</v>
       </c>
@@ -6862,8 +6898,14 @@
       <c r="AA24">
         <v>1.2800000000000001E-2</v>
       </c>
-    </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AC24">
+        <v>0.107</v>
+      </c>
+      <c r="AD24">
+        <v>9.9000000000000005E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A25" s="19" t="s">
         <v>26</v>
       </c>
@@ -6907,8 +6949,14 @@
         <f t="shared" si="3"/>
         <v>0.89999999999999858</v>
       </c>
-    </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AC25">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="AD25">
+        <v>9.1999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A26" s="19" t="s">
         <v>27</v>
       </c>
@@ -6956,8 +7004,14 @@
         <f>P29-D26</f>
         <v>2.5</v>
       </c>
-    </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AC26">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="AD26">
+        <v>0.16900000000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A27" s="19" t="s">
         <v>28</v>
       </c>
@@ -7004,8 +7058,14 @@
       <c r="AA27">
         <v>3.7000000000000002E-3</v>
       </c>
-    </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AC27">
+        <v>0.107</v>
+      </c>
+      <c r="AD27">
+        <v>0.127</v>
+      </c>
+    </row>
+    <row r="28" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A28" s="19" t="s">
         <v>29</v>
       </c>
@@ -7053,8 +7113,14 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AC28">
+        <v>8.6999999999999994E-2</v>
+      </c>
+      <c r="AD28">
+        <v>9.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A29" s="19" t="s">
         <v>30</v>
       </c>
@@ -7098,8 +7164,14 @@
         <f>P26-D29</f>
         <v>2.1999999999999993</v>
       </c>
-    </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AC29">
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="AD29">
+        <v>8.5999999999999993E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A30" s="19" t="s">
         <v>31</v>
       </c>
@@ -7132,8 +7204,14 @@
         <f t="shared" si="3"/>
         <v>-19.100000000000001</v>
       </c>
-    </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AC30">
+        <v>9.7000000000000003E-2</v>
+      </c>
+      <c r="AD30">
+        <v>0.10299999999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A31" s="19" t="s">
         <v>32</v>
       </c>
@@ -7183,8 +7261,14 @@
         <f t="shared" si="3"/>
         <v>1.8999999999999986</v>
       </c>
-    </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AC31">
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="AD31">
+        <v>8.8999999999999996E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A32" s="19" t="s">
         <v>33</v>
       </c>
@@ -7229,8 +7313,14 @@
       <c r="AA32">
         <v>4.1999999999999997E-3</v>
       </c>
-    </row>
-    <row r="33" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AC32">
+        <v>9.2999999999999999E-2</v>
+      </c>
+      <c r="AD32">
+        <v>0.13800000000000001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A33" s="19" t="s">
         <v>34</v>
       </c>
@@ -7277,8 +7367,14 @@
       <c r="AA33">
         <v>3.8999999999999998E-3</v>
       </c>
-    </row>
-    <row r="34" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AC33">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="AD33">
+        <v>8.5000000000000006E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A34" s="22" t="s">
         <v>35</v>
       </c>
@@ -7329,7 +7425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A35" s="22" t="s">
         <v>36</v>
       </c>
@@ -7382,7 +7478,7 @@
         <v>3.6000000000000014</v>
       </c>
     </row>
-    <row r="36" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A36" s="22" t="s">
         <v>37</v>
       </c>
@@ -7431,7 +7527,7 @@
         <v>2.1999999999999993</v>
       </c>
     </row>
-    <row r="37" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A37" s="22" t="s">
         <v>38</v>
       </c>
@@ -7482,7 +7578,7 @@
         <v>1.8999999999999986</v>
       </c>
     </row>
-    <row r="38" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A38" s="22" t="s">
         <v>39</v>
       </c>
@@ -7516,7 +7612,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="39" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A39" s="22" t="s">
         <v>40</v>
       </c>
@@ -7567,7 +7663,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A40" s="22" t="s">
         <v>41</v>
       </c>
@@ -7601,7 +7697,7 @@
         <v>-20.8</v>
       </c>
     </row>
-    <row r="41" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A41" s="22" t="s">
         <v>42</v>
       </c>
@@ -7652,7 +7748,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A42" s="22" t="s">
         <v>43</v>
       </c>
@@ -7686,7 +7782,7 @@
         <v>-20.100000000000001</v>
       </c>
     </row>
-    <row r="43" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A43" s="22" t="s">
         <v>44</v>
       </c>
@@ -7737,7 +7833,7 @@
         <v>1.6000000000000014</v>
       </c>
     </row>
-    <row r="44" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A44" s="22" t="s">
         <v>45</v>
       </c>
@@ -7780,7 +7876,7 @@
         <v>-0.39999999999999858</v>
       </c>
     </row>
-    <row r="45" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A45" s="22" t="s">
         <v>46</v>
       </c>
@@ -7825,7 +7921,7 @@
         <v>1.8999999999999986</v>
       </c>
     </row>
-    <row r="46" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A46" s="22" t="s">
         <v>47</v>
       </c>
@@ -7874,7 +7970,7 @@
         <v>2.2000000000000028</v>
       </c>
     </row>
-    <row r="47" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A47" s="22" t="s">
         <v>48</v>
       </c>
@@ -7910,7 +8006,7 @@
         <v>-31.1</v>
       </c>
     </row>
-    <row r="48" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A48" s="22" t="s">
         <v>49</v>
       </c>
@@ -8949,10 +9045,10 @@
         <v>12.700000000000003</v>
       </c>
       <c r="AC66">
-        <v>0.16500000000000001</v>
+        <v>0.158</v>
       </c>
       <c r="AD66">
-        <v>0.184</v>
+        <v>0.182</v>
       </c>
     </row>
     <row r="67" spans="1:30" x14ac:dyDescent="0.2">
@@ -9006,6 +9102,12 @@
       <c r="X67">
         <f t="shared" ref="X67:X130" si="5">P67-D67</f>
         <v>7.5</v>
+      </c>
+      <c r="AC67">
+        <v>0.14099999999999999</v>
+      </c>
+      <c r="AD67">
+        <v>0.14000000000000001</v>
       </c>
     </row>
     <row r="68" spans="1:30" x14ac:dyDescent="0.2">
@@ -9059,6 +9161,12 @@
       <c r="AA68">
         <v>2.18E-2</v>
       </c>
+      <c r="AC68">
+        <v>0.24099999999999999</v>
+      </c>
+      <c r="AD68">
+        <v>0.20499999999999999</v>
+      </c>
     </row>
     <row r="69" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A69" s="19" t="s">
@@ -9112,6 +9220,12 @@
       </c>
       <c r="AA69">
         <v>1.9800000000000002E-2</v>
+      </c>
+      <c r="AC69">
+        <v>0.158</v>
+      </c>
+      <c r="AD69">
+        <v>0.157</v>
       </c>
     </row>
     <row r="70" spans="1:30" x14ac:dyDescent="0.2">
@@ -9165,6 +9279,12 @@
       <c r="AA70">
         <v>2.06E-2</v>
       </c>
+      <c r="AC70">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="AD70">
+        <v>0.20200000000000001</v>
+      </c>
     </row>
     <row r="71" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A71" s="19" t="s">
@@ -9218,6 +9338,12 @@
       </c>
       <c r="AA71">
         <v>1.9900000000000001E-2</v>
+      </c>
+      <c r="AC71">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="AD71">
+        <v>0.152</v>
       </c>
     </row>
     <row r="72" spans="1:30" x14ac:dyDescent="0.2">
@@ -9301,6 +9427,12 @@
       <c r="AA73">
         <v>1.72E-2</v>
       </c>
+      <c r="AC73">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="AD73">
+        <v>0.14399999999999999</v>
+      </c>
     </row>
     <row r="74" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A74" s="19" t="s">
@@ -9353,6 +9485,12 @@
       <c r="AA74">
         <v>1.49E-2</v>
       </c>
+      <c r="AC74">
+        <v>0.113</v>
+      </c>
+      <c r="AD74">
+        <v>0.16500000000000001</v>
+      </c>
     </row>
     <row r="75" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A75" s="19" t="s">
@@ -9405,6 +9543,12 @@
       <c r="X75">
         <f t="shared" si="5"/>
         <v>-0.10000000000000142</v>
+      </c>
+      <c r="AC75">
+        <v>0.127</v>
+      </c>
+      <c r="AD75">
+        <v>0.17899999999999999</v>
       </c>
     </row>
     <row r="76" spans="1:30" x14ac:dyDescent="0.2">
@@ -9458,6 +9602,12 @@
       <c r="AA76">
         <v>1.4E-2</v>
       </c>
+      <c r="AC76">
+        <v>0.115</v>
+      </c>
+      <c r="AD76">
+        <v>0.129</v>
+      </c>
     </row>
     <row r="77" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A77" s="19" t="s">
@@ -9513,6 +9663,12 @@
       </c>
       <c r="AA77">
         <v>2.0199999999999999E-2</v>
+      </c>
+      <c r="AC77">
+        <v>0.155</v>
+      </c>
+      <c r="AD77">
+        <v>0.152</v>
       </c>
     </row>
     <row r="78" spans="1:30" x14ac:dyDescent="0.2">
@@ -9566,6 +9722,12 @@
       <c r="AA78">
         <v>1.9599999999999999E-2</v>
       </c>
+      <c r="AC78">
+        <v>0.13</v>
+      </c>
+      <c r="AD78">
+        <v>0.26</v>
+      </c>
     </row>
     <row r="79" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A79" s="19" t="s">
@@ -9619,6 +9781,12 @@
       </c>
       <c r="AA79">
         <v>1.54E-2</v>
+      </c>
+      <c r="AC79">
+        <v>0.14699999999999999</v>
+      </c>
+      <c r="AD79">
+        <v>0.153</v>
       </c>
     </row>
     <row r="80" spans="1:30" x14ac:dyDescent="0.2">
@@ -9672,8 +9840,14 @@
       <c r="AA80">
         <v>1.9E-2</v>
       </c>
-    </row>
-    <row r="81" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AC80">
+        <v>0.13</v>
+      </c>
+      <c r="AD80">
+        <v>0.14499999999999999</v>
+      </c>
+    </row>
+    <row r="81" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A81" s="19" t="s">
         <v>82</v>
       </c>
@@ -9726,8 +9900,14 @@
       <c r="AA81">
         <v>0.02</v>
       </c>
-    </row>
-    <row r="82" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AC81">
+        <v>0.127</v>
+      </c>
+      <c r="AD81">
+        <v>0.156</v>
+      </c>
+    </row>
+    <row r="82" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A82" s="25" t="s">
         <v>83</v>
       </c>
@@ -9759,7 +9939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A83" s="22" t="s">
         <v>84</v>
       </c>
@@ -9812,7 +9992,7 @@
         <v>1.1999999999999993</v>
       </c>
     </row>
-    <row r="84" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A84" s="22" t="s">
         <v>85</v>
       </c>
@@ -9866,7 +10046,7 @@
         <v>2.0500000000000001E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A85" s="22" t="s">
         <v>86</v>
       </c>
@@ -9902,7 +10082,7 @@
         <v>-22</v>
       </c>
     </row>
-    <row r="86" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A86" s="22" t="s">
         <v>87</v>
       </c>
@@ -9954,7 +10134,7 @@
         <v>2.1000000000000001E-2</v>
       </c>
     </row>
-    <row r="87" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A87" s="25" t="s">
         <v>88</v>
       </c>
@@ -9982,7 +10162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A88" s="25" t="s">
         <v>89</v>
       </c>
@@ -10010,7 +10190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A89" s="22" t="s">
         <v>90</v>
       </c>
@@ -10064,7 +10244,7 @@
         <v>1.7100000000000001E-2</v>
       </c>
     </row>
-    <row r="90" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A90" s="22" t="s">
         <v>91</v>
       </c>
@@ -10116,7 +10296,7 @@
         <v>2.1499999999999998E-2</v>
       </c>
     </row>
-    <row r="91" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A91" s="22" t="s">
         <v>92</v>
       </c>
@@ -10170,7 +10350,7 @@
         <v>1.5800000000000002E-2</v>
       </c>
     </row>
-    <row r="92" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A92" s="22" t="s">
         <v>93</v>
       </c>
@@ -10219,7 +10399,7 @@
         <v>14.8</v>
       </c>
     </row>
-    <row r="93" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A93" s="22" t="s">
         <v>94</v>
       </c>
@@ -10270,7 +10450,7 @@
         <v>5.3000000000000007</v>
       </c>
     </row>
-    <row r="94" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A94" s="22" t="s">
         <v>95</v>
       </c>
@@ -10322,7 +10502,7 @@
         <v>1.83E-2</v>
       </c>
     </row>
-    <row r="95" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A95" s="22" t="s">
         <v>96</v>
       </c>
@@ -10373,7 +10553,7 @@
         <v>13.099999999999998</v>
       </c>
     </row>
-    <row r="96" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A96" s="22" t="s">
         <v>97</v>
       </c>
@@ -11555,6 +11735,12 @@
       <c r="AA114">
         <v>1.26E-2</v>
       </c>
+      <c r="AC114">
+        <v>0.13</v>
+      </c>
+      <c r="AD114">
+        <v>0.153</v>
+      </c>
     </row>
     <row r="115" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A115" s="19" t="s">
@@ -11608,6 +11794,12 @@
       </c>
       <c r="AA115">
         <v>1.09E-2</v>
+      </c>
+      <c r="AC115">
+        <v>0.157</v>
+      </c>
+      <c r="AD115">
+        <v>0.28000000000000003</v>
       </c>
     </row>
     <row r="116" spans="1:30" x14ac:dyDescent="0.2">
@@ -11661,6 +11853,12 @@
       <c r="AA116">
         <v>1.8599999999999998E-2</v>
       </c>
+      <c r="AC116">
+        <v>0.17699999999999999</v>
+      </c>
+      <c r="AD116">
+        <v>0.18</v>
+      </c>
     </row>
     <row r="117" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A117" s="19" t="s">
@@ -11714,6 +11912,12 @@
       </c>
       <c r="AA117">
         <v>1.06E-2</v>
+      </c>
+      <c r="AC117">
+        <v>0.18</v>
+      </c>
+      <c r="AD117">
+        <v>0.22700000000000001</v>
       </c>
     </row>
     <row r="118" spans="1:30" x14ac:dyDescent="0.2">
@@ -11767,6 +11971,12 @@
       <c r="AA118">
         <v>9.9000000000000008E-3</v>
       </c>
+      <c r="AC118">
+        <v>0.17</v>
+      </c>
+      <c r="AD118">
+        <v>0.17699999999999999</v>
+      </c>
     </row>
     <row r="119" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A119" s="19" t="s">
@@ -11822,6 +12032,12 @@
       </c>
       <c r="AA119">
         <v>1.0699999999999999E-2</v>
+      </c>
+      <c r="AC119">
+        <v>0.152</v>
+      </c>
+      <c r="AD119">
+        <v>0.16500000000000001</v>
       </c>
     </row>
     <row r="120" spans="1:30" x14ac:dyDescent="0.2">
@@ -11875,6 +12091,12 @@
       <c r="AA120">
         <v>8.3999999999999995E-3</v>
       </c>
+      <c r="AC120">
+        <v>0.154</v>
+      </c>
+      <c r="AD120">
+        <v>0.22700000000000001</v>
+      </c>
     </row>
     <row r="121" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A121" s="19" t="s">
@@ -11928,6 +12150,12 @@
       </c>
       <c r="AA121">
         <v>8.8000000000000005E-3</v>
+      </c>
+      <c r="AC121">
+        <v>0.15</v>
+      </c>
+      <c r="AD121">
+        <v>0.159</v>
       </c>
     </row>
     <row r="122" spans="1:30" x14ac:dyDescent="0.2">
@@ -11981,6 +12209,12 @@
       <c r="AA122">
         <v>1.8800000000000001E-2</v>
       </c>
+      <c r="AC122">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="AD122">
+        <v>0.18</v>
+      </c>
     </row>
     <row r="123" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A123" s="19" t="s">
@@ -12036,6 +12270,12 @@
       </c>
       <c r="AA123">
         <v>1.3599999999999999E-2</v>
+      </c>
+      <c r="AC123">
+        <v>0.14399999999999999</v>
+      </c>
+      <c r="AD123">
+        <v>0.17199999999999999</v>
       </c>
     </row>
     <row r="124" spans="1:30" x14ac:dyDescent="0.2">
@@ -12089,6 +12329,12 @@
       <c r="AA124">
         <v>1.12E-2</v>
       </c>
+      <c r="AC124">
+        <v>0.19400000000000001</v>
+      </c>
+      <c r="AD124">
+        <v>0.21</v>
+      </c>
     </row>
     <row r="125" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A125" s="19" t="s">
@@ -12142,6 +12388,12 @@
       </c>
       <c r="AA125">
         <v>8.8999999999999999E-3</v>
+      </c>
+      <c r="AC125">
+        <v>0.14799999999999999</v>
+      </c>
+      <c r="AD125">
+        <v>0.16900000000000001</v>
       </c>
     </row>
     <row r="126" spans="1:30" x14ac:dyDescent="0.2">
@@ -12195,6 +12447,12 @@
       <c r="AA126">
         <v>2.0799999999999999E-2</v>
       </c>
+      <c r="AC126">
+        <v>0.21299999999999999</v>
+      </c>
+      <c r="AD126">
+        <v>0.25700000000000001</v>
+      </c>
     </row>
     <row r="127" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A127" s="19" t="s">
@@ -12248,6 +12506,12 @@
       </c>
       <c r="AA127">
         <v>1.3599999999999999E-2</v>
+      </c>
+      <c r="AC127">
+        <v>0.151</v>
+      </c>
+      <c r="AD127">
+        <v>0.183</v>
       </c>
     </row>
     <row r="128" spans="1:30" x14ac:dyDescent="0.2">
@@ -12301,8 +12565,14 @@
       <c r="AA128">
         <v>7.4999999999999997E-3</v>
       </c>
-    </row>
-    <row r="129" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AC128">
+        <v>0.153</v>
+      </c>
+      <c r="AD128">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="129" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A129" s="19" t="s">
         <v>130</v>
       </c>
@@ -12355,8 +12625,14 @@
       <c r="AA129">
         <v>9.5999999999999992E-3</v>
       </c>
-    </row>
-    <row r="130" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AC129">
+        <v>0.19</v>
+      </c>
+      <c r="AD129">
+        <v>0.19400000000000001</v>
+      </c>
+    </row>
+    <row r="130" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A130" s="22" t="s">
         <v>131</v>
       </c>
@@ -12410,7 +12686,7 @@
         <v>1.6E-2</v>
       </c>
     </row>
-    <row r="131" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A131" s="22" t="s">
         <v>132</v>
       </c>
@@ -12466,7 +12742,7 @@
         <v>1.03E-2</v>
       </c>
     </row>
-    <row r="132" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A132" s="22" t="s">
         <v>133</v>
       </c>
@@ -12520,7 +12796,7 @@
         <v>1.6400000000000001E-2</v>
       </c>
     </row>
-    <row r="133" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A133" s="22" t="s">
         <v>134</v>
       </c>
@@ -12574,7 +12850,7 @@
         <v>1.04E-2</v>
       </c>
     </row>
-    <row r="134" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A134" s="22" t="s">
         <v>135</v>
       </c>
@@ -12626,7 +12902,7 @@
         <v>2.1100000000000001E-2</v>
       </c>
     </row>
-    <row r="135" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A135" s="22" t="s">
         <v>136</v>
       </c>
@@ -12680,7 +12956,7 @@
         <v>7.7999999999999996E-3</v>
       </c>
     </row>
-    <row r="136" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A136" s="22" t="s">
         <v>137</v>
       </c>
@@ -12732,7 +13008,7 @@
         <v>5.4999999999999997E-3</v>
       </c>
     </row>
-    <row r="137" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A137" s="22" t="s">
         <v>138</v>
       </c>
@@ -12786,7 +13062,7 @@
         <v>7.1999999999999998E-3</v>
       </c>
     </row>
-    <row r="138" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A138" s="22" t="s">
         <v>139</v>
       </c>
@@ -12838,7 +13114,7 @@
         <v>1.41E-2</v>
       </c>
     </row>
-    <row r="139" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A139" s="22" t="s">
         <v>140</v>
       </c>
@@ -12892,7 +13168,7 @@
         <v>1.1900000000000001E-2</v>
       </c>
     </row>
-    <row r="140" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A140" s="22" t="s">
         <v>141</v>
       </c>
@@ -12944,7 +13220,7 @@
         <v>1.2E-2</v>
       </c>
     </row>
-    <row r="141" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A141" s="22" t="s">
         <v>142</v>
       </c>
@@ -12998,7 +13274,7 @@
         <v>1.14E-2</v>
       </c>
     </row>
-    <row r="142" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A142" s="22" t="s">
         <v>143</v>
       </c>
@@ -13050,7 +13326,7 @@
         <v>6.4999999999999997E-3</v>
       </c>
     </row>
-    <row r="143" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A143" s="22" t="s">
         <v>144</v>
       </c>
@@ -13103,7 +13379,7 @@
         <v>2.3999999999999986</v>
       </c>
     </row>
-    <row r="144" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A144" s="22" t="s">
         <v>145</v>
       </c>
@@ -14210,6 +14486,12 @@
       <c r="AA162">
         <v>1.7100000000000001E-2</v>
       </c>
+      <c r="AC162">
+        <v>0.13900000000000001</v>
+      </c>
+      <c r="AD162">
+        <v>0.22900000000000001</v>
+      </c>
     </row>
     <row r="163" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A163" s="19" t="s">
@@ -14263,6 +14545,12 @@
       </c>
       <c r="AA163">
         <v>1.29E-2</v>
+      </c>
+      <c r="AC163">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="AD163">
+        <v>0.13200000000000001</v>
       </c>
     </row>
     <row r="164" spans="1:30" x14ac:dyDescent="0.2">
@@ -14316,6 +14604,12 @@
       <c r="AA164">
         <v>1.37E-2</v>
       </c>
+      <c r="AC164">
+        <v>0.151</v>
+      </c>
+      <c r="AD164">
+        <v>0.16</v>
+      </c>
     </row>
     <row r="165" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A165" s="19" t="s">
@@ -14369,6 +14663,12 @@
       </c>
       <c r="AA165">
         <v>1.2200000000000001E-2</v>
+      </c>
+      <c r="AC165">
+        <v>0.16900000000000001</v>
+      </c>
+      <c r="AD165">
+        <v>0.14899999999999999</v>
       </c>
     </row>
     <row r="166" spans="1:30" x14ac:dyDescent="0.2">
@@ -14422,6 +14722,12 @@
       <c r="AA166">
         <v>1.06E-2</v>
       </c>
+      <c r="AC166">
+        <v>0.157</v>
+      </c>
+      <c r="AD166">
+        <v>0.14899999999999999</v>
+      </c>
     </row>
     <row r="167" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A167" s="19" t="s">
@@ -14475,6 +14781,12 @@
       </c>
       <c r="AA167">
         <v>9.1000000000000004E-3</v>
+      </c>
+      <c r="AC167">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="AD167">
+        <v>0.161</v>
       </c>
     </row>
     <row r="168" spans="1:30" x14ac:dyDescent="0.2">
@@ -14528,6 +14840,12 @@
       <c r="AA168">
         <v>9.7999999999999997E-3</v>
       </c>
+      <c r="AC168">
+        <v>0.14099999999999999</v>
+      </c>
+      <c r="AD168">
+        <v>0.188</v>
+      </c>
     </row>
     <row r="169" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A169" s="19" t="s">
@@ -14581,6 +14899,12 @@
       </c>
       <c r="AA169">
         <v>6.4000000000000003E-3</v>
+      </c>
+      <c r="AC169">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="AD169">
+        <v>0.14499999999999999</v>
       </c>
     </row>
     <row r="170" spans="1:30" x14ac:dyDescent="0.2">
@@ -14634,6 +14958,12 @@
       <c r="AA170">
         <v>1.8100000000000002E-2</v>
       </c>
+      <c r="AC170">
+        <v>0.153</v>
+      </c>
+      <c r="AD170">
+        <v>0.18099999999999999</v>
+      </c>
     </row>
     <row r="171" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A171" s="19" t="s">
@@ -14687,6 +15017,12 @@
       </c>
       <c r="AA171">
         <v>1.04E-2</v>
+      </c>
+      <c r="AC171">
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="AD171">
+        <v>0.14299999999999999</v>
       </c>
     </row>
     <row r="172" spans="1:30" x14ac:dyDescent="0.2">
@@ -14740,6 +15076,12 @@
       <c r="AA172">
         <v>1.43E-2</v>
       </c>
+      <c r="AC172">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AD172">
+        <v>0.14299999999999999</v>
+      </c>
     </row>
     <row r="173" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A173" s="19" t="s">
@@ -14793,6 +15135,12 @@
       </c>
       <c r="AA173">
         <v>1.04E-2</v>
+      </c>
+      <c r="AC173">
+        <v>0.153</v>
+      </c>
+      <c r="AD173">
+        <v>0.12</v>
       </c>
     </row>
     <row r="174" spans="1:30" x14ac:dyDescent="0.2">
@@ -14846,6 +15194,12 @@
       <c r="AA174">
         <v>2.76E-2</v>
       </c>
+      <c r="AC174">
+        <v>0.123</v>
+      </c>
+      <c r="AD174">
+        <v>0.15</v>
+      </c>
     </row>
     <row r="175" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A175" s="19" t="s">
@@ -14899,6 +15253,12 @@
       </c>
       <c r="AA175">
         <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="AC175">
+        <v>0.15</v>
+      </c>
+      <c r="AD175">
+        <v>0.13500000000000001</v>
       </c>
     </row>
     <row r="176" spans="1:30" x14ac:dyDescent="0.2">
@@ -14952,8 +15312,14 @@
       <c r="AA176">
         <v>2.3699999999999999E-2</v>
       </c>
-    </row>
-    <row r="177" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AC176">
+        <v>0.154</v>
+      </c>
+      <c r="AD176">
+        <v>0.17199999999999999</v>
+      </c>
+    </row>
+    <row r="177" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A177" s="19" t="s">
         <v>178</v>
       </c>
@@ -15006,8 +15372,14 @@
       <c r="AA177">
         <v>1.37E-2</v>
       </c>
-    </row>
-    <row r="178" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AC177">
+        <v>0.151</v>
+      </c>
+      <c r="AD177">
+        <v>0.16900000000000001</v>
+      </c>
+    </row>
+    <row r="178" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A178" s="22" t="s">
         <v>179</v>
       </c>
@@ -15061,7 +15433,7 @@
         <v>1.14E-2</v>
       </c>
     </row>
-    <row r="179" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A179" s="22" t="s">
         <v>180</v>
       </c>
@@ -15117,7 +15489,7 @@
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="180" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A180" s="22" t="s">
         <v>181</v>
       </c>
@@ -15169,7 +15541,7 @@
         <v>1.29E-2</v>
       </c>
     </row>
-    <row r="181" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A181" s="22" t="s">
         <v>182</v>
       </c>
@@ -15223,7 +15595,7 @@
         <v>1.1599999999999999E-2</v>
       </c>
     </row>
-    <row r="182" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A182" s="22" t="s">
         <v>183</v>
       </c>
@@ -15275,7 +15647,7 @@
         <v>1.0200000000000001E-2</v>
       </c>
     </row>
-    <row r="183" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A183" s="22" t="s">
         <v>184</v>
       </c>
@@ -15329,7 +15701,7 @@
         <v>1.1599999999999999E-2</v>
       </c>
     </row>
-    <row r="184" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A184" s="22" t="s">
         <v>185</v>
       </c>
@@ -15381,7 +15753,7 @@
         <v>2.69E-2</v>
       </c>
     </row>
-    <row r="185" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A185" s="22" t="s">
         <v>186</v>
       </c>
@@ -15435,7 +15807,7 @@
         <v>1.0200000000000001E-2</v>
       </c>
     </row>
-    <row r="186" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A186" s="22" t="s">
         <v>187</v>
       </c>
@@ -15487,7 +15859,7 @@
         <v>9.4999999999999998E-3</v>
       </c>
     </row>
-    <row r="187" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A187" s="22" t="s">
         <v>188</v>
       </c>
@@ -15541,7 +15913,7 @@
         <v>1.41E-2</v>
       </c>
     </row>
-    <row r="188" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A188" s="22" t="s">
         <v>189</v>
       </c>
@@ -15593,7 +15965,7 @@
         <v>1.6899999999999998E-2</v>
       </c>
     </row>
-    <row r="189" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A189" s="22" t="s">
         <v>190</v>
       </c>
@@ -15647,7 +16019,7 @@
         <v>1.0500000000000001E-2</v>
       </c>
     </row>
-    <row r="190" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A190" s="22" t="s">
         <v>191</v>
       </c>
@@ -15699,7 +16071,7 @@
         <v>1.9800000000000002E-2</v>
       </c>
     </row>
-    <row r="191" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A191" s="22" t="s">
         <v>192</v>
       </c>
@@ -15753,7 +16125,7 @@
         <v>1.0800000000000001E-2</v>
       </c>
     </row>
-    <row r="192" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A192" s="22" t="s">
         <v>193</v>
       </c>
@@ -16950,6 +17322,12 @@
       <c r="AA210">
         <v>1.4E-2</v>
       </c>
+      <c r="AC210">
+        <v>0.17299999999999999</v>
+      </c>
+      <c r="AD210">
+        <v>0.19500000000000001</v>
+      </c>
     </row>
     <row r="211" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A211" s="19" t="s">
@@ -17003,6 +17381,12 @@
       </c>
       <c r="AA211">
         <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="AC211">
+        <v>0.12</v>
+      </c>
+      <c r="AD211">
+        <v>0.14799999999999999</v>
       </c>
     </row>
     <row r="212" spans="1:30" x14ac:dyDescent="0.2">
@@ -17056,6 +17440,12 @@
       <c r="AA212">
         <v>7.7999999999999996E-3</v>
       </c>
+      <c r="AC212">
+        <v>0.19</v>
+      </c>
+      <c r="AD212">
+        <v>0.252</v>
+      </c>
     </row>
     <row r="213" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A213" s="19" t="s">
@@ -17111,6 +17501,12 @@
       </c>
       <c r="AA213">
         <v>1.01E-2</v>
+      </c>
+      <c r="AC213">
+        <v>0.115</v>
+      </c>
+      <c r="AD213">
+        <v>0.126</v>
       </c>
     </row>
     <row r="214" spans="1:30" x14ac:dyDescent="0.2">
@@ -17164,6 +17560,12 @@
       <c r="AA214">
         <v>1.5900000000000001E-2</v>
       </c>
+      <c r="AC214">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="AD214">
+        <v>0.17100000000000001</v>
+      </c>
     </row>
     <row r="215" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A215" s="19" t="s">
@@ -17217,6 +17619,12 @@
       </c>
       <c r="AA215">
         <v>1.5800000000000002E-2</v>
+      </c>
+      <c r="AC215">
+        <v>0.18099999999999999</v>
+      </c>
+      <c r="AD215">
+        <v>0.151</v>
       </c>
     </row>
     <row r="216" spans="1:30" x14ac:dyDescent="0.2">
@@ -17270,6 +17678,12 @@
       <c r="AA216">
         <v>1.1900000000000001E-2</v>
       </c>
+      <c r="AC216">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="AD216">
+        <v>0.13</v>
+      </c>
     </row>
     <row r="217" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A217" s="19" t="s">
@@ -17323,6 +17737,12 @@
       </c>
       <c r="AA217">
         <v>1.17E-2</v>
+      </c>
+      <c r="AC217">
+        <v>0.14399999999999999</v>
+      </c>
+      <c r="AD217">
+        <v>0.16800000000000001</v>
       </c>
     </row>
     <row r="218" spans="1:30" x14ac:dyDescent="0.2">
@@ -17376,6 +17796,12 @@
       <c r="AA218">
         <v>1.2800000000000001E-2</v>
       </c>
+      <c r="AC218">
+        <v>0.16900000000000001</v>
+      </c>
+      <c r="AD218">
+        <v>0.19500000000000001</v>
+      </c>
     </row>
     <row r="219" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A219" s="19" t="s">
@@ -17429,6 +17855,12 @@
       </c>
       <c r="AA219">
         <v>1.7500000000000002E-2</v>
+      </c>
+      <c r="AC219">
+        <v>0.16</v>
+      </c>
+      <c r="AD219">
+        <v>0.16200000000000001</v>
       </c>
     </row>
     <row r="220" spans="1:30" x14ac:dyDescent="0.2">
@@ -17482,6 +17914,12 @@
       <c r="AA220">
         <v>8.8999999999999999E-3</v>
       </c>
+      <c r="AC220">
+        <v>0.11700000000000001</v>
+      </c>
+      <c r="AD220">
+        <v>0.14199999999999999</v>
+      </c>
     </row>
     <row r="221" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A221" s="19" t="s">
@@ -17535,6 +17973,12 @@
       </c>
       <c r="AA221">
         <v>1.2800000000000001E-2</v>
+      </c>
+      <c r="AC221">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="AD221">
+        <v>0.17100000000000001</v>
       </c>
     </row>
     <row r="222" spans="1:30" x14ac:dyDescent="0.2">
@@ -17588,6 +18032,12 @@
       <c r="AA222">
         <v>1.41E-2</v>
       </c>
+      <c r="AC222">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="AD222">
+        <v>0.16500000000000001</v>
+      </c>
     </row>
     <row r="223" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A223" s="19" t="s">
@@ -17641,6 +18091,12 @@
       </c>
       <c r="AA223">
         <v>1.9300000000000001E-2</v>
+      </c>
+      <c r="AC223">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="AD223">
+        <v>0.111</v>
       </c>
     </row>
     <row r="224" spans="1:30" x14ac:dyDescent="0.2">
@@ -17694,6 +18150,12 @@
       <c r="AA224">
         <v>1.9300000000000001E-2</v>
       </c>
+      <c r="AC224">
+        <v>0.12</v>
+      </c>
+      <c r="AD224">
+        <v>0.15</v>
+      </c>
     </row>
     <row r="225" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A225" s="19" t="s">
@@ -17747,6 +18209,12 @@
       </c>
       <c r="AA225">
         <v>1.35E-2</v>
+      </c>
+      <c r="AC225">
+        <v>0.108</v>
+      </c>
+      <c r="AD225">
+        <v>0.14699999999999999</v>
       </c>
     </row>
     <row r="226" spans="1:30" x14ac:dyDescent="0.2">
@@ -22844,10 +23312,10 @@
         <v>3.04E-2</v>
       </c>
       <c r="AC354">
-        <v>0.16300000000000001</v>
+        <v>0.13200000000000001</v>
       </c>
       <c r="AD354">
-        <v>0.24099999999999999</v>
+        <v>0.159</v>
       </c>
     </row>
     <row r="355" spans="1:30" x14ac:dyDescent="0.2">
@@ -22904,10 +23372,10 @@
         <v>2.53E-2</v>
       </c>
       <c r="AC355">
-        <v>0.193</v>
+        <v>9.5000000000000001E-2</v>
       </c>
       <c r="AD355">
-        <v>0.19700000000000001</v>
+        <v>0.155</v>
       </c>
     </row>
     <row r="356" spans="1:30" x14ac:dyDescent="0.2">
@@ -22962,10 +23430,10 @@
         <v>3.0499999999999999E-2</v>
       </c>
       <c r="AC356">
-        <v>0.19800000000000001</v>
+        <v>0.156</v>
       </c>
       <c r="AD356">
-        <v>0.191</v>
+        <v>0.157</v>
       </c>
     </row>
     <row r="357" spans="1:30" x14ac:dyDescent="0.2">
@@ -23022,10 +23490,10 @@
         <v>2.0400000000000001E-2</v>
       </c>
       <c r="AC357">
-        <v>0.214</v>
+        <v>0.14899999999999999</v>
       </c>
       <c r="AD357">
-        <v>0.19600000000000001</v>
+        <v>0.155</v>
       </c>
     </row>
     <row r="358" spans="1:30" x14ac:dyDescent="0.2">
@@ -23080,10 +23548,10 @@
         <v>2.7300000000000001E-2</v>
       </c>
       <c r="AC358">
-        <v>0.2</v>
+        <v>0.14499999999999999</v>
       </c>
       <c r="AD358">
-        <v>0.192</v>
+        <v>0.158</v>
       </c>
     </row>
     <row r="359" spans="1:30" x14ac:dyDescent="0.2">
@@ -23140,10 +23608,10 @@
         <v>2.2100000000000002E-2</v>
       </c>
       <c r="AC359">
-        <v>0.18</v>
+        <v>0.13100000000000001</v>
       </c>
       <c r="AD359">
-        <v>0.18</v>
+        <v>0.159</v>
       </c>
     </row>
     <row r="360" spans="1:30" x14ac:dyDescent="0.2">
@@ -23198,10 +23666,10 @@
         <v>2.4799999999999999E-2</v>
       </c>
       <c r="AC360">
-        <v>0.19400000000000001</v>
+        <v>0.13400000000000001</v>
       </c>
       <c r="AD360">
-        <v>0.184</v>
+        <v>0.161</v>
       </c>
     </row>
     <row r="361" spans="1:30" x14ac:dyDescent="0.2">
@@ -23258,10 +23726,10 @@
         <v>2.5899999999999999E-2</v>
       </c>
       <c r="AC361">
-        <v>0.157</v>
+        <v>0.126</v>
       </c>
       <c r="AD361">
-        <v>0.16400000000000001</v>
+        <v>0.14899999999999999</v>
       </c>
     </row>
     <row r="362" spans="1:30" x14ac:dyDescent="0.2">
@@ -23316,10 +23784,10 @@
         <v>2.4E-2</v>
       </c>
       <c r="AC362">
-        <v>0.19800000000000001</v>
+        <v>0.154</v>
       </c>
       <c r="AD362">
-        <v>0.20799999999999999</v>
+        <v>0.159</v>
       </c>
     </row>
     <row r="363" spans="1:30" x14ac:dyDescent="0.2">
@@ -23376,10 +23844,10 @@
         <v>1.4200000000000001E-2</v>
       </c>
       <c r="AC363">
-        <v>0.215</v>
+        <v>0.14299999999999999</v>
       </c>
       <c r="AD363">
-        <v>0.157</v>
+        <v>0.127</v>
       </c>
     </row>
     <row r="364" spans="1:30" x14ac:dyDescent="0.2">
@@ -23434,10 +23902,10 @@
         <v>2.1700000000000001E-2</v>
       </c>
       <c r="AC364">
-        <v>0.184</v>
+        <v>0.13700000000000001</v>
       </c>
       <c r="AD364">
-        <v>0.16900000000000001</v>
+        <v>0.159</v>
       </c>
     </row>
     <row r="365" spans="1:30" x14ac:dyDescent="0.2">
@@ -23494,10 +23962,10 @@
         <v>1.7600000000000001E-2</v>
       </c>
       <c r="AC365">
-        <v>0.17499999999999999</v>
+        <v>0.129</v>
       </c>
       <c r="AD365">
-        <v>0.17</v>
+        <v>0.156</v>
       </c>
     </row>
     <row r="366" spans="1:30" x14ac:dyDescent="0.2">
@@ -23552,10 +24020,10 @@
         <v>3.1600000000000003E-2</v>
       </c>
       <c r="AC366">
-        <v>0.20899999999999999</v>
+        <v>0.14899999999999999</v>
       </c>
       <c r="AD366">
-        <v>0.19800000000000001</v>
+        <v>0.161</v>
       </c>
     </row>
     <row r="367" spans="1:30" x14ac:dyDescent="0.2">
@@ -23612,10 +24080,10 @@
         <v>2.6800000000000001E-2</v>
       </c>
       <c r="AC367">
-        <v>0.18099999999999999</v>
+        <v>0.13100000000000001</v>
       </c>
       <c r="AD367">
-        <v>0.20499999999999999</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="368" spans="1:30" x14ac:dyDescent="0.2">
@@ -23670,10 +24138,10 @@
         <v>2.7E-2</v>
       </c>
       <c r="AC368">
-        <v>0.186</v>
+        <v>0.126</v>
       </c>
       <c r="AD368">
-        <v>0.19500000000000001</v>
+        <v>0.17299999999999999</v>
       </c>
     </row>
     <row r="369" spans="1:30" x14ac:dyDescent="0.2">
@@ -23732,10 +24200,10 @@
         <v>2.5700000000000001E-2</v>
       </c>
       <c r="AC369">
-        <v>0.17</v>
+        <v>0.129</v>
       </c>
       <c r="AD369">
-        <v>0.182</v>
+        <v>0.13200000000000001</v>
       </c>
     </row>
     <row r="370" spans="1:30" x14ac:dyDescent="0.2">
@@ -25540,6 +26008,12 @@
       <c r="AA402">
         <v>6.3E-3</v>
       </c>
+      <c r="AC402">
+        <v>0.114</v>
+      </c>
+      <c r="AD402">
+        <v>0.184</v>
+      </c>
     </row>
     <row r="403" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A403" s="19" t="s">
@@ -25592,6 +26066,12 @@
       <c r="X403">
         <f t="shared" si="17"/>
         <v>5.7000000000000028</v>
+      </c>
+      <c r="AC403">
+        <v>0.105</v>
+      </c>
+      <c r="AD403">
+        <v>0.125</v>
       </c>
     </row>
     <row r="404" spans="1:30" x14ac:dyDescent="0.2">
@@ -25647,6 +26127,12 @@
       <c r="AA404">
         <v>4.5999999999999999E-3</v>
       </c>
+      <c r="AC404">
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="AD404">
+        <v>0.111</v>
+      </c>
     </row>
     <row r="405" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A405" s="19" t="s">
@@ -25702,6 +26188,12 @@
       </c>
       <c r="AA405">
         <v>4.5999999999999999E-3</v>
+      </c>
+      <c r="AC405">
+        <v>0.109</v>
+      </c>
+      <c r="AD405">
+        <v>0.115</v>
       </c>
     </row>
     <row r="406" spans="1:30" x14ac:dyDescent="0.2">
@@ -25755,6 +26247,12 @@
       <c r="AA406">
         <v>0</v>
       </c>
+      <c r="AC406">
+        <v>0.111</v>
+      </c>
+      <c r="AD406">
+        <v>0.11899999999999999</v>
+      </c>
     </row>
     <row r="407" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A407" s="19" t="s">
@@ -25805,6 +26303,12 @@
       <c r="X407">
         <f t="shared" si="17"/>
         <v>-4.6999999999999957</v>
+      </c>
+      <c r="AC407">
+        <v>0.108</v>
+      </c>
+      <c r="AD407">
+        <v>9.8000000000000004E-2</v>
       </c>
     </row>
     <row r="408" spans="1:30" x14ac:dyDescent="0.2">
@@ -25858,6 +26362,12 @@
       <c r="AA408">
         <v>4.4000000000000003E-3</v>
       </c>
+      <c r="AC408">
+        <v>0.11899999999999999</v>
+      </c>
+      <c r="AD408">
+        <v>0.126</v>
+      </c>
     </row>
     <row r="409" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A409" s="19" t="s">
@@ -25911,6 +26421,12 @@
       </c>
       <c r="AA409">
         <v>5.7999999999999996E-3</v>
+      </c>
+      <c r="AC409">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="AD409">
+        <v>0.12</v>
       </c>
     </row>
     <row r="410" spans="1:30" x14ac:dyDescent="0.2">
@@ -25964,6 +26480,12 @@
       <c r="AA410">
         <v>7.1000000000000004E-3</v>
       </c>
+      <c r="AC410">
+        <v>0.11700000000000001</v>
+      </c>
+      <c r="AD410">
+        <v>0.13100000000000001</v>
+      </c>
     </row>
     <row r="411" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A411" s="19" t="s">
@@ -26017,6 +26539,12 @@
       </c>
       <c r="AA411">
         <v>7.1999999999999998E-3</v>
+      </c>
+      <c r="AC411">
+        <v>0.11700000000000001</v>
+      </c>
+      <c r="AD411">
+        <v>0.121</v>
       </c>
     </row>
     <row r="412" spans="1:30" x14ac:dyDescent="0.2">
@@ -26070,6 +26598,12 @@
       <c r="AA412">
         <v>3.7000000000000002E-3</v>
       </c>
+      <c r="AC412">
+        <v>0.127</v>
+      </c>
+      <c r="AD412">
+        <v>0.17</v>
+      </c>
     </row>
     <row r="413" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A413" s="19" t="s">
@@ -26120,6 +26654,12 @@
       <c r="X413">
         <f t="shared" si="17"/>
         <v>5.7999999999999972</v>
+      </c>
+      <c r="AC413">
+        <v>0.122</v>
+      </c>
+      <c r="AD413">
+        <v>0.14499999999999999</v>
       </c>
     </row>
     <row r="414" spans="1:30" x14ac:dyDescent="0.2">
@@ -28061,6 +28601,12 @@
       <c r="AA450">
         <v>1.3100000000000001E-2</v>
       </c>
+      <c r="AC450">
+        <v>0.121</v>
+      </c>
+      <c r="AD450">
+        <v>0.121</v>
+      </c>
     </row>
     <row r="451" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A451" s="19" t="s">
@@ -28116,6 +28662,12 @@
       </c>
       <c r="AA451">
         <v>1.2E-2</v>
+      </c>
+      <c r="AC451">
+        <v>0.13</v>
+      </c>
+      <c r="AD451">
+        <v>0.189</v>
       </c>
     </row>
     <row r="452" spans="1:30" x14ac:dyDescent="0.2">
@@ -28171,6 +28723,12 @@
       <c r="AA452">
         <v>8.9999999999999993E-3</v>
       </c>
+      <c r="AC452">
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="AD452">
+        <v>0.13300000000000001</v>
+      </c>
     </row>
     <row r="453" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A453" s="19" t="s">
@@ -28224,6 +28782,12 @@
       </c>
       <c r="AA453">
         <v>8.3000000000000001E-3</v>
+      </c>
+      <c r="AC453">
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="AD453">
+        <v>0.122</v>
       </c>
     </row>
     <row r="454" spans="1:30" x14ac:dyDescent="0.2">
@@ -28277,6 +28841,12 @@
       <c r="AA454">
         <v>1.26E-2</v>
       </c>
+      <c r="AC454">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="AD454">
+        <v>0.13700000000000001</v>
+      </c>
     </row>
     <row r="455" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A455" s="19" t="s">
@@ -28330,6 +28900,12 @@
       </c>
       <c r="AA455">
         <v>8.3999999999999995E-3</v>
+      </c>
+      <c r="AC455">
+        <v>0.13900000000000001</v>
+      </c>
+      <c r="AD455">
+        <v>0.13300000000000001</v>
       </c>
     </row>
     <row r="456" spans="1:30" x14ac:dyDescent="0.2">
@@ -28383,6 +28959,12 @@
       <c r="AA456">
         <v>4.3E-3</v>
       </c>
+      <c r="AC456">
+        <v>0.112</v>
+      </c>
+      <c r="AD456">
+        <v>0.11700000000000001</v>
+      </c>
     </row>
     <row r="457" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A457" s="19" t="s">
@@ -28433,6 +29015,12 @@
       <c r="X457">
         <f t="shared" si="19"/>
         <v>0.30000000000000071</v>
+      </c>
+      <c r="AC457">
+        <v>0.108</v>
+      </c>
+      <c r="AD457">
+        <v>0.11700000000000001</v>
       </c>
     </row>
     <row r="458" spans="1:30" x14ac:dyDescent="0.2">
@@ -28486,6 +29074,12 @@
       <c r="AA458">
         <v>1.04E-2</v>
       </c>
+      <c r="AC458">
+        <v>0.155</v>
+      </c>
+      <c r="AD458">
+        <v>0.13</v>
+      </c>
     </row>
     <row r="459" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A459" s="19" t="s">
@@ -28539,6 +29133,12 @@
       </c>
       <c r="AA459">
         <v>1.1299999999999999E-2</v>
+      </c>
+      <c r="AC459">
+        <v>0.159</v>
+      </c>
+      <c r="AD459">
+        <v>0.124</v>
       </c>
     </row>
     <row r="460" spans="1:30" x14ac:dyDescent="0.2">
@@ -28589,6 +29189,12 @@
         <f t="shared" si="19"/>
         <v>0.80000000000000426</v>
       </c>
+      <c r="AC460">
+        <v>0.19400000000000001</v>
+      </c>
+      <c r="AD460">
+        <v>0.18</v>
+      </c>
     </row>
     <row r="461" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A461" s="19" t="s">
@@ -28642,6 +29248,12 @@
       </c>
       <c r="AA461">
         <v>9.4999999999999998E-3</v>
+      </c>
+      <c r="AC461">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="AD461">
+        <v>0.126</v>
       </c>
     </row>
     <row r="462" spans="1:30" x14ac:dyDescent="0.2">
@@ -28695,6 +29307,12 @@
       <c r="AA462">
         <v>8.8000000000000005E-3</v>
       </c>
+      <c r="AC462">
+        <v>0.16200000000000001</v>
+      </c>
+      <c r="AD462">
+        <v>0.11700000000000001</v>
+      </c>
     </row>
     <row r="463" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A463" s="19" t="s">
@@ -28748,6 +29366,12 @@
       </c>
       <c r="AA463">
         <v>5.4999999999999997E-3</v>
+      </c>
+      <c r="AC463">
+        <v>0.127</v>
+      </c>
+      <c r="AD463">
+        <v>0.151</v>
       </c>
     </row>
     <row r="464" spans="1:30" x14ac:dyDescent="0.2">
@@ -28801,8 +29425,14 @@
       <c r="AA464">
         <v>1.0200000000000001E-2</v>
       </c>
-    </row>
-    <row r="465" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AC464">
+        <v>0.14899999999999999</v>
+      </c>
+      <c r="AD464">
+        <v>0.126</v>
+      </c>
+    </row>
+    <row r="465" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A465" s="19" t="s">
         <v>466</v>
       </c>
@@ -28852,8 +29482,14 @@
         <f t="shared" si="19"/>
         <v>0.30000000000000071</v>
       </c>
-    </row>
-    <row r="466" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AC465">
+        <v>0.14899999999999999</v>
+      </c>
+      <c r="AD465">
+        <v>0.16300000000000001</v>
+      </c>
+    </row>
+    <row r="466" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A466" s="22" t="s">
         <v>467</v>
       </c>
@@ -28907,7 +29543,7 @@
         <v>8.6E-3</v>
       </c>
     </row>
-    <row r="467" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="467" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A467" s="22" t="s">
         <v>468</v>
       </c>
@@ -28963,7 +29599,7 @@
         <v>1.7100000000000001E-2</v>
       </c>
     </row>
-    <row r="468" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="468" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A468" s="22" t="s">
         <v>469</v>
       </c>
@@ -29017,7 +29653,7 @@
         <v>1.04E-2</v>
       </c>
     </row>
-    <row r="469" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="469" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A469" s="22" t="s">
         <v>470</v>
       </c>
@@ -29068,7 +29704,7 @@
         <v>-0.29999999999999716</v>
       </c>
     </row>
-    <row r="470" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="470" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A470" s="22" t="s">
         <v>471</v>
       </c>
@@ -29120,7 +29756,7 @@
         <v>8.6E-3</v>
       </c>
     </row>
-    <row r="471" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="471" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A471" s="22" t="s">
         <v>472</v>
       </c>
@@ -29171,7 +29807,7 @@
         <v>-0.10000000000000142</v>
       </c>
     </row>
-    <row r="472" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="472" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A472" s="22" t="s">
         <v>473</v>
       </c>
@@ -29223,7 +29859,7 @@
         <v>6.8999999999999999E-3</v>
       </c>
     </row>
-    <row r="473" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="473" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A473" s="22" t="s">
         <v>474</v>
       </c>
@@ -29274,7 +29910,7 @@
         <v>-11.299999999999997</v>
       </c>
     </row>
-    <row r="474" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="474" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A474" s="22" t="s">
         <v>475</v>
       </c>
@@ -29323,7 +29959,7 @@
         <v>4.3000000000000007</v>
       </c>
     </row>
-    <row r="475" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="475" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A475" s="22" t="s">
         <v>476</v>
       </c>
@@ -29374,7 +30010,7 @@
         <v>-6.9000000000000021</v>
       </c>
     </row>
-    <row r="476" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="476" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A476" s="22" t="s">
         <v>477</v>
       </c>
@@ -29426,7 +30062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="477" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="477" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A477" s="22" t="s">
         <v>478</v>
       </c>
@@ -29480,7 +30116,7 @@
         <v>6.6E-3</v>
       </c>
     </row>
-    <row r="478" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="478" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A478" s="22" t="s">
         <v>479</v>
       </c>
@@ -29532,7 +30168,7 @@
         <v>6.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="479" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="479" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A479" s="22" t="s">
         <v>480</v>
       </c>
@@ -29586,7 +30222,7 @@
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="480" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="480" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A480" s="22" t="s">
         <v>481</v>
       </c>

</xml_diff>

<commit_message>
working on new heights data
</commit_message>
<xml_diff>
--- a/data/observation_datasheet.xlsx
+++ b/data/observation_datasheet.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1228" uniqueCount="579">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1230" uniqueCount="581">
   <si>
     <t>ID</t>
   </si>
@@ -1775,6 +1775,12 @@
   </si>
   <si>
     <t>tough2</t>
+  </si>
+  <si>
+    <t>ht.prebudset</t>
+  </si>
+  <si>
+    <t>ht.date</t>
   </si>
 </sst>
 </file>
@@ -2380,7 +2386,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="94">
+  <cellStyleXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -2423,6 +2429,8 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2531,7 +2539,7 @@
     <xf numFmtId="0" fontId="21" fillId="38" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="94">
+  <cellStyles count="96">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -2586,6 +2594,7 @@
     <cellStyle name="Followed Hyperlink" xfId="89" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="91" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="93" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="95" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
@@ -2617,6 +2626,7 @@
     <cellStyle name="Hyperlink" xfId="88" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="90" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="92" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="94" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -5492,13 +5502,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF481"/>
+  <dimension ref="A1:AH481"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="86" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B430" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AF475" sqref="AF475"/>
+      <selection pane="bottomRight" activeCell="AG450" sqref="AG450"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5515,7 +5525,7 @@
     <col min="23" max="30" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>487</v>
       </c>
@@ -5600,8 +5610,14 @@
       <c r="AF1" s="50" t="s">
         <v>578</v>
       </c>
-    </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG1" s="50" t="s">
+        <v>579</v>
+      </c>
+      <c r="AH1" s="50" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="2" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
         <v>3</v>
       </c>
@@ -5666,8 +5682,14 @@
       <c r="AF2">
         <v>0.34</v>
       </c>
-    </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG2">
+        <v>78.400000000000006</v>
+      </c>
+      <c r="AH2">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="3" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
         <v>4</v>
       </c>
@@ -5734,8 +5756,14 @@
       <c r="AF3">
         <v>0.17</v>
       </c>
-    </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG3">
+        <v>58.6</v>
+      </c>
+      <c r="AH3">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="4" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
         <v>5</v>
       </c>
@@ -5800,8 +5828,14 @@
       <c r="AF4">
         <v>0.45</v>
       </c>
-    </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG4">
+        <v>53.4</v>
+      </c>
+      <c r="AH4">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="5" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>6</v>
       </c>
@@ -5866,8 +5900,14 @@
       <c r="AF5">
         <v>0.24</v>
       </c>
-    </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG5">
+        <v>66.8</v>
+      </c>
+      <c r="AH5">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="6" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
         <v>7</v>
       </c>
@@ -5930,8 +5970,14 @@
       <c r="AF6">
         <v>0.41</v>
       </c>
-    </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG6">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="AH6">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="7" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
         <v>8</v>
       </c>
@@ -5996,8 +6042,14 @@
       <c r="AF7">
         <v>0.22</v>
       </c>
-    </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG7">
+        <v>61.6</v>
+      </c>
+      <c r="AH7">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="8" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
         <v>9</v>
       </c>
@@ -6060,8 +6112,14 @@
       <c r="AF8">
         <v>0.34</v>
       </c>
-    </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG8">
+        <v>66.7</v>
+      </c>
+      <c r="AH8">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="9" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
         <v>10</v>
       </c>
@@ -6126,8 +6184,14 @@
       <c r="AF9">
         <v>0.28000000000000003</v>
       </c>
-    </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG9">
+        <v>29.5</v>
+      </c>
+      <c r="AH9">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="10" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
         <v>11</v>
       </c>
@@ -6190,8 +6254,14 @@
       <c r="AF10">
         <v>0.46</v>
       </c>
-    </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG10">
+        <v>52.5</v>
+      </c>
+      <c r="AH10">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="11" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
         <v>12</v>
       </c>
@@ -6258,8 +6328,14 @@
       <c r="AF11">
         <v>0.28000000000000003</v>
       </c>
-    </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG11">
+        <v>48.9</v>
+      </c>
+      <c r="AH11">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="12" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
         <v>13</v>
       </c>
@@ -6316,8 +6392,14 @@
       <c r="AF12">
         <v>0.33</v>
       </c>
-    </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG12">
+        <v>22.1</v>
+      </c>
+      <c r="AH12">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="13" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A13" s="14" t="s">
         <v>14</v>
       </c>
@@ -6379,8 +6461,14 @@
       <c r="AE13">
         <v>0.36</v>
       </c>
-    </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG13">
+        <v>25.9</v>
+      </c>
+      <c r="AH13">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="14" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A14" s="14" t="s">
         <v>15</v>
       </c>
@@ -6440,8 +6528,14 @@
       <c r="AE14">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG14">
+        <v>20.3</v>
+      </c>
+      <c r="AH14">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="15" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>16</v>
       </c>
@@ -6506,8 +6600,14 @@
       <c r="AF15">
         <v>0.35</v>
       </c>
-    </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG15">
+        <v>31</v>
+      </c>
+      <c r="AH15">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="16" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A16" s="14" t="s">
         <v>17</v>
       </c>
@@ -6567,8 +6667,14 @@
       <c r="AE16">
         <v>0.27</v>
       </c>
-    </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG16">
+        <v>53.4</v>
+      </c>
+      <c r="AH16">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="17" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A17" s="14" t="s">
         <v>18</v>
       </c>
@@ -6633,8 +6739,14 @@
       <c r="AF17">
         <v>0.28000000000000003</v>
       </c>
-    </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG17">
+        <v>25.1</v>
+      </c>
+      <c r="AH17">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="18" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A18" s="19" t="s">
         <v>19</v>
       </c>
@@ -6700,7 +6812,7 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A19" s="19" t="s">
         <v>20</v>
       </c>
@@ -6768,7 +6880,7 @@
         <v>0.37</v>
       </c>
     </row>
-    <row r="20" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A20" s="19" t="s">
         <v>21</v>
       </c>
@@ -6832,7 +6944,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="21" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A21" s="19" t="s">
         <v>22</v>
       </c>
@@ -6898,7 +7010,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="22" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A22" s="19" t="s">
         <v>23</v>
       </c>
@@ -6962,7 +7074,7 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="23" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A23" s="19" t="s">
         <v>24</v>
       </c>
@@ -7028,7 +7140,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="24" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A24" s="19" t="s">
         <v>25</v>
       </c>
@@ -7089,7 +7201,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="25" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A25" s="19" t="s">
         <v>26</v>
       </c>
@@ -7149,7 +7261,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="26" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A26" s="19" t="s">
         <v>27</v>
       </c>
@@ -7213,7 +7325,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="27" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A27" s="19" t="s">
         <v>28</v>
       </c>
@@ -7270,7 +7382,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="28" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A28" s="19" t="s">
         <v>29</v>
       </c>
@@ -7334,7 +7446,7 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="29" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A29" s="19" t="s">
         <v>30</v>
       </c>
@@ -7394,7 +7506,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="30" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A30" s="19" t="s">
         <v>31</v>
       </c>
@@ -7452,7 +7564,7 @@
         <v>0.26</v>
       </c>
     </row>
-    <row r="31" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A31" s="19" t="s">
         <v>32</v>
       </c>
@@ -7518,7 +7630,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="32" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A32" s="19" t="s">
         <v>33</v>
       </c>
@@ -8578,7 +8690,7 @@
         <v>0.32</v>
       </c>
     </row>
-    <row r="49" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A49" s="22" t="s">
         <v>50</v>
       </c>
@@ -8638,7 +8750,7 @@
         <v>0.31</v>
       </c>
     </row>
-    <row r="50" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A50" s="14" t="s">
         <v>51</v>
       </c>
@@ -8703,8 +8815,14 @@
       <c r="AF50">
         <v>0.35</v>
       </c>
-    </row>
-    <row r="51" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG50">
+        <v>93.9</v>
+      </c>
+      <c r="AH50">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="51" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A51" s="14" t="s">
         <v>52</v>
       </c>
@@ -8771,8 +8889,14 @@
       <c r="AF51">
         <v>0.35</v>
       </c>
-    </row>
-    <row r="52" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG51">
+        <v>134.19999999999999</v>
+      </c>
+      <c r="AH51">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="52" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A52" s="14" t="s">
         <v>53</v>
       </c>
@@ -8837,8 +8961,14 @@
       <c r="AF52">
         <v>0.31</v>
       </c>
-    </row>
-    <row r="53" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG52">
+        <v>70.599999999999994</v>
+      </c>
+      <c r="AH52">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="53" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A53" s="14" t="s">
         <v>54</v>
       </c>
@@ -8903,8 +9033,14 @@
       <c r="AF53">
         <v>0.34</v>
       </c>
-    </row>
-    <row r="54" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG53">
+        <v>84.7</v>
+      </c>
+      <c r="AH53">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="54" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A54" s="14" t="s">
         <v>55</v>
       </c>
@@ -8967,8 +9103,14 @@
       <c r="AF54">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="55" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG54">
+        <v>57.7</v>
+      </c>
+      <c r="AH54">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="55" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A55" s="14" t="s">
         <v>56</v>
       </c>
@@ -9033,8 +9175,14 @@
       <c r="AF55">
         <v>0.41</v>
       </c>
-    </row>
-    <row r="56" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG55">
+        <v>57.1</v>
+      </c>
+      <c r="AH55">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="56" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A56" s="14" t="s">
         <v>57</v>
       </c>
@@ -9097,8 +9245,14 @@
       <c r="AF56">
         <v>0.35</v>
       </c>
-    </row>
-    <row r="57" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG56">
+        <v>46.2</v>
+      </c>
+      <c r="AH56">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="57" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A57" s="14" t="s">
         <v>58</v>
       </c>
@@ -9163,8 +9317,14 @@
       <c r="AF57">
         <v>0.44</v>
       </c>
-    </row>
-    <row r="58" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG57">
+        <v>102.2</v>
+      </c>
+      <c r="AH57">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="58" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A58" s="14" t="s">
         <v>59</v>
       </c>
@@ -9227,8 +9387,14 @@
       <c r="AF58">
         <v>0.36</v>
       </c>
-    </row>
-    <row r="59" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG58">
+        <v>77.2</v>
+      </c>
+      <c r="AH58">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="59" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A59" s="14" t="s">
         <v>60</v>
       </c>
@@ -9293,8 +9459,14 @@
       <c r="AF59">
         <v>0.38</v>
       </c>
-    </row>
-    <row r="60" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG59">
+        <v>68.5</v>
+      </c>
+      <c r="AH59">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="60" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A60" s="14" t="s">
         <v>61</v>
       </c>
@@ -9357,8 +9529,14 @@
       <c r="AF60">
         <v>0.43</v>
       </c>
-    </row>
-    <row r="61" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG60">
+        <v>67.099999999999994</v>
+      </c>
+      <c r="AH60">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="61" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A61" s="25" t="s">
         <v>62</v>
       </c>
@@ -9386,7 +9564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A62" s="14" t="s">
         <v>63</v>
       </c>
@@ -9449,8 +9627,14 @@
       <c r="AF62">
         <v>0.34</v>
       </c>
-    </row>
-    <row r="63" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG62">
+        <v>61.6</v>
+      </c>
+      <c r="AH62">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="63" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A63" s="14" t="s">
         <v>64</v>
       </c>
@@ -9515,8 +9699,14 @@
       <c r="AF63">
         <v>0.41</v>
       </c>
-    </row>
-    <row r="64" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG63">
+        <v>92.5</v>
+      </c>
+      <c r="AH63">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="64" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A64" s="14" t="s">
         <v>65</v>
       </c>
@@ -9579,8 +9769,14 @@
       <c r="AF64">
         <v>0.39</v>
       </c>
-    </row>
-    <row r="65" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG64">
+        <v>81.400000000000006</v>
+      </c>
+      <c r="AH64">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="65" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A65" s="14" t="s">
         <v>66</v>
       </c>
@@ -9645,8 +9841,14 @@
       <c r="AF65">
         <v>0.17</v>
       </c>
-    </row>
-    <row r="66" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG65">
+        <v>80.099999999999994</v>
+      </c>
+      <c r="AH65">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="66" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A66" s="19" t="s">
         <v>67</v>
       </c>
@@ -9709,7 +9911,7 @@
         <v>0.39</v>
       </c>
     </row>
-    <row r="67" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A67" s="19" t="s">
         <v>68</v>
       </c>
@@ -9774,7 +9976,7 @@
         <v>0.26</v>
       </c>
     </row>
-    <row r="68" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A68" s="19" t="s">
         <v>69</v>
       </c>
@@ -9838,7 +10040,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="69" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A69" s="19" t="s">
         <v>70</v>
       </c>
@@ -9904,7 +10106,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="70" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A70" s="19" t="s">
         <v>71</v>
       </c>
@@ -9968,7 +10170,7 @@
         <v>0.38</v>
       </c>
     </row>
-    <row r="71" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A71" s="19" t="s">
         <v>72</v>
       </c>
@@ -10034,7 +10236,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="72" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A72" s="25" t="s">
         <v>73</v>
       </c>
@@ -10062,7 +10264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A73" s="19" t="s">
         <v>74</v>
       </c>
@@ -10128,7 +10330,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="74" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A74" s="19" t="s">
         <v>75</v>
       </c>
@@ -10192,7 +10394,7 @@
         <v>0.39</v>
       </c>
     </row>
-    <row r="75" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A75" s="19" t="s">
         <v>76</v>
       </c>
@@ -10257,7 +10459,7 @@
         <v>0.37</v>
       </c>
     </row>
-    <row r="76" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A76" s="19" t="s">
         <v>77</v>
       </c>
@@ -10321,7 +10523,7 @@
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="77" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A77" s="19" t="s">
         <v>78</v>
       </c>
@@ -10389,7 +10591,7 @@
         <v>0.32</v>
       </c>
     </row>
-    <row r="78" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A78" s="19" t="s">
         <v>79</v>
       </c>
@@ -10453,7 +10655,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="79" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A79" s="19" t="s">
         <v>80</v>
       </c>
@@ -10519,7 +10721,7 @@
         <v>0.26</v>
       </c>
     </row>
-    <row r="80" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A80" s="19" t="s">
         <v>81</v>
       </c>
@@ -11521,7 +11723,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="97" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A97" s="22" t="s">
         <v>98</v>
       </c>
@@ -11587,7 +11789,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="98" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A98" s="14" t="s">
         <v>99</v>
       </c>
@@ -11660,8 +11862,14 @@
       <c r="AF98">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="99" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG98">
+        <v>43.4</v>
+      </c>
+      <c r="AH98">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="99" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A99" s="14" t="s">
         <v>100</v>
       </c>
@@ -11734,8 +11942,14 @@
       <c r="AF99">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="100" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG99">
+        <v>36.200000000000003</v>
+      </c>
+      <c r="AH99">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="100" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A100" s="14" t="s">
         <v>101</v>
       </c>
@@ -11811,8 +12025,14 @@
       <c r="AF100">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="101" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG100">
+        <v>35.299999999999997</v>
+      </c>
+      <c r="AH100">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="101" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A101" s="14" t="s">
         <v>102</v>
       </c>
@@ -11877,8 +12097,14 @@
       <c r="AF101">
         <v>0.21</v>
       </c>
-    </row>
-    <row r="102" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG101">
+        <v>65.400000000000006</v>
+      </c>
+      <c r="AH101">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="102" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A102" s="14" t="s">
         <v>103</v>
       </c>
@@ -11954,8 +12180,14 @@
       <c r="AF102">
         <v>0.28999999999999998</v>
       </c>
-    </row>
-    <row r="103" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG102">
+        <v>60.2</v>
+      </c>
+      <c r="AH102">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="103" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A103" s="14" t="s">
         <v>104</v>
       </c>
@@ -12020,8 +12252,14 @@
       <c r="AF103">
         <v>0.32</v>
       </c>
-    </row>
-    <row r="104" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG103">
+        <v>45.4</v>
+      </c>
+      <c r="AH103">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="104" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A104" s="14" t="s">
         <v>105</v>
       </c>
@@ -12097,8 +12335,14 @@
       <c r="AF104">
         <v>0.31</v>
       </c>
-    </row>
-    <row r="105" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG104">
+        <v>57.5</v>
+      </c>
+      <c r="AH104">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="105" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A105" s="14" t="s">
         <v>106</v>
       </c>
@@ -12176,8 +12420,14 @@
       <c r="AF105">
         <v>0.28000000000000003</v>
       </c>
-    </row>
-    <row r="106" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG105">
+        <v>37.4</v>
+      </c>
+      <c r="AH105">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="106" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A106" s="14" t="s">
         <v>107</v>
       </c>
@@ -12240,8 +12490,14 @@
       <c r="AF106">
         <v>0.33</v>
       </c>
-    </row>
-    <row r="107" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG106">
+        <v>46.9</v>
+      </c>
+      <c r="AH106">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="107" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A107" s="14" t="s">
         <v>108</v>
       </c>
@@ -12306,8 +12562,14 @@
       <c r="AF107">
         <v>0.33</v>
       </c>
-    </row>
-    <row r="108" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG107">
+        <v>43.5</v>
+      </c>
+      <c r="AH107">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="108" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A108" s="14" t="s">
         <v>109</v>
       </c>
@@ -12383,8 +12645,14 @@
       <c r="AF108">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="109" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG108">
+        <v>47.6</v>
+      </c>
+      <c r="AH108">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="109" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A109" s="14" t="s">
         <v>110</v>
       </c>
@@ -12449,8 +12717,14 @@
       <c r="AF109">
         <v>0.26</v>
       </c>
-    </row>
-    <row r="110" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG109">
+        <v>51</v>
+      </c>
+      <c r="AH109">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="110" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A110" s="14" t="s">
         <v>111</v>
       </c>
@@ -12513,8 +12787,14 @@
       <c r="AF110">
         <v>0.31</v>
       </c>
-    </row>
-    <row r="111" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG110">
+        <v>49.9</v>
+      </c>
+      <c r="AH110">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="111" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A111" s="14" t="s">
         <v>112</v>
       </c>
@@ -12579,8 +12859,14 @@
       <c r="AF111">
         <v>0.28999999999999998</v>
       </c>
-    </row>
-    <row r="112" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG111">
+        <v>47.3</v>
+      </c>
+      <c r="AH111">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="112" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A112" s="14" t="s">
         <v>113</v>
       </c>
@@ -12643,8 +12929,14 @@
       <c r="AF112">
         <v>0.28000000000000003</v>
       </c>
-    </row>
-    <row r="113" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG112">
+        <v>59.7</v>
+      </c>
+      <c r="AH112">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="113" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A113" s="14" t="s">
         <v>114</v>
       </c>
@@ -12711,8 +13003,14 @@
       <c r="AF113">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="114" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG113">
+        <v>62.1</v>
+      </c>
+      <c r="AH113">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="114" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A114" s="19" t="s">
         <v>115</v>
       </c>
@@ -12778,7 +13076,7 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="115" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A115" s="19" t="s">
         <v>116</v>
       </c>
@@ -12844,7 +13142,7 @@
         <v>0.19</v>
       </c>
     </row>
-    <row r="116" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A116" s="19" t="s">
         <v>117</v>
       </c>
@@ -12908,7 +13206,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="117" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A117" s="19" t="s">
         <v>118</v>
       </c>
@@ -12974,7 +13272,7 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="118" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A118" s="19" t="s">
         <v>119</v>
       </c>
@@ -13038,7 +13336,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="119" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A119" s="19" t="s">
         <v>120</v>
       </c>
@@ -13106,7 +13404,7 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="120" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A120" s="19" t="s">
         <v>121</v>
       </c>
@@ -13170,7 +13468,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="121" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A121" s="19" t="s">
         <v>122</v>
       </c>
@@ -13236,7 +13534,7 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="122" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A122" s="19" t="s">
         <v>123</v>
       </c>
@@ -13300,7 +13598,7 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="123" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A123" s="19" t="s">
         <v>124</v>
       </c>
@@ -13368,7 +13666,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="124" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A124" s="19" t="s">
         <v>125</v>
       </c>
@@ -13432,7 +13730,7 @@
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="125" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A125" s="19" t="s">
         <v>126</v>
       </c>
@@ -13498,7 +13796,7 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="126" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A126" s="19" t="s">
         <v>127</v>
       </c>
@@ -13562,7 +13860,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="127" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A127" s="19" t="s">
         <v>128</v>
       </c>
@@ -13628,7 +13926,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="128" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A128" s="19" t="s">
         <v>129</v>
       </c>
@@ -14737,7 +15035,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="145" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A145" s="22" t="s">
         <v>146</v>
       </c>
@@ -14803,7 +15101,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="146" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A146" s="14" t="s">
         <v>147</v>
       </c>
@@ -14868,8 +15166,14 @@
       <c r="AF146">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="147" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG146">
+        <v>79.099999999999994</v>
+      </c>
+      <c r="AH146">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="147" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A147" s="14" t="s">
         <v>148</v>
       </c>
@@ -14934,8 +15238,14 @@
       <c r="AF147">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="148" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG147">
+        <v>68</v>
+      </c>
+      <c r="AH147">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="148" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A148" s="14" t="s">
         <v>149</v>
       </c>
@@ -14998,8 +15308,14 @@
       <c r="AF148">
         <v>0.36</v>
       </c>
-    </row>
-    <row r="149" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG148">
+        <v>62.6</v>
+      </c>
+      <c r="AH148">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="149" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A149" s="14" t="s">
         <v>150</v>
       </c>
@@ -15066,8 +15382,14 @@
       <c r="AF149">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="150" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG149">
+        <v>64.8</v>
+      </c>
+      <c r="AH149">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="150" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A150" s="14" t="s">
         <v>151</v>
       </c>
@@ -15130,8 +15452,14 @@
       <c r="AF150">
         <v>0.49</v>
       </c>
-    </row>
-    <row r="151" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG150">
+        <v>67.400000000000006</v>
+      </c>
+      <c r="AH150">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="151" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A151" s="14" t="s">
         <v>152</v>
       </c>
@@ -15196,8 +15524,14 @@
       <c r="AF151">
         <v>0.17</v>
       </c>
-    </row>
-    <row r="152" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG151">
+        <v>56.2</v>
+      </c>
+      <c r="AH151">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="152" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A152" s="14" t="s">
         <v>153</v>
       </c>
@@ -15260,8 +15594,14 @@
       <c r="AF152">
         <v>0.31</v>
       </c>
-    </row>
-    <row r="153" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG152">
+        <v>68.8</v>
+      </c>
+      <c r="AH152">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="153" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A153" s="14" t="s">
         <v>154</v>
       </c>
@@ -15326,8 +15666,14 @@
       <c r="AF153">
         <v>0.35</v>
       </c>
-    </row>
-    <row r="154" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG153">
+        <v>86.8</v>
+      </c>
+      <c r="AH153">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="154" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A154" s="14" t="s">
         <v>155</v>
       </c>
@@ -15390,8 +15736,14 @@
       <c r="AF154">
         <v>0.39</v>
       </c>
-    </row>
-    <row r="155" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG154">
+        <v>75.599999999999994</v>
+      </c>
+      <c r="AH154">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="155" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A155" s="14" t="s">
         <v>156</v>
       </c>
@@ -15456,8 +15808,14 @@
       <c r="AF155">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="156" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG155">
+        <v>56.7</v>
+      </c>
+      <c r="AH155">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="156" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A156" s="14" t="s">
         <v>157</v>
       </c>
@@ -15520,8 +15878,14 @@
       <c r="AF156">
         <v>0.39</v>
       </c>
-    </row>
-    <row r="157" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG156">
+        <v>77.400000000000006</v>
+      </c>
+      <c r="AH156">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="157" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A157" s="14" t="s">
         <v>158</v>
       </c>
@@ -15586,8 +15950,14 @@
       <c r="AF157">
         <v>0.28000000000000003</v>
       </c>
-    </row>
-    <row r="158" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG157">
+        <v>77.599999999999994</v>
+      </c>
+      <c r="AH157">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="158" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A158" s="14" t="s">
         <v>159</v>
       </c>
@@ -15650,8 +16020,14 @@
       <c r="AF158">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="159" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG158">
+        <v>75.2</v>
+      </c>
+      <c r="AH158">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="159" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A159" s="14" t="s">
         <v>160</v>
       </c>
@@ -15716,8 +16092,14 @@
       <c r="AF159">
         <v>0.37</v>
       </c>
-    </row>
-    <row r="160" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG159">
+        <v>65</v>
+      </c>
+      <c r="AH159">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="160" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A160" s="14" t="s">
         <v>161</v>
       </c>
@@ -15780,8 +16162,14 @@
       <c r="AF160">
         <v>0.49</v>
       </c>
-    </row>
-    <row r="161" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG160">
+        <v>77.2</v>
+      </c>
+      <c r="AH160">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="161" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A161" s="14" t="s">
         <v>162</v>
       </c>
@@ -15846,8 +16234,14 @@
       <c r="AF161">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="162" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG161">
+        <v>56.2</v>
+      </c>
+      <c r="AH161">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="162" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A162" s="19" t="s">
         <v>163</v>
       </c>
@@ -15913,7 +16307,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="163" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A163" s="19" t="s">
         <v>164</v>
       </c>
@@ -15979,7 +16373,7 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="164" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A164" s="19" t="s">
         <v>165</v>
       </c>
@@ -16043,7 +16437,7 @@
         <v>0.36</v>
       </c>
     </row>
-    <row r="165" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A165" s="19" t="s">
         <v>166</v>
       </c>
@@ -16109,7 +16503,7 @@
         <v>0.38</v>
       </c>
     </row>
-    <row r="166" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A166" s="19" t="s">
         <v>167</v>
       </c>
@@ -16173,7 +16567,7 @@
         <v>0.32</v>
       </c>
     </row>
-    <row r="167" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A167" s="19" t="s">
         <v>168</v>
       </c>
@@ -16239,7 +16633,7 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="168" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A168" s="19" t="s">
         <v>169</v>
       </c>
@@ -16303,7 +16697,7 @@
         <v>0.26</v>
       </c>
     </row>
-    <row r="169" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A169" s="19" t="s">
         <v>170</v>
       </c>
@@ -16369,7 +16763,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="170" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A170" s="19" t="s">
         <v>171</v>
       </c>
@@ -16433,7 +16827,7 @@
         <v>0.37</v>
       </c>
     </row>
-    <row r="171" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A171" s="19" t="s">
         <v>172</v>
       </c>
@@ -16499,7 +16893,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="172" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A172" s="19" t="s">
         <v>173</v>
       </c>
@@ -16563,7 +16957,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="173" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A173" s="19" t="s">
         <v>174</v>
       </c>
@@ -16629,7 +17023,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="174" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A174" s="19" t="s">
         <v>175</v>
       </c>
@@ -16693,7 +17087,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="175" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A175" s="19" t="s">
         <v>176</v>
       </c>
@@ -16759,7 +17153,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="176" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A176" s="19" t="s">
         <v>177</v>
       </c>
@@ -17867,7 +18261,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="193" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A193" s="22" t="s">
         <v>194</v>
       </c>
@@ -17933,7 +18327,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="194" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A194" s="14" t="s">
         <v>195</v>
       </c>
@@ -18019,8 +18413,14 @@
       <c r="AF194">
         <v>0.44</v>
       </c>
-    </row>
-    <row r="195" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG194">
+        <v>62.5</v>
+      </c>
+      <c r="AH194">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="195" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A195" s="14" t="s">
         <v>196</v>
       </c>
@@ -18099,8 +18499,14 @@
       <c r="AF195">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="196" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG195">
+        <v>57</v>
+      </c>
+      <c r="AH195">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="196" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A196" s="14" t="s">
         <v>197</v>
       </c>
@@ -18163,8 +18569,14 @@
       <c r="AF196">
         <v>0.39</v>
       </c>
-    </row>
-    <row r="197" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG196">
+        <v>62.5</v>
+      </c>
+      <c r="AH196">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="197" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A197" s="14" t="s">
         <v>198</v>
       </c>
@@ -18229,8 +18641,14 @@
       <c r="AF197">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="198" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG197">
+        <v>43</v>
+      </c>
+      <c r="AH197">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="198" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A198" s="14" t="s">
         <v>199</v>
       </c>
@@ -18306,8 +18724,14 @@
       <c r="AF198">
         <v>0.42</v>
       </c>
-    </row>
-    <row r="199" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG198">
+        <v>46</v>
+      </c>
+      <c r="AH198">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="199" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A199" s="14" t="s">
         <v>200</v>
       </c>
@@ -18372,8 +18796,14 @@
       <c r="AF199">
         <v>0.43</v>
       </c>
-    </row>
-    <row r="200" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG199">
+        <v>52.7</v>
+      </c>
+      <c r="AH199">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="200" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A200" s="14" t="s">
         <v>201</v>
       </c>
@@ -18436,8 +18866,14 @@
       <c r="AF200">
         <v>0.43</v>
       </c>
-    </row>
-    <row r="201" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG200">
+        <v>55.3</v>
+      </c>
+      <c r="AH200">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="201" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A201" s="14" t="s">
         <v>202</v>
       </c>
@@ -18502,8 +18938,14 @@
       <c r="AF201">
         <v>0.38</v>
       </c>
-    </row>
-    <row r="202" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG201">
+        <v>55.8</v>
+      </c>
+      <c r="AH201">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="202" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A202" s="14" t="s">
         <v>203</v>
       </c>
@@ -18566,8 +19008,14 @@
       <c r="AF202">
         <v>0.46</v>
       </c>
-    </row>
-    <row r="203" spans="1:32" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AG202">
+        <v>65.2</v>
+      </c>
+      <c r="AH202">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="203" spans="1:34" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A203" s="14" t="s">
         <v>204</v>
       </c>
@@ -18635,8 +19083,14 @@
       <c r="AF203">
         <v>0.41</v>
       </c>
-    </row>
-    <row r="204" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AG203">
+        <v>61.2</v>
+      </c>
+      <c r="AH203">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="204" spans="1:34" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A204" s="14" t="s">
         <v>205</v>
       </c>
@@ -18699,8 +19153,14 @@
       <c r="AF204">
         <v>0.28000000000000003</v>
       </c>
-    </row>
-    <row r="205" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AG204">
+        <v>58.9</v>
+      </c>
+      <c r="AH204">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="205" spans="1:34" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A205" s="14" t="s">
         <v>206</v>
       </c>
@@ -18778,8 +19238,14 @@
       <c r="AF205">
         <v>0.37</v>
       </c>
-    </row>
-    <row r="206" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AG205">
+        <v>61</v>
+      </c>
+      <c r="AH205">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="206" spans="1:34" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A206" s="14" t="s">
         <v>207</v>
       </c>
@@ -18855,8 +19321,14 @@
       <c r="AF206">
         <v>0.32</v>
       </c>
-    </row>
-    <row r="207" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AG206">
+        <v>60.6</v>
+      </c>
+      <c r="AH206">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="207" spans="1:34" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A207" s="14" t="s">
         <v>208</v>
       </c>
@@ -18923,8 +19395,14 @@
       <c r="AF207">
         <v>0.11</v>
       </c>
-    </row>
-    <row r="208" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG207">
+        <v>63.4</v>
+      </c>
+      <c r="AH207">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="208" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A208" s="14" t="s">
         <v>209</v>
       </c>
@@ -19000,8 +19478,14 @@
       <c r="AF208">
         <v>0.34</v>
       </c>
-    </row>
-    <row r="209" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG208">
+        <v>59.9</v>
+      </c>
+      <c r="AH208">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="209" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A209" s="14" t="s">
         <v>210</v>
       </c>
@@ -19066,8 +19550,14 @@
       <c r="AF209">
         <v>0.28000000000000003</v>
       </c>
-    </row>
-    <row r="210" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG209">
+        <v>60.5</v>
+      </c>
+      <c r="AH209">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="210" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A210" s="19" t="s">
         <v>211</v>
       </c>
@@ -19133,7 +19623,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="211" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A211" s="19" t="s">
         <v>212</v>
       </c>
@@ -19199,7 +19689,7 @@
         <v>0.49</v>
       </c>
     </row>
-    <row r="212" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A212" s="19" t="s">
         <v>213</v>
       </c>
@@ -19263,7 +19753,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="213" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A213" s="19" t="s">
         <v>214</v>
       </c>
@@ -19331,7 +19821,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="214" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A214" s="19" t="s">
         <v>215</v>
       </c>
@@ -19395,7 +19885,7 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="215" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A215" s="19" t="s">
         <v>216</v>
       </c>
@@ -19461,7 +19951,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="216" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A216" s="19" t="s">
         <v>217</v>
       </c>
@@ -19525,7 +20015,7 @@
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="217" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A217" s="19" t="s">
         <v>218</v>
       </c>
@@ -19591,7 +20081,7 @@
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="218" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A218" s="19" t="s">
         <v>219</v>
       </c>
@@ -19655,7 +20145,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="219" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A219" s="19" t="s">
         <v>220</v>
       </c>
@@ -19721,7 +20211,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="220" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A220" s="19" t="s">
         <v>221</v>
       </c>
@@ -19785,7 +20275,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="221" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A221" s="19" t="s">
         <v>222</v>
       </c>
@@ -19851,7 +20341,7 @@
         <v>0.38</v>
       </c>
     </row>
-    <row r="222" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A222" s="19" t="s">
         <v>223</v>
       </c>
@@ -19915,7 +20405,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="223" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A223" s="19" t="s">
         <v>224</v>
       </c>
@@ -19981,7 +20471,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="224" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A224" s="19" t="s">
         <v>225</v>
       </c>
@@ -24151,7 +24641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="337" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A337" s="22" t="s">
         <v>338</v>
       </c>
@@ -24179,7 +24669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="338" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A338" s="14" t="s">
         <v>339</v>
       </c>
@@ -24265,8 +24755,14 @@
       <c r="AF338">
         <v>1.05</v>
       </c>
-    </row>
-    <row r="339" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG338">
+        <v>72.599999999999994</v>
+      </c>
+      <c r="AH338">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="339" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A339" s="14" t="s">
         <v>340</v>
       </c>
@@ -24352,8 +24848,14 @@
       <c r="AF339">
         <v>0.65</v>
       </c>
-    </row>
-    <row r="340" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG339">
+        <v>89.9</v>
+      </c>
+      <c r="AH339">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="340" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A340" s="14" t="s">
         <v>341</v>
       </c>
@@ -24429,8 +24931,14 @@
       <c r="AF340">
         <v>0.39</v>
       </c>
-    </row>
-    <row r="341" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG340">
+        <v>95.3</v>
+      </c>
+      <c r="AH340">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="341" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A341" s="14" t="s">
         <v>342</v>
       </c>
@@ -24508,8 +25016,14 @@
       <c r="AF341">
         <v>0.61</v>
       </c>
-    </row>
-    <row r="342" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG341">
+        <v>79</v>
+      </c>
+      <c r="AH341">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="342" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A342" s="14" t="s">
         <v>343</v>
       </c>
@@ -24585,8 +25099,14 @@
       <c r="AF342">
         <v>0.77</v>
       </c>
-    </row>
-    <row r="343" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG342">
+        <v>87.9</v>
+      </c>
+      <c r="AH342">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="343" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A343" s="14" t="s">
         <v>344</v>
       </c>
@@ -24664,8 +25184,14 @@
       <c r="AF343">
         <v>0.39</v>
       </c>
-    </row>
-    <row r="344" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG343">
+        <v>81.5</v>
+      </c>
+      <c r="AH343">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="344" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A344" s="14" t="s">
         <v>345</v>
       </c>
@@ -24741,8 +25267,14 @@
       <c r="AF344">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="345" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG344">
+        <v>78.2</v>
+      </c>
+      <c r="AH344">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="345" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A345" s="14" t="s">
         <v>346</v>
       </c>
@@ -24820,8 +25352,14 @@
       <c r="AF345">
         <v>0.46</v>
       </c>
-    </row>
-    <row r="346" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG345">
+        <v>63.4</v>
+      </c>
+      <c r="AH345">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="346" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A346" s="14" t="s">
         <v>347</v>
       </c>
@@ -24897,8 +25435,14 @@
       <c r="AF346">
         <v>0.56000000000000005</v>
       </c>
-    </row>
-    <row r="347" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG346">
+        <v>72.2</v>
+      </c>
+      <c r="AH346">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="347" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A347" s="14" t="s">
         <v>348</v>
       </c>
@@ -24976,8 +25520,14 @@
       <c r="AF347">
         <v>0.76</v>
       </c>
-    </row>
-    <row r="348" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG347">
+        <v>67.7</v>
+      </c>
+      <c r="AH347">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="348" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A348" s="14" t="s">
         <v>349</v>
       </c>
@@ -25053,8 +25603,14 @@
       <c r="AF348">
         <v>0.51</v>
       </c>
-    </row>
-    <row r="349" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG348">
+        <v>84.2</v>
+      </c>
+      <c r="AH348">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="349" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A349" s="14" t="s">
         <v>350</v>
       </c>
@@ -25132,8 +25688,14 @@
       <c r="AF349">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="350" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG349">
+        <v>81.8</v>
+      </c>
+      <c r="AH349">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="350" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A350" s="14" t="s">
         <v>351</v>
       </c>
@@ -25209,8 +25771,14 @@
       <c r="AF350">
         <v>0.59</v>
       </c>
-    </row>
-    <row r="351" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG350">
+        <v>92.7</v>
+      </c>
+      <c r="AH350">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="351" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A351" s="14" t="s">
         <v>352</v>
       </c>
@@ -25290,8 +25858,14 @@
       <c r="AF351">
         <v>0.27</v>
       </c>
-    </row>
-    <row r="352" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG351">
+        <v>81.8</v>
+      </c>
+      <c r="AH351">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="352" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A352" s="14" t="s">
         <v>353</v>
       </c>
@@ -25367,8 +25941,14 @@
       <c r="AF352">
         <v>0.48</v>
       </c>
-    </row>
-    <row r="353" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG352">
+        <v>76.7</v>
+      </c>
+      <c r="AH352">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="353" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A353" s="14" t="s">
         <v>354</v>
       </c>
@@ -25433,8 +26013,14 @@
       <c r="AF353">
         <v>0.68</v>
       </c>
-    </row>
-    <row r="354" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG353">
+        <v>80.900000000000006</v>
+      </c>
+      <c r="AH353">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="354" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A354" s="19" t="s">
         <v>355</v>
       </c>
@@ -25499,8 +26085,14 @@
       <c r="AF354">
         <v>0.46</v>
       </c>
-    </row>
-    <row r="355" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG354">
+        <v>95.4</v>
+      </c>
+      <c r="AH354">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="355" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A355" s="19" t="s">
         <v>356</v>
       </c>
@@ -25565,8 +26157,14 @@
       <c r="AF355">
         <v>0.52</v>
       </c>
-    </row>
-    <row r="356" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG355">
+        <v>123</v>
+      </c>
+      <c r="AH355">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="356" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A356" s="19" t="s">
         <v>357</v>
       </c>
@@ -25629,8 +26227,14 @@
       <c r="AF356">
         <v>0.46</v>
       </c>
-    </row>
-    <row r="357" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG356">
+        <v>93.1</v>
+      </c>
+      <c r="AH356">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="357" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A357" s="19" t="s">
         <v>358</v>
       </c>
@@ -25695,8 +26299,14 @@
       <c r="AF357">
         <v>0.43</v>
       </c>
-    </row>
-    <row r="358" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG357">
+        <v>90.6</v>
+      </c>
+      <c r="AH357">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="358" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A358" s="19" t="s">
         <v>359</v>
       </c>
@@ -25759,8 +26369,14 @@
       <c r="AF358">
         <v>0.63</v>
       </c>
-    </row>
-    <row r="359" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG358">
+        <v>90.4</v>
+      </c>
+      <c r="AH358">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="359" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A359" s="19" t="s">
         <v>360</v>
       </c>
@@ -25825,8 +26441,14 @@
       <c r="AF359">
         <v>0.42</v>
       </c>
-    </row>
-    <row r="360" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG359">
+        <v>93.4</v>
+      </c>
+      <c r="AH359">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="360" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A360" s="19" t="s">
         <v>361</v>
       </c>
@@ -25889,8 +26511,14 @@
       <c r="AF360">
         <v>0.47</v>
       </c>
-    </row>
-    <row r="361" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG360">
+        <v>75.599999999999994</v>
+      </c>
+      <c r="AH360">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="361" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A361" s="19" t="s">
         <v>362</v>
       </c>
@@ -25955,8 +26583,14 @@
       <c r="AF361">
         <v>0.37</v>
       </c>
-    </row>
-    <row r="362" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG361">
+        <v>84.8</v>
+      </c>
+      <c r="AH361">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="362" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A362" s="19" t="s">
         <v>363</v>
       </c>
@@ -26019,8 +26653,14 @@
       <c r="AF362">
         <v>0.63</v>
       </c>
-    </row>
-    <row r="363" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG362">
+        <v>134.80000000000001</v>
+      </c>
+      <c r="AH362">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="363" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A363" s="19" t="s">
         <v>364</v>
       </c>
@@ -26085,8 +26725,14 @@
       <c r="AF363">
         <v>0.53</v>
       </c>
-    </row>
-    <row r="364" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG363">
+        <v>110.6</v>
+      </c>
+      <c r="AH363">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="364" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A364" s="19" t="s">
         <v>365</v>
       </c>
@@ -26149,8 +26795,14 @@
       <c r="AF364">
         <v>0.75</v>
       </c>
-    </row>
-    <row r="365" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG364">
+        <v>94.8</v>
+      </c>
+      <c r="AH364">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="365" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A365" s="19" t="s">
         <v>366</v>
       </c>
@@ -26215,8 +26867,14 @@
       <c r="AF365">
         <v>0.62</v>
       </c>
-    </row>
-    <row r="366" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG365">
+        <v>147.6</v>
+      </c>
+      <c r="AH365">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="366" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A366" s="19" t="s">
         <v>367</v>
       </c>
@@ -26279,8 +26937,14 @@
       <c r="AF366">
         <v>0.39</v>
       </c>
-    </row>
-    <row r="367" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG366">
+        <v>97.3</v>
+      </c>
+      <c r="AH366">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="367" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A367" s="19" t="s">
         <v>368</v>
       </c>
@@ -26345,8 +27009,14 @@
       <c r="AF367">
         <v>0.82</v>
       </c>
-    </row>
-    <row r="368" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG367">
+        <v>92.6</v>
+      </c>
+      <c r="AH367">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="368" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A368" s="19" t="s">
         <v>369</v>
       </c>
@@ -26409,8 +27079,14 @@
       <c r="AF368">
         <v>0.51</v>
       </c>
-    </row>
-    <row r="369" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG368">
+        <v>100.7</v>
+      </c>
+      <c r="AH368">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="369" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A369" s="19" t="s">
         <v>370</v>
       </c>
@@ -26477,8 +27153,14 @@
       <c r="AF369">
         <v>0.47</v>
       </c>
-    </row>
-    <row r="370" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG369">
+        <v>94.8</v>
+      </c>
+      <c r="AH369">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="370" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A370" s="22" t="s">
         <v>371</v>
       </c>
@@ -26544,7 +27226,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="371" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="371" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A371" s="22" t="s">
         <v>372</v>
       </c>
@@ -26610,7 +27292,7 @@
         <v>0.53</v>
       </c>
     </row>
-    <row r="372" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="372" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A372" s="22" t="s">
         <v>373</v>
       </c>
@@ -26674,7 +27356,7 @@
         <v>0.68</v>
       </c>
     </row>
-    <row r="373" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="373" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A373" s="22" t="s">
         <v>374</v>
       </c>
@@ -26740,7 +27422,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="374" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="374" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A374" s="22" t="s">
         <v>375</v>
       </c>
@@ -26804,7 +27486,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="375" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="375" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A375" s="22" t="s">
         <v>376</v>
       </c>
@@ -26870,7 +27552,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="376" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="376" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A376" s="22" t="s">
         <v>377</v>
       </c>
@@ -26934,7 +27616,7 @@
         <v>0.43</v>
       </c>
     </row>
-    <row r="377" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="377" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A377" s="22" t="s">
         <v>378</v>
       </c>
@@ -27000,7 +27682,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="378" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="378" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A378" s="22" t="s">
         <v>379</v>
       </c>
@@ -27064,7 +27746,7 @@
         <v>0.59</v>
       </c>
     </row>
-    <row r="379" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="379" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A379" s="22" t="s">
         <v>380</v>
       </c>
@@ -27130,7 +27812,7 @@
         <v>0.51</v>
       </c>
     </row>
-    <row r="380" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="380" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A380" s="22" t="s">
         <v>381</v>
       </c>
@@ -27194,7 +27876,7 @@
         <v>0.43</v>
       </c>
     </row>
-    <row r="381" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="381" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A381" s="22" t="s">
         <v>382</v>
       </c>
@@ -27260,7 +27942,7 @@
         <v>0.49</v>
       </c>
     </row>
-    <row r="382" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="382" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A382" s="22" t="s">
         <v>383</v>
       </c>
@@ -27324,7 +28006,7 @@
         <v>0.87</v>
       </c>
     </row>
-    <row r="383" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="383" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A383" s="22" t="s">
         <v>384</v>
       </c>
@@ -27392,7 +28074,7 @@
         <v>0.38</v>
       </c>
     </row>
-    <row r="384" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="384" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A384" s="22" t="s">
         <v>385</v>
       </c>
@@ -27456,7 +28138,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="385" spans="1:32" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="385" spans="1:34" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A385" s="25" t="s">
         <v>386</v>
       </c>
@@ -27485,7 +28167,7 @@
       </c>
       <c r="AA385"/>
     </row>
-    <row r="386" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="386" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A386" s="14" t="s">
         <v>387</v>
       </c>
@@ -27550,8 +28232,14 @@
       <c r="AF386">
         <v>0.34</v>
       </c>
-    </row>
-    <row r="387" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG386">
+        <v>46.3</v>
+      </c>
+      <c r="AH386">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="387" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A387" s="14" t="s">
         <v>388</v>
       </c>
@@ -27618,8 +28306,14 @@
       <c r="AF387">
         <v>0.55000000000000004</v>
       </c>
-    </row>
-    <row r="388" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG387">
+        <v>66</v>
+      </c>
+      <c r="AH387">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="388" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A388" s="25" t="s">
         <v>389</v>
       </c>
@@ -27650,8 +28344,11 @@
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="389" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AH388">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="389" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A389" s="14" t="s">
         <v>390</v>
       </c>
@@ -27718,8 +28415,14 @@
       <c r="AF389">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="390" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG389">
+        <v>48.3</v>
+      </c>
+      <c r="AH389">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="390" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A390" s="14" t="s">
         <v>391</v>
       </c>
@@ -27784,8 +28487,14 @@
       <c r="AF390">
         <v>0.44</v>
       </c>
-    </row>
-    <row r="391" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG390">
+        <v>53.3</v>
+      </c>
+      <c r="AH390">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="391" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A391" s="14" t="s">
         <v>392</v>
       </c>
@@ -27850,8 +28559,14 @@
       <c r="AF391">
         <v>0.35</v>
       </c>
-    </row>
-    <row r="392" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG391">
+        <v>53.8</v>
+      </c>
+      <c r="AH391">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="392" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A392" s="14" t="s">
         <v>393</v>
       </c>
@@ -27914,8 +28629,14 @@
       <c r="AF392">
         <v>0.36</v>
       </c>
-    </row>
-    <row r="393" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG392">
+        <v>60.6</v>
+      </c>
+      <c r="AH392">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="393" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A393" s="14" t="s">
         <v>394</v>
       </c>
@@ -27980,8 +28701,14 @@
       <c r="AF393">
         <v>0.32</v>
       </c>
-    </row>
-    <row r="394" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG393">
+        <v>41.4</v>
+      </c>
+      <c r="AH393">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="394" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A394" s="14" t="s">
         <v>395</v>
       </c>
@@ -28044,8 +28771,14 @@
       <c r="AF394">
         <v>0.56999999999999995</v>
       </c>
-    </row>
-    <row r="395" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG394">
+        <v>54.3</v>
+      </c>
+      <c r="AH394">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="395" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A395" s="14" t="s">
         <v>396</v>
       </c>
@@ -28110,8 +28843,14 @@
       <c r="AF395">
         <v>0.37</v>
       </c>
-    </row>
-    <row r="396" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG395">
+        <v>43.7</v>
+      </c>
+      <c r="AH395">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="396" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A396" s="14" t="s">
         <v>397</v>
       </c>
@@ -28174,8 +28913,14 @@
       <c r="AF396">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="397" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG396">
+        <v>44.6</v>
+      </c>
+      <c r="AH396">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="397" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A397" s="14" t="s">
         <v>398</v>
       </c>
@@ -28234,8 +28979,11 @@
       <c r="AD397">
         <v>0.122</v>
       </c>
-    </row>
-    <row r="398" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AH397">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="398" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A398" s="14" t="s">
         <v>399</v>
       </c>
@@ -28298,8 +29046,14 @@
       <c r="AF398">
         <v>0.41</v>
       </c>
-    </row>
-    <row r="399" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG398">
+        <v>61.3</v>
+      </c>
+      <c r="AH398">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="399" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A399" s="14" t="s">
         <v>400</v>
       </c>
@@ -28366,8 +29120,14 @@
       <c r="AF399">
         <v>0.24</v>
       </c>
-    </row>
-    <row r="400" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG399">
+        <v>45.7</v>
+      </c>
+      <c r="AH399">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="400" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A400" s="14" t="s">
         <v>401</v>
       </c>
@@ -28430,8 +29190,14 @@
       <c r="AF400">
         <v>0.55000000000000004</v>
       </c>
-    </row>
-    <row r="401" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG400">
+        <v>69.099999999999994</v>
+      </c>
+      <c r="AH400">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="401" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A401" s="14" t="s">
         <v>402</v>
       </c>
@@ -28496,8 +29262,14 @@
       <c r="AF401">
         <v>0.32</v>
       </c>
-    </row>
-    <row r="402" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG401">
+        <v>58.5</v>
+      </c>
+      <c r="AH401">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="402" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A402" s="19" t="s">
         <v>403</v>
       </c>
@@ -28563,7 +29335,7 @@
         <v>0.38</v>
       </c>
     </row>
-    <row r="403" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="403" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A403" s="19" t="s">
         <v>404</v>
       </c>
@@ -28631,7 +29403,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="404" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="404" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A404" s="19" t="s">
         <v>405</v>
       </c>
@@ -28697,7 +29469,7 @@
         <v>0.43</v>
       </c>
     </row>
-    <row r="405" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="405" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A405" s="19" t="s">
         <v>406</v>
       </c>
@@ -28765,7 +29537,7 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="406" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="406" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A406" s="19" t="s">
         <v>407</v>
       </c>
@@ -28829,7 +29601,7 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="407" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="407" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A407" s="19" t="s">
         <v>408</v>
       </c>
@@ -28895,7 +29667,7 @@
         <v>0.32</v>
       </c>
     </row>
-    <row r="408" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="408" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A408" s="19" t="s">
         <v>409</v>
       </c>
@@ -28959,7 +29731,7 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="409" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="409" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A409" s="19" t="s">
         <v>410</v>
       </c>
@@ -29025,7 +29797,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="410" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="410" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A410" s="19" t="s">
         <v>411</v>
       </c>
@@ -29089,7 +29861,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="411" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="411" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A411" s="19" t="s">
         <v>412</v>
       </c>
@@ -29155,7 +29927,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="412" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="412" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A412" s="19" t="s">
         <v>413</v>
       </c>
@@ -29219,7 +29991,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="413" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="413" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A413" s="19" t="s">
         <v>414</v>
       </c>
@@ -29285,7 +30057,7 @@
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="414" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="414" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A414" s="19" t="s">
         <v>415</v>
       </c>
@@ -29349,7 +30121,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="415" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="415" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A415" s="19" t="s">
         <v>416</v>
       </c>
@@ -29415,7 +30187,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="416" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="416" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A416" s="19" t="s">
         <v>417</v>
       </c>
@@ -29479,7 +30251,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="417" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="417" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A417" s="19" t="s">
         <v>418</v>
       </c>
@@ -29545,7 +30317,7 @@
         <v>0.26</v>
       </c>
     </row>
-    <row r="418" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="418" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A418" s="22" t="s">
         <v>419</v>
       </c>
@@ -29610,8 +30382,14 @@
       <c r="AF418">
         <v>0.35</v>
       </c>
-    </row>
-    <row r="419" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG418">
+        <v>53.9</v>
+      </c>
+      <c r="AH418">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="419" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A419" s="22" t="s">
         <v>420</v>
       </c>
@@ -29678,8 +30456,14 @@
       <c r="AF419">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="420" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG419">
+        <v>47.8</v>
+      </c>
+      <c r="AH419">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="420" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A420" s="22" t="s">
         <v>421</v>
       </c>
@@ -29744,8 +30528,14 @@
       <c r="AF420">
         <v>0.33</v>
       </c>
-    </row>
-    <row r="421" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG420">
+        <v>61.6</v>
+      </c>
+      <c r="AH420">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="421" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A421" s="22" t="s">
         <v>422</v>
       </c>
@@ -29810,8 +30600,14 @@
       <c r="AF421">
         <v>0.31</v>
       </c>
-    </row>
-    <row r="422" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG421">
+        <v>61.4</v>
+      </c>
+      <c r="AH421">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="422" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A422" s="22" t="s">
         <v>423</v>
       </c>
@@ -29874,8 +30670,14 @@
       <c r="AF422">
         <v>0.34</v>
       </c>
-    </row>
-    <row r="423" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG422">
+        <v>55.3</v>
+      </c>
+      <c r="AH422">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="423" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A423" s="22" t="s">
         <v>424</v>
       </c>
@@ -29940,8 +30742,14 @@
       <c r="AF423">
         <v>0.32</v>
       </c>
-    </row>
-    <row r="424" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG423">
+        <v>62.9</v>
+      </c>
+      <c r="AH423">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="424" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A424" s="22" t="s">
         <v>425</v>
       </c>
@@ -30004,8 +30812,14 @@
       <c r="AF424">
         <v>0.32</v>
       </c>
-    </row>
-    <row r="425" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG424">
+        <v>55</v>
+      </c>
+      <c r="AH424">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="425" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A425" s="22" t="s">
         <v>426</v>
       </c>
@@ -30070,8 +30884,14 @@
       <c r="AF425">
         <v>0.28999999999999998</v>
       </c>
-    </row>
-    <row r="426" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG425">
+        <v>64</v>
+      </c>
+      <c r="AH425">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="426" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A426" s="22" t="s">
         <v>427</v>
       </c>
@@ -30134,8 +30954,14 @@
       <c r="AF426">
         <v>0.31</v>
       </c>
-    </row>
-    <row r="427" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG426">
+        <v>65.3</v>
+      </c>
+      <c r="AH426">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="427" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A427" s="22" t="s">
         <v>428</v>
       </c>
@@ -30200,8 +31026,14 @@
       <c r="AF427">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="428" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG427">
+        <v>69.7</v>
+      </c>
+      <c r="AH427">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="428" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A428" s="22" t="s">
         <v>429</v>
       </c>
@@ -30264,8 +31096,14 @@
       <c r="AF428">
         <v>0.32</v>
       </c>
-    </row>
-    <row r="429" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG428">
+        <v>61.3</v>
+      </c>
+      <c r="AH428">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="429" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A429" s="22" t="s">
         <v>430</v>
       </c>
@@ -30330,8 +31168,14 @@
       <c r="AF429">
         <v>0.22</v>
       </c>
-    </row>
-    <row r="430" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG429">
+        <v>49.2</v>
+      </c>
+      <c r="AH429">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="430" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A430" s="22" t="s">
         <v>431</v>
       </c>
@@ -30394,8 +31238,14 @@
       <c r="AF430">
         <v>0.36</v>
       </c>
-    </row>
-    <row r="431" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG430">
+        <v>52.6</v>
+      </c>
+      <c r="AH430">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="431" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A431" s="22" t="s">
         <v>432</v>
       </c>
@@ -30458,8 +31308,14 @@
       <c r="AF431">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="432" spans="1:32" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AG431">
+        <v>54.2</v>
+      </c>
+      <c r="AH431">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="432" spans="1:34" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A432" s="22" t="s">
         <v>433</v>
       </c>
@@ -30522,8 +31378,14 @@
       <c r="AF432" s="5">
         <v>0.34</v>
       </c>
-    </row>
-    <row r="433" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG432" s="5">
+        <v>44.7</v>
+      </c>
+      <c r="AH432">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="433" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A433" s="22" t="s">
         <v>434</v>
       </c>
@@ -30588,8 +31450,14 @@
       <c r="AF433" s="5">
         <v>0.21</v>
       </c>
-    </row>
-    <row r="434" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG433" s="5">
+        <v>56.7</v>
+      </c>
+      <c r="AH433">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="434" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A434" s="14" t="s">
         <v>435</v>
       </c>
@@ -30654,8 +31522,14 @@
       <c r="AF434">
         <v>0.42</v>
       </c>
-    </row>
-    <row r="435" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG434" s="5">
+        <v>48</v>
+      </c>
+      <c r="AH434">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="435" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A435" s="14" t="s">
         <v>436</v>
       </c>
@@ -30722,8 +31596,14 @@
       <c r="AF435">
         <v>0.87</v>
       </c>
-    </row>
-    <row r="436" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG435" s="5">
+        <v>31.5</v>
+      </c>
+      <c r="AH435">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="436" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A436" s="14" t="s">
         <v>437</v>
       </c>
@@ -30788,8 +31668,14 @@
       <c r="AF436">
         <v>0.67</v>
       </c>
-    </row>
-    <row r="437" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG436" s="5">
+        <v>45.1</v>
+      </c>
+      <c r="AH436">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="437" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A437" s="14" t="s">
         <v>438</v>
       </c>
@@ -30856,8 +31742,14 @@
       <c r="AF437">
         <v>0.57999999999999996</v>
       </c>
-    </row>
-    <row r="438" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG437" s="5">
+        <v>33.299999999999997</v>
+      </c>
+      <c r="AH437">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="438" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A438" s="14" t="s">
         <v>439</v>
       </c>
@@ -30920,8 +31812,14 @@
       <c r="AF438">
         <v>0.96</v>
       </c>
-    </row>
-    <row r="439" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG438" s="5">
+        <v>22.2</v>
+      </c>
+      <c r="AH438">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="439" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A439" s="14" t="s">
         <v>440</v>
       </c>
@@ -30984,8 +31882,14 @@
       <c r="AF439">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="440" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG439" s="5">
+        <v>29.1</v>
+      </c>
+      <c r="AH439">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="440" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A440" s="14" t="s">
         <v>441</v>
       </c>
@@ -31048,8 +31952,14 @@
       <c r="AF440">
         <v>0.98</v>
       </c>
-    </row>
-    <row r="441" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG440" s="5">
+        <v>25.6</v>
+      </c>
+      <c r="AH440">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="441" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A441" s="25" t="s">
         <v>442</v>
       </c>
@@ -31076,8 +31986,11 @@
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="442" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AH441">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="442" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A442" s="14" t="s">
         <v>443</v>
       </c>
@@ -31140,8 +32053,14 @@
       <c r="AF442">
         <v>0.69</v>
       </c>
-    </row>
-    <row r="443" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG442">
+        <v>32.4</v>
+      </c>
+      <c r="AH442">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="443" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A443" s="14" t="s">
         <v>444</v>
       </c>
@@ -31208,8 +32127,14 @@
       <c r="AF443">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="444" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG443">
+        <v>26</v>
+      </c>
+      <c r="AH443">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="444" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A444" s="14" t="s">
         <v>445</v>
       </c>
@@ -31272,8 +32197,14 @@
       <c r="AF444">
         <v>0.62</v>
       </c>
-    </row>
-    <row r="445" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG444">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="AH444">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="445" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A445" s="14" t="s">
         <v>446</v>
       </c>
@@ -31338,8 +32269,14 @@
       <c r="AF445">
         <v>0.61</v>
       </c>
-    </row>
-    <row r="446" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG445">
+        <v>20.2</v>
+      </c>
+      <c r="AH445">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="446" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A446" s="14" t="s">
         <v>447</v>
       </c>
@@ -31402,8 +32339,14 @@
       <c r="AF446">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="447" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG446">
+        <v>29.9</v>
+      </c>
+      <c r="AH446">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="447" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A447" s="14" t="s">
         <v>448</v>
       </c>
@@ -31468,8 +32411,14 @@
       <c r="AF447">
         <v>0.64</v>
       </c>
-    </row>
-    <row r="448" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG447">
+        <v>26.1</v>
+      </c>
+      <c r="AH447">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="448" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A448" s="14" t="s">
         <v>449</v>
       </c>
@@ -31532,8 +32481,14 @@
       <c r="AF448">
         <v>0.46</v>
       </c>
-    </row>
-    <row r="449" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG448">
+        <v>41.3</v>
+      </c>
+      <c r="AH448">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="449" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A449" s="14" t="s">
         <v>450</v>
       </c>
@@ -31592,8 +32547,14 @@
       <c r="AF449">
         <v>0.48</v>
       </c>
-    </row>
-    <row r="450" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG449">
+        <v>21</v>
+      </c>
+      <c r="AH449">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="450" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A450" s="19" t="s">
         <v>451</v>
       </c>
@@ -31659,7 +32620,7 @@
         <v>0.48</v>
       </c>
     </row>
-    <row r="451" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="451" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A451" s="19" t="s">
         <v>452</v>
       </c>
@@ -31727,7 +32688,7 @@
         <v>0.53</v>
       </c>
     </row>
-    <row r="452" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="452" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A452" s="19" t="s">
         <v>453</v>
       </c>
@@ -31793,7 +32754,7 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="453" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="453" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A453" s="19" t="s">
         <v>454</v>
       </c>
@@ -31859,7 +32820,7 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="454" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="454" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A454" s="19" t="s">
         <v>455</v>
       </c>
@@ -31923,7 +32884,7 @@
         <v>0.74</v>
       </c>
     </row>
-    <row r="455" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="455" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A455" s="19" t="s">
         <v>456</v>
       </c>
@@ -31989,7 +32950,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="456" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="456" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A456" s="19" t="s">
         <v>457</v>
       </c>
@@ -32053,7 +33014,7 @@
         <v>0.71</v>
       </c>
     </row>
-    <row r="457" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="457" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A457" s="19" t="s">
         <v>458</v>
       </c>
@@ -32119,7 +33080,7 @@
         <v>0.56999999999999995</v>
       </c>
     </row>
-    <row r="458" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="458" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A458" s="19" t="s">
         <v>459</v>
       </c>
@@ -32183,7 +33144,7 @@
         <v>0.49</v>
       </c>
     </row>
-    <row r="459" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="459" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A459" s="19" t="s">
         <v>460</v>
       </c>
@@ -32249,7 +33210,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="460" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="460" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A460" s="19" t="s">
         <v>461</v>
       </c>
@@ -32313,7 +33274,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="461" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="461" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A461" s="19" t="s">
         <v>462</v>
       </c>
@@ -32379,7 +33340,7 @@
         <v>0.48</v>
       </c>
     </row>
-    <row r="462" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="462" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A462" s="19" t="s">
         <v>463</v>
       </c>
@@ -32443,7 +33404,7 @@
         <v>0.63</v>
       </c>
     </row>
-    <row r="463" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="463" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A463" s="19" t="s">
         <v>464</v>
       </c>
@@ -32509,7 +33470,7 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="464" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="464" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A464" s="19" t="s">
         <v>465</v>
       </c>

</xml_diff>

<commit_message>
rgr plots and models
</commit_message>
<xml_diff>
--- a/data/observation_datasheet.xlsx
+++ b/data/observation_datasheet.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28209"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/CatherineChamberlain/Documents/git/chillfreeze/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/catchamberlain/Documents/git/chillfreeze/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B9F42F9-D7CB-5446-A1D4-7E9548370530}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" activeTab="1"/>
+    <workbookView xWindow="7040" yWindow="3220" windowWidth="31580" windowHeight="19540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="observation_datasheet" sheetId="1" r:id="rId1"/>
@@ -19,13 +20,10 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Feb19 Breakdown'!$A$1:$J$61</definedName>
   </definedNames>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -33,6 +31,9 @@
         <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
   </extLst>
 </workbook>
 </file>
@@ -1786,7 +1787,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -2908,8 +2909,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:M481"/>
@@ -5501,14 +5502,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AH481"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="86" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B430" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="P24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AG450" sqref="AG450"/>
+      <selection pane="bottomRight" activeCell="AG52" sqref="AG52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5519,10 +5520,8 @@
     <col min="4" max="4" width="10.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="10.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="13" width="10.85546875" hidden="1" customWidth="1"/>
-    <col min="14" max="19" width="0" hidden="1" customWidth="1"/>
-    <col min="20" max="22" width="10.7109375" hidden="1" customWidth="1"/>
-    <col min="23" max="30" width="0" hidden="1" customWidth="1"/>
+    <col min="8" max="13" width="10.85546875" customWidth="1"/>
+    <col min="14" max="30" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.2">
@@ -6811,6 +6810,12 @@
       <c r="AF18">
         <v>0.52</v>
       </c>
+      <c r="AG18">
+        <v>66.3</v>
+      </c>
+      <c r="AH18">
+        <v>192</v>
+      </c>
     </row>
     <row r="19" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A19" s="19" t="s">
@@ -6878,6 +6883,12 @@
       </c>
       <c r="AF19">
         <v>0.37</v>
+      </c>
+      <c r="AG19">
+        <v>65.099999999999994</v>
+      </c>
+      <c r="AH19">
+        <v>192</v>
       </c>
     </row>
     <row r="20" spans="1:34" x14ac:dyDescent="0.2">
@@ -6943,6 +6954,12 @@
       <c r="AF20">
         <v>0.44</v>
       </c>
+      <c r="AG20">
+        <v>80</v>
+      </c>
+      <c r="AH20">
+        <v>192</v>
+      </c>
     </row>
     <row r="21" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A21" s="19" t="s">
@@ -7008,6 +7025,12 @@
       </c>
       <c r="AF21">
         <v>0.35</v>
+      </c>
+      <c r="AG21">
+        <v>33.9</v>
+      </c>
+      <c r="AH21">
+        <v>192</v>
       </c>
     </row>
     <row r="22" spans="1:34" x14ac:dyDescent="0.2">
@@ -7073,6 +7096,12 @@
       <c r="AF22">
         <v>0.24</v>
       </c>
+      <c r="AG22">
+        <v>81.8</v>
+      </c>
+      <c r="AH22">
+        <v>192</v>
+      </c>
     </row>
     <row r="23" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A23" s="19" t="s">
@@ -7138,6 +7167,12 @@
       </c>
       <c r="AF23">
         <v>0.5</v>
+      </c>
+      <c r="AG23">
+        <v>59.8</v>
+      </c>
+      <c r="AH23">
+        <v>192</v>
       </c>
     </row>
     <row r="24" spans="1:34" x14ac:dyDescent="0.2">
@@ -7200,6 +7235,12 @@
       <c r="AF24">
         <v>0.33</v>
       </c>
+      <c r="AG24">
+        <v>55.2</v>
+      </c>
+      <c r="AH24">
+        <v>192</v>
+      </c>
     </row>
     <row r="25" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A25" s="19" t="s">
@@ -7259,6 +7300,12 @@
       </c>
       <c r="AF25">
         <v>0.22</v>
+      </c>
+      <c r="AG25">
+        <v>47.8</v>
+      </c>
+      <c r="AH25">
+        <v>192</v>
       </c>
     </row>
     <row r="26" spans="1:34" x14ac:dyDescent="0.2">
@@ -7324,6 +7371,12 @@
       <c r="AF26">
         <v>0.17</v>
       </c>
+      <c r="AG26">
+        <v>39.700000000000003</v>
+      </c>
+      <c r="AH26">
+        <v>192</v>
+      </c>
     </row>
     <row r="27" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A27" s="19" t="s">
@@ -7380,6 +7433,12 @@
       </c>
       <c r="AE27">
         <v>0.14000000000000001</v>
+      </c>
+      <c r="AG27">
+        <v>22.5</v>
+      </c>
+      <c r="AH27">
+        <v>192</v>
       </c>
     </row>
     <row r="28" spans="1:34" x14ac:dyDescent="0.2">
@@ -7445,6 +7504,12 @@
       <c r="AF28">
         <v>0.23</v>
       </c>
+      <c r="AG28">
+        <v>60.5</v>
+      </c>
+      <c r="AH28">
+        <v>192</v>
+      </c>
     </row>
     <row r="29" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A29" s="19" t="s">
@@ -7504,6 +7569,12 @@
       </c>
       <c r="AF29">
         <v>0.33</v>
+      </c>
+      <c r="AG29">
+        <v>44.8</v>
+      </c>
+      <c r="AH29">
+        <v>192</v>
       </c>
     </row>
     <row r="30" spans="1:34" x14ac:dyDescent="0.2">
@@ -7563,6 +7634,12 @@
       <c r="AF30">
         <v>0.26</v>
       </c>
+      <c r="AG30">
+        <v>52.7</v>
+      </c>
+      <c r="AH30">
+        <v>192</v>
+      </c>
     </row>
     <row r="31" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A31" s="19" t="s">
@@ -7628,6 +7705,12 @@
       </c>
       <c r="AF31">
         <v>0.28000000000000003</v>
+      </c>
+      <c r="AG31">
+        <v>32.1</v>
+      </c>
+      <c r="AH31">
+        <v>192</v>
       </c>
     </row>
     <row r="32" spans="1:34" x14ac:dyDescent="0.2">
@@ -7687,8 +7770,14 @@
       <c r="AF32">
         <v>0.57999999999999996</v>
       </c>
-    </row>
-    <row r="33" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG32">
+        <v>65</v>
+      </c>
+      <c r="AH32">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="33" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A33" s="19" t="s">
         <v>34</v>
       </c>
@@ -7747,8 +7836,14 @@
       <c r="AF33">
         <v>0.22</v>
       </c>
-    </row>
-    <row r="34" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG33">
+        <v>52.5</v>
+      </c>
+      <c r="AH33">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="34" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A34" s="22" t="s">
         <v>35</v>
       </c>
@@ -7813,8 +7908,14 @@
       <c r="AF34">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="35" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG34">
+        <v>65.599999999999994</v>
+      </c>
+      <c r="AH34">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="35" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A35" s="22" t="s">
         <v>36</v>
       </c>
@@ -7881,8 +7982,14 @@
       <c r="AF35">
         <v>0.34</v>
       </c>
-    </row>
-    <row r="36" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG35">
+        <v>69.8</v>
+      </c>
+      <c r="AH35">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="36" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A36" s="22" t="s">
         <v>37</v>
       </c>
@@ -7945,8 +8052,14 @@
       <c r="AF36">
         <v>0.57999999999999996</v>
       </c>
-    </row>
-    <row r="37" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG36">
+        <v>72.099999999999994</v>
+      </c>
+      <c r="AH36">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="37" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A37" s="22" t="s">
         <v>38</v>
       </c>
@@ -8011,8 +8124,14 @@
       <c r="AF37">
         <v>0.34</v>
       </c>
-    </row>
-    <row r="38" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG37">
+        <v>54.8</v>
+      </c>
+      <c r="AH37">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="38" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A38" s="22" t="s">
         <v>39</v>
       </c>
@@ -8075,8 +8194,14 @@
       <c r="AF38">
         <v>0.32</v>
       </c>
-    </row>
-    <row r="39" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG38">
+        <v>60.9</v>
+      </c>
+      <c r="AH38">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="39" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A39" s="22" t="s">
         <v>40</v>
       </c>
@@ -8141,8 +8266,14 @@
       <c r="AF39">
         <v>0.34</v>
       </c>
-    </row>
-    <row r="40" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG39">
+        <v>78.2</v>
+      </c>
+      <c r="AH39">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="40" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A40" s="22" t="s">
         <v>41</v>
       </c>
@@ -8199,8 +8330,14 @@
       <c r="AF40">
         <v>0.19</v>
       </c>
-    </row>
-    <row r="41" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG40">
+        <v>56.9</v>
+      </c>
+      <c r="AH40">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="41" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A41" s="22" t="s">
         <v>42</v>
       </c>
@@ -8265,8 +8402,14 @@
       <c r="AF41">
         <v>0.21</v>
       </c>
-    </row>
-    <row r="42" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG41">
+        <v>66.099999999999994</v>
+      </c>
+      <c r="AH41">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="42" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A42" s="22" t="s">
         <v>43</v>
       </c>
@@ -8323,8 +8466,14 @@
       <c r="AF42">
         <v>0.28999999999999998</v>
       </c>
-    </row>
-    <row r="43" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG42">
+        <v>57.9</v>
+      </c>
+      <c r="AH42">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="43" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A43" s="22" t="s">
         <v>44</v>
       </c>
@@ -8389,8 +8538,14 @@
       <c r="AF43">
         <v>0.33</v>
       </c>
-    </row>
-    <row r="44" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG43">
+        <v>71.099999999999994</v>
+      </c>
+      <c r="AH43">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="44" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A44" s="22" t="s">
         <v>45</v>
       </c>
@@ -8447,8 +8602,14 @@
       <c r="AF44">
         <v>0.44</v>
       </c>
-    </row>
-    <row r="45" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG44">
+        <v>45.5</v>
+      </c>
+      <c r="AH44">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="45" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A45" s="22" t="s">
         <v>46</v>
       </c>
@@ -8507,8 +8668,14 @@
       <c r="AF45">
         <v>0.47</v>
       </c>
-    </row>
-    <row r="46" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG45">
+        <v>51.6</v>
+      </c>
+      <c r="AH45">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="46" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A46" s="22" t="s">
         <v>47</v>
       </c>
@@ -8571,8 +8738,14 @@
       <c r="AF46">
         <v>0.31</v>
       </c>
-    </row>
-    <row r="47" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG46">
+        <v>75</v>
+      </c>
+      <c r="AH46">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="47" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A47" s="22" t="s">
         <v>48</v>
       </c>
@@ -8631,8 +8804,14 @@
       <c r="AF47">
         <v>0.46</v>
       </c>
-    </row>
-    <row r="48" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG47">
+        <v>53.3</v>
+      </c>
+      <c r="AH47">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="48" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A48" s="22" t="s">
         <v>49</v>
       </c>
@@ -8689,6 +8868,12 @@
       <c r="AF48">
         <v>0.32</v>
       </c>
+      <c r="AG48">
+        <v>54.3</v>
+      </c>
+      <c r="AH48">
+        <v>192</v>
+      </c>
     </row>
     <row r="49" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A49" s="22" t="s">
@@ -8749,6 +8934,12 @@
       <c r="AF49">
         <v>0.31</v>
       </c>
+      <c r="AG49">
+        <v>49.6</v>
+      </c>
+      <c r="AH49">
+        <v>192</v>
+      </c>
     </row>
     <row r="50" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A50" s="14" t="s">
@@ -8890,7 +9081,7 @@
         <v>0.35</v>
       </c>
       <c r="AG51">
-        <v>134.19999999999999</v>
+        <v>121.8</v>
       </c>
       <c r="AH51">
         <v>191</v>
@@ -9910,6 +10101,12 @@
       <c r="AF66">
         <v>0.39</v>
       </c>
+      <c r="AG66">
+        <v>79.3</v>
+      </c>
+      <c r="AH66">
+        <v>192</v>
+      </c>
     </row>
     <row r="67" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A67" s="19" t="s">
@@ -9974,6 +10171,12 @@
       </c>
       <c r="AF67">
         <v>0.26</v>
+      </c>
+      <c r="AG67">
+        <v>35.9</v>
+      </c>
+      <c r="AH67">
+        <v>192</v>
       </c>
     </row>
     <row r="68" spans="1:34" x14ac:dyDescent="0.2">
@@ -10039,6 +10242,12 @@
       <c r="AF68">
         <v>0.17</v>
       </c>
+      <c r="AG68">
+        <v>72.099999999999994</v>
+      </c>
+      <c r="AH68">
+        <v>192</v>
+      </c>
     </row>
     <row r="69" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A69" s="19" t="s">
@@ -10104,6 +10313,12 @@
       </c>
       <c r="AF69">
         <v>0.3</v>
+      </c>
+      <c r="AG69">
+        <v>53.9</v>
+      </c>
+      <c r="AH69">
+        <v>192</v>
       </c>
     </row>
     <row r="70" spans="1:34" x14ac:dyDescent="0.2">
@@ -10169,6 +10384,12 @@
       <c r="AF70">
         <v>0.38</v>
       </c>
+      <c r="AG70">
+        <v>61.1</v>
+      </c>
+      <c r="AH70">
+        <v>192</v>
+      </c>
     </row>
     <row r="71" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A71" s="19" t="s">
@@ -10234,6 +10455,12 @@
       </c>
       <c r="AF71">
         <v>0.21</v>
+      </c>
+      <c r="AG71">
+        <v>48.1</v>
+      </c>
+      <c r="AH71">
+        <v>192</v>
       </c>
     </row>
     <row r="72" spans="1:34" x14ac:dyDescent="0.2">
@@ -10329,6 +10556,12 @@
       <c r="AF73">
         <v>0.25</v>
       </c>
+      <c r="AG73">
+        <v>60.5</v>
+      </c>
+      <c r="AH73">
+        <v>192</v>
+      </c>
     </row>
     <row r="74" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A74" s="19" t="s">
@@ -10393,6 +10626,12 @@
       <c r="AF74">
         <v>0.39</v>
       </c>
+      <c r="AG74">
+        <v>73.8</v>
+      </c>
+      <c r="AH74">
+        <v>192</v>
+      </c>
     </row>
     <row r="75" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A75" s="19" t="s">
@@ -10457,6 +10696,12 @@
       </c>
       <c r="AF75">
         <v>0.37</v>
+      </c>
+      <c r="AG75">
+        <v>23.5</v>
+      </c>
+      <c r="AH75">
+        <v>192</v>
       </c>
     </row>
     <row r="76" spans="1:34" x14ac:dyDescent="0.2">
@@ -10522,6 +10767,12 @@
       <c r="AF76">
         <v>0.28999999999999998</v>
       </c>
+      <c r="AG76">
+        <v>77.3</v>
+      </c>
+      <c r="AH76">
+        <v>192</v>
+      </c>
     </row>
     <row r="77" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A77" s="19" t="s">
@@ -10589,6 +10840,12 @@
       </c>
       <c r="AF77">
         <v>0.32</v>
+      </c>
+      <c r="AG77">
+        <v>50.2</v>
+      </c>
+      <c r="AH77">
+        <v>192</v>
       </c>
     </row>
     <row r="78" spans="1:34" x14ac:dyDescent="0.2">
@@ -10654,6 +10911,12 @@
       <c r="AF78">
         <v>0.25</v>
       </c>
+      <c r="AG78">
+        <v>62.9</v>
+      </c>
+      <c r="AH78">
+        <v>192</v>
+      </c>
     </row>
     <row r="79" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A79" s="19" t="s">
@@ -10719,6 +10982,12 @@
       </c>
       <c r="AF79">
         <v>0.26</v>
+      </c>
+      <c r="AG79">
+        <v>62.8</v>
+      </c>
+      <c r="AH79">
+        <v>192</v>
       </c>
     </row>
     <row r="80" spans="1:34" x14ac:dyDescent="0.2">
@@ -10784,8 +11053,14 @@
       <c r="AF80">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="81" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG80">
+        <v>62.6</v>
+      </c>
+      <c r="AH80">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="81" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A81" s="19" t="s">
         <v>82</v>
       </c>
@@ -10850,8 +11125,11 @@
       <c r="AF81">
         <v>0.27</v>
       </c>
-    </row>
-    <row r="82" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG81">
+        <v>71.2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A82" s="25" t="s">
         <v>83</v>
       </c>
@@ -10883,7 +11161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A83" s="22" t="s">
         <v>84</v>
       </c>
@@ -10950,8 +11228,14 @@
       <c r="AF83">
         <v>0.33</v>
       </c>
-    </row>
-    <row r="84" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG83">
+        <v>51.5</v>
+      </c>
+      <c r="AH83">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="84" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A84" s="22" t="s">
         <v>85</v>
       </c>
@@ -11016,8 +11300,14 @@
       <c r="AF84">
         <v>0.28999999999999998</v>
       </c>
-    </row>
-    <row r="85" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG84">
+        <v>67.900000000000006</v>
+      </c>
+      <c r="AH84">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="85" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A85" s="22" t="s">
         <v>86</v>
       </c>
@@ -11082,8 +11372,14 @@
       <c r="AF85">
         <v>0.26</v>
       </c>
-    </row>
-    <row r="86" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG85">
+        <v>64.8</v>
+      </c>
+      <c r="AH85">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="86" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A86" s="22" t="s">
         <v>87</v>
       </c>
@@ -11146,8 +11442,14 @@
       <c r="AF86">
         <v>0.28000000000000003</v>
       </c>
-    </row>
-    <row r="87" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG86">
+        <v>66.400000000000006</v>
+      </c>
+      <c r="AH86">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="87" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A87" s="25" t="s">
         <v>88</v>
       </c>
@@ -11175,7 +11477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A88" s="25" t="s">
         <v>89</v>
       </c>
@@ -11203,7 +11505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A89" s="22" t="s">
         <v>90</v>
       </c>
@@ -11268,8 +11570,14 @@
       <c r="AF89">
         <v>0.28000000000000003</v>
       </c>
-    </row>
-    <row r="90" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG89">
+        <v>73.2</v>
+      </c>
+      <c r="AH89">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="90" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A90" s="22" t="s">
         <v>91</v>
       </c>
@@ -11332,8 +11640,14 @@
       <c r="AF90">
         <v>0.37</v>
       </c>
-    </row>
-    <row r="91" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG90">
+        <v>51.1</v>
+      </c>
+      <c r="AH90">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="91" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A91" s="22" t="s">
         <v>92</v>
       </c>
@@ -11398,8 +11712,14 @@
       <c r="AF91">
         <v>0.21</v>
       </c>
-    </row>
-    <row r="92" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG91">
+        <v>73.5</v>
+      </c>
+      <c r="AH91">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="92" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A92" s="22" t="s">
         <v>93</v>
       </c>
@@ -11462,8 +11782,14 @@
       <c r="AF92">
         <v>0.36</v>
       </c>
-    </row>
-    <row r="93" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG92">
+        <v>80.5</v>
+      </c>
+      <c r="AH92">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="93" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A93" s="22" t="s">
         <v>94</v>
       </c>
@@ -11528,8 +11854,14 @@
       <c r="AF93">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="94" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG93">
+        <v>59.8</v>
+      </c>
+      <c r="AH93">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="94" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A94" s="22" t="s">
         <v>95</v>
       </c>
@@ -11592,8 +11924,14 @@
       <c r="AF94">
         <v>0.19</v>
       </c>
-    </row>
-    <row r="95" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG94">
+        <v>90.8</v>
+      </c>
+      <c r="AH94">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="95" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A95" s="22" t="s">
         <v>96</v>
       </c>
@@ -11658,8 +11996,14 @@
       <c r="AF95">
         <v>0.24</v>
       </c>
-    </row>
-    <row r="96" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG95">
+        <v>78.8</v>
+      </c>
+      <c r="AH95">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="96" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A96" s="22" t="s">
         <v>97</v>
       </c>
@@ -11722,6 +12066,12 @@
       <c r="AF96">
         <v>0.28000000000000003</v>
       </c>
+      <c r="AG96">
+        <v>65.099999999999994</v>
+      </c>
+      <c r="AH96">
+        <v>192</v>
+      </c>
     </row>
     <row r="97" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A97" s="22" t="s">
@@ -11787,6 +12137,12 @@
       </c>
       <c r="AF97">
         <v>0.4</v>
+      </c>
+      <c r="AG97">
+        <v>90.2</v>
+      </c>
+      <c r="AH97">
+        <v>192</v>
       </c>
     </row>
     <row r="98" spans="1:34" x14ac:dyDescent="0.2">
@@ -13075,6 +13431,12 @@
       <c r="AF114">
         <v>0.23</v>
       </c>
+      <c r="AG114">
+        <v>51.9</v>
+      </c>
+      <c r="AH114">
+        <v>192</v>
+      </c>
     </row>
     <row r="115" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A115" s="19" t="s">
@@ -13140,6 +13502,12 @@
       </c>
       <c r="AF115">
         <v>0.19</v>
+      </c>
+      <c r="AG115">
+        <v>64.7</v>
+      </c>
+      <c r="AH115">
+        <v>192</v>
       </c>
     </row>
     <row r="116" spans="1:34" x14ac:dyDescent="0.2">
@@ -13205,6 +13573,12 @@
       <c r="AF116">
         <v>0.22</v>
       </c>
+      <c r="AG116">
+        <v>42.4</v>
+      </c>
+      <c r="AH116">
+        <v>192</v>
+      </c>
     </row>
     <row r="117" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A117" s="19" t="s">
@@ -13270,6 +13644,12 @@
       </c>
       <c r="AF117">
         <v>0.27</v>
+      </c>
+      <c r="AG117">
+        <v>41.3</v>
+      </c>
+      <c r="AH117">
+        <v>192</v>
       </c>
     </row>
     <row r="118" spans="1:34" x14ac:dyDescent="0.2">
@@ -13335,6 +13715,12 @@
       <c r="AF118">
         <v>0.18</v>
       </c>
+      <c r="AG118">
+        <v>46</v>
+      </c>
+      <c r="AH118">
+        <v>192</v>
+      </c>
     </row>
     <row r="119" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A119" s="19" t="s">
@@ -13402,6 +13788,12 @@
       </c>
       <c r="AF119">
         <v>0.27</v>
+      </c>
+      <c r="AG119">
+        <v>49.1</v>
+      </c>
+      <c r="AH119">
+        <v>192</v>
       </c>
     </row>
     <row r="120" spans="1:34" x14ac:dyDescent="0.2">
@@ -13467,6 +13859,12 @@
       <c r="AF120">
         <v>0.33</v>
       </c>
+      <c r="AG120">
+        <v>55.2</v>
+      </c>
+      <c r="AH120">
+        <v>192</v>
+      </c>
     </row>
     <row r="121" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A121" s="19" t="s">
@@ -13532,6 +13930,12 @@
       </c>
       <c r="AF121">
         <v>0.27</v>
+      </c>
+      <c r="AG121">
+        <v>36.1</v>
+      </c>
+      <c r="AH121">
+        <v>192</v>
       </c>
     </row>
     <row r="122" spans="1:34" x14ac:dyDescent="0.2">
@@ -13597,6 +14001,12 @@
       <c r="AF122">
         <v>0.24</v>
       </c>
+      <c r="AG122">
+        <v>57.5</v>
+      </c>
+      <c r="AH122">
+        <v>192</v>
+      </c>
     </row>
     <row r="123" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A123" s="19" t="s">
@@ -13664,6 +14074,12 @@
       </c>
       <c r="AF123">
         <v>0.28000000000000003</v>
+      </c>
+      <c r="AG123">
+        <v>48.2</v>
+      </c>
+      <c r="AH123">
+        <v>192</v>
       </c>
     </row>
     <row r="124" spans="1:34" x14ac:dyDescent="0.2">
@@ -13729,6 +14145,12 @@
       <c r="AF124">
         <v>0.28999999999999998</v>
       </c>
+      <c r="AG124">
+        <v>54.3</v>
+      </c>
+      <c r="AH124">
+        <v>192</v>
+      </c>
     </row>
     <row r="125" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A125" s="19" t="s">
@@ -13794,6 +14216,12 @@
       </c>
       <c r="AF125">
         <v>0.23</v>
+      </c>
+      <c r="AG125">
+        <v>49.7</v>
+      </c>
+      <c r="AH125">
+        <v>192</v>
       </c>
     </row>
     <row r="126" spans="1:34" x14ac:dyDescent="0.2">
@@ -13859,6 +14287,12 @@
       <c r="AF126">
         <v>0.21</v>
       </c>
+      <c r="AG126">
+        <v>55.5</v>
+      </c>
+      <c r="AH126">
+        <v>192</v>
+      </c>
     </row>
     <row r="127" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A127" s="19" t="s">
@@ -13924,6 +14358,12 @@
       </c>
       <c r="AF127">
         <v>0.15</v>
+      </c>
+      <c r="AG127">
+        <v>54.1</v>
+      </c>
+      <c r="AH127">
+        <v>192</v>
       </c>
     </row>
     <row r="128" spans="1:34" x14ac:dyDescent="0.2">
@@ -13989,8 +14429,14 @@
       <c r="AF128">
         <v>0.31</v>
       </c>
-    </row>
-    <row r="129" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG128">
+        <v>55.9</v>
+      </c>
+      <c r="AH128">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="129" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A129" s="19" t="s">
         <v>130</v>
       </c>
@@ -14055,8 +14501,14 @@
       <c r="AF129">
         <v>0.28999999999999998</v>
       </c>
-    </row>
-    <row r="130" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG129">
+        <v>46.9</v>
+      </c>
+      <c r="AH129">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="130" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A130" s="22" t="s">
         <v>131</v>
       </c>
@@ -14121,8 +14573,14 @@
       <c r="AF130">
         <v>0.33</v>
       </c>
-    </row>
-    <row r="131" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG130">
+        <v>63.4</v>
+      </c>
+      <c r="AH130">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="131" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A131" s="22" t="s">
         <v>132</v>
       </c>
@@ -14189,8 +14647,14 @@
       <c r="AF131">
         <v>0.12</v>
       </c>
-    </row>
-    <row r="132" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG131">
+        <v>63.5</v>
+      </c>
+      <c r="AH131">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="132" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A132" s="22" t="s">
         <v>133</v>
       </c>
@@ -14255,8 +14719,14 @@
       <c r="AF132">
         <v>0.34</v>
       </c>
-    </row>
-    <row r="133" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG132">
+        <v>46.4</v>
+      </c>
+      <c r="AH132">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="133" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A133" s="22" t="s">
         <v>134</v>
       </c>
@@ -14321,8 +14791,14 @@
       <c r="AF133">
         <v>0.31</v>
       </c>
-    </row>
-    <row r="134" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG133">
+        <v>64.900000000000006</v>
+      </c>
+      <c r="AH133">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="134" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A134" s="22" t="s">
         <v>135</v>
       </c>
@@ -14385,8 +14861,14 @@
       <c r="AF134">
         <v>0.33</v>
       </c>
-    </row>
-    <row r="135" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG134">
+        <v>63.5</v>
+      </c>
+      <c r="AH134">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="135" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A135" s="22" t="s">
         <v>136</v>
       </c>
@@ -14451,8 +14933,14 @@
       <c r="AF135">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="136" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG135">
+        <v>46.2</v>
+      </c>
+      <c r="AH135">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="136" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A136" s="22" t="s">
         <v>137</v>
       </c>
@@ -14515,8 +15003,14 @@
       <c r="AF136">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="137" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG136">
+        <v>60.8</v>
+      </c>
+      <c r="AH136">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="137" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A137" s="22" t="s">
         <v>138</v>
       </c>
@@ -14581,8 +15075,14 @@
       <c r="AF137">
         <v>0.24</v>
       </c>
-    </row>
-    <row r="138" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG137">
+        <v>43.6</v>
+      </c>
+      <c r="AH137">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="138" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A138" s="22" t="s">
         <v>139</v>
       </c>
@@ -14645,8 +15145,14 @@
       <c r="AF138">
         <v>0.22</v>
       </c>
-    </row>
-    <row r="139" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG138">
+        <v>81.099999999999994</v>
+      </c>
+      <c r="AH138">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="139" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A139" s="22" t="s">
         <v>140</v>
       </c>
@@ -14711,8 +15217,14 @@
       <c r="AF139">
         <v>0.19</v>
       </c>
-    </row>
-    <row r="140" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG139">
+        <v>56</v>
+      </c>
+      <c r="AH139">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="140" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A140" s="22" t="s">
         <v>141</v>
       </c>
@@ -14775,8 +15287,14 @@
       <c r="AF140">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="141" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG140">
+        <v>51.3</v>
+      </c>
+      <c r="AH140">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="141" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A141" s="22" t="s">
         <v>142</v>
       </c>
@@ -14841,8 +15359,14 @@
       <c r="AF141">
         <v>0.22</v>
       </c>
-    </row>
-    <row r="142" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG141">
+        <v>41.9</v>
+      </c>
+      <c r="AH141">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="142" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A142" s="22" t="s">
         <v>143</v>
       </c>
@@ -14905,8 +15429,14 @@
       <c r="AF142">
         <v>0.12</v>
       </c>
-    </row>
-    <row r="143" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG142">
+        <v>64.900000000000006</v>
+      </c>
+      <c r="AH142">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="143" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A143" s="22" t="s">
         <v>144</v>
       </c>
@@ -14970,8 +15500,14 @@
       <c r="AF143">
         <v>0.12</v>
       </c>
-    </row>
-    <row r="144" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG143">
+        <v>50.6</v>
+      </c>
+      <c r="AH143">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="144" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A144" s="22" t="s">
         <v>145</v>
       </c>
@@ -15034,6 +15570,12 @@
       <c r="AF144">
         <v>0.14000000000000001</v>
       </c>
+      <c r="AG144">
+        <v>57.2</v>
+      </c>
+      <c r="AH144">
+        <v>192</v>
+      </c>
     </row>
     <row r="145" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A145" s="22" t="s">
@@ -15099,6 +15641,12 @@
       </c>
       <c r="AF145">
         <v>0.18</v>
+      </c>
+      <c r="AG145">
+        <v>43.7</v>
+      </c>
+      <c r="AH145">
+        <v>192</v>
       </c>
     </row>
     <row r="146" spans="1:34" x14ac:dyDescent="0.2">
@@ -16306,6 +16854,12 @@
       <c r="AF162">
         <v>0.21</v>
       </c>
+      <c r="AG162">
+        <v>91.2</v>
+      </c>
+      <c r="AH162">
+        <v>192</v>
+      </c>
     </row>
     <row r="163" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A163" s="19" t="s">
@@ -16371,6 +16925,12 @@
       </c>
       <c r="AF163">
         <v>0.23</v>
+      </c>
+      <c r="AG163">
+        <v>86.7</v>
+      </c>
+      <c r="AH163">
+        <v>192</v>
       </c>
     </row>
     <row r="164" spans="1:34" x14ac:dyDescent="0.2">
@@ -16436,6 +16996,12 @@
       <c r="AF164">
         <v>0.36</v>
       </c>
+      <c r="AG164">
+        <v>45.6</v>
+      </c>
+      <c r="AH164">
+        <v>192</v>
+      </c>
     </row>
     <row r="165" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A165" s="19" t="s">
@@ -16501,6 +17067,12 @@
       </c>
       <c r="AF165">
         <v>0.38</v>
+      </c>
+      <c r="AG165">
+        <v>77.400000000000006</v>
+      </c>
+      <c r="AH165">
+        <v>192</v>
       </c>
     </row>
     <row r="166" spans="1:34" x14ac:dyDescent="0.2">
@@ -16566,6 +17138,12 @@
       <c r="AF166">
         <v>0.32</v>
       </c>
+      <c r="AG166">
+        <v>82.4</v>
+      </c>
+      <c r="AH166">
+        <v>192</v>
+      </c>
     </row>
     <row r="167" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A167" s="19" t="s">
@@ -16631,6 +17209,12 @@
       </c>
       <c r="AF167">
         <v>0.27</v>
+      </c>
+      <c r="AG167">
+        <v>83.7</v>
+      </c>
+      <c r="AH167">
+        <v>192</v>
       </c>
     </row>
     <row r="168" spans="1:34" x14ac:dyDescent="0.2">
@@ -16696,6 +17280,12 @@
       <c r="AF168">
         <v>0.26</v>
       </c>
+      <c r="AG168">
+        <v>69.5</v>
+      </c>
+      <c r="AH168">
+        <v>192</v>
+      </c>
     </row>
     <row r="169" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A169" s="19" t="s">
@@ -16761,6 +17351,12 @@
       </c>
       <c r="AF169">
         <v>0.17</v>
+      </c>
+      <c r="AG169">
+        <v>69.3</v>
+      </c>
+      <c r="AH169">
+        <v>192</v>
       </c>
     </row>
     <row r="170" spans="1:34" x14ac:dyDescent="0.2">
@@ -16826,6 +17422,12 @@
       <c r="AF170">
         <v>0.37</v>
       </c>
+      <c r="AG170">
+        <v>82.4</v>
+      </c>
+      <c r="AH170">
+        <v>192</v>
+      </c>
     </row>
     <row r="171" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A171" s="19" t="s">
@@ -16891,6 +17493,12 @@
       </c>
       <c r="AF171">
         <v>0.21</v>
+      </c>
+      <c r="AG171">
+        <v>64.900000000000006</v>
+      </c>
+      <c r="AH171">
+        <v>192</v>
       </c>
     </row>
     <row r="172" spans="1:34" x14ac:dyDescent="0.2">
@@ -16956,6 +17564,12 @@
       <c r="AF172">
         <v>0.18</v>
       </c>
+      <c r="AG172">
+        <v>58.9</v>
+      </c>
+      <c r="AH172">
+        <v>192</v>
+      </c>
     </row>
     <row r="173" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A173" s="19" t="s">
@@ -17021,6 +17635,12 @@
       </c>
       <c r="AF173">
         <v>0.3</v>
+      </c>
+      <c r="AG173">
+        <v>85.2</v>
+      </c>
+      <c r="AH173">
+        <v>192</v>
       </c>
     </row>
     <row r="174" spans="1:34" x14ac:dyDescent="0.2">
@@ -17086,6 +17706,12 @@
       <c r="AF174">
         <v>0.21</v>
       </c>
+      <c r="AG174">
+        <v>78.5</v>
+      </c>
+      <c r="AH174">
+        <v>192</v>
+      </c>
     </row>
     <row r="175" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A175" s="19" t="s">
@@ -17151,6 +17777,12 @@
       </c>
       <c r="AF175">
         <v>0.3</v>
+      </c>
+      <c r="AG175">
+        <v>75.2</v>
+      </c>
+      <c r="AH175">
+        <v>192</v>
       </c>
     </row>
     <row r="176" spans="1:34" x14ac:dyDescent="0.2">
@@ -17216,8 +17848,14 @@
       <c r="AF176">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="177" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG176">
+        <v>105.7</v>
+      </c>
+      <c r="AH176">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="177" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A177" s="19" t="s">
         <v>178</v>
       </c>
@@ -17282,8 +17920,14 @@
       <c r="AF177">
         <v>0.24</v>
       </c>
-    </row>
-    <row r="178" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG177">
+        <v>84.7</v>
+      </c>
+      <c r="AH177">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="178" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A178" s="22" t="s">
         <v>179</v>
       </c>
@@ -17348,8 +17992,14 @@
       <c r="AF178">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="179" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG178">
+        <v>75.599999999999994</v>
+      </c>
+      <c r="AH178">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="179" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A179" s="22" t="s">
         <v>180</v>
       </c>
@@ -17416,8 +18066,14 @@
       <c r="AF179">
         <v>0.33</v>
       </c>
-    </row>
-    <row r="180" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG179">
+        <v>76.5</v>
+      </c>
+      <c r="AH179">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="180" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A180" s="22" t="s">
         <v>181</v>
       </c>
@@ -17480,8 +18136,14 @@
       <c r="AF180">
         <v>0.19</v>
       </c>
-    </row>
-    <row r="181" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG180">
+        <v>66.900000000000006</v>
+      </c>
+      <c r="AH180">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="181" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A181" s="22" t="s">
         <v>182</v>
       </c>
@@ -17546,8 +18208,14 @@
       <c r="AF181">
         <v>0.16</v>
       </c>
-    </row>
-    <row r="182" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG181">
+        <v>74.5</v>
+      </c>
+      <c r="AH181">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="182" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A182" s="22" t="s">
         <v>183</v>
       </c>
@@ -17610,8 +18278,14 @@
       <c r="AF182">
         <v>0.21</v>
       </c>
-    </row>
-    <row r="183" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG182">
+        <v>58.4</v>
+      </c>
+      <c r="AH182">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="183" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A183" s="22" t="s">
         <v>184</v>
       </c>
@@ -17676,8 +18350,14 @@
       <c r="AF183">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="184" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG183">
+        <v>80.599999999999994</v>
+      </c>
+      <c r="AH183">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="184" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A184" s="22" t="s">
         <v>185</v>
       </c>
@@ -17740,8 +18420,14 @@
       <c r="AF184">
         <v>0.38</v>
       </c>
-    </row>
-    <row r="185" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG184">
+        <v>73.5</v>
+      </c>
+      <c r="AH184">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="185" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A185" s="22" t="s">
         <v>186</v>
       </c>
@@ -17806,8 +18492,14 @@
       <c r="AF185">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="186" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG185">
+        <v>81.3</v>
+      </c>
+      <c r="AH185">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="186" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A186" s="22" t="s">
         <v>187</v>
       </c>
@@ -17870,8 +18562,14 @@
       <c r="AF186">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="187" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG186">
+        <v>77.099999999999994</v>
+      </c>
+      <c r="AH186">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="187" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A187" s="22" t="s">
         <v>188</v>
       </c>
@@ -17936,8 +18634,14 @@
       <c r="AF187">
         <v>0.12</v>
       </c>
-    </row>
-    <row r="188" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG187">
+        <v>75.400000000000006</v>
+      </c>
+      <c r="AH187">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="188" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A188" s="22" t="s">
         <v>189</v>
       </c>
@@ -18000,8 +18704,14 @@
       <c r="AF188">
         <v>0.34</v>
       </c>
-    </row>
-    <row r="189" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG188">
+        <v>78</v>
+      </c>
+      <c r="AH188">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="189" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A189" s="22" t="s">
         <v>190</v>
       </c>
@@ -18066,8 +18776,14 @@
       <c r="AF189">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="190" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG189">
+        <v>79.8</v>
+      </c>
+      <c r="AH189">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="190" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A190" s="22" t="s">
         <v>191</v>
       </c>
@@ -18130,8 +18846,14 @@
       <c r="AF190">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="191" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG190">
+        <v>103.3</v>
+      </c>
+      <c r="AH190">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="191" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A191" s="22" t="s">
         <v>192</v>
       </c>
@@ -18196,8 +18918,14 @@
       <c r="AF191">
         <v>0.19</v>
       </c>
-    </row>
-    <row r="192" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG191">
+        <v>74.3</v>
+      </c>
+      <c r="AH191">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="192" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A192" s="22" t="s">
         <v>193</v>
       </c>
@@ -18260,6 +18988,12 @@
       <c r="AF192">
         <v>0.16</v>
       </c>
+      <c r="AG192">
+        <v>79.7</v>
+      </c>
+      <c r="AH192">
+        <v>192</v>
+      </c>
     </row>
     <row r="193" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A193" s="22" t="s">
@@ -18325,6 +19059,12 @@
       </c>
       <c r="AF193">
         <v>0.17</v>
+      </c>
+      <c r="AG193">
+        <v>76.900000000000006</v>
+      </c>
+      <c r="AH193">
+        <v>192</v>
       </c>
     </row>
     <row r="194" spans="1:34" x14ac:dyDescent="0.2">
@@ -19622,6 +20362,12 @@
       <c r="AF210">
         <v>0.22</v>
       </c>
+      <c r="AG210">
+        <v>52.5</v>
+      </c>
+      <c r="AH210">
+        <v>192</v>
+      </c>
     </row>
     <row r="211" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A211" s="19" t="s">
@@ -19687,6 +20433,12 @@
       </c>
       <c r="AF211">
         <v>0.49</v>
+      </c>
+      <c r="AG211">
+        <v>48.2</v>
+      </c>
+      <c r="AH211">
+        <v>192</v>
       </c>
     </row>
     <row r="212" spans="1:34" x14ac:dyDescent="0.2">
@@ -19752,6 +20504,12 @@
       <c r="AF212">
         <v>0.33</v>
       </c>
+      <c r="AG212">
+        <v>63.8</v>
+      </c>
+      <c r="AH212">
+        <v>192</v>
+      </c>
     </row>
     <row r="213" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A213" s="19" t="s">
@@ -19819,6 +20577,12 @@
       </c>
       <c r="AF213">
         <v>0.33</v>
+      </c>
+      <c r="AG213">
+        <v>54.2</v>
+      </c>
+      <c r="AH213">
+        <v>192</v>
       </c>
     </row>
     <row r="214" spans="1:34" x14ac:dyDescent="0.2">
@@ -19884,6 +20648,12 @@
       <c r="AF214">
         <v>0.34</v>
       </c>
+      <c r="AG214">
+        <v>40.5</v>
+      </c>
+      <c r="AH214">
+        <v>192</v>
+      </c>
     </row>
     <row r="215" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A215" s="19" t="s">
@@ -19949,6 +20719,12 @@
       </c>
       <c r="AF215">
         <v>0.25</v>
+      </c>
+      <c r="AG215">
+        <v>65.099999999999994</v>
+      </c>
+      <c r="AH215">
+        <v>192</v>
       </c>
     </row>
     <row r="216" spans="1:34" x14ac:dyDescent="0.2">
@@ -20014,6 +20790,12 @@
       <c r="AF216">
         <v>0.56000000000000005</v>
       </c>
+      <c r="AG216">
+        <v>61.6</v>
+      </c>
+      <c r="AH216">
+        <v>192</v>
+      </c>
     </row>
     <row r="217" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A217" s="19" t="s">
@@ -20079,6 +20861,12 @@
       </c>
       <c r="AF217">
         <v>0.28999999999999998</v>
+      </c>
+      <c r="AG217">
+        <v>90.1</v>
+      </c>
+      <c r="AH217">
+        <v>192</v>
       </c>
     </row>
     <row r="218" spans="1:34" x14ac:dyDescent="0.2">
@@ -20144,6 +20932,12 @@
       <c r="AF218">
         <v>0.21</v>
       </c>
+      <c r="AG218">
+        <v>57.5</v>
+      </c>
+      <c r="AH218">
+        <v>192</v>
+      </c>
     </row>
     <row r="219" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A219" s="19" t="s">
@@ -20209,6 +21003,12 @@
       </c>
       <c r="AF219">
         <v>0.25</v>
+      </c>
+      <c r="AG219">
+        <v>52.1</v>
+      </c>
+      <c r="AH219">
+        <v>192</v>
       </c>
     </row>
     <row r="220" spans="1:34" x14ac:dyDescent="0.2">
@@ -20274,6 +21074,12 @@
       <c r="AF220">
         <v>0.21</v>
       </c>
+      <c r="AG220">
+        <v>57.6</v>
+      </c>
+      <c r="AH220">
+        <v>192</v>
+      </c>
     </row>
     <row r="221" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A221" s="19" t="s">
@@ -20339,6 +21145,12 @@
       </c>
       <c r="AF221">
         <v>0.38</v>
+      </c>
+      <c r="AG221">
+        <v>47.2</v>
+      </c>
+      <c r="AH221">
+        <v>192</v>
       </c>
     </row>
     <row r="222" spans="1:34" x14ac:dyDescent="0.2">
@@ -20404,6 +21216,12 @@
       <c r="AF222">
         <v>0.33</v>
       </c>
+      <c r="AG222">
+        <v>64.3</v>
+      </c>
+      <c r="AH222">
+        <v>192</v>
+      </c>
     </row>
     <row r="223" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A223" s="19" t="s">
@@ -20469,6 +21287,12 @@
       </c>
       <c r="AF223">
         <v>0.18</v>
+      </c>
+      <c r="AG223">
+        <v>50</v>
+      </c>
+      <c r="AH223">
+        <v>192</v>
       </c>
     </row>
     <row r="224" spans="1:34" x14ac:dyDescent="0.2">
@@ -20534,8 +21358,14 @@
       <c r="AF224">
         <v>0.23</v>
       </c>
-    </row>
-    <row r="225" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG224">
+        <v>54.9</v>
+      </c>
+      <c r="AH224">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="225" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A225" s="19" t="s">
         <v>226</v>
       </c>
@@ -20600,8 +21430,14 @@
       <c r="AF225">
         <v>0.44</v>
       </c>
-    </row>
-    <row r="226" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG225">
+        <v>57.8</v>
+      </c>
+      <c r="AH225">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="226" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A226" s="22" t="s">
         <v>227</v>
       </c>
@@ -20666,8 +21502,14 @@
       <c r="AF226">
         <v>0.15</v>
       </c>
-    </row>
-    <row r="227" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG226">
+        <v>63.4</v>
+      </c>
+      <c r="AH226">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="227" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A227" s="22" t="s">
         <v>228</v>
       </c>
@@ -20734,8 +21576,14 @@
       <c r="AF227">
         <v>0.32</v>
       </c>
-    </row>
-    <row r="228" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG227">
+        <v>53.7</v>
+      </c>
+      <c r="AH227">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="228" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A228" s="22" t="s">
         <v>229</v>
       </c>
@@ -20798,8 +21646,14 @@
       <c r="AF228">
         <v>0.42</v>
       </c>
-    </row>
-    <row r="229" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG228">
+        <v>56.3</v>
+      </c>
+      <c r="AH228">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="229" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A229" s="22" t="s">
         <v>230</v>
       </c>
@@ -20864,8 +21718,14 @@
       <c r="AF229">
         <v>0.35</v>
       </c>
-    </row>
-    <row r="230" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG229">
+        <v>35</v>
+      </c>
+      <c r="AH229">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="230" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A230" s="22" t="s">
         <v>231</v>
       </c>
@@ -20928,8 +21788,14 @@
       <c r="AF230">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="231" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG230">
+        <v>89</v>
+      </c>
+      <c r="AH230">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="231" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A231" s="22" t="s">
         <v>232</v>
       </c>
@@ -20994,8 +21860,14 @@
       <c r="AF231">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="232" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG231">
+        <v>56.1</v>
+      </c>
+      <c r="AH231">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="232" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A232" s="22" t="s">
         <v>233</v>
       </c>
@@ -21058,8 +21930,14 @@
       <c r="AF232">
         <v>0.31</v>
       </c>
-    </row>
-    <row r="233" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG232">
+        <v>39.1</v>
+      </c>
+      <c r="AH232">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="233" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A233" s="22" t="s">
         <v>234</v>
       </c>
@@ -21124,8 +22002,14 @@
       <c r="AF233">
         <v>0.52</v>
       </c>
-    </row>
-    <row r="234" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG233">
+        <v>45.3</v>
+      </c>
+      <c r="AH233">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="234" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A234" s="22" t="s">
         <v>235</v>
       </c>
@@ -21188,8 +22072,14 @@
       <c r="AF234">
         <v>0.37</v>
       </c>
-    </row>
-    <row r="235" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG234">
+        <v>59.7</v>
+      </c>
+      <c r="AH234">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="235" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A235" s="22" t="s">
         <v>236</v>
       </c>
@@ -21254,8 +22144,14 @@
       <c r="AF235">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="236" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG235">
+        <v>57.4</v>
+      </c>
+      <c r="AH235">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="236" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A236" s="22" t="s">
         <v>237</v>
       </c>
@@ -21318,8 +22214,14 @@
       <c r="AF236">
         <v>0.31</v>
       </c>
-    </row>
-    <row r="237" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG236">
+        <v>59.1</v>
+      </c>
+      <c r="AH236">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="237" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A237" s="22" t="s">
         <v>238</v>
       </c>
@@ -21386,8 +22288,14 @@
       <c r="AF237">
         <v>0.42</v>
       </c>
-    </row>
-    <row r="238" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG237">
+        <v>58.8</v>
+      </c>
+      <c r="AH237">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="238" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A238" s="22" t="s">
         <v>239</v>
       </c>
@@ -21450,8 +22358,14 @@
       <c r="AF238">
         <v>0.17</v>
       </c>
-    </row>
-    <row r="239" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG238">
+        <v>64.5</v>
+      </c>
+      <c r="AH238">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="239" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A239" s="22" t="s">
         <v>240</v>
       </c>
@@ -21516,8 +22430,14 @@
       <c r="AF239">
         <v>0.49</v>
       </c>
-    </row>
-    <row r="240" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG239">
+        <v>60.5</v>
+      </c>
+      <c r="AH239">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="240" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A240" s="22" t="s">
         <v>241</v>
       </c>
@@ -21580,8 +22500,14 @@
       <c r="AF240">
         <v>0.32</v>
       </c>
-    </row>
-    <row r="241" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG240">
+        <v>56.8</v>
+      </c>
+      <c r="AH240">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="241" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A241" s="22" t="s">
         <v>242</v>
       </c>
@@ -21648,8 +22574,14 @@
       <c r="AF241">
         <v>0.14000000000000001</v>
       </c>
-    </row>
-    <row r="242" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG241">
+        <v>63.9</v>
+      </c>
+      <c r="AH241">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="242" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A242" s="14" t="s">
         <v>243</v>
       </c>
@@ -21679,7 +22611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A243" s="14" t="s">
         <v>244</v>
       </c>
@@ -21730,7 +22662,7 @@
         <v>-0.70000000000000284</v>
       </c>
     </row>
-    <row r="244" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A244" s="14" t="s">
         <v>245</v>
       </c>
@@ -21779,7 +22711,7 @@
         <v>-0.40000000000000568</v>
       </c>
     </row>
-    <row r="245" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A245" s="14" t="s">
         <v>246</v>
       </c>
@@ -21830,7 +22762,7 @@
         <v>-0.59999999999999787</v>
       </c>
     </row>
-    <row r="246" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A246" s="14" t="s">
         <v>247</v>
       </c>
@@ -21858,7 +22790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="247" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A247" s="14" t="s">
         <v>248</v>
       </c>
@@ -21886,7 +22818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="248" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A248" s="14" t="s">
         <v>249</v>
       </c>
@@ -21920,7 +22852,7 @@
         <v>-28.3</v>
       </c>
     </row>
-    <row r="249" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A249" s="14" t="s">
         <v>250</v>
       </c>
@@ -21948,7 +22880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="250" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A250" s="14" t="s">
         <v>251</v>
       </c>
@@ -21976,7 +22908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="251" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A251" s="14" t="s">
         <v>252</v>
       </c>
@@ -22012,7 +22944,7 @@
         <v>-34.1</v>
       </c>
     </row>
-    <row r="252" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A252" s="14" t="s">
         <v>253</v>
       </c>
@@ -22046,7 +22978,7 @@
         <v>-27.7</v>
       </c>
     </row>
-    <row r="253" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A253" s="14" t="s">
         <v>254</v>
       </c>
@@ -22074,7 +23006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="254" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A254" s="14" t="s">
         <v>255</v>
       </c>
@@ -22108,7 +23040,7 @@
         <v>-30.3</v>
       </c>
     </row>
-    <row r="255" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A255" s="14" t="s">
         <v>256</v>
       </c>
@@ -22136,7 +23068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="256" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A256" s="14" t="s">
         <v>257</v>
       </c>
@@ -27225,6 +28157,12 @@
       <c r="AF370">
         <v>0.5</v>
       </c>
+      <c r="AG370">
+        <v>88.7</v>
+      </c>
+      <c r="AH370">
+        <v>192</v>
+      </c>
     </row>
     <row r="371" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A371" s="22" t="s">
@@ -27290,6 +28228,12 @@
       </c>
       <c r="AF371">
         <v>0.53</v>
+      </c>
+      <c r="AG371">
+        <v>81.3</v>
+      </c>
+      <c r="AH371">
+        <v>192</v>
       </c>
     </row>
     <row r="372" spans="1:34" x14ac:dyDescent="0.2">
@@ -27355,6 +28299,12 @@
       <c r="AF372">
         <v>0.68</v>
       </c>
+      <c r="AG372">
+        <v>101.3</v>
+      </c>
+      <c r="AH372">
+        <v>192</v>
+      </c>
     </row>
     <row r="373" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A373" s="22" t="s">
@@ -27420,6 +28370,12 @@
       </c>
       <c r="AF373">
         <v>0.35</v>
+      </c>
+      <c r="AG373">
+        <v>105.7</v>
+      </c>
+      <c r="AH373">
+        <v>192</v>
       </c>
     </row>
     <row r="374" spans="1:34" x14ac:dyDescent="0.2">
@@ -27485,6 +28441,12 @@
       <c r="AF374">
         <v>0.44</v>
       </c>
+      <c r="AG374">
+        <v>115.1</v>
+      </c>
+      <c r="AH374">
+        <v>192</v>
+      </c>
     </row>
     <row r="375" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A375" s="22" t="s">
@@ -27550,6 +28512,12 @@
       </c>
       <c r="AF375">
         <v>0.35</v>
+      </c>
+      <c r="AG375">
+        <v>110.6</v>
+      </c>
+      <c r="AH375">
+        <v>192</v>
       </c>
     </row>
     <row r="376" spans="1:34" x14ac:dyDescent="0.2">
@@ -27615,6 +28583,12 @@
       <c r="AF376">
         <v>0.43</v>
       </c>
+      <c r="AG376">
+        <v>176.5</v>
+      </c>
+      <c r="AH376">
+        <v>192</v>
+      </c>
     </row>
     <row r="377" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A377" s="22" t="s">
@@ -27680,6 +28654,12 @@
       </c>
       <c r="AF377">
         <v>0.44</v>
+      </c>
+      <c r="AG377">
+        <v>156.1</v>
+      </c>
+      <c r="AH377">
+        <v>192</v>
       </c>
     </row>
     <row r="378" spans="1:34" x14ac:dyDescent="0.2">
@@ -27745,6 +28725,12 @@
       <c r="AF378">
         <v>0.59</v>
       </c>
+      <c r="AG378">
+        <v>127.8</v>
+      </c>
+      <c r="AH378">
+        <v>192</v>
+      </c>
     </row>
     <row r="379" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A379" s="22" t="s">
@@ -27810,6 +28796,12 @@
       </c>
       <c r="AF379">
         <v>0.51</v>
+      </c>
+      <c r="AG379">
+        <v>73.900000000000006</v>
+      </c>
+      <c r="AH379">
+        <v>192</v>
       </c>
     </row>
     <row r="380" spans="1:34" x14ac:dyDescent="0.2">
@@ -27875,6 +28867,12 @@
       <c r="AF380">
         <v>0.43</v>
       </c>
+      <c r="AG380">
+        <v>80.5</v>
+      </c>
+      <c r="AH380">
+        <v>192</v>
+      </c>
     </row>
     <row r="381" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A381" s="22" t="s">
@@ -27940,6 +28938,12 @@
       </c>
       <c r="AF381">
         <v>0.49</v>
+      </c>
+      <c r="AG381">
+        <v>116.9</v>
+      </c>
+      <c r="AH381">
+        <v>192</v>
       </c>
     </row>
     <row r="382" spans="1:34" x14ac:dyDescent="0.2">
@@ -28005,6 +29009,12 @@
       <c r="AF382">
         <v>0.87</v>
       </c>
+      <c r="AG382">
+        <v>129.5</v>
+      </c>
+      <c r="AH382">
+        <v>192</v>
+      </c>
     </row>
     <row r="383" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A383" s="22" t="s">
@@ -28072,6 +29082,12 @@
       </c>
       <c r="AF383">
         <v>0.38</v>
+      </c>
+      <c r="AG383">
+        <v>128.4</v>
+      </c>
+      <c r="AH383">
+        <v>192</v>
       </c>
     </row>
     <row r="384" spans="1:34" x14ac:dyDescent="0.2">
@@ -28137,6 +29153,12 @@
       <c r="AF384">
         <v>0.91</v>
       </c>
+      <c r="AG384">
+        <v>141.30000000000001</v>
+      </c>
+      <c r="AH384">
+        <v>192</v>
+      </c>
     </row>
     <row r="385" spans="1:34" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A385" s="25" t="s">
@@ -29334,6 +30356,12 @@
       <c r="AF402">
         <v>0.38</v>
       </c>
+      <c r="AG402">
+        <v>64.3</v>
+      </c>
+      <c r="AH402">
+        <v>192</v>
+      </c>
     </row>
     <row r="403" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A403" s="19" t="s">
@@ -29401,6 +30429,12 @@
       </c>
       <c r="AF403">
         <v>0.22</v>
+      </c>
+      <c r="AG403">
+        <v>55.5</v>
+      </c>
+      <c r="AH403">
+        <v>192</v>
       </c>
     </row>
     <row r="404" spans="1:34" x14ac:dyDescent="0.2">
@@ -29468,6 +30502,12 @@
       <c r="AF404">
         <v>0.43</v>
       </c>
+      <c r="AG404">
+        <v>54.8</v>
+      </c>
+      <c r="AH404">
+        <v>192</v>
+      </c>
     </row>
     <row r="405" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A405" s="19" t="s">
@@ -29535,6 +30575,12 @@
       </c>
       <c r="AF405">
         <v>0.27</v>
+      </c>
+      <c r="AG405">
+        <v>44.6</v>
+      </c>
+      <c r="AH405">
+        <v>192</v>
       </c>
     </row>
     <row r="406" spans="1:34" x14ac:dyDescent="0.2">
@@ -29600,6 +30646,12 @@
       <c r="AF406">
         <v>0.27</v>
       </c>
+      <c r="AG406">
+        <v>61.3</v>
+      </c>
+      <c r="AH406">
+        <v>192</v>
+      </c>
     </row>
     <row r="407" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A407" s="19" t="s">
@@ -29665,6 +30717,12 @@
       </c>
       <c r="AF407">
         <v>0.32</v>
+      </c>
+      <c r="AG407">
+        <v>50.1</v>
+      </c>
+      <c r="AH407">
+        <v>192</v>
       </c>
     </row>
     <row r="408" spans="1:34" x14ac:dyDescent="0.2">
@@ -29730,6 +30788,12 @@
       <c r="AF408">
         <v>0.34</v>
       </c>
+      <c r="AG408">
+        <v>66.3</v>
+      </c>
+      <c r="AH408">
+        <v>192</v>
+      </c>
     </row>
     <row r="409" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A409" s="19" t="s">
@@ -29795,6 +30859,12 @@
       </c>
       <c r="AF409">
         <v>0.25</v>
+      </c>
+      <c r="AG409">
+        <v>50.8</v>
+      </c>
+      <c r="AH409">
+        <v>192</v>
       </c>
     </row>
     <row r="410" spans="1:34" x14ac:dyDescent="0.2">
@@ -29860,6 +30930,12 @@
       <c r="AF410">
         <v>0.17</v>
       </c>
+      <c r="AG410">
+        <v>47.8</v>
+      </c>
+      <c r="AH410">
+        <v>192</v>
+      </c>
     </row>
     <row r="411" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A411" s="19" t="s">
@@ -29925,6 +31001,12 @@
       </c>
       <c r="AF411">
         <v>0.22</v>
+      </c>
+      <c r="AG411">
+        <v>52.2</v>
+      </c>
+      <c r="AH411">
+        <v>192</v>
       </c>
     </row>
     <row r="412" spans="1:34" x14ac:dyDescent="0.2">
@@ -29990,6 +31072,12 @@
       <c r="AF412">
         <v>0.4</v>
       </c>
+      <c r="AG412">
+        <v>57.6</v>
+      </c>
+      <c r="AH412">
+        <v>192</v>
+      </c>
     </row>
     <row r="413" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A413" s="19" t="s">
@@ -30055,6 +31143,12 @@
       </c>
       <c r="AF413">
         <v>0.28999999999999998</v>
+      </c>
+      <c r="AG413">
+        <v>49.3</v>
+      </c>
+      <c r="AH413">
+        <v>192</v>
       </c>
     </row>
     <row r="414" spans="1:34" x14ac:dyDescent="0.2">
@@ -30120,6 +31214,12 @@
       <c r="AF414">
         <v>0.42</v>
       </c>
+      <c r="AG414">
+        <v>59.9</v>
+      </c>
+      <c r="AH414">
+        <v>192</v>
+      </c>
     </row>
     <row r="415" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A415" s="19" t="s">
@@ -30185,6 +31285,12 @@
       </c>
       <c r="AF415">
         <v>0.4</v>
+      </c>
+      <c r="AG415">
+        <v>59.5</v>
+      </c>
+      <c r="AH415">
+        <v>192</v>
       </c>
     </row>
     <row r="416" spans="1:34" x14ac:dyDescent="0.2">
@@ -30250,6 +31356,12 @@
       <c r="AF416">
         <v>0.42</v>
       </c>
+      <c r="AG416">
+        <v>58.3</v>
+      </c>
+      <c r="AH416">
+        <v>192</v>
+      </c>
     </row>
     <row r="417" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A417" s="19" t="s">
@@ -30315,6 +31427,12 @@
       </c>
       <c r="AF417">
         <v>0.26</v>
+      </c>
+      <c r="AG417">
+        <v>53.3</v>
+      </c>
+      <c r="AH417">
+        <v>192</v>
       </c>
     </row>
     <row r="418" spans="1:34" x14ac:dyDescent="0.2">
@@ -31829,7 +32947,9 @@
       <c r="C439" s="15">
         <v>43528</v>
       </c>
-      <c r="D439" s="16"/>
+      <c r="D439" s="16">
+        <v>30.6</v>
+      </c>
       <c r="E439" s="15">
         <v>43458</v>
       </c>
@@ -31865,7 +32985,7 @@
       </c>
       <c r="X439">
         <f t="shared" si="19"/>
-        <v>30.6</v>
+        <v>0</v>
       </c>
       <c r="AA439">
         <v>5.3E-3</v>
@@ -32619,6 +33739,12 @@
       <c r="AF450">
         <v>0.48</v>
       </c>
+      <c r="AG450">
+        <v>36.9</v>
+      </c>
+      <c r="AH450">
+        <v>192</v>
+      </c>
     </row>
     <row r="451" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A451" s="19" t="s">
@@ -32686,6 +33812,12 @@
       </c>
       <c r="AF451">
         <v>0.53</v>
+      </c>
+      <c r="AG451">
+        <v>31.2</v>
+      </c>
+      <c r="AH451">
+        <v>192</v>
       </c>
     </row>
     <row r="452" spans="1:34" x14ac:dyDescent="0.2">
@@ -32753,6 +33885,12 @@
       <c r="AF452">
         <v>0.67</v>
       </c>
+      <c r="AG452">
+        <v>32.299999999999997</v>
+      </c>
+      <c r="AH452">
+        <v>192</v>
+      </c>
     </row>
     <row r="453" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A453" s="19" t="s">
@@ -32818,6 +33956,12 @@
       </c>
       <c r="AF453">
         <v>0.52</v>
+      </c>
+      <c r="AG453">
+        <v>31.3</v>
+      </c>
+      <c r="AH453">
+        <v>192</v>
       </c>
     </row>
     <row r="454" spans="1:34" x14ac:dyDescent="0.2">
@@ -32883,6 +34027,12 @@
       <c r="AF454">
         <v>0.74</v>
       </c>
+      <c r="AG454">
+        <v>34.1</v>
+      </c>
+      <c r="AH454">
+        <v>192</v>
+      </c>
     </row>
     <row r="455" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A455" s="19" t="s">
@@ -32948,6 +34098,12 @@
       </c>
       <c r="AF455">
         <v>0.65</v>
+      </c>
+      <c r="AG455">
+        <v>28.1</v>
+      </c>
+      <c r="AH455">
+        <v>192</v>
       </c>
     </row>
     <row r="456" spans="1:34" x14ac:dyDescent="0.2">
@@ -33013,6 +34169,12 @@
       <c r="AF456">
         <v>0.71</v>
       </c>
+      <c r="AG456">
+        <v>21.2</v>
+      </c>
+      <c r="AH456">
+        <v>192</v>
+      </c>
     </row>
     <row r="457" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A457" s="19" t="s">
@@ -33078,6 +34240,12 @@
       </c>
       <c r="AF457">
         <v>0.56999999999999995</v>
+      </c>
+      <c r="AG457">
+        <v>25.5</v>
+      </c>
+      <c r="AH457">
+        <v>192</v>
       </c>
     </row>
     <row r="458" spans="1:34" x14ac:dyDescent="0.2">
@@ -33143,6 +34311,12 @@
       <c r="AF458">
         <v>0.49</v>
       </c>
+      <c r="AG458">
+        <v>25.4</v>
+      </c>
+      <c r="AH458">
+        <v>192</v>
+      </c>
     </row>
     <row r="459" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A459" s="19" t="s">
@@ -33208,6 +34382,12 @@
       </c>
       <c r="AF459">
         <v>0.6</v>
+      </c>
+      <c r="AG459">
+        <v>21.5</v>
+      </c>
+      <c r="AH459">
+        <v>192</v>
       </c>
     </row>
     <row r="460" spans="1:34" x14ac:dyDescent="0.2">
@@ -33273,6 +34453,12 @@
       <c r="AF460">
         <v>0.28000000000000003</v>
       </c>
+      <c r="AG460">
+        <v>35.299999999999997</v>
+      </c>
+      <c r="AH460">
+        <v>192</v>
+      </c>
     </row>
     <row r="461" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A461" s="19" t="s">
@@ -33338,6 +34524,12 @@
       </c>
       <c r="AF461">
         <v>0.48</v>
+      </c>
+      <c r="AG461">
+        <v>29.8</v>
+      </c>
+      <c r="AH461">
+        <v>192</v>
       </c>
     </row>
     <row r="462" spans="1:34" x14ac:dyDescent="0.2">
@@ -33403,6 +34595,12 @@
       <c r="AF462">
         <v>0.63</v>
       </c>
+      <c r="AG462">
+        <v>27.7</v>
+      </c>
+      <c r="AH462">
+        <v>192</v>
+      </c>
     </row>
     <row r="463" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A463" s="19" t="s">
@@ -33468,6 +34666,12 @@
       </c>
       <c r="AF463">
         <v>0.67</v>
+      </c>
+      <c r="AG463">
+        <v>33.700000000000003</v>
+      </c>
+      <c r="AH463">
+        <v>192</v>
       </c>
     </row>
     <row r="464" spans="1:34" x14ac:dyDescent="0.2">
@@ -33533,8 +34737,14 @@
       <c r="AF464">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="465" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG464">
+        <v>25.4</v>
+      </c>
+      <c r="AH464">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="465" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A465" s="19" t="s">
         <v>466</v>
       </c>
@@ -33599,8 +34809,14 @@
       <c r="AF465">
         <v>0.78</v>
       </c>
-    </row>
-    <row r="466" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG465">
+        <v>43.7</v>
+      </c>
+      <c r="AH465">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="466" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A466" s="22" t="s">
         <v>467</v>
       </c>
@@ -33665,8 +34881,14 @@
       <c r="AF466">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="467" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG466">
+        <v>56.6</v>
+      </c>
+      <c r="AH466">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="467" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A467" s="22" t="s">
         <v>468</v>
       </c>
@@ -33733,8 +34955,14 @@
       <c r="AF467">
         <v>0.67</v>
       </c>
-    </row>
-    <row r="468" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG467">
+        <v>44.4</v>
+      </c>
+      <c r="AH467">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="468" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A468" s="22" t="s">
         <v>469</v>
       </c>
@@ -33799,8 +35027,14 @@
       <c r="AF468">
         <v>0.59</v>
       </c>
-    </row>
-    <row r="469" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG468">
+        <v>35.9</v>
+      </c>
+      <c r="AH468">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="469" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A469" s="22" t="s">
         <v>470</v>
       </c>
@@ -33865,8 +35099,14 @@
       <c r="AF469">
         <v>0.59</v>
       </c>
-    </row>
-    <row r="470" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG469">
+        <v>31.5</v>
+      </c>
+      <c r="AH469">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="470" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A470" s="22" t="s">
         <v>471</v>
       </c>
@@ -33929,8 +35169,14 @@
       <c r="AF470">
         <v>0.37</v>
       </c>
-    </row>
-    <row r="471" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG470">
+        <v>36.1</v>
+      </c>
+      <c r="AH470">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="471" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A471" s="22" t="s">
         <v>472</v>
       </c>
@@ -33995,8 +35241,14 @@
       <c r="AF471">
         <v>0.44</v>
       </c>
-    </row>
-    <row r="472" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG471">
+        <v>31.6</v>
+      </c>
+      <c r="AH471">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="472" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A472" s="22" t="s">
         <v>473</v>
       </c>
@@ -34059,8 +35311,14 @@
       <c r="AF472">
         <v>0.82</v>
       </c>
-    </row>
-    <row r="473" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG472">
+        <v>40</v>
+      </c>
+      <c r="AH472">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="473" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A473" s="22" t="s">
         <v>474</v>
       </c>
@@ -34125,8 +35383,14 @@
       <c r="AF473">
         <v>0.67</v>
       </c>
-    </row>
-    <row r="474" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG473">
+        <v>26.5</v>
+      </c>
+      <c r="AH473">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="474" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A474" s="22" t="s">
         <v>475</v>
       </c>
@@ -34189,8 +35453,14 @@
       <c r="AF474">
         <v>0.78</v>
       </c>
-    </row>
-    <row r="475" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG474">
+        <v>27.6</v>
+      </c>
+      <c r="AH474">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="475" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A475" s="22" t="s">
         <v>476</v>
       </c>
@@ -34255,8 +35525,14 @@
       <c r="AF475">
         <v>0.51</v>
       </c>
-    </row>
-    <row r="476" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG475">
+        <v>24.3</v>
+      </c>
+      <c r="AH475">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="476" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A476" s="22" t="s">
         <v>477</v>
       </c>
@@ -34319,8 +35595,14 @@
       <c r="AF476">
         <v>0.66</v>
       </c>
-    </row>
-    <row r="477" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG476">
+        <v>36</v>
+      </c>
+      <c r="AH476">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="477" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A477" s="22" t="s">
         <v>478</v>
       </c>
@@ -34385,8 +35667,14 @@
       <c r="AF477">
         <v>0.54</v>
       </c>
-    </row>
-    <row r="478" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG477">
+        <v>24.1</v>
+      </c>
+      <c r="AH477">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="478" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A478" s="22" t="s">
         <v>479</v>
       </c>
@@ -34449,8 +35737,14 @@
       <c r="AF478">
         <v>0.74</v>
       </c>
-    </row>
-    <row r="479" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG478">
+        <v>35.799999999999997</v>
+      </c>
+      <c r="AH478">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="479" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A479" s="22" t="s">
         <v>480</v>
       </c>
@@ -34515,8 +35809,14 @@
       <c r="AF479">
         <v>0.53</v>
       </c>
-    </row>
-    <row r="480" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG479">
+        <v>31.1</v>
+      </c>
+      <c r="AH479">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="480" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A480" s="22" t="s">
         <v>481</v>
       </c>
@@ -34579,8 +35879,14 @@
       <c r="AF480">
         <v>0.67</v>
       </c>
-    </row>
-    <row r="481" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AG480">
+        <v>44.1</v>
+      </c>
+      <c r="AH480">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="481" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A481" s="22" t="s">
         <v>482</v>
       </c>
@@ -34647,6 +35953,12 @@
       <c r="AF481">
         <v>0.59</v>
       </c>
+      <c r="AG481">
+        <v>35.1</v>
+      </c>
+      <c r="AH481">
+        <v>192</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -34655,7 +35967,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -36452,7 +37764,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J61"/>
+  <autoFilter ref="A1:J61" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>

</xml_diff>

<commit_message>
updated phenol and budset data
</commit_message>
<xml_diff>
--- a/data/observation_datasheet.xlsx
+++ b/data/observation_datasheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/catchamberlain/Documents/git/chillfreeze/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D8C68D9-A0D1-3945-9CE2-FB4CB41D605B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95B915EB-A847-D847-969E-C4871EADDAB9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7040" yWindow="3220" windowWidth="31580" windowHeight="19540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7040" yWindow="3220" windowWidth="31580" windowHeight="19540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="observation_datasheet" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1229" uniqueCount="580">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1232" uniqueCount="583">
   <si>
     <t>ID</t>
   </si>
@@ -1779,6 +1779,15 @@
   </si>
   <si>
     <t>ht.date</t>
+  </si>
+  <si>
+    <t>phenol</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>budset</t>
   </si>
 </sst>
 </file>
@@ -2905,7 +2914,7 @@
   </sheetPr>
   <dimension ref="A1:M481"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D80" sqref="D80"/>
     </sheetView>
   </sheetViews>
@@ -5406,13 +5415,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AH481"/>
+  <dimension ref="A1:AJ481"/>
   <sheetViews>
-    <sheetView zoomScale="86" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="P24" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="86" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="U2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AG52" sqref="AG52"/>
+      <selection pane="bottomRight" activeCell="AJ428" sqref="AJ428"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5427,7 +5436,7 @@
     <col min="14" max="30" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>487</v>
       </c>
@@ -5518,8 +5527,14 @@
       <c r="AH1" s="49" t="s">
         <v>579</v>
       </c>
-    </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI1" s="49" t="s">
+        <v>580</v>
+      </c>
+      <c r="AJ1" s="49" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="2" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
         <v>3</v>
       </c>
@@ -5590,8 +5605,12 @@
       <c r="AH2">
         <v>191</v>
       </c>
-    </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI2">
+        <v>-0.14000000000000001</v>
+      </c>
+      <c r="AJ2" s="1"/>
+    </row>
+    <row r="3" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
         <v>4</v>
       </c>
@@ -5664,8 +5683,11 @@
       <c r="AH3">
         <v>191</v>
       </c>
-    </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI3">
+        <v>-0.05</v>
+      </c>
+    </row>
+    <row r="4" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
         <v>5</v>
       </c>
@@ -5736,8 +5758,11 @@
       <c r="AH4">
         <v>191</v>
       </c>
-    </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI4">
+        <v>-0.26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
         <v>6</v>
       </c>
@@ -5808,8 +5833,11 @@
       <c r="AH5">
         <v>191</v>
       </c>
-    </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI5">
+        <v>-0.23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
         <v>7</v>
       </c>
@@ -5878,8 +5906,11 @@
       <c r="AH6">
         <v>191</v>
       </c>
-    </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI6">
+        <v>-0.26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
         <v>8</v>
       </c>
@@ -5950,8 +5981,11 @@
       <c r="AH7">
         <v>191</v>
       </c>
-    </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI7">
+        <v>-0.02</v>
+      </c>
+    </row>
+    <row r="8" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
         <v>9</v>
       </c>
@@ -6020,8 +6054,11 @@
       <c r="AH8">
         <v>191</v>
       </c>
-    </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI8">
+        <v>-0.06</v>
+      </c>
+    </row>
+    <row r="9" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
         <v>10</v>
       </c>
@@ -6092,8 +6129,11 @@
       <c r="AH9">
         <v>191</v>
       </c>
-    </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI9">
+        <v>-0.33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
         <v>11</v>
       </c>
@@ -6162,8 +6202,11 @@
       <c r="AH10">
         <v>191</v>
       </c>
-    </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI10">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="11" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
         <v>12</v>
       </c>
@@ -6236,8 +6279,11 @@
       <c r="AH11">
         <v>191</v>
       </c>
-    </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI11">
+        <v>-0.26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
         <v>13</v>
       </c>
@@ -6300,8 +6346,14 @@
       <c r="AH12">
         <v>191</v>
       </c>
-    </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI12">
+        <v>-0.13</v>
+      </c>
+      <c r="AJ12" s="1">
+        <v>43676</v>
+      </c>
+    </row>
+    <row r="13" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A13" s="13" t="s">
         <v>14</v>
       </c>
@@ -6369,8 +6421,11 @@
       <c r="AH13">
         <v>191</v>
       </c>
-    </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI13">
+        <v>-0.19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A14" s="13" t="s">
         <v>15</v>
       </c>
@@ -6436,8 +6491,11 @@
       <c r="AH14">
         <v>191</v>
       </c>
-    </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI14">
+        <v>-0.18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A15" s="13" t="s">
         <v>16</v>
       </c>
@@ -6508,8 +6566,11 @@
       <c r="AH15">
         <v>191</v>
       </c>
-    </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI15">
+        <v>-7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A16" s="13" t="s">
         <v>17</v>
       </c>
@@ -6575,8 +6636,11 @@
       <c r="AH16">
         <v>191</v>
       </c>
-    </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI16">
+        <v>-0.02</v>
+      </c>
+    </row>
+    <row r="17" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A17" s="13" t="s">
         <v>18</v>
       </c>
@@ -6647,8 +6711,11 @@
       <c r="AH17">
         <v>191</v>
       </c>
-    </row>
-    <row r="18" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI17">
+        <v>-0.06</v>
+      </c>
+    </row>
+    <row r="18" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A18" s="18" t="s">
         <v>19</v>
       </c>
@@ -6720,7 +6787,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="19" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A19" s="18" t="s">
         <v>20</v>
       </c>
@@ -6794,7 +6861,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="20" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A20" s="18" t="s">
         <v>21</v>
       </c>
@@ -6864,7 +6931,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="21" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A21" s="18" t="s">
         <v>22</v>
       </c>
@@ -6935,8 +7002,11 @@
       <c r="AH21">
         <v>192</v>
       </c>
-    </row>
-    <row r="22" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AJ21" s="1">
+        <v>43676</v>
+      </c>
+    </row>
+    <row r="22" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A22" s="18" t="s">
         <v>23</v>
       </c>
@@ -7006,7 +7076,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="23" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A23" s="18" t="s">
         <v>24</v>
       </c>
@@ -7078,7 +7148,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="24" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A24" s="18" t="s">
         <v>25</v>
       </c>
@@ -7145,7 +7215,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="25" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A25" s="18" t="s">
         <v>26</v>
       </c>
@@ -7211,7 +7281,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="26" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A26" s="18" t="s">
         <v>27</v>
       </c>
@@ -7281,7 +7351,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="27" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A27" s="18" t="s">
         <v>28</v>
       </c>
@@ -7344,7 +7414,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="28" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A28" s="18" t="s">
         <v>29</v>
       </c>
@@ -7414,7 +7484,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="29" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A29" s="18" t="s">
         <v>30</v>
       </c>
@@ -7480,7 +7550,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="30" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A30" s="18" t="s">
         <v>31</v>
       </c>
@@ -7544,7 +7614,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="31" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A31" s="18" t="s">
         <v>32</v>
       </c>
@@ -7616,7 +7686,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="32" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A32" s="18" t="s">
         <v>33</v>
       </c>
@@ -11976,7 +12046,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="97" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A97" s="21" t="s">
         <v>98</v>
       </c>
@@ -12048,7 +12118,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="98" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A98" s="13" t="s">
         <v>99</v>
       </c>
@@ -12127,8 +12197,11 @@
       <c r="AH98">
         <v>191</v>
       </c>
-    </row>
-    <row r="99" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI98">
+        <v>-0.05</v>
+      </c>
+    </row>
+    <row r="99" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A99" s="13" t="s">
         <v>100</v>
       </c>
@@ -12207,8 +12280,11 @@
       <c r="AH99">
         <v>191</v>
       </c>
-    </row>
-    <row r="100" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI99">
+        <v>-0.02</v>
+      </c>
+    </row>
+    <row r="100" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A100" s="13" t="s">
         <v>101</v>
       </c>
@@ -12290,8 +12366,11 @@
       <c r="AH100">
         <v>191</v>
       </c>
-    </row>
-    <row r="101" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI100">
+        <v>-0.03</v>
+      </c>
+    </row>
+    <row r="101" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A101" s="13" t="s">
         <v>102</v>
       </c>
@@ -12362,8 +12441,11 @@
       <c r="AH101">
         <v>191</v>
       </c>
-    </row>
-    <row r="102" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A102" s="13" t="s">
         <v>103</v>
       </c>
@@ -12445,8 +12527,11 @@
       <c r="AH102">
         <v>191</v>
       </c>
-    </row>
-    <row r="103" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI102">
+        <v>-0.03</v>
+      </c>
+    </row>
+    <row r="103" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A103" s="13" t="s">
         <v>104</v>
       </c>
@@ -12517,8 +12602,11 @@
       <c r="AH103">
         <v>191</v>
       </c>
-    </row>
-    <row r="104" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI103">
+        <v>-0.04</v>
+      </c>
+    </row>
+    <row r="104" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A104" s="13" t="s">
         <v>105</v>
       </c>
@@ -12600,8 +12688,11 @@
       <c r="AH104">
         <v>191</v>
       </c>
-    </row>
-    <row r="105" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI104">
+        <v>-0.08</v>
+      </c>
+    </row>
+    <row r="105" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A105" s="13" t="s">
         <v>106</v>
       </c>
@@ -12685,8 +12776,11 @@
       <c r="AH105">
         <v>191</v>
       </c>
-    </row>
-    <row r="106" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI105">
+        <v>-0.08</v>
+      </c>
+    </row>
+    <row r="106" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A106" s="13" t="s">
         <v>107</v>
       </c>
@@ -12755,8 +12849,11 @@
       <c r="AH106">
         <v>191</v>
       </c>
-    </row>
-    <row r="107" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI106">
+        <v>-0.12</v>
+      </c>
+    </row>
+    <row r="107" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A107" s="13" t="s">
         <v>108</v>
       </c>
@@ -12827,8 +12924,11 @@
       <c r="AH107">
         <v>191</v>
       </c>
-    </row>
-    <row r="108" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI107">
+        <v>-0.08</v>
+      </c>
+    </row>
+    <row r="108" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A108" s="13" t="s">
         <v>109</v>
       </c>
@@ -12910,8 +13010,11 @@
       <c r="AH108">
         <v>191</v>
       </c>
-    </row>
-    <row r="109" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI108">
+        <v>-0.04</v>
+      </c>
+    </row>
+    <row r="109" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A109" s="13" t="s">
         <v>110</v>
       </c>
@@ -12982,8 +13085,11 @@
       <c r="AH109">
         <v>191</v>
       </c>
-    </row>
-    <row r="110" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI109">
+        <v>-0.03</v>
+      </c>
+    </row>
+    <row r="110" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A110" s="13" t="s">
         <v>111</v>
       </c>
@@ -13052,8 +13158,11 @@
       <c r="AH110">
         <v>191</v>
       </c>
-    </row>
-    <row r="111" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI110">
+        <v>-0.06</v>
+      </c>
+    </row>
+    <row r="111" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A111" s="13" t="s">
         <v>112</v>
       </c>
@@ -13124,8 +13233,11 @@
       <c r="AH111">
         <v>191</v>
       </c>
-    </row>
-    <row r="112" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI111">
+        <v>-0.05</v>
+      </c>
+    </row>
+    <row r="112" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A112" s="13" t="s">
         <v>113</v>
       </c>
@@ -13194,8 +13306,11 @@
       <c r="AH112">
         <v>191</v>
       </c>
-    </row>
-    <row r="113" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI112">
+        <v>-0.11</v>
+      </c>
+    </row>
+    <row r="113" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A113" s="13" t="s">
         <v>114</v>
       </c>
@@ -13268,8 +13383,11 @@
       <c r="AH113">
         <v>191</v>
       </c>
-    </row>
-    <row r="114" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI113">
+        <v>-0.1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A114" s="18" t="s">
         <v>115</v>
       </c>
@@ -13341,7 +13459,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="115" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A115" s="18" t="s">
         <v>116</v>
       </c>
@@ -13413,7 +13531,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="116" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A116" s="18" t="s">
         <v>117</v>
       </c>
@@ -13483,7 +13601,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="117" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A117" s="18" t="s">
         <v>118</v>
       </c>
@@ -13555,7 +13673,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="118" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A118" s="18" t="s">
         <v>119</v>
       </c>
@@ -13625,7 +13743,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="119" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A119" s="18" t="s">
         <v>120</v>
       </c>
@@ -13699,7 +13817,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="120" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A120" s="18" t="s">
         <v>121</v>
       </c>
@@ -13769,7 +13887,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="121" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A121" s="18" t="s">
         <v>122</v>
       </c>
@@ -13841,7 +13959,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="122" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A122" s="18" t="s">
         <v>123</v>
       </c>
@@ -13911,7 +14029,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="123" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A123" s="18" t="s">
         <v>124</v>
       </c>
@@ -13985,7 +14103,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="124" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A124" s="18" t="s">
         <v>125</v>
       </c>
@@ -14055,7 +14173,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="125" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A125" s="18" t="s">
         <v>126</v>
       </c>
@@ -14127,7 +14245,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="126" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A126" s="18" t="s">
         <v>127</v>
       </c>
@@ -14197,7 +14315,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="127" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A127" s="18" t="s">
         <v>128</v>
       </c>
@@ -14269,7 +14387,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="128" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A128" s="18" t="s">
         <v>129</v>
       </c>
@@ -18898,7 +19016,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="193" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A193" s="21" t="s">
         <v>194</v>
       </c>
@@ -18970,7 +19088,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="194" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A194" s="13" t="s">
         <v>195</v>
       </c>
@@ -19062,8 +19180,11 @@
       <c r="AH194">
         <v>191</v>
       </c>
-    </row>
-    <row r="195" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI194">
+        <v>-0.21</v>
+      </c>
+    </row>
+    <row r="195" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A195" s="13" t="s">
         <v>196</v>
       </c>
@@ -19148,8 +19269,11 @@
       <c r="AH195">
         <v>191</v>
       </c>
-    </row>
-    <row r="196" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI195">
+        <v>-0.2</v>
+      </c>
+    </row>
+    <row r="196" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A196" s="13" t="s">
         <v>197</v>
       </c>
@@ -19218,8 +19342,11 @@
       <c r="AH196">
         <v>191</v>
       </c>
-    </row>
-    <row r="197" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI196">
+        <v>-0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="197" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A197" s="13" t="s">
         <v>198</v>
       </c>
@@ -19290,8 +19417,11 @@
       <c r="AH197">
         <v>191</v>
       </c>
-    </row>
-    <row r="198" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI197">
+        <v>-0.2</v>
+      </c>
+    </row>
+    <row r="198" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A198" s="13" t="s">
         <v>199</v>
       </c>
@@ -19373,8 +19503,11 @@
       <c r="AH198">
         <v>191</v>
       </c>
-    </row>
-    <row r="199" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI198">
+        <v>-0.1</v>
+      </c>
+    </row>
+    <row r="199" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A199" s="13" t="s">
         <v>200</v>
       </c>
@@ -19445,8 +19578,11 @@
       <c r="AH199">
         <v>191</v>
       </c>
-    </row>
-    <row r="200" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI199">
+        <v>-0.15</v>
+      </c>
+    </row>
+    <row r="200" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A200" s="13" t="s">
         <v>201</v>
       </c>
@@ -19515,8 +19651,11 @@
       <c r="AH200">
         <v>191</v>
       </c>
-    </row>
-    <row r="201" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI200">
+        <v>-0.23</v>
+      </c>
+    </row>
+    <row r="201" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A201" s="13" t="s">
         <v>202</v>
       </c>
@@ -19587,8 +19726,11 @@
       <c r="AH201">
         <v>191</v>
       </c>
-    </row>
-    <row r="202" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI201">
+        <v>-0.27</v>
+      </c>
+    </row>
+    <row r="202" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A202" s="13" t="s">
         <v>203</v>
       </c>
@@ -19657,8 +19799,11 @@
       <c r="AH202">
         <v>191</v>
       </c>
-    </row>
-    <row r="203" spans="1:34" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AI202">
+        <v>-0.25</v>
+      </c>
+    </row>
+    <row r="203" spans="1:35" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A203" s="13" t="s">
         <v>204</v>
       </c>
@@ -19732,8 +19877,11 @@
       <c r="AH203">
         <v>191</v>
       </c>
-    </row>
-    <row r="204" spans="1:34" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AI203">
+        <v>-0.21</v>
+      </c>
+    </row>
+    <row r="204" spans="1:35" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A204" s="13" t="s">
         <v>205</v>
       </c>
@@ -19802,8 +19950,11 @@
       <c r="AH204">
         <v>191</v>
       </c>
-    </row>
-    <row r="205" spans="1:34" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AI204">
+        <v>-0.22</v>
+      </c>
+    </row>
+    <row r="205" spans="1:35" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A205" s="13" t="s">
         <v>206</v>
       </c>
@@ -19887,8 +20038,11 @@
       <c r="AH205">
         <v>191</v>
       </c>
-    </row>
-    <row r="206" spans="1:34" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AI205">
+        <v>-0.24</v>
+      </c>
+    </row>
+    <row r="206" spans="1:35" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A206" s="13" t="s">
         <v>207</v>
       </c>
@@ -19970,8 +20124,11 @@
       <c r="AH206">
         <v>191</v>
       </c>
-    </row>
-    <row r="207" spans="1:34" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AI206">
+        <v>-0.23</v>
+      </c>
+    </row>
+    <row r="207" spans="1:35" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A207" s="13" t="s">
         <v>208</v>
       </c>
@@ -20044,8 +20201,11 @@
       <c r="AH207">
         <v>191</v>
       </c>
-    </row>
-    <row r="208" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI207">
+        <v>-0.06</v>
+      </c>
+    </row>
+    <row r="208" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A208" s="13" t="s">
         <v>209</v>
       </c>
@@ -20127,8 +20287,11 @@
       <c r="AH208">
         <v>191</v>
       </c>
-    </row>
-    <row r="209" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI208">
+        <v>-0.26</v>
+      </c>
+    </row>
+    <row r="209" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A209" s="13" t="s">
         <v>210</v>
       </c>
@@ -20199,8 +20362,11 @@
       <c r="AH209">
         <v>191</v>
       </c>
-    </row>
-    <row r="210" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI209">
+        <v>-0.26</v>
+      </c>
+    </row>
+    <row r="210" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A210" s="18" t="s">
         <v>211</v>
       </c>
@@ -20272,7 +20438,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="211" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A211" s="18" t="s">
         <v>212</v>
       </c>
@@ -20344,7 +20510,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="212" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A212" s="18" t="s">
         <v>213</v>
       </c>
@@ -20414,7 +20580,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="213" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A213" s="18" t="s">
         <v>214</v>
       </c>
@@ -20488,7 +20654,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="214" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A214" s="18" t="s">
         <v>215</v>
       </c>
@@ -20558,7 +20724,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="215" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A215" s="18" t="s">
         <v>216</v>
       </c>
@@ -20630,7 +20796,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="216" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A216" s="18" t="s">
         <v>217</v>
       </c>
@@ -20700,7 +20866,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="217" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A217" s="18" t="s">
         <v>218</v>
       </c>
@@ -20772,7 +20938,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="218" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A218" s="18" t="s">
         <v>219</v>
       </c>
@@ -20842,7 +21008,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="219" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A219" s="18" t="s">
         <v>220</v>
       </c>
@@ -20914,7 +21080,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="220" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A220" s="18" t="s">
         <v>221</v>
       </c>
@@ -20984,7 +21150,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="221" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A221" s="18" t="s">
         <v>222</v>
       </c>
@@ -21056,7 +21222,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="222" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A222" s="18" t="s">
         <v>223</v>
       </c>
@@ -21126,7 +21292,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="223" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A223" s="18" t="s">
         <v>224</v>
       </c>
@@ -21198,7 +21364,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="224" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A224" s="18" t="s">
         <v>225</v>
       </c>
@@ -22410,7 +22576,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="241" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A241" s="21" t="s">
         <v>242</v>
       </c>
@@ -22483,8 +22649,11 @@
       <c r="AH241">
         <v>192</v>
       </c>
-    </row>
-    <row r="242" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AJ241" s="1">
+        <v>43676</v>
+      </c>
+    </row>
+    <row r="242" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A242" s="13" t="s">
         <v>243</v>
       </c>
@@ -22514,7 +22683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A243" s="13" t="s">
         <v>244</v>
       </c>
@@ -22565,7 +22734,7 @@
         <v>-0.70000000000000284</v>
       </c>
     </row>
-    <row r="244" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A244" s="13" t="s">
         <v>245</v>
       </c>
@@ -22614,7 +22783,7 @@
         <v>-0.40000000000000568</v>
       </c>
     </row>
-    <row r="245" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A245" s="13" t="s">
         <v>246</v>
       </c>
@@ -22665,7 +22834,7 @@
         <v>-0.59999999999999787</v>
       </c>
     </row>
-    <row r="246" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A246" s="13" t="s">
         <v>247</v>
       </c>
@@ -22693,7 +22862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="247" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A247" s="13" t="s">
         <v>248</v>
       </c>
@@ -22721,7 +22890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="248" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A248" s="13" t="s">
         <v>249</v>
       </c>
@@ -22755,7 +22924,7 @@
         <v>-28.3</v>
       </c>
     </row>
-    <row r="249" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A249" s="13" t="s">
         <v>250</v>
       </c>
@@ -22783,7 +22952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="250" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A250" s="13" t="s">
         <v>251</v>
       </c>
@@ -22811,7 +22980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="251" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A251" s="13" t="s">
         <v>252</v>
       </c>
@@ -22847,7 +23016,7 @@
         <v>-34.1</v>
       </c>
     </row>
-    <row r="252" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A252" s="13" t="s">
         <v>253</v>
       </c>
@@ -22881,7 +23050,7 @@
         <v>-27.7</v>
       </c>
     </row>
-    <row r="253" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A253" s="13" t="s">
         <v>254</v>
       </c>
@@ -22909,7 +23078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="254" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A254" s="13" t="s">
         <v>255</v>
       </c>
@@ -22943,7 +23112,7 @@
         <v>-30.3</v>
       </c>
     </row>
-    <row r="255" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A255" s="13" t="s">
         <v>256</v>
       </c>
@@ -22971,7 +23140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="256" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A256" s="13" t="s">
         <v>257</v>
       </c>
@@ -29063,7 +29232,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="385" spans="1:34" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="385" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A385" s="24" t="s">
         <v>386</v>
       </c>
@@ -29091,8 +29260,9 @@
         <v>0</v>
       </c>
       <c r="AA385"/>
-    </row>
-    <row r="386" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI385"/>
+    </row>
+    <row r="386" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A386" s="13" t="s">
         <v>387</v>
       </c>
@@ -29163,8 +29333,9 @@
       <c r="AH386">
         <v>191</v>
       </c>
-    </row>
-    <row r="387" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI386" s="5"/>
+    </row>
+    <row r="387" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A387" s="13" t="s">
         <v>388</v>
       </c>
@@ -29238,7 +29409,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="388" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="388" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A388" s="24" t="s">
         <v>389</v>
       </c>
@@ -29273,7 +29444,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="389" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="389" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A389" s="13" t="s">
         <v>390</v>
       </c>
@@ -29347,7 +29518,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="390" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="390" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A390" s="13" t="s">
         <v>391</v>
       </c>
@@ -29419,7 +29590,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="391" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="391" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A391" s="13" t="s">
         <v>392</v>
       </c>
@@ -29491,7 +29662,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="392" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="392" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A392" s="13" t="s">
         <v>393</v>
       </c>
@@ -29560,8 +29731,11 @@
       <c r="AH392">
         <v>191</v>
       </c>
-    </row>
-    <row r="393" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AJ392" s="1">
+        <v>43676</v>
+      </c>
+    </row>
+    <row r="393" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A393" s="13" t="s">
         <v>394</v>
       </c>
@@ -29633,7 +29807,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="394" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="394" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A394" s="13" t="s">
         <v>395</v>
       </c>
@@ -29703,7 +29877,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="395" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="395" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A395" s="13" t="s">
         <v>396</v>
       </c>
@@ -29775,7 +29949,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="396" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="396" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A396" s="13" t="s">
         <v>397</v>
       </c>
@@ -29845,7 +30019,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="397" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="397" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A397" s="13" t="s">
         <v>398</v>
       </c>
@@ -29908,7 +30082,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="398" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="398" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A398" s="13" t="s">
         <v>399</v>
       </c>
@@ -29978,7 +30152,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="399" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="399" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A399" s="13" t="s">
         <v>400</v>
       </c>
@@ -30052,7 +30226,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="400" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="400" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A400" s="13" t="s">
         <v>401</v>
       </c>
@@ -30122,7 +30296,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="401" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="401" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A401" s="13" t="s">
         <v>402</v>
       </c>
@@ -30193,8 +30367,11 @@
       <c r="AH401">
         <v>191</v>
       </c>
-    </row>
-    <row r="402" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AJ401" s="1">
+        <v>43671</v>
+      </c>
+    </row>
+    <row r="402" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A402" s="18" t="s">
         <v>403</v>
       </c>
@@ -30265,8 +30442,11 @@
       <c r="AH402">
         <v>192</v>
       </c>
-    </row>
-    <row r="403" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AJ402" s="1">
+        <v>43676</v>
+      </c>
+    </row>
+    <row r="403" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A403" s="18" t="s">
         <v>404</v>
       </c>
@@ -30340,7 +30520,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="404" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="404" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A404" s="18" t="s">
         <v>405</v>
       </c>
@@ -30412,7 +30592,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="405" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="405" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A405" s="18" t="s">
         <v>406</v>
       </c>
@@ -30486,7 +30666,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="406" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="406" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A406" s="18" t="s">
         <v>407</v>
       </c>
@@ -30556,7 +30736,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="407" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="407" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A407" s="18" t="s">
         <v>408</v>
       </c>
@@ -30627,8 +30807,11 @@
       <c r="AH407">
         <v>192</v>
       </c>
-    </row>
-    <row r="408" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AJ407" s="1">
+        <v>43671</v>
+      </c>
+    </row>
+    <row r="408" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A408" s="18" t="s">
         <v>409</v>
       </c>
@@ -30698,7 +30881,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="409" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="409" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A409" s="18" t="s">
         <v>410</v>
       </c>
@@ -30770,7 +30953,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="410" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="410" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A410" s="18" t="s">
         <v>411</v>
       </c>
@@ -30840,7 +31023,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="411" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="411" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A411" s="18" t="s">
         <v>412</v>
       </c>
@@ -30912,7 +31095,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="412" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="412" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A412" s="18" t="s">
         <v>413</v>
       </c>
@@ -30982,7 +31165,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="413" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="413" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A413" s="18" t="s">
         <v>414</v>
       </c>
@@ -31054,7 +31237,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="414" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="414" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A414" s="18" t="s">
         <v>415</v>
       </c>
@@ -31124,7 +31307,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="415" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="415" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A415" s="18" t="s">
         <v>416</v>
       </c>
@@ -31195,8 +31378,11 @@
       <c r="AH415">
         <v>192</v>
       </c>
-    </row>
-    <row r="416" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AJ415" s="1">
+        <v>43676</v>
+      </c>
+    </row>
+    <row r="416" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A416" s="18" t="s">
         <v>417</v>
       </c>
@@ -31266,7 +31452,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="417" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="417" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A417" s="18" t="s">
         <v>418</v>
       </c>
@@ -31338,7 +31524,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="418" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="418" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A418" s="21" t="s">
         <v>419</v>
       </c>
@@ -31410,7 +31596,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="419" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="419" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A419" s="21" t="s">
         <v>420</v>
       </c>
@@ -31484,7 +31670,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="420" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="420" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A420" s="21" t="s">
         <v>421</v>
       </c>
@@ -31556,7 +31742,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="421" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="421" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A421" s="21" t="s">
         <v>422</v>
       </c>
@@ -31628,7 +31814,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="422" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="422" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A422" s="21" t="s">
         <v>423</v>
       </c>
@@ -31698,7 +31884,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="423" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="423" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A423" s="21" t="s">
         <v>424</v>
       </c>
@@ -31770,7 +31956,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="424" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="424" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A424" s="21" t="s">
         <v>425</v>
       </c>
@@ -31840,7 +32026,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="425" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="425" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A425" s="21" t="s">
         <v>426</v>
       </c>
@@ -31912,7 +32098,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="426" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="426" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A426" s="21" t="s">
         <v>427</v>
       </c>
@@ -31982,7 +32168,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="427" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="427" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A427" s="21" t="s">
         <v>428</v>
       </c>
@@ -32053,8 +32239,11 @@
       <c r="AH427">
         <v>191</v>
       </c>
-    </row>
-    <row r="428" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AJ427" s="1">
+        <v>43676</v>
+      </c>
+    </row>
+    <row r="428" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A428" s="21" t="s">
         <v>429</v>
       </c>
@@ -32124,7 +32313,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="429" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="429" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A429" s="21" t="s">
         <v>430</v>
       </c>
@@ -32196,7 +32385,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="430" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="430" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A430" s="21" t="s">
         <v>431</v>
       </c>
@@ -32266,7 +32455,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="431" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="431" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A431" s="21" t="s">
         <v>432</v>
       </c>
@@ -32336,7 +32525,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="432" spans="1:34" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="432" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A432" s="21" t="s">
         <v>433</v>
       </c>
@@ -32405,8 +32594,9 @@
       <c r="AH432">
         <v>191</v>
       </c>
-    </row>
-    <row r="433" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI432"/>
+    </row>
+    <row r="433" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A433" s="21" t="s">
         <v>434</v>
       </c>
@@ -32477,8 +32667,9 @@
       <c r="AH433">
         <v>191</v>
       </c>
-    </row>
-    <row r="434" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI433" s="5"/>
+    </row>
+    <row r="434" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A434" s="13" t="s">
         <v>435</v>
       </c>
@@ -32549,8 +32740,11 @@
       <c r="AH434">
         <v>191</v>
       </c>
-    </row>
-    <row r="435" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI434">
+        <v>-0.03</v>
+      </c>
+    </row>
+    <row r="435" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A435" s="13" t="s">
         <v>436</v>
       </c>
@@ -32623,8 +32817,11 @@
       <c r="AH435">
         <v>191</v>
       </c>
-    </row>
-    <row r="436" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI435">
+        <v>-0.03</v>
+      </c>
+    </row>
+    <row r="436" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A436" s="13" t="s">
         <v>437</v>
       </c>
@@ -32695,8 +32892,11 @@
       <c r="AH436">
         <v>191</v>
       </c>
-    </row>
-    <row r="437" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI436">
+        <v>-0.06</v>
+      </c>
+    </row>
+    <row r="437" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A437" s="13" t="s">
         <v>438</v>
       </c>
@@ -32769,8 +32969,11 @@
       <c r="AH437">
         <v>191</v>
       </c>
-    </row>
-    <row r="438" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI437">
+        <v>-0.11</v>
+      </c>
+    </row>
+    <row r="438" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A438" s="13" t="s">
         <v>439</v>
       </c>
@@ -32839,8 +33042,11 @@
       <c r="AH438">
         <v>191</v>
       </c>
-    </row>
-    <row r="439" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI438">
+        <v>-0.03</v>
+      </c>
+    </row>
+    <row r="439" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A439" s="13" t="s">
         <v>440</v>
       </c>
@@ -32911,8 +33117,11 @@
       <c r="AH439">
         <v>191</v>
       </c>
-    </row>
-    <row r="440" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI439">
+        <v>-0.03</v>
+      </c>
+    </row>
+    <row r="440" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A440" s="13" t="s">
         <v>441</v>
       </c>
@@ -32981,8 +33190,11 @@
       <c r="AH440">
         <v>191</v>
       </c>
-    </row>
-    <row r="441" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI440">
+        <v>-0.03</v>
+      </c>
+    </row>
+    <row r="441" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A441" s="24" t="s">
         <v>442</v>
       </c>
@@ -33012,8 +33224,11 @@
       <c r="AH441">
         <v>191</v>
       </c>
-    </row>
-    <row r="442" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI441" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="442" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A442" s="13" t="s">
         <v>443</v>
       </c>
@@ -33082,8 +33297,11 @@
       <c r="AH442">
         <v>191</v>
       </c>
-    </row>
-    <row r="443" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI442">
+        <v>-0.05</v>
+      </c>
+    </row>
+    <row r="443" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A443" s="13" t="s">
         <v>444</v>
       </c>
@@ -33156,8 +33374,11 @@
       <c r="AH443">
         <v>191</v>
       </c>
-    </row>
-    <row r="444" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI443">
+        <v>-0.02</v>
+      </c>
+    </row>
+    <row r="444" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A444" s="13" t="s">
         <v>445</v>
       </c>
@@ -33226,8 +33447,11 @@
       <c r="AH444">
         <v>191</v>
       </c>
-    </row>
-    <row r="445" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI444">
+        <v>-0.02</v>
+      </c>
+    </row>
+    <row r="445" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A445" s="13" t="s">
         <v>446</v>
       </c>
@@ -33298,8 +33522,11 @@
       <c r="AH445">
         <v>191</v>
       </c>
-    </row>
-    <row r="446" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI445">
+        <v>-0.08</v>
+      </c>
+    </row>
+    <row r="446" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A446" s="13" t="s">
         <v>447</v>
       </c>
@@ -33368,8 +33595,11 @@
       <c r="AH446">
         <v>191</v>
       </c>
-    </row>
-    <row r="447" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI446">
+        <v>-7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="447" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A447" s="13" t="s">
         <v>448</v>
       </c>
@@ -33440,8 +33670,11 @@
       <c r="AH447">
         <v>191</v>
       </c>
-    </row>
-    <row r="448" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI447">
+        <v>-0.05</v>
+      </c>
+    </row>
+    <row r="448" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A448" s="13" t="s">
         <v>449</v>
       </c>
@@ -33510,8 +33743,11 @@
       <c r="AH448">
         <v>191</v>
       </c>
-    </row>
-    <row r="449" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI448">
+        <v>-0.16</v>
+      </c>
+    </row>
+    <row r="449" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A449" s="13" t="s">
         <v>450</v>
       </c>
@@ -33576,8 +33812,11 @@
       <c r="AH449">
         <v>191</v>
       </c>
-    </row>
-    <row r="450" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI449">
+        <v>-0.02</v>
+      </c>
+    </row>
+    <row r="450" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A450" s="18" t="s">
         <v>451</v>
       </c>
@@ -33649,7 +33888,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="451" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="451" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A451" s="18" t="s">
         <v>452</v>
       </c>
@@ -33723,7 +33962,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="452" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="452" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A452" s="18" t="s">
         <v>453</v>
       </c>
@@ -33795,7 +34034,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="453" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="453" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A453" s="18" t="s">
         <v>454</v>
       </c>
@@ -33867,7 +34106,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="454" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="454" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A454" s="18" t="s">
         <v>455</v>
       </c>
@@ -33937,7 +34176,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="455" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="455" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A455" s="18" t="s">
         <v>456</v>
       </c>
@@ -34009,7 +34248,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="456" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="456" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A456" s="18" t="s">
         <v>457</v>
       </c>
@@ -34079,7 +34318,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="457" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="457" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A457" s="18" t="s">
         <v>458</v>
       </c>
@@ -34151,7 +34390,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="458" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="458" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A458" s="18" t="s">
         <v>459</v>
       </c>
@@ -34221,7 +34460,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="459" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="459" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A459" s="18" t="s">
         <v>460</v>
       </c>
@@ -34293,7 +34532,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="460" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="460" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A460" s="18" t="s">
         <v>461</v>
       </c>
@@ -34363,7 +34602,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="461" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="461" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A461" s="18" t="s">
         <v>462</v>
       </c>
@@ -34435,7 +34674,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="462" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="462" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A462" s="18" t="s">
         <v>463</v>
       </c>
@@ -34505,7 +34744,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="463" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="463" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A463" s="18" t="s">
         <v>464</v>
       </c>
@@ -34577,7 +34816,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="464" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="464" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A464" s="18" t="s">
         <v>465</v>
       </c>

</xml_diff>

<commit_message>
adding refs and obs
</commit_message>
<xml_diff>
--- a/data/observation_datasheet.xlsx
+++ b/data/observation_datasheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/catchamberlain/Documents/git/chillfreeze/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33D57EEC-E86D-6144-B3C4-B4C702053392}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{651912EC-3D5A-9B46-AD0B-938D0B1903AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="460" windowWidth="19040" windowHeight="13760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3420" yWindow="460" windowWidth="32400" windowHeight="21640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="observation_datasheet" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1226" uniqueCount="586">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1227" uniqueCount="587">
   <si>
     <t>ID</t>
   </si>
@@ -1798,13 +1798,16 @@
   </si>
   <si>
     <t>meristem</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="27">
+  <fonts count="28">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1996,6 +1999,12 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Rockwell"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <name val="Rockwell"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2535,7 +2544,7 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -2599,6 +2608,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="39" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="98">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -5453,10 +5464,10 @@
   <dimension ref="A1:AN481"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="86" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AI466" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AC389" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AK479" sqref="AK479"/>
+      <selection pane="bottomRight" activeCell="AM387" sqref="AM387"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -5840,6 +5851,12 @@
       <c r="AJ4" s="1">
         <v>43784</v>
       </c>
+      <c r="AL4">
+        <v>46.728999999999999</v>
+      </c>
+      <c r="AM4">
+        <v>9.0980000000000008</v>
+      </c>
       <c r="AN4">
         <v>1</v>
       </c>
@@ -6184,6 +6201,15 @@
       <c r="AJ8" s="1">
         <v>43788</v>
       </c>
+      <c r="AK8">
+        <v>117.1</v>
+      </c>
+      <c r="AL8">
+        <v>61.079000000000001</v>
+      </c>
+      <c r="AM8" s="58">
+        <v>41.905000000000001</v>
+      </c>
       <c r="AN8">
         <v>0</v>
       </c>
@@ -6353,6 +6379,15 @@
       <c r="AJ10" s="1">
         <v>43795</v>
       </c>
+      <c r="AK10">
+        <v>86</v>
+      </c>
+      <c r="AL10">
+        <v>47.75</v>
+      </c>
+      <c r="AM10">
+        <v>17.507000000000001</v>
+      </c>
       <c r="AN10">
         <v>0</v>
       </c>
@@ -6435,6 +6470,15 @@
       </c>
       <c r="AJ11" s="60">
         <v>43788</v>
+      </c>
+      <c r="AK11">
+        <v>76.599999999999994</v>
+      </c>
+      <c r="AL11">
+        <v>53.427999999999997</v>
+      </c>
+      <c r="AM11">
+        <v>18.248000000000001</v>
       </c>
       <c r="AN11">
         <v>1</v>
@@ -6509,12 +6553,6 @@
       <c r="AJ12" s="1">
         <v>43676</v>
       </c>
-      <c r="AL12">
-        <v>0.21304000000000001</v>
-      </c>
-      <c r="AM12">
-        <v>0.38613999999999998</v>
-      </c>
     </row>
     <row r="13" spans="1:40">
       <c r="A13" s="13" t="s">
@@ -6678,6 +6716,12 @@
       <c r="AK14">
         <v>64.599999999999994</v>
       </c>
+      <c r="AL14">
+        <v>16.561</v>
+      </c>
+      <c r="AM14">
+        <v>7.9969999999999999</v>
+      </c>
       <c r="AN14">
         <v>0</v>
       </c>
@@ -6761,6 +6805,12 @@
       </c>
       <c r="AK15">
         <v>91.3</v>
+      </c>
+      <c r="AL15">
+        <v>22.065999999999999</v>
+      </c>
+      <c r="AM15">
+        <v>11.009</v>
       </c>
       <c r="AN15">
         <v>0</v>
@@ -6841,6 +6891,12 @@
       <c r="AK16">
         <v>91.4</v>
       </c>
+      <c r="AL16">
+        <v>29.123000000000001</v>
+      </c>
+      <c r="AM16">
+        <v>16.253</v>
+      </c>
       <c r="AN16">
         <v>0</v>
       </c>
@@ -6922,6 +6978,15 @@
       <c r="AJ17" s="60">
         <v>43788</v>
       </c>
+      <c r="AK17">
+        <v>98.9</v>
+      </c>
+      <c r="AL17">
+        <v>38.459000000000003</v>
+      </c>
+      <c r="AM17">
+        <v>15.836</v>
+      </c>
       <c r="AN17">
         <v>0</v>
       </c>
@@ -7000,6 +7065,15 @@
       <c r="AJ18" s="1">
         <v>43802</v>
       </c>
+      <c r="AK18">
+        <v>105.8</v>
+      </c>
+      <c r="AL18">
+        <v>48.615000000000002</v>
+      </c>
+      <c r="AM18">
+        <v>19.937000000000001</v>
+      </c>
       <c r="AN18">
         <v>0</v>
       </c>
@@ -7079,6 +7153,15 @@
       </c>
       <c r="AJ19" s="1">
         <v>43802</v>
+      </c>
+      <c r="AK19">
+        <v>94.1</v>
+      </c>
+      <c r="AL19">
+        <v>45.57</v>
+      </c>
+      <c r="AM19">
+        <v>20.704000000000001</v>
       </c>
       <c r="AN19">
         <v>0</v>
@@ -7159,6 +7242,12 @@
       <c r="AK20">
         <v>89.4</v>
       </c>
+      <c r="AL20">
+        <v>51.46</v>
+      </c>
+      <c r="AM20">
+        <v>15.625</v>
+      </c>
       <c r="AN20">
         <v>0</v>
       </c>
@@ -7239,6 +7328,12 @@
       </c>
       <c r="AK21">
         <v>33.9</v>
+      </c>
+      <c r="AL21" s="54">
+        <v>9.06</v>
+      </c>
+      <c r="AM21" s="54">
+        <v>1.3720000000000001</v>
       </c>
     </row>
     <row r="22" spans="1:40">
@@ -7313,6 +7408,15 @@
       <c r="AJ22" s="1">
         <v>43795</v>
       </c>
+      <c r="AK22">
+        <v>105.5</v>
+      </c>
+      <c r="AL22">
+        <v>45.045000000000002</v>
+      </c>
+      <c r="AM22">
+        <v>19.29</v>
+      </c>
       <c r="AN22">
         <v>0</v>
       </c>
@@ -7390,6 +7494,15 @@
       </c>
       <c r="AJ23" s="1">
         <v>43802</v>
+      </c>
+      <c r="AK23">
+        <v>86.7</v>
+      </c>
+      <c r="AL23">
+        <v>46.901000000000003</v>
+      </c>
+      <c r="AM23">
+        <v>17.094000000000001</v>
       </c>
       <c r="AN23">
         <v>0</v>
@@ -7464,6 +7577,12 @@
       <c r="AJ24" s="60">
         <v>43788</v>
       </c>
+      <c r="AL24">
+        <v>41.08</v>
+      </c>
+      <c r="AM24">
+        <v>14.714</v>
+      </c>
       <c r="AN24">
         <v>0</v>
       </c>
@@ -7535,6 +7654,15 @@
       </c>
       <c r="AJ25" s="1">
         <v>43802</v>
+      </c>
+      <c r="AK25">
+        <v>85.6</v>
+      </c>
+      <c r="AL25">
+        <v>32.012</v>
+      </c>
+      <c r="AM25">
+        <v>11.324</v>
       </c>
       <c r="AN25">
         <v>0</v>
@@ -7609,6 +7737,18 @@
       <c r="AH26">
         <v>192</v>
       </c>
+      <c r="AJ26" s="1">
+        <v>43808</v>
+      </c>
+      <c r="AK26">
+        <v>62.3</v>
+      </c>
+      <c r="AL26">
+        <v>28.997</v>
+      </c>
+      <c r="AM26">
+        <v>11.202</v>
+      </c>
       <c r="AN26">
         <v>0</v>
       </c>
@@ -7677,6 +7817,15 @@
       </c>
       <c r="AJ27" s="60">
         <v>43788</v>
+      </c>
+      <c r="AK27">
+        <v>93.5</v>
+      </c>
+      <c r="AL27">
+        <v>28.436</v>
+      </c>
+      <c r="AM27">
+        <v>17.710999999999999</v>
       </c>
       <c r="AN27">
         <v>0</v>
@@ -7754,6 +7903,15 @@
       <c r="AJ28" s="1">
         <v>43802</v>
       </c>
+      <c r="AK28">
+        <v>99.2</v>
+      </c>
+      <c r="AL28">
+        <v>47.604999999999997</v>
+      </c>
+      <c r="AM28">
+        <v>17.161999999999999</v>
+      </c>
       <c r="AN28">
         <v>0</v>
       </c>
@@ -7825,6 +7983,15 @@
       </c>
       <c r="AJ29" s="1">
         <v>43795</v>
+      </c>
+      <c r="AK29">
+        <v>90.7</v>
+      </c>
+      <c r="AL29">
+        <v>51.835999999999999</v>
+      </c>
+      <c r="AM29">
+        <v>17.163599999999999</v>
       </c>
       <c r="AN29">
         <v>0</v>
@@ -7896,6 +8063,15 @@
       <c r="AJ30" s="1">
         <v>43802</v>
       </c>
+      <c r="AK30">
+        <v>86.4</v>
+      </c>
+      <c r="AL30">
+        <v>39.006</v>
+      </c>
+      <c r="AM30">
+        <v>15.47</v>
+      </c>
       <c r="AN30">
         <v>0</v>
       </c>
@@ -7976,6 +8152,12 @@
       </c>
       <c r="AK31">
         <v>32.5</v>
+      </c>
+      <c r="AL31" s="54">
+        <v>4.923</v>
+      </c>
+      <c r="AM31" s="54">
+        <v>1.1919999999999999</v>
       </c>
     </row>
     <row r="32" spans="1:40">
@@ -8044,6 +8226,15 @@
       <c r="AJ32" s="1">
         <v>43802</v>
       </c>
+      <c r="AK32">
+        <v>96.3</v>
+      </c>
+      <c r="AL32" s="54">
+        <v>52.914999999999999</v>
+      </c>
+      <c r="AM32" s="54">
+        <v>27.782</v>
+      </c>
       <c r="AN32">
         <v>0</v>
       </c>
@@ -8115,6 +8306,15 @@
       </c>
       <c r="AJ33" s="1">
         <v>43795</v>
+      </c>
+      <c r="AK33">
+        <v>88.1</v>
+      </c>
+      <c r="AL33" s="54">
+        <v>52.204999999999998</v>
+      </c>
+      <c r="AM33" s="54">
+        <v>28.206</v>
       </c>
       <c r="AN33">
         <v>0</v>
@@ -8368,6 +8568,15 @@
       <c r="AJ36" s="1">
         <v>43795</v>
       </c>
+      <c r="AK36">
+        <v>101.5</v>
+      </c>
+      <c r="AL36">
+        <v>35.659999999999997</v>
+      </c>
+      <c r="AM36">
+        <v>18.07</v>
+      </c>
       <c r="AN36">
         <v>0</v>
       </c>
@@ -8446,8 +8655,14 @@
       <c r="AJ37" s="1">
         <v>43784</v>
       </c>
+      <c r="AK37">
+        <v>71.900000000000006</v>
+      </c>
       <c r="AL37">
-        <v>71.900000000000006</v>
+        <v>50.259</v>
+      </c>
+      <c r="AM37">
+        <v>21.195</v>
       </c>
       <c r="AN37">
         <v>1</v>
@@ -8525,6 +8740,15 @@
       <c r="AJ38" s="1">
         <v>43795</v>
       </c>
+      <c r="AK38">
+        <v>98.7</v>
+      </c>
+      <c r="AL38">
+        <v>27.88</v>
+      </c>
+      <c r="AM38">
+        <v>13.516999999999999</v>
+      </c>
       <c r="AN38">
         <v>0</v>
       </c>
@@ -8602,6 +8826,15 @@
       </c>
       <c r="AJ39" s="60">
         <v>43788</v>
+      </c>
+      <c r="AK39">
+        <v>104.9</v>
+      </c>
+      <c r="AL39">
+        <v>36.222000000000001</v>
+      </c>
+      <c r="AM39">
+        <v>18.007999999999999</v>
       </c>
       <c r="AN39">
         <v>0</v>
@@ -8760,6 +8993,15 @@
       <c r="AJ41" s="60">
         <v>43788</v>
       </c>
+      <c r="AK41">
+        <v>91.3</v>
+      </c>
+      <c r="AL41">
+        <v>42.029000000000003</v>
+      </c>
+      <c r="AM41">
+        <v>28.564</v>
+      </c>
       <c r="AN41">
         <v>0</v>
       </c>
@@ -8830,6 +9072,15 @@
       <c r="AJ42" s="1">
         <v>43795</v>
       </c>
+      <c r="AK42">
+        <v>99.1</v>
+      </c>
+      <c r="AL42">
+        <v>34.15</v>
+      </c>
+      <c r="AM42">
+        <v>26.965</v>
+      </c>
       <c r="AN42">
         <v>0</v>
       </c>
@@ -8984,6 +9235,18 @@
       <c r="AH44">
         <v>192</v>
       </c>
+      <c r="AJ44" s="1">
+        <v>43808</v>
+      </c>
+      <c r="AK44">
+        <v>89.9</v>
+      </c>
+      <c r="AL44">
+        <v>20.965</v>
+      </c>
+      <c r="AM44">
+        <v>11.0282</v>
+      </c>
       <c r="AN44">
         <v>0</v>
       </c>
@@ -9055,6 +9318,15 @@
       </c>
       <c r="AJ45" s="1">
         <v>43802</v>
+      </c>
+      <c r="AK45">
+        <v>78.900000000000006</v>
+      </c>
+      <c r="AL45">
+        <v>39.368000000000002</v>
+      </c>
+      <c r="AM45">
+        <v>12.1286</v>
       </c>
       <c r="AN45">
         <v>0</v>
@@ -9132,6 +9404,15 @@
       <c r="AJ46" s="60">
         <v>43788</v>
       </c>
+      <c r="AK46">
+        <v>100.5</v>
+      </c>
+      <c r="AL46">
+        <v>46.207000000000001</v>
+      </c>
+      <c r="AM46">
+        <v>27.184000000000001</v>
+      </c>
       <c r="AN46">
         <v>0</v>
       </c>
@@ -9283,6 +9564,15 @@
       <c r="AJ48" s="1">
         <v>43802</v>
       </c>
+      <c r="AK48">
+        <v>70.3</v>
+      </c>
+      <c r="AL48">
+        <v>36.29</v>
+      </c>
+      <c r="AM48">
+        <v>13.664</v>
+      </c>
       <c r="AN48">
         <v>0</v>
       </c>
@@ -9355,6 +9645,15 @@
       <c r="AJ49" s="1">
         <v>43795</v>
       </c>
+      <c r="AK49">
+        <v>90.3</v>
+      </c>
+      <c r="AL49">
+        <v>53.326999999999998</v>
+      </c>
+      <c r="AM49">
+        <v>17.728000000000002</v>
+      </c>
       <c r="AN49">
         <v>0</v>
       </c>
@@ -9433,6 +9732,19 @@
       <c r="AI50">
         <v>0.01</v>
       </c>
+      <c r="AJ50" s="1">
+        <v>43802</v>
+      </c>
+      <c r="AK50">
+        <v>90.4</v>
+      </c>
+      <c r="AL50">
+        <v>32.715000000000003</v>
+      </c>
+      <c r="AM50">
+        <f>54.84+29.14</f>
+        <v>83.98</v>
+      </c>
       <c r="AN50">
         <v>0</v>
       </c>
@@ -9512,6 +9824,9 @@
       </c>
       <c r="AI51">
         <v>-0.01</v>
+      </c>
+      <c r="AJ51" s="1">
+        <v>43817</v>
       </c>
       <c r="AN51">
         <v>1</v>
@@ -9591,6 +9906,9 @@
       <c r="AI52">
         <v>0.02</v>
       </c>
+      <c r="AJ52" s="1">
+        <v>43812</v>
+      </c>
       <c r="AN52">
         <v>1</v>
       </c>
@@ -9671,6 +9989,16 @@
       </c>
       <c r="AJ53" s="1">
         <v>43795</v>
+      </c>
+      <c r="AK53">
+        <v>123.3</v>
+      </c>
+      <c r="AL53">
+        <v>40.98</v>
+      </c>
+      <c r="AM53">
+        <f>39.775+34.1529</f>
+        <v>73.927899999999994</v>
       </c>
       <c r="AN53">
         <v>1</v>
@@ -9748,6 +10076,18 @@
       <c r="AI54">
         <v>0.03</v>
       </c>
+      <c r="AJ54" s="1">
+        <v>43810</v>
+      </c>
+      <c r="AK54">
+        <v>88</v>
+      </c>
+      <c r="AL54">
+        <v>26.31</v>
+      </c>
+      <c r="AM54">
+        <v>63.338999999999999</v>
+      </c>
       <c r="AN54">
         <v>0</v>
       </c>
@@ -9825,6 +10165,9 @@
       </c>
       <c r="AI55">
         <v>0.09</v>
+      </c>
+      <c r="AJ55" s="1">
+        <v>43815</v>
       </c>
       <c r="AN55">
         <v>1</v>
@@ -9902,6 +10245,9 @@
       <c r="AI56">
         <v>-0.12</v>
       </c>
+      <c r="AJ56" s="1">
+        <v>43815</v>
+      </c>
       <c r="AN56">
         <v>1</v>
       </c>
@@ -9982,6 +10328,15 @@
       </c>
       <c r="AJ57" s="1">
         <v>43795</v>
+      </c>
+      <c r="AK57">
+        <v>138.1</v>
+      </c>
+      <c r="AL57">
+        <v>28.597000000000001</v>
+      </c>
+      <c r="AM57">
+        <v>54.738999999999997</v>
       </c>
       <c r="AN57">
         <v>0</v>
@@ -10059,6 +10414,9 @@
       <c r="AI58">
         <v>-0.22</v>
       </c>
+      <c r="AJ58" s="1">
+        <v>43819</v>
+      </c>
       <c r="AN58">
         <v>0</v>
       </c>
@@ -10136,6 +10494,18 @@
       </c>
       <c r="AI59">
         <v>0.05</v>
+      </c>
+      <c r="AJ59" s="1">
+        <v>43810</v>
+      </c>
+      <c r="AK59">
+        <v>102</v>
+      </c>
+      <c r="AL59">
+        <v>24.870999999999999</v>
+      </c>
+      <c r="AM59">
+        <v>57.475000000000001</v>
       </c>
       <c r="AN59">
         <v>1</v>
@@ -10212,6 +10582,9 @@
       </c>
       <c r="AI60">
         <v>0.01</v>
+      </c>
+      <c r="AJ60" s="1">
+        <v>43812</v>
       </c>
       <c r="AN60">
         <v>0</v>
@@ -10317,6 +10690,9 @@
       <c r="AI62">
         <v>-0.02</v>
       </c>
+      <c r="AJ62" s="1">
+        <v>43812</v>
+      </c>
       <c r="AN62">
         <v>0</v>
       </c>
@@ -10394,6 +10770,9 @@
       </c>
       <c r="AI63">
         <v>0.02</v>
+      </c>
+      <c r="AJ63" s="1">
+        <v>43815</v>
       </c>
       <c r="AN63">
         <v>1</v>
@@ -10471,6 +10850,9 @@
       <c r="AI64">
         <v>0.05</v>
       </c>
+      <c r="AJ64" s="1">
+        <v>43812</v>
+      </c>
       <c r="AN64">
         <v>0</v>
       </c>
@@ -10549,6 +10931,9 @@
       <c r="AI65">
         <v>0.06</v>
       </c>
+      <c r="AJ65" s="1">
+        <v>43817</v>
+      </c>
       <c r="AN65">
         <v>1</v>
       </c>
@@ -10621,6 +11006,18 @@
       <c r="AH66">
         <v>192</v>
       </c>
+      <c r="AJ66" s="1">
+        <v>43808</v>
+      </c>
+      <c r="AK66">
+        <v>106.7</v>
+      </c>
+      <c r="AL66">
+        <v>36.982999999999997</v>
+      </c>
+      <c r="AM66">
+        <v>52.216999999999999</v>
+      </c>
       <c r="AN66">
         <v>0</v>
       </c>
@@ -10694,6 +11091,9 @@
       </c>
       <c r="AH67">
         <v>192</v>
+      </c>
+      <c r="AJ67" s="1">
+        <v>43812</v>
       </c>
       <c r="AN67">
         <v>0</v>
@@ -10768,6 +11168,9 @@
       <c r="AH68">
         <v>192</v>
       </c>
+      <c r="AJ68" s="1">
+        <v>43808</v>
+      </c>
       <c r="AN68">
         <v>1</v>
       </c>
@@ -10842,6 +11245,18 @@
       </c>
       <c r="AH69">
         <v>192</v>
+      </c>
+      <c r="AJ69" s="1">
+        <v>43804</v>
+      </c>
+      <c r="AK69">
+        <v>80</v>
+      </c>
+      <c r="AL69">
+        <v>23.21</v>
+      </c>
+      <c r="AM69">
+        <v>53.511000000000003</v>
       </c>
       <c r="AN69">
         <v>0</v>
@@ -10916,6 +11331,9 @@
       <c r="AH70">
         <v>192</v>
       </c>
+      <c r="AJ70" s="1">
+        <v>43812</v>
+      </c>
       <c r="AN70">
         <v>0</v>
       </c>
@@ -10990,6 +11408,19 @@
       </c>
       <c r="AH71">
         <v>192</v>
+      </c>
+      <c r="AJ71" s="1">
+        <v>43808</v>
+      </c>
+      <c r="AK71">
+        <v>89.1</v>
+      </c>
+      <c r="AL71">
+        <v>44.048000000000002</v>
+      </c>
+      <c r="AM71">
+        <f>SUM(37.901+29.86)</f>
+        <v>67.760999999999996</v>
       </c>
       <c r="AN71">
         <v>1</v>
@@ -11097,6 +11528,15 @@
       <c r="AJ73" s="1">
         <v>43802</v>
       </c>
+      <c r="AK73">
+        <v>121.7</v>
+      </c>
+      <c r="AL73">
+        <v>29.327000000000002</v>
+      </c>
+      <c r="AM73">
+        <v>56.384999999999998</v>
+      </c>
       <c r="AN73">
         <v>1</v>
       </c>
@@ -11173,6 +11613,15 @@
       <c r="AJ74" s="1">
         <v>43795</v>
       </c>
+      <c r="AK74">
+        <v>113.1</v>
+      </c>
+      <c r="AL74">
+        <v>35.520000000000003</v>
+      </c>
+      <c r="AM74">
+        <v>61.741</v>
+      </c>
       <c r="AN74">
         <v>0</v>
       </c>
@@ -11246,6 +11695,18 @@
       </c>
       <c r="AH75">
         <v>192</v>
+      </c>
+      <c r="AJ75" s="1">
+        <v>43810</v>
+      </c>
+      <c r="AK75">
+        <v>71</v>
+      </c>
+      <c r="AL75">
+        <v>4.5670000000000002</v>
+      </c>
+      <c r="AM75">
+        <v>12.4</v>
       </c>
       <c r="AN75">
         <v>1</v>
@@ -11323,6 +11784,16 @@
       <c r="AJ76" s="1">
         <v>43802</v>
       </c>
+      <c r="AK76">
+        <v>96.4</v>
+      </c>
+      <c r="AL76">
+        <v>34.603000000000002</v>
+      </c>
+      <c r="AM76">
+        <f>32.575+28.582</f>
+        <v>61.157000000000004</v>
+      </c>
       <c r="AN76">
         <v>0</v>
       </c>
@@ -11402,6 +11873,16 @@
       </c>
       <c r="AJ77" s="1">
         <v>43795</v>
+      </c>
+      <c r="AK77">
+        <v>101.1</v>
+      </c>
+      <c r="AL77">
+        <v>31.62</v>
+      </c>
+      <c r="AM77">
+        <f>47.817+27.138</f>
+        <v>74.954999999999998</v>
       </c>
       <c r="AN77">
         <v>1</v>
@@ -11476,6 +11957,9 @@
       <c r="AH78">
         <v>192</v>
       </c>
+      <c r="AJ78" s="1">
+        <v>43812</v>
+      </c>
       <c r="AN78">
         <v>0</v>
       </c>
@@ -11554,8 +12038,15 @@
       <c r="AJ79" s="1">
         <v>43784</v>
       </c>
+      <c r="AK79">
+        <v>58</v>
+      </c>
       <c r="AL79">
-        <v>58</v>
+        <v>39.640999999999998</v>
+      </c>
+      <c r="AM79">
+        <f>30.069+41.965</f>
+        <v>72.034000000000006</v>
       </c>
       <c r="AN79">
         <v>1</v>
@@ -11630,6 +12121,18 @@
       <c r="AH80">
         <v>192</v>
       </c>
+      <c r="AJ80" s="1">
+        <v>43810</v>
+      </c>
+      <c r="AK80">
+        <v>84</v>
+      </c>
+      <c r="AL80">
+        <v>30.963000000000001</v>
+      </c>
+      <c r="AM80">
+        <v>51.052</v>
+      </c>
       <c r="AN80">
         <v>0</v>
       </c>
@@ -11702,6 +12205,22 @@
       <c r="AG81">
         <v>71.2</v>
       </c>
+      <c r="AH81">
+        <v>192</v>
+      </c>
+      <c r="AJ81" s="1">
+        <v>43810</v>
+      </c>
+      <c r="AK81">
+        <v>106</v>
+      </c>
+      <c r="AL81">
+        <v>32.720999999999997</v>
+      </c>
+      <c r="AM81">
+        <f>SUM(42.242+8.694)</f>
+        <v>50.936</v>
+      </c>
       <c r="AN81">
         <v>0</v>
       </c>
@@ -11811,6 +12330,18 @@
       <c r="AH83">
         <v>192</v>
       </c>
+      <c r="AJ83" s="1">
+        <v>43804</v>
+      </c>
+      <c r="AK83">
+        <v>77.8</v>
+      </c>
+      <c r="AL83">
+        <v>32.859000000000002</v>
+      </c>
+      <c r="AM83">
+        <v>55.296999999999997</v>
+      </c>
       <c r="AN83">
         <v>0</v>
       </c>
@@ -11886,6 +12417,9 @@
       <c r="AH84">
         <v>192</v>
       </c>
+      <c r="AJ84" s="1">
+        <v>43819</v>
+      </c>
       <c r="AN84">
         <v>0</v>
       </c>
@@ -11960,6 +12494,9 @@
       </c>
       <c r="AH85">
         <v>192</v>
+      </c>
+      <c r="AJ85" s="1">
+        <v>43812</v>
       </c>
       <c r="AN85">
         <v>0</v>
@@ -12033,6 +12570,9 @@
       </c>
       <c r="AH86">
         <v>192</v>
+      </c>
+      <c r="AJ86" s="1">
+        <v>43812</v>
       </c>
       <c r="AN86">
         <v>0</v>
@@ -12165,6 +12705,18 @@
       <c r="AH89">
         <v>192</v>
       </c>
+      <c r="AJ89" s="1">
+        <v>43808</v>
+      </c>
+      <c r="AK89">
+        <v>145</v>
+      </c>
+      <c r="AL89">
+        <v>32.256</v>
+      </c>
+      <c r="AM89">
+        <v>64.66</v>
+      </c>
       <c r="AN89">
         <v>1</v>
       </c>
@@ -12238,6 +12790,9 @@
       <c r="AH90">
         <v>192</v>
       </c>
+      <c r="AJ90" s="1">
+        <v>43808</v>
+      </c>
       <c r="AN90">
         <v>0</v>
       </c>
@@ -12312,6 +12867,9 @@
       </c>
       <c r="AH91">
         <v>192</v>
+      </c>
+      <c r="AJ91" s="1">
+        <v>43812</v>
       </c>
       <c r="AN91">
         <v>1</v>
@@ -12386,6 +12944,9 @@
       <c r="AH92">
         <v>192</v>
       </c>
+      <c r="AJ92" s="1">
+        <v>43819</v>
+      </c>
       <c r="AN92">
         <v>0</v>
       </c>
@@ -12460,6 +13021,9 @@
       </c>
       <c r="AH93">
         <v>192</v>
+      </c>
+      <c r="AJ93" s="1">
+        <v>43817</v>
       </c>
       <c r="AN93">
         <v>0</v>
@@ -12537,6 +13101,16 @@
       <c r="AJ94" s="1">
         <v>43802</v>
       </c>
+      <c r="AK94">
+        <v>131.1</v>
+      </c>
+      <c r="AL94">
+        <v>40.173000000000002</v>
+      </c>
+      <c r="AM94">
+        <f>SUM(50.256+21.893)</f>
+        <v>72.149000000000001</v>
+      </c>
       <c r="AN94">
         <v>0</v>
       </c>
@@ -12611,6 +13185,18 @@
       </c>
       <c r="AH95">
         <v>192</v>
+      </c>
+      <c r="AJ95" s="1">
+        <v>43810</v>
+      </c>
+      <c r="AK95">
+        <v>90</v>
+      </c>
+      <c r="AL95">
+        <v>38.130000000000003</v>
+      </c>
+      <c r="AM95">
+        <v>64.090999999999994</v>
       </c>
       <c r="AN95">
         <v>0</v>
@@ -12685,6 +13271,18 @@
       <c r="AH96">
         <v>192</v>
       </c>
+      <c r="AJ96" s="1">
+        <v>43810</v>
+      </c>
+      <c r="AK96">
+        <v>112</v>
+      </c>
+      <c r="AL96">
+        <v>31.54</v>
+      </c>
+      <c r="AM96">
+        <v>63.902999999999999</v>
+      </c>
       <c r="AN96">
         <v>0</v>
       </c>
@@ -12760,6 +13358,9 @@
       <c r="AH97">
         <v>192</v>
       </c>
+      <c r="AJ97" s="1">
+        <v>43812</v>
+      </c>
       <c r="AN97">
         <v>1</v>
       </c>
@@ -13319,6 +13920,18 @@
       </c>
       <c r="AI103">
         <v>-0.04</v>
+      </c>
+      <c r="AJ103" s="1">
+        <v>43808</v>
+      </c>
+      <c r="AK103">
+        <v>83.3</v>
+      </c>
+      <c r="AL103">
+        <v>28.085000000000001</v>
+      </c>
+      <c r="AM103">
+        <v>11.177</v>
       </c>
       <c r="AN103">
         <v>1</v>
@@ -13594,6 +14207,18 @@
       <c r="AI106">
         <v>-0.12</v>
       </c>
+      <c r="AJ106" s="1">
+        <v>43808</v>
+      </c>
+      <c r="AK106">
+        <v>82.9</v>
+      </c>
+      <c r="AL106">
+        <v>33.956000000000003</v>
+      </c>
+      <c r="AM106">
+        <v>14.358700000000001</v>
+      </c>
       <c r="AN106">
         <v>0</v>
       </c>
@@ -13675,6 +14300,15 @@
       <c r="AJ107" s="1">
         <v>43795</v>
       </c>
+      <c r="AK107">
+        <v>77.5</v>
+      </c>
+      <c r="AL107">
+        <v>24.992000000000001</v>
+      </c>
+      <c r="AM107">
+        <v>10.414999999999999</v>
+      </c>
       <c r="AN107">
         <v>1</v>
       </c>
@@ -13769,6 +14403,12 @@
       </c>
       <c r="AK108">
         <v>95.2</v>
+      </c>
+      <c r="AL108">
+        <v>35.116</v>
+      </c>
+      <c r="AM108">
+        <v>17.396999999999998</v>
       </c>
       <c r="AN108">
         <v>0</v>
@@ -13937,7 +14577,16 @@
         <v>-0.06</v>
       </c>
       <c r="AJ110" s="1">
-        <v>43802</v>
+        <v>43808</v>
+      </c>
+      <c r="AK110">
+        <v>55.7</v>
+      </c>
+      <c r="AL110">
+        <v>27.004999999999999</v>
+      </c>
+      <c r="AM110">
+        <v>8.1170000000000009</v>
       </c>
       <c r="AN110">
         <v>1</v>
@@ -14108,6 +14757,15 @@
       <c r="AJ112" s="1">
         <v>43802</v>
       </c>
+      <c r="AK112">
+        <v>79.5</v>
+      </c>
+      <c r="AL112">
+        <v>25.321000000000002</v>
+      </c>
+      <c r="AM112">
+        <v>8.8490000000000002</v>
+      </c>
       <c r="AN112">
         <v>0</v>
       </c>
@@ -14275,6 +14933,18 @@
       <c r="AH114">
         <v>192</v>
       </c>
+      <c r="AJ114" s="1">
+        <v>43804</v>
+      </c>
+      <c r="AK114">
+        <v>121.4</v>
+      </c>
+      <c r="AL114">
+        <v>42.174999999999997</v>
+      </c>
+      <c r="AM114">
+        <v>19.635000000000002</v>
+      </c>
       <c r="AN114">
         <v>0</v>
       </c>
@@ -14352,6 +15022,15 @@
       </c>
       <c r="AJ115" s="60">
         <v>43788</v>
+      </c>
+      <c r="AK115">
+        <v>79.900000000000006</v>
+      </c>
+      <c r="AL115">
+        <v>30.548999999999999</v>
+      </c>
+      <c r="AM115">
+        <v>8.0570000000000004</v>
       </c>
       <c r="AN115">
         <v>0</v>
@@ -14426,6 +15105,18 @@
       <c r="AH116">
         <v>192</v>
       </c>
+      <c r="AJ116" s="1">
+        <v>43808</v>
+      </c>
+      <c r="AK116">
+        <v>115.1</v>
+      </c>
+      <c r="AL116">
+        <v>22.882000000000001</v>
+      </c>
+      <c r="AM116">
+        <v>15.782999999999999</v>
+      </c>
       <c r="AN116">
         <v>0</v>
       </c>
@@ -14503,6 +15194,15 @@
       </c>
       <c r="AJ117" s="60">
         <v>43788</v>
+      </c>
+      <c r="AK117">
+        <v>42.2</v>
+      </c>
+      <c r="AL117">
+        <v>16.234000000000002</v>
+      </c>
+      <c r="AM117">
+        <v>4.0250000000000004</v>
       </c>
       <c r="AN117">
         <v>1</v>
@@ -15172,6 +15872,18 @@
       <c r="AH125">
         <v>192</v>
       </c>
+      <c r="AJ125" s="1">
+        <v>43812</v>
+      </c>
+      <c r="AK125" s="59">
+        <v>130.6</v>
+      </c>
+      <c r="AL125" s="59">
+        <v>26.45</v>
+      </c>
+      <c r="AM125" s="59">
+        <v>21.797000000000001</v>
+      </c>
       <c r="AN125">
         <v>0</v>
       </c>
@@ -15248,6 +15960,15 @@
       <c r="AJ126" s="1">
         <v>43802</v>
       </c>
+      <c r="AK126">
+        <v>89.1</v>
+      </c>
+      <c r="AL126">
+        <v>24.364999999999998</v>
+      </c>
+      <c r="AM126">
+        <v>11.7904</v>
+      </c>
       <c r="AN126">
         <v>0</v>
       </c>
@@ -15325,6 +16046,15 @@
       </c>
       <c r="AJ127" s="1">
         <v>43795</v>
+      </c>
+      <c r="AK127">
+        <v>76.400000000000006</v>
+      </c>
+      <c r="AL127">
+        <v>34.853999999999999</v>
+      </c>
+      <c r="AM127">
+        <v>8.1319999999999997</v>
       </c>
       <c r="AN127">
         <v>0</v>
@@ -15399,6 +16129,18 @@
       <c r="AH128">
         <v>192</v>
       </c>
+      <c r="AJ128" s="1">
+        <v>43808</v>
+      </c>
+      <c r="AK128">
+        <v>55.6</v>
+      </c>
+      <c r="AL128">
+        <v>8.7089999999999996</v>
+      </c>
+      <c r="AM128">
+        <v>3.169</v>
+      </c>
       <c r="AN128">
         <v>0</v>
       </c>
@@ -15474,6 +16216,18 @@
       <c r="AH129">
         <v>192</v>
       </c>
+      <c r="AJ129" s="1">
+        <v>43804</v>
+      </c>
+      <c r="AK129">
+        <v>54.3</v>
+      </c>
+      <c r="AL129">
+        <v>14.672000000000001</v>
+      </c>
+      <c r="AM129">
+        <v>4.2229999999999999</v>
+      </c>
       <c r="AN129">
         <v>0</v>
       </c>
@@ -15552,6 +16306,15 @@
       <c r="AJ130" s="1">
         <v>43795</v>
       </c>
+      <c r="AK130">
+        <v>85.5</v>
+      </c>
+      <c r="AL130">
+        <v>47.933999999999997</v>
+      </c>
+      <c r="AM130">
+        <v>12.968</v>
+      </c>
       <c r="AN130">
         <v>0</v>
       </c>
@@ -15716,6 +16479,9 @@
       <c r="AH132">
         <v>192</v>
       </c>
+      <c r="AJ132" s="1">
+        <v>43815</v>
+      </c>
       <c r="AN132">
         <v>0</v>
       </c>
@@ -15790,6 +16556,18 @@
       </c>
       <c r="AH133">
         <v>192</v>
+      </c>
+      <c r="AJ133" s="1">
+        <v>43788</v>
+      </c>
+      <c r="AK133">
+        <v>90.8</v>
+      </c>
+      <c r="AL133">
+        <v>41.335999999999999</v>
+      </c>
+      <c r="AM133">
+        <v>15.704000000000001</v>
       </c>
       <c r="AN133">
         <v>0</v>
@@ -15867,8 +16645,11 @@
       <c r="AJ134" s="1">
         <v>43707</v>
       </c>
-      <c r="AL134">
+      <c r="AL134" s="54">
         <v>9.1739999999999995</v>
+      </c>
+      <c r="AM134" s="54">
+        <v>6.76</v>
       </c>
     </row>
     <row r="135" spans="1:40">
@@ -15941,6 +16722,18 @@
       </c>
       <c r="AH135">
         <v>192</v>
+      </c>
+      <c r="AJ135" s="1">
+        <v>43804</v>
+      </c>
+      <c r="AK135">
+        <v>78.400000000000006</v>
+      </c>
+      <c r="AL135" s="54">
+        <v>24.734000000000002</v>
+      </c>
+      <c r="AM135" s="54">
+        <v>14.427</v>
       </c>
       <c r="AN135">
         <v>1</v>
@@ -16021,6 +16814,12 @@
       <c r="AK136">
         <v>79.099999999999994</v>
       </c>
+      <c r="AL136" s="54">
+        <v>19.748999999999999</v>
+      </c>
+      <c r="AM136" s="54">
+        <v>7.3310000000000004</v>
+      </c>
       <c r="AN136">
         <v>0</v>
       </c>
@@ -16098,6 +16897,15 @@
       </c>
       <c r="AJ137" s="1">
         <v>43802</v>
+      </c>
+      <c r="AK137">
+        <v>82</v>
+      </c>
+      <c r="AL137" s="54">
+        <v>46.158000000000001</v>
+      </c>
+      <c r="AM137" s="54">
+        <v>13.629</v>
       </c>
       <c r="AN137">
         <v>1</v>
@@ -16338,6 +17146,18 @@
       <c r="AH140">
         <v>192</v>
       </c>
+      <c r="AJ140" s="1">
+        <v>43808</v>
+      </c>
+      <c r="AK140">
+        <v>81</v>
+      </c>
+      <c r="AL140">
+        <v>28.7</v>
+      </c>
+      <c r="AM140" s="58">
+        <v>13.82</v>
+      </c>
       <c r="AN140">
         <v>1</v>
       </c>
@@ -16415,6 +17235,15 @@
       </c>
       <c r="AJ141" s="1">
         <v>43802</v>
+      </c>
+      <c r="AK141">
+        <v>103.9</v>
+      </c>
+      <c r="AL141">
+        <v>35.567</v>
+      </c>
+      <c r="AM141">
+        <v>19.741</v>
       </c>
       <c r="AN141">
         <v>1</v>
@@ -16581,6 +17410,12 @@
       <c r="AK143">
         <v>48.1</v>
       </c>
+      <c r="AL143">
+        <v>20.939</v>
+      </c>
+      <c r="AM143" s="58">
+        <v>7.4160000000000004</v>
+      </c>
       <c r="AN143">
         <v>1</v>
       </c>
@@ -16660,6 +17495,12 @@
       <c r="AK144">
         <v>92.5</v>
       </c>
+      <c r="AL144">
+        <v>29.396000000000001</v>
+      </c>
+      <c r="AM144" s="58">
+        <v>16.510999999999999</v>
+      </c>
       <c r="AN144">
         <v>0</v>
       </c>
@@ -16735,6 +17576,9 @@
       <c r="AH145">
         <v>192</v>
       </c>
+      <c r="AJ145" s="1">
+        <v>43815</v>
+      </c>
       <c r="AN145">
         <v>0</v>
       </c>
@@ -16819,6 +17663,12 @@
       <c r="AK146">
         <v>105.9</v>
       </c>
+      <c r="AL146">
+        <v>36.939</v>
+      </c>
+      <c r="AM146">
+        <v>22.279</v>
+      </c>
       <c r="AN146">
         <v>0</v>
       </c>
@@ -16900,6 +17750,9 @@
       <c r="AJ147" s="1">
         <v>43795</v>
       </c>
+      <c r="AK147" s="61"/>
+      <c r="AL147" s="59"/>
+      <c r="AM147" s="59"/>
       <c r="AN147">
         <v>0</v>
       </c>
@@ -16979,6 +17832,15 @@
       <c r="AJ148" s="1">
         <v>43795</v>
       </c>
+      <c r="AK148" s="1">
+        <v>104.5</v>
+      </c>
+      <c r="AL148">
+        <v>37.536000000000001</v>
+      </c>
+      <c r="AM148">
+        <v>19.337</v>
+      </c>
       <c r="AN148">
         <v>0</v>
       </c>
@@ -17061,6 +17923,15 @@
       </c>
       <c r="AJ149" s="1">
         <v>43802</v>
+      </c>
+      <c r="AK149">
+        <v>123.4</v>
+      </c>
+      <c r="AL149">
+        <v>28.774999999999999</v>
+      </c>
+      <c r="AM149">
+        <v>17.116900000000001</v>
       </c>
       <c r="AN149">
         <v>0</v>
@@ -17141,6 +18012,15 @@
       <c r="AJ150" s="1">
         <v>43788</v>
       </c>
+      <c r="AK150">
+        <v>122.7</v>
+      </c>
+      <c r="AL150">
+        <v>43.746000000000002</v>
+      </c>
+      <c r="AM150">
+        <v>18.969000000000001</v>
+      </c>
       <c r="AN150">
         <v>0</v>
       </c>
@@ -17221,6 +18101,15 @@
       </c>
       <c r="AJ151" s="1">
         <v>43795</v>
+      </c>
+      <c r="AK151">
+        <v>107.7</v>
+      </c>
+      <c r="AL151">
+        <v>37.08</v>
+      </c>
+      <c r="AM151">
+        <v>18.968</v>
       </c>
       <c r="AN151">
         <v>0</v>
@@ -17301,6 +18190,15 @@
       <c r="AJ152" s="1">
         <v>43795</v>
       </c>
+      <c r="AK152">
+        <v>107</v>
+      </c>
+      <c r="AL152">
+        <v>35.99</v>
+      </c>
+      <c r="AM152">
+        <v>15.005000000000001</v>
+      </c>
       <c r="AN152">
         <v>0</v>
       </c>
@@ -17381,6 +18279,15 @@
       </c>
       <c r="AJ153" s="1">
         <v>43802</v>
+      </c>
+      <c r="AK153">
+        <v>153.80000000000001</v>
+      </c>
+      <c r="AL153">
+        <v>31.33</v>
+      </c>
+      <c r="AM153">
+        <v>27.158999999999999</v>
       </c>
       <c r="AN153">
         <v>0</v>
@@ -17461,6 +18368,15 @@
       <c r="AJ154" s="1">
         <v>43802</v>
       </c>
+      <c r="AK154">
+        <v>118</v>
+      </c>
+      <c r="AL154">
+        <v>36.923999999999999</v>
+      </c>
+      <c r="AM154">
+        <v>17.27</v>
+      </c>
       <c r="AN154">
         <v>0</v>
       </c>
@@ -17538,6 +18454,18 @@
       </c>
       <c r="AI155">
         <v>0.01</v>
+      </c>
+      <c r="AJ155" s="1">
+        <v>43808</v>
+      </c>
+      <c r="AK155">
+        <v>137.9</v>
+      </c>
+      <c r="AL155">
+        <v>27.434000000000001</v>
+      </c>
+      <c r="AM155">
+        <v>21.846</v>
       </c>
       <c r="AN155">
         <v>0</v>
@@ -17618,6 +18546,15 @@
       <c r="AJ156" s="1">
         <v>43802</v>
       </c>
+      <c r="AK156">
+        <v>123.9</v>
+      </c>
+      <c r="AL156">
+        <v>33.106000000000002</v>
+      </c>
+      <c r="AM156">
+        <v>17.760000000000002</v>
+      </c>
       <c r="AN156">
         <v>0</v>
       </c>
@@ -17695,6 +18632,9 @@
       </c>
       <c r="AI157">
         <v>0.05</v>
+      </c>
+      <c r="AJ157" s="1">
+        <v>43817</v>
       </c>
       <c r="AN157">
         <v>0</v>
@@ -17772,6 +18712,18 @@
       <c r="AI158">
         <v>0.04</v>
       </c>
+      <c r="AJ158" s="1">
+        <v>43802</v>
+      </c>
+      <c r="AK158">
+        <v>128</v>
+      </c>
+      <c r="AL158">
+        <v>31.32</v>
+      </c>
+      <c r="AM158">
+        <v>18.975000000000001</v>
+      </c>
       <c r="AN158">
         <v>0</v>
       </c>
@@ -17852,6 +18804,15 @@
       </c>
       <c r="AJ159" s="1">
         <v>43802</v>
+      </c>
+      <c r="AK159">
+        <v>125.2</v>
+      </c>
+      <c r="AL159">
+        <v>50.411999999999999</v>
+      </c>
+      <c r="AM159">
+        <v>23.645</v>
       </c>
       <c r="AN159">
         <v>0</v>
@@ -17932,6 +18893,15 @@
       <c r="AJ160" s="1">
         <v>43802</v>
       </c>
+      <c r="AK160">
+        <v>126.7</v>
+      </c>
+      <c r="AL160">
+        <v>40.091000000000001</v>
+      </c>
+      <c r="AM160">
+        <v>26.504999999999999</v>
+      </c>
       <c r="AN160">
         <v>0</v>
       </c>
@@ -18013,6 +18983,15 @@
       <c r="AJ161" s="1">
         <v>43795</v>
       </c>
+      <c r="AK161">
+        <v>79.2</v>
+      </c>
+      <c r="AL161">
+        <v>36.814999999999998</v>
+      </c>
+      <c r="AM161">
+        <v>17.047999999999998</v>
+      </c>
       <c r="AN161">
         <v>0</v>
       </c>
@@ -18088,6 +19067,12 @@
       <c r="AH162">
         <v>192</v>
       </c>
+      <c r="AJ162" s="1">
+        <v>43812</v>
+      </c>
+      <c r="AK162" s="62"/>
+      <c r="AL162" s="62"/>
+      <c r="AM162" s="62"/>
       <c r="AN162">
         <v>0</v>
       </c>
@@ -18162,6 +19147,18 @@
       </c>
       <c r="AH163">
         <v>192</v>
+      </c>
+      <c r="AJ163" s="1">
+        <v>43808</v>
+      </c>
+      <c r="AK163">
+        <v>132.1</v>
+      </c>
+      <c r="AL163">
+        <v>17.161000000000001</v>
+      </c>
+      <c r="AM163">
+        <v>14.278</v>
       </c>
       <c r="AN163">
         <v>0</v>
@@ -18236,6 +19233,9 @@
       <c r="AH164">
         <v>192</v>
       </c>
+      <c r="AJ164" s="1">
+        <v>43812</v>
+      </c>
       <c r="AN164">
         <v>1</v>
       </c>
@@ -18310,6 +19310,18 @@
       </c>
       <c r="AH165">
         <v>192</v>
+      </c>
+      <c r="AJ165" s="1">
+        <v>43804</v>
+      </c>
+      <c r="AK165">
+        <v>119.7</v>
+      </c>
+      <c r="AL165">
+        <v>43.22</v>
+      </c>
+      <c r="AM165">
+        <v>22.923999999999999</v>
       </c>
       <c r="AN165">
         <v>1</v>
@@ -18387,6 +19399,15 @@
       <c r="AJ166" s="1">
         <v>43802</v>
       </c>
+      <c r="AK166">
+        <v>141.1</v>
+      </c>
+      <c r="AL166">
+        <v>34.098999999999997</v>
+      </c>
+      <c r="AM166">
+        <v>17.491</v>
+      </c>
       <c r="AN166">
         <v>0</v>
       </c>
@@ -18464,6 +19485,15 @@
       </c>
       <c r="AJ167" s="1">
         <v>43802</v>
+      </c>
+      <c r="AK167">
+        <v>136.30000000000001</v>
+      </c>
+      <c r="AL167">
+        <v>27.215</v>
+      </c>
+      <c r="AM167">
+        <v>18.605</v>
       </c>
       <c r="AN167">
         <v>1</v>
@@ -18538,6 +19568,9 @@
       <c r="AH168">
         <v>192</v>
       </c>
+      <c r="AJ168" s="1">
+        <v>43812</v>
+      </c>
       <c r="AN168">
         <v>0</v>
       </c>
@@ -18615,6 +19648,15 @@
       </c>
       <c r="AJ169" s="1">
         <v>43802</v>
+      </c>
+      <c r="AK169">
+        <v>105</v>
+      </c>
+      <c r="AL169">
+        <v>36.484000000000002</v>
+      </c>
+      <c r="AM169">
+        <v>21.888000000000002</v>
       </c>
       <c r="AN169">
         <v>0</v>
@@ -18695,6 +19737,12 @@
       <c r="AK170">
         <v>94.2</v>
       </c>
+      <c r="AL170">
+        <v>24.484000000000002</v>
+      </c>
+      <c r="AM170">
+        <v>26.373999999999999</v>
+      </c>
       <c r="AN170">
         <v>0</v>
       </c>
@@ -18769,6 +19817,18 @@
       </c>
       <c r="AH171">
         <v>192</v>
+      </c>
+      <c r="AJ171" s="1">
+        <v>43810</v>
+      </c>
+      <c r="AK171" s="59">
+        <v>135</v>
+      </c>
+      <c r="AL171" s="59">
+        <v>39.110999999999997</v>
+      </c>
+      <c r="AM171" s="59">
+        <v>26.13</v>
       </c>
       <c r="AN171">
         <v>1</v>
@@ -18843,6 +19903,18 @@
       <c r="AH172">
         <v>192</v>
       </c>
+      <c r="AJ172" s="1">
+        <v>43804</v>
+      </c>
+      <c r="AK172">
+        <v>110.4</v>
+      </c>
+      <c r="AL172">
+        <v>49.71</v>
+      </c>
+      <c r="AM172">
+        <v>18.116</v>
+      </c>
       <c r="AN172">
         <v>0</v>
       </c>
@@ -18919,7 +19991,16 @@
         <v>192</v>
       </c>
       <c r="AJ173" s="1">
-        <v>43795</v>
+        <v>43808</v>
+      </c>
+      <c r="AK173">
+        <v>116.5</v>
+      </c>
+      <c r="AL173">
+        <v>34.225000000000001</v>
+      </c>
+      <c r="AM173">
+        <v>20.355</v>
       </c>
       <c r="AN173">
         <v>1</v>
@@ -18997,6 +20078,15 @@
       <c r="AJ174" s="1">
         <v>43795</v>
       </c>
+      <c r="AK174">
+        <v>100.8</v>
+      </c>
+      <c r="AL174">
+        <v>38.984999999999999</v>
+      </c>
+      <c r="AM174">
+        <v>14.478999999999999</v>
+      </c>
       <c r="AN174">
         <v>0</v>
       </c>
@@ -19074,6 +20164,15 @@
       </c>
       <c r="AJ175" s="1">
         <v>43802</v>
+      </c>
+      <c r="AK175">
+        <v>114.7</v>
+      </c>
+      <c r="AL175">
+        <v>49.220999999999997</v>
+      </c>
+      <c r="AM175">
+        <v>22.003</v>
       </c>
       <c r="AN175">
         <v>0</v>
@@ -19151,6 +20250,15 @@
       <c r="AJ176" s="1">
         <v>43802</v>
       </c>
+      <c r="AK176">
+        <v>147.30000000000001</v>
+      </c>
+      <c r="AL176">
+        <v>47.116999999999997</v>
+      </c>
+      <c r="AM176">
+        <v>36.427</v>
+      </c>
       <c r="AN176">
         <v>0</v>
       </c>
@@ -19229,6 +20337,15 @@
       <c r="AJ177" s="1">
         <v>43795</v>
       </c>
+      <c r="AK177">
+        <v>116</v>
+      </c>
+      <c r="AL177">
+        <v>39.893999999999998</v>
+      </c>
+      <c r="AM177">
+        <v>13.89</v>
+      </c>
       <c r="AN177">
         <v>0</v>
       </c>
@@ -19304,6 +20421,18 @@
       <c r="AH178">
         <v>192</v>
       </c>
+      <c r="AJ178" s="1">
+        <v>43819</v>
+      </c>
+      <c r="AK178">
+        <v>116</v>
+      </c>
+      <c r="AL178">
+        <v>39.893999999999998</v>
+      </c>
+      <c r="AM178">
+        <v>13.89</v>
+      </c>
       <c r="AN178">
         <v>0</v>
       </c>
@@ -19380,6 +20509,9 @@
       </c>
       <c r="AH179">
         <v>192</v>
+      </c>
+      <c r="AJ179" s="1">
+        <v>43815</v>
       </c>
       <c r="AN179">
         <v>0</v>
@@ -19454,6 +20586,9 @@
       <c r="AH180">
         <v>192</v>
       </c>
+      <c r="AJ180" s="1">
+        <v>43812</v>
+      </c>
       <c r="AN180">
         <v>1</v>
       </c>
@@ -19530,7 +20665,16 @@
         <v>192</v>
       </c>
       <c r="AJ181" s="60">
-        <v>43788</v>
+        <v>43804</v>
+      </c>
+      <c r="AK181">
+        <v>129.1</v>
+      </c>
+      <c r="AL181">
+        <v>33.32</v>
+      </c>
+      <c r="AM181">
+        <v>26.06</v>
       </c>
       <c r="AN181">
         <v>0</v>
@@ -19611,6 +20755,12 @@
       <c r="AK182">
         <v>129.69999999999999</v>
       </c>
+      <c r="AL182">
+        <v>31.265000000000001</v>
+      </c>
+      <c r="AM182">
+        <v>20.396999999999998</v>
+      </c>
       <c r="AN182">
         <v>0</v>
       </c>
@@ -19685,6 +20835,18 @@
       </c>
       <c r="AH183">
         <v>192</v>
+      </c>
+      <c r="AJ183" s="1">
+        <v>43804</v>
+      </c>
+      <c r="AK183">
+        <v>135.30000000000001</v>
+      </c>
+      <c r="AL183">
+        <v>47.655999999999999</v>
+      </c>
+      <c r="AM183">
+        <v>28.49</v>
       </c>
       <c r="AN183">
         <v>0</v>
@@ -19759,6 +20921,9 @@
       <c r="AH184">
         <v>192</v>
       </c>
+      <c r="AJ184" s="1">
+        <v>43815</v>
+      </c>
       <c r="AN184">
         <v>0</v>
       </c>
@@ -19833,6 +20998,18 @@
       </c>
       <c r="AH185">
         <v>192</v>
+      </c>
+      <c r="AJ185" s="1">
+        <v>43810</v>
+      </c>
+      <c r="AK185" s="59">
+        <v>135</v>
+      </c>
+      <c r="AL185" s="59">
+        <v>39.110999999999997</v>
+      </c>
+      <c r="AM185" s="59">
+        <v>26.13</v>
       </c>
       <c r="AN185">
         <v>0</v>
@@ -19907,6 +21084,9 @@
       <c r="AH186">
         <v>192</v>
       </c>
+      <c r="AJ186" s="61">
+        <v>43802</v>
+      </c>
       <c r="AN186">
         <v>0</v>
       </c>
@@ -19984,6 +21164,15 @@
       </c>
       <c r="AJ187" s="1">
         <v>43802</v>
+      </c>
+      <c r="AK187">
+        <v>102.6</v>
+      </c>
+      <c r="AL187">
+        <v>38.308999999999997</v>
+      </c>
+      <c r="AM187">
+        <v>17.498000000000001</v>
       </c>
       <c r="AN187">
         <v>0</v>
@@ -20058,6 +21247,9 @@
       <c r="AH188">
         <v>192</v>
       </c>
+      <c r="AJ188" s="1">
+        <v>43812</v>
+      </c>
       <c r="AN188">
         <v>0</v>
       </c>
@@ -20132,6 +21324,9 @@
       </c>
       <c r="AH189">
         <v>192</v>
+      </c>
+      <c r="AJ189" s="61">
+        <v>43795</v>
       </c>
       <c r="AN189">
         <v>0</v>
@@ -20206,6 +21401,9 @@
       <c r="AH190">
         <v>192</v>
       </c>
+      <c r="AJ190" s="1">
+        <v>43815</v>
+      </c>
       <c r="AN190">
         <v>0</v>
       </c>
@@ -20283,6 +21481,15 @@
       </c>
       <c r="AJ191" s="60">
         <v>43788</v>
+      </c>
+      <c r="AK191">
+        <v>108.1</v>
+      </c>
+      <c r="AL191">
+        <v>32.243000000000002</v>
+      </c>
+      <c r="AM191">
+        <v>18.350000000000001</v>
       </c>
       <c r="AN191">
         <v>0</v>
@@ -20357,6 +21564,18 @@
       <c r="AH192">
         <v>192</v>
       </c>
+      <c r="AJ192" s="1">
+        <v>43802</v>
+      </c>
+      <c r="AK192">
+        <v>129.30000000000001</v>
+      </c>
+      <c r="AL192">
+        <v>40.254800000000003</v>
+      </c>
+      <c r="AM192">
+        <v>27.907</v>
+      </c>
       <c r="AN192">
         <v>0</v>
       </c>
@@ -20431,6 +21650,18 @@
       </c>
       <c r="AH193">
         <v>192</v>
+      </c>
+      <c r="AJ193" s="1">
+        <v>43804</v>
+      </c>
+      <c r="AK193">
+        <v>143</v>
+      </c>
+      <c r="AL193">
+        <v>36.539000000000001</v>
+      </c>
+      <c r="AM193">
+        <v>17.591000000000001</v>
       </c>
       <c r="AN193">
         <v>0</v>
@@ -22833,6 +24064,15 @@
       <c r="AJ220" s="1">
         <v>43795</v>
       </c>
+      <c r="AK220">
+        <v>78.099999999999994</v>
+      </c>
+      <c r="AL220">
+        <v>37.579000000000001</v>
+      </c>
+      <c r="AM220">
+        <v>18.972000000000001</v>
+      </c>
       <c r="AN220">
         <v>1</v>
       </c>
@@ -22990,6 +24230,15 @@
       <c r="AJ222" s="1">
         <v>43795</v>
       </c>
+      <c r="AK222">
+        <v>94</v>
+      </c>
+      <c r="AL222">
+        <v>45.377000000000002</v>
+      </c>
+      <c r="AM222">
+        <v>11.895</v>
+      </c>
       <c r="AN222">
         <v>0</v>
       </c>
@@ -24001,6 +25250,12 @@
       </c>
       <c r="AK234">
         <v>90.1</v>
+      </c>
+      <c r="AL234">
+        <v>40.945</v>
+      </c>
+      <c r="AM234" s="58">
+        <v>18.376000000000001</v>
       </c>
       <c r="AN234">
         <v>1</v>
@@ -27711,7 +28966,9 @@
       <c r="AI338">
         <v>-0.03</v>
       </c>
-      <c r="AJ338" s="1"/>
+      <c r="AJ338" s="1">
+        <v>43817</v>
+      </c>
       <c r="AN338">
         <v>1</v>
       </c>
@@ -27810,6 +29067,9 @@
       </c>
       <c r="AI339">
         <v>-0.11</v>
+      </c>
+      <c r="AJ339" s="1">
+        <v>43815</v>
       </c>
       <c r="AN339">
         <v>1</v>
@@ -27903,6 +29163,15 @@
       <c r="AJ340" s="60">
         <v>43788</v>
       </c>
+      <c r="AK340">
+        <v>159.80000000000001</v>
+      </c>
+      <c r="AL340">
+        <v>60.844000000000001</v>
+      </c>
+      <c r="AM340">
+        <v>47.293999999999997</v>
+      </c>
       <c r="AN340">
         <v>0</v>
       </c>
@@ -27993,6 +29262,9 @@
       </c>
       <c r="AI341">
         <v>0.01</v>
+      </c>
+      <c r="AJ341" s="1">
+        <v>43812</v>
       </c>
       <c r="AN341">
         <v>0</v>
@@ -28290,6 +29562,15 @@
       <c r="AJ344" s="60">
         <v>43788</v>
       </c>
+      <c r="AK344">
+        <v>164.4</v>
+      </c>
+      <c r="AL344">
+        <v>50.744999999999997</v>
+      </c>
+      <c r="AM344">
+        <v>33.097999999999999</v>
+      </c>
       <c r="AN344">
         <v>1</v>
       </c>
@@ -28380,6 +29661,9 @@
       </c>
       <c r="AI345">
         <v>-0.05</v>
+      </c>
+      <c r="AJ345" s="1">
+        <v>43812</v>
       </c>
       <c r="AN345">
         <v>1</v>
@@ -28473,6 +29757,12 @@
       <c r="AJ346" s="1">
         <v>43795</v>
       </c>
+      <c r="AL346">
+        <v>44.975000000000001</v>
+      </c>
+      <c r="AM346">
+        <v>30.506</v>
+      </c>
       <c r="AN346">
         <v>0</v>
       </c>
@@ -28566,6 +29856,15 @@
       </c>
       <c r="AJ347" s="1">
         <v>43802</v>
+      </c>
+      <c r="AK347">
+        <v>138</v>
+      </c>
+      <c r="AL347">
+        <v>63.503</v>
+      </c>
+      <c r="AM347">
+        <v>28.75</v>
       </c>
       <c r="AN347">
         <v>0</v>
@@ -28656,6 +29955,18 @@
       <c r="AI348">
         <v>-0.11</v>
       </c>
+      <c r="AJ348" s="1">
+        <v>43808</v>
+      </c>
+      <c r="AK348">
+        <v>163.9</v>
+      </c>
+      <c r="AL348">
+        <v>32.470999999999997</v>
+      </c>
+      <c r="AM348">
+        <v>24.41</v>
+      </c>
       <c r="AN348">
         <v>1</v>
       </c>
@@ -28746,6 +30057,18 @@
       </c>
       <c r="AI349">
         <v>-0.03</v>
+      </c>
+      <c r="AJ349" s="1">
+        <v>43808</v>
+      </c>
+      <c r="AK349">
+        <v>172.3</v>
+      </c>
+      <c r="AL349">
+        <v>37.972000000000001</v>
+      </c>
+      <c r="AM349">
+        <v>31.768000000000001</v>
       </c>
       <c r="AN349">
         <v>1</v>
@@ -28836,6 +30159,9 @@
       <c r="AI350">
         <v>-0.05</v>
       </c>
+      <c r="AJ350" s="1">
+        <v>43812</v>
+      </c>
       <c r="AN350">
         <v>0</v>
       </c>
@@ -28934,6 +30260,12 @@
       </c>
       <c r="AK351">
         <v>139.5</v>
+      </c>
+      <c r="AL351">
+        <v>43.264000000000003</v>
+      </c>
+      <c r="AM351">
+        <v>30.239000000000001</v>
       </c>
       <c r="AN351">
         <v>1</v>
@@ -29026,6 +30358,15 @@
       </c>
       <c r="AJ352" s="1">
         <v>43802</v>
+      </c>
+      <c r="AK352">
+        <v>180.1</v>
+      </c>
+      <c r="AL352">
+        <v>65.947000000000003</v>
+      </c>
+      <c r="AM352">
+        <v>44.816000000000003</v>
       </c>
       <c r="AN352">
         <v>1</v>
@@ -29108,6 +30449,15 @@
       <c r="AJ353" s="1">
         <v>43802</v>
       </c>
+      <c r="AK353">
+        <v>176.7</v>
+      </c>
+      <c r="AL353">
+        <v>64.632999999999996</v>
+      </c>
+      <c r="AM353">
+        <v>32.960999999999999</v>
+      </c>
       <c r="AN353">
         <v>1</v>
       </c>
@@ -29182,6 +30532,18 @@
       </c>
       <c r="AH354">
         <v>191</v>
+      </c>
+      <c r="AJ354" s="1">
+        <v>43804</v>
+      </c>
+      <c r="AK354">
+        <v>157.9</v>
+      </c>
+      <c r="AL354">
+        <v>43.503</v>
+      </c>
+      <c r="AM354">
+        <v>41.232999999999997</v>
       </c>
       <c r="AN354">
         <v>0</v>
@@ -29343,6 +30705,9 @@
       <c r="AH356">
         <v>191</v>
       </c>
+      <c r="AJ356" s="1">
+        <v>43815</v>
+      </c>
       <c r="AN356">
         <v>0</v>
       </c>
@@ -29506,6 +30871,15 @@
       <c r="AJ358" s="1">
         <v>43795</v>
       </c>
+      <c r="AK358">
+        <v>154.69999999999999</v>
+      </c>
+      <c r="AL358">
+        <v>32.664999999999999</v>
+      </c>
+      <c r="AM358">
+        <v>29.33</v>
+      </c>
       <c r="AN358">
         <v>1</v>
       </c>
@@ -29583,6 +30957,15 @@
       </c>
       <c r="AJ359" s="1">
         <v>43795</v>
+      </c>
+      <c r="AK359">
+        <v>164</v>
+      </c>
+      <c r="AL359">
+        <v>52.341000000000001</v>
+      </c>
+      <c r="AM359">
+        <v>37.503999999999998</v>
       </c>
       <c r="AN359">
         <v>1</v>
@@ -29657,6 +31040,9 @@
       <c r="AH360">
         <v>191</v>
       </c>
+      <c r="AJ360" s="1">
+        <v>43815</v>
+      </c>
       <c r="AN360">
         <v>0</v>
       </c>
@@ -29731,6 +31117,18 @@
       </c>
       <c r="AH361">
         <v>191</v>
+      </c>
+      <c r="AJ361" s="1">
+        <v>43804</v>
+      </c>
+      <c r="AK361">
+        <v>152.30000000000001</v>
+      </c>
+      <c r="AL361">
+        <v>42.365000000000002</v>
+      </c>
+      <c r="AM361">
+        <v>36.171999999999997</v>
       </c>
       <c r="AN361">
         <v>1</v>
@@ -29805,6 +31203,9 @@
       <c r="AH362">
         <v>191</v>
       </c>
+      <c r="AJ362" s="1">
+        <v>43817</v>
+      </c>
       <c r="AN362">
         <v>0</v>
       </c>
@@ -29879,6 +31280,18 @@
       </c>
       <c r="AH363">
         <v>191</v>
+      </c>
+      <c r="AJ363" s="1">
+        <v>43804</v>
+      </c>
+      <c r="AK363">
+        <v>159.69999999999999</v>
+      </c>
+      <c r="AL363">
+        <v>50.02</v>
+      </c>
+      <c r="AM363">
+        <v>32.46</v>
       </c>
       <c r="AN363">
         <v>0</v>
@@ -29956,6 +31369,15 @@
       <c r="AJ364" s="60">
         <v>43788</v>
       </c>
+      <c r="AK364">
+        <v>141.1</v>
+      </c>
+      <c r="AL364">
+        <v>43.161999999999999</v>
+      </c>
+      <c r="AM364">
+        <v>36.591000000000001</v>
+      </c>
       <c r="AN364">
         <v>0</v>
       </c>
@@ -30119,6 +31541,15 @@
       <c r="AJ366" s="1">
         <v>43795</v>
       </c>
+      <c r="AK366">
+        <v>148.19999999999999</v>
+      </c>
+      <c r="AL366">
+        <v>50.33</v>
+      </c>
+      <c r="AM366">
+        <v>38.69</v>
+      </c>
       <c r="AN366">
         <v>1</v>
       </c>
@@ -30193,6 +31624,18 @@
       </c>
       <c r="AH367">
         <v>191</v>
+      </c>
+      <c r="AJ367" s="1">
+        <v>43808</v>
+      </c>
+      <c r="AK367">
+        <v>146.6</v>
+      </c>
+      <c r="AL367">
+        <v>41.207999999999998</v>
+      </c>
+      <c r="AM367">
+        <v>45.886000000000003</v>
       </c>
       <c r="AN367">
         <v>1</v>
@@ -30273,6 +31716,12 @@
       <c r="AK368">
         <v>146.69999999999999</v>
       </c>
+      <c r="AL368">
+        <v>59.863999999999997</v>
+      </c>
+      <c r="AM368">
+        <v>39.972000000000001</v>
+      </c>
       <c r="AN368">
         <v>0</v>
       </c>
@@ -30352,6 +31801,15 @@
       </c>
       <c r="AJ369" s="60">
         <v>43788</v>
+      </c>
+      <c r="AK369">
+        <v>147.69999999999999</v>
+      </c>
+      <c r="AL369">
+        <v>51.131999999999998</v>
+      </c>
+      <c r="AM369">
+        <v>37.78</v>
       </c>
       <c r="AN369">
         <v>1</v>
@@ -30432,13 +31890,13 @@
         <v>43784</v>
       </c>
       <c r="AK370">
-        <v>150.30000000000001</v>
+        <v>153.19999999999999</v>
       </c>
       <c r="AL370">
-        <v>33.31</v>
+        <v>49.003999999999998</v>
       </c>
       <c r="AM370">
-        <v>35.24</v>
+        <v>29.876000000000001</v>
       </c>
       <c r="AN370">
         <v>0</v>
@@ -30517,6 +31975,15 @@
       </c>
       <c r="AJ371" s="1">
         <v>43795</v>
+      </c>
+      <c r="AK371">
+        <v>136.1</v>
+      </c>
+      <c r="AL371">
+        <v>42.207000000000001</v>
+      </c>
+      <c r="AM371">
+        <v>34.497999999999998</v>
       </c>
       <c r="AN371">
         <v>0</v>
@@ -30591,6 +32058,9 @@
       <c r="AH372">
         <v>192</v>
       </c>
+      <c r="AJ372" s="1">
+        <v>43812</v>
+      </c>
       <c r="AN372">
         <v>0</v>
       </c>
@@ -30665,6 +32135,18 @@
       </c>
       <c r="AH373">
         <v>192</v>
+      </c>
+      <c r="AJ373" s="1">
+        <v>43808</v>
+      </c>
+      <c r="AK373">
+        <v>133.30000000000001</v>
+      </c>
+      <c r="AL373">
+        <v>44.712000000000003</v>
+      </c>
+      <c r="AM373">
+        <v>32.674999999999997</v>
       </c>
       <c r="AN373">
         <v>1</v>
@@ -30742,6 +32224,15 @@
       <c r="AJ374" s="1">
         <v>43802</v>
       </c>
+      <c r="AK374">
+        <v>155.6</v>
+      </c>
+      <c r="AL374">
+        <v>46.911999999999999</v>
+      </c>
+      <c r="AM374">
+        <v>28.13</v>
+      </c>
       <c r="AN374">
         <v>1</v>
       </c>
@@ -30819,6 +32310,15 @@
       </c>
       <c r="AJ375" s="1">
         <v>43795</v>
+      </c>
+      <c r="AK375">
+        <v>143.69999999999999</v>
+      </c>
+      <c r="AL375">
+        <v>38.396999999999998</v>
+      </c>
+      <c r="AM375">
+        <v>29.658999999999999</v>
       </c>
       <c r="AN375">
         <v>0</v>
@@ -30896,6 +32396,15 @@
       <c r="AJ376" s="1">
         <v>43802</v>
       </c>
+      <c r="AK376">
+        <v>179.8</v>
+      </c>
+      <c r="AL376">
+        <v>32.645000000000003</v>
+      </c>
+      <c r="AM376">
+        <v>36.828000000000003</v>
+      </c>
       <c r="AN376">
         <v>1</v>
       </c>
@@ -30970,6 +32479,18 @@
       </c>
       <c r="AH377">
         <v>192</v>
+      </c>
+      <c r="AJ377" s="1">
+        <v>43808</v>
+      </c>
+      <c r="AK377">
+        <v>174.5</v>
+      </c>
+      <c r="AL377">
+        <v>47.103999999999999</v>
+      </c>
+      <c r="AM377">
+        <v>35.063000000000002</v>
       </c>
       <c r="AN377">
         <v>1</v>
@@ -31044,6 +32565,18 @@
       <c r="AH378">
         <v>192</v>
       </c>
+      <c r="AJ378" s="1">
+        <v>43808</v>
+      </c>
+      <c r="AK378">
+        <v>173.7</v>
+      </c>
+      <c r="AL378">
+        <v>60.593000000000004</v>
+      </c>
+      <c r="AM378">
+        <v>41.24</v>
+      </c>
       <c r="AN378">
         <v>0</v>
       </c>
@@ -31118,6 +32651,15 @@
       </c>
       <c r="AH379">
         <v>192</v>
+      </c>
+      <c r="AJ379" s="1">
+        <v>43804</v>
+      </c>
+      <c r="AL379">
+        <v>45.886000000000003</v>
+      </c>
+      <c r="AM379">
+        <v>32.707999999999998</v>
       </c>
       <c r="AN379">
         <v>1</v>
@@ -31195,6 +32737,15 @@
       <c r="AJ380" s="1">
         <v>43795</v>
       </c>
+      <c r="AK380">
+        <v>135.1</v>
+      </c>
+      <c r="AL380">
+        <v>33.31</v>
+      </c>
+      <c r="AM380">
+        <v>35.24</v>
+      </c>
       <c r="AN380">
         <v>0</v>
       </c>
@@ -31272,6 +32823,15 @@
       </c>
       <c r="AJ381" s="1">
         <v>43795</v>
+      </c>
+      <c r="AK381">
+        <v>153.5</v>
+      </c>
+      <c r="AL381">
+        <v>46.161999999999999</v>
+      </c>
+      <c r="AM381">
+        <v>37.997</v>
       </c>
       <c r="AN381">
         <v>1</v>
@@ -31349,6 +32909,15 @@
       <c r="AJ382" s="1">
         <v>43802</v>
       </c>
+      <c r="AK382">
+        <v>159.69999999999999</v>
+      </c>
+      <c r="AL382">
+        <v>43.91</v>
+      </c>
+      <c r="AM382">
+        <v>37.643999999999998</v>
+      </c>
       <c r="AN382">
         <v>1</v>
       </c>
@@ -31425,6 +32994,18 @@
       </c>
       <c r="AH383">
         <v>192</v>
+      </c>
+      <c r="AJ383" s="1">
+        <v>43804</v>
+      </c>
+      <c r="AK383">
+        <v>154.30000000000001</v>
+      </c>
+      <c r="AL383">
+        <v>68.319999999999993</v>
+      </c>
+      <c r="AM383">
+        <v>38.625</v>
       </c>
       <c r="AN383">
         <v>1</v>
@@ -31499,6 +33080,18 @@
       <c r="AH384">
         <v>192</v>
       </c>
+      <c r="AJ384" s="1">
+        <v>43808</v>
+      </c>
+      <c r="AK384">
+        <v>174.9</v>
+      </c>
+      <c r="AL384">
+        <v>53.124000000000002</v>
+      </c>
+      <c r="AM384">
+        <v>40.250999999999998</v>
+      </c>
       <c r="AN384">
         <v>1</v>
       </c>
@@ -34490,6 +36083,12 @@
       <c r="AK420">
         <v>55</v>
       </c>
+      <c r="AL420">
+        <v>22.31</v>
+      </c>
+      <c r="AM420" s="58">
+        <v>8.1869999999999994</v>
+      </c>
       <c r="AN420">
         <v>0</v>
       </c>
@@ -34653,6 +36252,15 @@
       <c r="AJ422" s="1">
         <v>43795</v>
       </c>
+      <c r="AK422">
+        <v>44.5</v>
+      </c>
+      <c r="AL422">
+        <v>11.691700000000001</v>
+      </c>
+      <c r="AM422" s="58">
+        <v>5.1230000000000002</v>
+      </c>
       <c r="AN422">
         <v>0</v>
       </c>
@@ -34988,6 +36596,12 @@
       <c r="AK426">
         <v>58.8</v>
       </c>
+      <c r="AL426">
+        <v>13.544</v>
+      </c>
+      <c r="AM426" s="58">
+        <v>6.67</v>
+      </c>
       <c r="AN426">
         <v>0</v>
       </c>
@@ -35148,6 +36762,15 @@
       <c r="AJ428" s="60">
         <v>43788</v>
       </c>
+      <c r="AK428">
+        <v>45.5</v>
+      </c>
+      <c r="AL428">
+        <v>13.948</v>
+      </c>
+      <c r="AM428" s="58">
+        <v>7.5970000000000004</v>
+      </c>
       <c r="AN428">
         <v>0</v>
       </c>
@@ -35648,6 +37271,15 @@
       <c r="AJ434" s="1">
         <v>43795</v>
       </c>
+      <c r="AK434">
+        <v>108</v>
+      </c>
+      <c r="AL434">
+        <v>40.438000000000002</v>
+      </c>
+      <c r="AM434" s="58">
+        <v>28.445</v>
+      </c>
       <c r="AN434">
         <v>0</v>
       </c>
@@ -35727,6 +37359,18 @@
       </c>
       <c r="AI435">
         <v>-0.03</v>
+      </c>
+      <c r="AJ435" s="1">
+        <v>43808</v>
+      </c>
+      <c r="AK435">
+        <v>114.9</v>
+      </c>
+      <c r="AL435">
+        <v>26.030999999999999</v>
+      </c>
+      <c r="AM435" s="58">
+        <v>17.332999999999998</v>
       </c>
       <c r="AN435">
         <v>1</v>
@@ -35809,6 +37453,15 @@
       <c r="AJ436" s="1">
         <v>43802</v>
       </c>
+      <c r="AK436">
+        <v>59.3</v>
+      </c>
+      <c r="AL436">
+        <v>11.361000000000001</v>
+      </c>
+      <c r="AM436" s="58">
+        <v>9.0449999999999999</v>
+      </c>
       <c r="AN436">
         <v>1</v>
       </c>
@@ -35888,6 +37541,18 @@
       </c>
       <c r="AI437">
         <v>-0.11</v>
+      </c>
+      <c r="AJ437" s="1">
+        <v>43810</v>
+      </c>
+      <c r="AK437">
+        <v>95</v>
+      </c>
+      <c r="AL437">
+        <v>29.408000000000001</v>
+      </c>
+      <c r="AM437" s="58">
+        <v>12.881</v>
       </c>
       <c r="AN437">
         <v>1</v>
@@ -35971,6 +37636,12 @@
       <c r="AK438">
         <v>83.6</v>
       </c>
+      <c r="AL438">
+        <v>8</v>
+      </c>
+      <c r="AM438">
+        <v>8.3170000000000002</v>
+      </c>
       <c r="AN438">
         <v>0</v>
       </c>
@@ -36051,6 +37722,15 @@
       </c>
       <c r="AJ439" s="1">
         <v>43802</v>
+      </c>
+      <c r="AK439">
+        <v>92.9</v>
+      </c>
+      <c r="AL439">
+        <v>11.07</v>
+      </c>
+      <c r="AM439">
+        <v>9.1869999999999994</v>
       </c>
       <c r="AN439">
         <v>1</v>
@@ -36130,6 +37810,15 @@
       </c>
       <c r="AJ440" s="1">
         <v>43802</v>
+      </c>
+      <c r="AK440">
+        <v>67.7</v>
+      </c>
+      <c r="AL440">
+        <v>27.782</v>
+      </c>
+      <c r="AM440">
+        <v>13.417999999999999</v>
       </c>
       <c r="AN440">
         <v>0</v>
@@ -36244,6 +37933,15 @@
       <c r="AJ442" s="1">
         <v>43802</v>
       </c>
+      <c r="AK442">
+        <v>46.8</v>
+      </c>
+      <c r="AL442">
+        <v>8.5389999999999997</v>
+      </c>
+      <c r="AM442">
+        <v>3.3130000000000002</v>
+      </c>
       <c r="AN442">
         <v>0</v>
       </c>
@@ -36412,6 +38110,18 @@
       <c r="AI444">
         <v>-0.02</v>
       </c>
+      <c r="AJ444" s="1">
+        <v>43804</v>
+      </c>
+      <c r="AK444">
+        <v>43.8</v>
+      </c>
+      <c r="AL444">
+        <v>6.4320000000000004</v>
+      </c>
+      <c r="AM444">
+        <v>3.01</v>
+      </c>
       <c r="AN444">
         <v>1</v>
       </c>
@@ -36668,6 +38378,18 @@
       <c r="AI447">
         <v>-0.05</v>
       </c>
+      <c r="AJ447" s="1">
+        <v>43808</v>
+      </c>
+      <c r="AK447">
+        <v>94.1</v>
+      </c>
+      <c r="AL447">
+        <v>20.312999999999999</v>
+      </c>
+      <c r="AM447">
+        <v>10.385</v>
+      </c>
       <c r="AN447">
         <v>1</v>
       </c>
@@ -36921,6 +38643,12 @@
       <c r="AK450">
         <v>85.5</v>
       </c>
+      <c r="AL450">
+        <v>28.27</v>
+      </c>
+      <c r="AM450">
+        <v>24.693000000000001</v>
+      </c>
       <c r="AN450">
         <v>1</v>
       </c>
@@ -37000,6 +38728,15 @@
       </c>
       <c r="AJ451" s="1">
         <v>43795</v>
+      </c>
+      <c r="AK451">
+        <v>87.2</v>
+      </c>
+      <c r="AL451">
+        <v>17.07</v>
+      </c>
+      <c r="AM451">
+        <v>11.138999999999999</v>
       </c>
       <c r="AN451">
         <v>1</v>
@@ -37082,6 +38819,12 @@
       <c r="AK452">
         <v>104.2</v>
       </c>
+      <c r="AL452">
+        <v>24.963000000000001</v>
+      </c>
+      <c r="AM452">
+        <v>26.277000000000001</v>
+      </c>
       <c r="AN452">
         <v>1</v>
       </c>
@@ -37156,6 +38899,18 @@
       </c>
       <c r="AH453">
         <v>192</v>
+      </c>
+      <c r="AJ453" s="1">
+        <v>43804</v>
+      </c>
+      <c r="AK453">
+        <v>86.2</v>
+      </c>
+      <c r="AL453">
+        <v>15.026</v>
+      </c>
+      <c r="AM453">
+        <v>14.356999999999999</v>
       </c>
       <c r="AN453">
         <v>1</v>
@@ -37233,6 +38988,15 @@
       <c r="AJ454" s="60">
         <v>43788</v>
       </c>
+      <c r="AK454">
+        <v>68.2</v>
+      </c>
+      <c r="AL454">
+        <v>32.677</v>
+      </c>
+      <c r="AM454">
+        <v>21.311</v>
+      </c>
       <c r="AN454">
         <v>1</v>
       </c>
@@ -37313,6 +39077,12 @@
       </c>
       <c r="AK455">
         <v>110.6</v>
+      </c>
+      <c r="AL455">
+        <v>29.187999999999999</v>
+      </c>
+      <c r="AM455">
+        <v>31.771000000000001</v>
       </c>
       <c r="AN455">
         <v>1</v>
@@ -37390,6 +39160,15 @@
       <c r="AJ456" s="1">
         <v>43802</v>
       </c>
+      <c r="AK456">
+        <v>92.7</v>
+      </c>
+      <c r="AL456">
+        <v>18.126000000000001</v>
+      </c>
+      <c r="AM456">
+        <v>14.127000000000001</v>
+      </c>
       <c r="AN456">
         <v>1</v>
       </c>
@@ -37467,6 +39246,15 @@
       </c>
       <c r="AJ457" s="1">
         <v>43802</v>
+      </c>
+      <c r="AK457">
+        <v>91.7</v>
+      </c>
+      <c r="AL457">
+        <v>14.551</v>
+      </c>
+      <c r="AM457">
+        <v>9.1669999999999998</v>
       </c>
       <c r="AN457">
         <v>1</v>
@@ -37541,6 +39329,18 @@
       <c r="AH458">
         <v>192</v>
       </c>
+      <c r="AJ458" s="1">
+        <v>43808</v>
+      </c>
+      <c r="AK458">
+        <v>78.8</v>
+      </c>
+      <c r="AL458">
+        <v>13.682</v>
+      </c>
+      <c r="AM458">
+        <v>6.2679999999999998</v>
+      </c>
       <c r="AN458">
         <v>1</v>
       </c>
@@ -37615,6 +39415,18 @@
       </c>
       <c r="AH459">
         <v>192</v>
+      </c>
+      <c r="AJ459" s="1">
+        <v>43804</v>
+      </c>
+      <c r="AK459">
+        <v>58.2</v>
+      </c>
+      <c r="AL459">
+        <v>28.78</v>
+      </c>
+      <c r="AM459">
+        <v>17.192</v>
       </c>
       <c r="AN459">
         <v>1</v>
@@ -37692,6 +39504,15 @@
       <c r="AJ460" s="1">
         <v>43795</v>
       </c>
+      <c r="AK460">
+        <v>44</v>
+      </c>
+      <c r="AL460">
+        <v>7.8609999999999998</v>
+      </c>
+      <c r="AM460">
+        <v>5.4329999999999998</v>
+      </c>
       <c r="AN460">
         <v>1</v>
       </c>
@@ -37772,6 +39593,12 @@
       </c>
       <c r="AK461">
         <v>81.8</v>
+      </c>
+      <c r="AL461">
+        <v>19.239999999999998</v>
+      </c>
+      <c r="AM461">
+        <v>10.67</v>
       </c>
       <c r="AN461">
         <v>1</v>
@@ -37852,6 +39679,12 @@
       <c r="AK462">
         <v>83.7</v>
       </c>
+      <c r="AL462">
+        <v>14.474</v>
+      </c>
+      <c r="AM462">
+        <v>7.7359999999999998</v>
+      </c>
       <c r="AN462">
         <v>1</v>
       </c>
@@ -37929,6 +39762,15 @@
       </c>
       <c r="AJ463" s="60">
         <v>43788</v>
+      </c>
+      <c r="AK463">
+        <v>99.1</v>
+      </c>
+      <c r="AL463">
+        <v>21.42</v>
+      </c>
+      <c r="AM463">
+        <v>19.736000000000001</v>
       </c>
       <c r="AN463">
         <v>1</v>
@@ -38006,6 +39848,15 @@
       <c r="AJ464" s="60">
         <v>43788</v>
       </c>
+      <c r="AK464">
+        <v>57.5</v>
+      </c>
+      <c r="AL464">
+        <v>11.803000000000001</v>
+      </c>
+      <c r="AM464">
+        <v>8.2560000000000002</v>
+      </c>
       <c r="AN464">
         <v>1</v>
       </c>
@@ -38087,6 +39938,12 @@
       <c r="AK465">
         <v>92.2</v>
       </c>
+      <c r="AL465">
+        <v>19.094000000000001</v>
+      </c>
+      <c r="AM465">
+        <v>16.87</v>
+      </c>
       <c r="AN465">
         <v>1</v>
       </c>
@@ -38165,6 +40022,15 @@
       <c r="AJ466" s="60">
         <v>43788</v>
       </c>
+      <c r="AK466">
+        <v>129.6</v>
+      </c>
+      <c r="AL466">
+        <v>28.695</v>
+      </c>
+      <c r="AM466">
+        <v>27.567</v>
+      </c>
       <c r="AN466">
         <v>1</v>
       </c>
@@ -38241,6 +40107,18 @@
       </c>
       <c r="AH467">
         <v>192</v>
+      </c>
+      <c r="AJ467" s="1">
+        <v>43804</v>
+      </c>
+      <c r="AK467">
+        <v>100.8</v>
+      </c>
+      <c r="AL467">
+        <v>25.395</v>
+      </c>
+      <c r="AM467">
+        <v>17.867000000000001</v>
       </c>
       <c r="AN467">
         <v>1</v>
@@ -38319,6 +40197,15 @@
       </c>
       <c r="AJ468" s="1">
         <v>43802</v>
+      </c>
+      <c r="AK468">
+        <v>121.3</v>
+      </c>
+      <c r="AL468">
+        <v>24.956</v>
+      </c>
+      <c r="AM468">
+        <v>18.277000000000001</v>
       </c>
       <c r="AN468">
         <v>1</v>
@@ -38486,6 +40373,12 @@
       <c r="AK470">
         <v>113.5</v>
       </c>
+      <c r="AL470">
+        <v>28.234000000000002</v>
+      </c>
+      <c r="AM470">
+        <v>24.268000000000001</v>
+      </c>
       <c r="AN470">
         <v>1</v>
       </c>
@@ -38560,6 +40453,18 @@
       </c>
       <c r="AH471">
         <v>192</v>
+      </c>
+      <c r="AJ471" s="1">
+        <v>43808</v>
+      </c>
+      <c r="AK471">
+        <v>36.700000000000003</v>
+      </c>
+      <c r="AL471">
+        <v>13.039</v>
+      </c>
+      <c r="AM471">
+        <v>5.0090000000000003</v>
       </c>
       <c r="AN471">
         <v>1</v>
@@ -38634,6 +40539,18 @@
       <c r="AH472">
         <v>192</v>
       </c>
+      <c r="AJ472" s="1">
+        <v>43810</v>
+      </c>
+      <c r="AK472">
+        <v>115</v>
+      </c>
+      <c r="AL472">
+        <v>22.66</v>
+      </c>
+      <c r="AM472">
+        <v>22.46</v>
+      </c>
       <c r="AN472">
         <v>1</v>
       </c>
@@ -38710,7 +40627,7 @@
         <v>192</v>
       </c>
       <c r="AJ473" s="1">
-        <v>43802</v>
+        <v>43812</v>
       </c>
       <c r="AN473">
         <v>1</v>
@@ -38785,6 +40702,18 @@
       <c r="AH474">
         <v>192</v>
       </c>
+      <c r="AJ474" s="1">
+        <v>43804</v>
+      </c>
+      <c r="AK474">
+        <v>61.5</v>
+      </c>
+      <c r="AL474">
+        <v>13.124000000000001</v>
+      </c>
+      <c r="AM474">
+        <v>6.6390000000000002</v>
+      </c>
       <c r="AN474">
         <v>1</v>
       </c>
@@ -38865,6 +40794,12 @@
       </c>
       <c r="AK475">
         <v>84.7</v>
+      </c>
+      <c r="AL475">
+        <v>29.082000000000001</v>
+      </c>
+      <c r="AM475">
+        <v>17.722000000000001</v>
       </c>
       <c r="AN475">
         <v>1</v>
@@ -38939,6 +40874,18 @@
       <c r="AH476">
         <v>192</v>
       </c>
+      <c r="AJ476" s="1">
+        <v>43804</v>
+      </c>
+      <c r="AK476">
+        <v>117.9</v>
+      </c>
+      <c r="AL476">
+        <v>33.619</v>
+      </c>
+      <c r="AM476">
+        <v>17.597000000000001</v>
+      </c>
       <c r="AN476">
         <v>1</v>
       </c>
@@ -39016,6 +40963,15 @@
       </c>
       <c r="AJ477" s="60">
         <v>43788</v>
+      </c>
+      <c r="AK477">
+        <v>44.1</v>
+      </c>
+      <c r="AL477">
+        <v>19.559000000000001</v>
+      </c>
+      <c r="AM477">
+        <v>7.5730000000000004</v>
       </c>
       <c r="AN477">
         <v>1</v>
@@ -39090,8 +41046,17 @@
       <c r="AH478">
         <v>192</v>
       </c>
+      <c r="AJ478" t="s">
+        <v>586</v>
+      </c>
       <c r="AK478">
         <v>79.900000000000006</v>
+      </c>
+      <c r="AL478">
+        <v>23.867000000000001</v>
+      </c>
+      <c r="AM478">
+        <v>16.097999999999999</v>
       </c>
       <c r="AN478">
         <v>1</v>
@@ -39170,6 +41135,15 @@
       </c>
       <c r="AJ479" s="1">
         <v>43795</v>
+      </c>
+      <c r="AK479">
+        <v>95</v>
+      </c>
+      <c r="AL479">
+        <v>33.32</v>
+      </c>
+      <c r="AM479">
+        <v>18.655999999999999</v>
       </c>
       <c r="AN479">
         <v>1</v>
@@ -39247,6 +41221,15 @@
       <c r="AJ480" s="1">
         <v>43784</v>
       </c>
+      <c r="AK480">
+        <v>70.900000000000006</v>
+      </c>
+      <c r="AL480">
+        <v>17.342600000000001</v>
+      </c>
+      <c r="AM480">
+        <v>9.76</v>
+      </c>
       <c r="AN480">
         <v>1</v>
       </c>
@@ -39323,6 +41306,18 @@
       </c>
       <c r="AH481">
         <v>192</v>
+      </c>
+      <c r="AJ481" s="1">
+        <v>43802</v>
+      </c>
+      <c r="AK481">
+        <v>107.4</v>
+      </c>
+      <c r="AL481">
+        <v>35.948</v>
+      </c>
+      <c r="AM481">
+        <v>17.353000000000002</v>
       </c>
       <c r="AN481">
         <v>1</v>

</xml_diff>

<commit_message>
lots of data and models
</commit_message>
<xml_diff>
--- a/data/observation_datasheet.xlsx
+++ b/data/observation_datasheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/catchamberlain/Documents/git/chillfreeze/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A4A3A15-643B-2347-8B1B-4F39B8D41923}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{553C78D9-9A03-F742-99DA-2844E8F3D086}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3420" yWindow="460" windowWidth="32400" windowHeight="21640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2535,7 +2535,7 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -2600,6 +2600,7 @@
     <xf numFmtId="14" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="98">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -5454,10 +5455,10 @@
   <dimension ref="A1:AN481"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="86" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AC195" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AC147" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AJ240" sqref="AJ240"/>
+      <selection pane="bottomRight" activeCell="AL483" sqref="AL483"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -17806,7 +17807,7 @@
       <c r="AJ147" s="1">
         <v>43795</v>
       </c>
-      <c r="AK147" s="56">
+      <c r="AK147" s="62">
         <v>99.7</v>
       </c>
       <c r="AL147" s="5">
@@ -25964,7 +25965,7 @@
         <v>13.58</v>
       </c>
     </row>
-    <row r="242" spans="1:39" hidden="1">
+    <row r="242" spans="1:39">
       <c r="A242" s="13" t="s">
         <v>241</v>
       </c>
@@ -25994,7 +25995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="1:39" hidden="1">
+    <row r="243" spans="1:39">
       <c r="A243" s="13" t="s">
         <v>242</v>
       </c>
@@ -26045,7 +26046,7 @@
         <v>-0.70000000000000284</v>
       </c>
     </row>
-    <row r="244" spans="1:39" hidden="1">
+    <row r="244" spans="1:39">
       <c r="A244" s="13" t="s">
         <v>243</v>
       </c>
@@ -26094,7 +26095,7 @@
         <v>-0.40000000000000568</v>
       </c>
     </row>
-    <row r="245" spans="1:39" hidden="1">
+    <row r="245" spans="1:39">
       <c r="A245" s="13" t="s">
         <v>244</v>
       </c>
@@ -26145,7 +26146,7 @@
         <v>-0.59999999999999787</v>
       </c>
     </row>
-    <row r="246" spans="1:39" hidden="1">
+    <row r="246" spans="1:39">
       <c r="A246" s="13" t="s">
         <v>245</v>
       </c>
@@ -26173,7 +26174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="247" spans="1:39" hidden="1">
+    <row r="247" spans="1:39">
       <c r="A247" s="13" t="s">
         <v>246</v>
       </c>
@@ -26201,7 +26202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="248" spans="1:39" hidden="1">
+    <row r="248" spans="1:39">
       <c r="A248" s="13" t="s">
         <v>247</v>
       </c>
@@ -26235,7 +26236,7 @@
         <v>-28.3</v>
       </c>
     </row>
-    <row r="249" spans="1:39" hidden="1">
+    <row r="249" spans="1:39">
       <c r="A249" s="13" t="s">
         <v>248</v>
       </c>
@@ -26263,7 +26264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="250" spans="1:39" hidden="1">
+    <row r="250" spans="1:39">
       <c r="A250" s="13" t="s">
         <v>249</v>
       </c>
@@ -26291,7 +26292,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="251" spans="1:39" hidden="1">
+    <row r="251" spans="1:39">
       <c r="A251" s="13" t="s">
         <v>250</v>
       </c>
@@ -26327,7 +26328,7 @@
         <v>-34.1</v>
       </c>
     </row>
-    <row r="252" spans="1:39" hidden="1">
+    <row r="252" spans="1:39">
       <c r="A252" s="13" t="s">
         <v>251</v>
       </c>
@@ -26361,7 +26362,7 @@
         <v>-27.7</v>
       </c>
     </row>
-    <row r="253" spans="1:39" hidden="1">
+    <row r="253" spans="1:39">
       <c r="A253" s="13" t="s">
         <v>252</v>
       </c>
@@ -26389,7 +26390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="254" spans="1:39" hidden="1">
+    <row r="254" spans="1:39">
       <c r="A254" s="13" t="s">
         <v>253</v>
       </c>
@@ -26423,7 +26424,7 @@
         <v>-30.3</v>
       </c>
     </row>
-    <row r="255" spans="1:39" hidden="1">
+    <row r="255" spans="1:39">
       <c r="A255" s="13" t="s">
         <v>254</v>
       </c>
@@ -26451,7 +26452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="256" spans="1:39" hidden="1">
+    <row r="256" spans="1:39">
       <c r="A256" s="13" t="s">
         <v>255</v>
       </c>
@@ -26479,7 +26480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="257" spans="1:24" hidden="1">
+    <row r="257" spans="1:24">
       <c r="A257" s="13" t="s">
         <v>256</v>
       </c>
@@ -26507,7 +26508,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="258" spans="1:24" hidden="1">
+    <row r="258" spans="1:24">
       <c r="A258" s="18" t="s">
         <v>257</v>
       </c>
@@ -26543,7 +26544,7 @@
         <v>-30.8</v>
       </c>
     </row>
-    <row r="259" spans="1:24" hidden="1">
+    <row r="259" spans="1:24">
       <c r="A259" s="18" t="s">
         <v>258</v>
       </c>
@@ -26579,7 +26580,7 @@
         <v>-35.9</v>
       </c>
     </row>
-    <row r="260" spans="1:24" hidden="1">
+    <row r="260" spans="1:24">
       <c r="A260" s="18" t="s">
         <v>259</v>
       </c>
@@ -26607,7 +26608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="261" spans="1:24" hidden="1">
+    <row r="261" spans="1:24">
       <c r="A261" s="18" t="s">
         <v>260</v>
       </c>
@@ -26635,7 +26636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="262" spans="1:24" hidden="1">
+    <row r="262" spans="1:24">
       <c r="A262" s="18" t="s">
         <v>261</v>
       </c>
@@ -26663,7 +26664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="263" spans="1:24" hidden="1">
+    <row r="263" spans="1:24">
       <c r="A263" s="18" t="s">
         <v>262</v>
       </c>
@@ -26691,7 +26692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="264" spans="1:24" hidden="1">
+    <row r="264" spans="1:24">
       <c r="A264" s="18" t="s">
         <v>263</v>
       </c>
@@ -26740,7 +26741,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="265" spans="1:24" hidden="1">
+    <row r="265" spans="1:24">
       <c r="A265" s="18" t="s">
         <v>264</v>
       </c>
@@ -26768,7 +26769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="266" spans="1:24" hidden="1">
+    <row r="266" spans="1:24">
       <c r="A266" s="18" t="s">
         <v>265</v>
       </c>
@@ -26817,7 +26818,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="267" spans="1:24" hidden="1">
+    <row r="267" spans="1:24">
       <c r="A267" s="18" t="s">
         <v>266</v>
       </c>
@@ -26845,7 +26846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="268" spans="1:24" hidden="1">
+    <row r="268" spans="1:24">
       <c r="A268" s="18" t="s">
         <v>267</v>
       </c>
@@ -26873,7 +26874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="269" spans="1:24" hidden="1">
+    <row r="269" spans="1:24">
       <c r="A269" s="18" t="s">
         <v>268</v>
       </c>
@@ -26901,7 +26902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="270" spans="1:24" hidden="1">
+    <row r="270" spans="1:24">
       <c r="A270" s="18" t="s">
         <v>269</v>
       </c>
@@ -26950,7 +26951,7 @@
         <v>9.9999999999997868E-2</v>
       </c>
     </row>
-    <row r="271" spans="1:24" hidden="1">
+    <row r="271" spans="1:24">
       <c r="A271" s="18" t="s">
         <v>270</v>
       </c>
@@ -26978,7 +26979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="272" spans="1:24" hidden="1">
+    <row r="272" spans="1:24">
       <c r="A272" s="18" t="s">
         <v>271</v>
       </c>
@@ -27027,7 +27028,7 @@
         <v>0.70000000000000284</v>
       </c>
     </row>
-    <row r="273" spans="1:24" hidden="1">
+    <row r="273" spans="1:24">
       <c r="A273" s="18" t="s">
         <v>272</v>
       </c>
@@ -27055,7 +27056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="274" spans="1:24" hidden="1">
+    <row r="274" spans="1:24">
       <c r="A274" s="21" t="s">
         <v>273</v>
       </c>
@@ -27085,7 +27086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="275" spans="1:24" hidden="1">
+    <row r="275" spans="1:24">
       <c r="A275" s="21" t="s">
         <v>274</v>
       </c>
@@ -27113,7 +27114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="276" spans="1:24" hidden="1">
+    <row r="276" spans="1:24">
       <c r="A276" s="21" t="s">
         <v>275</v>
       </c>
@@ -27141,7 +27142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="277" spans="1:24" hidden="1">
+    <row r="277" spans="1:24">
       <c r="A277" s="21" t="s">
         <v>276</v>
       </c>
@@ -27169,7 +27170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="278" spans="1:24" hidden="1">
+    <row r="278" spans="1:24">
       <c r="A278" s="21" t="s">
         <v>277</v>
       </c>
@@ -27197,7 +27198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="279" spans="1:24" hidden="1">
+    <row r="279" spans="1:24">
       <c r="A279" s="21" t="s">
         <v>278</v>
       </c>
@@ -27225,7 +27226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="280" spans="1:24" hidden="1">
+    <row r="280" spans="1:24">
       <c r="A280" s="21" t="s">
         <v>279</v>
       </c>
@@ -27253,7 +27254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="281" spans="1:24" hidden="1">
+    <row r="281" spans="1:24">
       <c r="A281" s="21" t="s">
         <v>280</v>
       </c>
@@ -27281,7 +27282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="282" spans="1:24" hidden="1">
+    <row r="282" spans="1:24">
       <c r="A282" s="21" t="s">
         <v>281</v>
       </c>
@@ -27309,7 +27310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="283" spans="1:24" hidden="1">
+    <row r="283" spans="1:24">
       <c r="A283" s="21" t="s">
         <v>282</v>
       </c>
@@ -27337,7 +27338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="284" spans="1:24" hidden="1">
+    <row r="284" spans="1:24">
       <c r="A284" s="21" t="s">
         <v>283</v>
       </c>
@@ -27365,7 +27366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="285" spans="1:24" hidden="1">
+    <row r="285" spans="1:24">
       <c r="A285" s="21" t="s">
         <v>284</v>
       </c>
@@ -27393,7 +27394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="286" spans="1:24" hidden="1">
+    <row r="286" spans="1:24">
       <c r="A286" s="21" t="s">
         <v>285</v>
       </c>
@@ -27421,7 +27422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="287" spans="1:24" hidden="1">
+    <row r="287" spans="1:24">
       <c r="A287" s="21" t="s">
         <v>286</v>
       </c>
@@ -27449,7 +27450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="288" spans="1:24" hidden="1">
+    <row r="288" spans="1:24">
       <c r="A288" s="21" t="s">
         <v>287</v>
       </c>
@@ -27477,7 +27478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="289" spans="1:27" hidden="1">
+    <row r="289" spans="1:27">
       <c r="A289" s="21" t="s">
         <v>288</v>
       </c>
@@ -27505,7 +27506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="290" spans="1:27" hidden="1">
+    <row r="290" spans="1:27">
       <c r="A290" s="13" t="s">
         <v>289</v>
       </c>
@@ -27535,7 +27536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="291" spans="1:27" hidden="1">
+    <row r="291" spans="1:27">
       <c r="A291" s="13" t="s">
         <v>290</v>
       </c>
@@ -27565,7 +27566,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="292" spans="1:27" hidden="1">
+    <row r="292" spans="1:27">
       <c r="A292" s="13" t="s">
         <v>291</v>
       </c>
@@ -27595,7 +27596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="293" spans="1:27" hidden="1">
+    <row r="293" spans="1:27">
       <c r="A293" s="13" t="s">
         <v>292</v>
       </c>
@@ -27625,7 +27626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="294" spans="1:27" hidden="1">
+    <row r="294" spans="1:27">
       <c r="A294" s="13" t="s">
         <v>293</v>
       </c>
@@ -27653,7 +27654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="295" spans="1:27" hidden="1">
+    <row r="295" spans="1:27">
       <c r="A295" s="13" t="s">
         <v>294</v>
       </c>
@@ -27681,7 +27682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="296" spans="1:27" hidden="1">
+    <row r="296" spans="1:27">
       <c r="A296" s="13" t="s">
         <v>295</v>
       </c>
@@ -27730,7 +27731,7 @@
         <v>1.1000000000000014</v>
       </c>
     </row>
-    <row r="297" spans="1:27" hidden="1">
+    <row r="297" spans="1:27">
       <c r="A297" s="13" t="s">
         <v>296</v>
       </c>
@@ -27758,7 +27759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="298" spans="1:27" hidden="1">
+    <row r="298" spans="1:27">
       <c r="A298" s="13" t="s">
         <v>297</v>
       </c>
@@ -27786,7 +27787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="299" spans="1:27" hidden="1">
+    <row r="299" spans="1:27">
       <c r="A299" s="13" t="s">
         <v>298</v>
       </c>
@@ -27837,7 +27838,7 @@
         <v>0.90000000000000213</v>
       </c>
     </row>
-    <row r="300" spans="1:27" hidden="1">
+    <row r="300" spans="1:27">
       <c r="A300" s="13" t="s">
         <v>299</v>
       </c>
@@ -27886,7 +27887,7 @@
         <v>-0.40000000000000213</v>
       </c>
     </row>
-    <row r="301" spans="1:27" hidden="1">
+    <row r="301" spans="1:27">
       <c r="A301" s="13" t="s">
         <v>300</v>
       </c>
@@ -27922,7 +27923,7 @@
         <v>-25.4</v>
       </c>
     </row>
-    <row r="302" spans="1:27" hidden="1">
+    <row r="302" spans="1:27">
       <c r="A302" s="13" t="s">
         <v>301</v>
       </c>
@@ -27950,7 +27951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="303" spans="1:27" hidden="1">
+    <row r="303" spans="1:27">
       <c r="A303" s="13" t="s">
         <v>302</v>
       </c>
@@ -27986,7 +27987,7 @@
         <v>-32.200000000000003</v>
       </c>
     </row>
-    <row r="304" spans="1:27" hidden="1">
+    <row r="304" spans="1:27">
       <c r="A304" s="13" t="s">
         <v>303</v>
       </c>
@@ -28038,7 +28039,7 @@
         <v>9.7999999999999997E-3</v>
       </c>
     </row>
-    <row r="305" spans="1:24" hidden="1">
+    <row r="305" spans="1:24">
       <c r="A305" s="13" t="s">
         <v>304</v>
       </c>
@@ -28066,7 +28067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="306" spans="1:24" hidden="1">
+    <row r="306" spans="1:24">
       <c r="A306" s="18" t="s">
         <v>305</v>
       </c>
@@ -28096,7 +28097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="307" spans="1:24" hidden="1">
+    <row r="307" spans="1:24">
       <c r="A307" s="18" t="s">
         <v>306</v>
       </c>
@@ -28124,7 +28125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="308" spans="1:24" hidden="1">
+    <row r="308" spans="1:24">
       <c r="A308" s="18" t="s">
         <v>307</v>
       </c>
@@ -28152,7 +28153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="309" spans="1:24" hidden="1">
+    <row r="309" spans="1:24">
       <c r="A309" s="18" t="s">
         <v>308</v>
       </c>
@@ -28180,7 +28181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="310" spans="1:24" hidden="1">
+    <row r="310" spans="1:24">
       <c r="A310" s="18" t="s">
         <v>309</v>
       </c>
@@ -28208,7 +28209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="311" spans="1:24" hidden="1">
+    <row r="311" spans="1:24">
       <c r="A311" s="18" t="s">
         <v>310</v>
       </c>
@@ -28236,7 +28237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="312" spans="1:24" hidden="1">
+    <row r="312" spans="1:24">
       <c r="A312" s="18" t="s">
         <v>311</v>
       </c>
@@ -28264,7 +28265,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="313" spans="1:24" hidden="1">
+    <row r="313" spans="1:24">
       <c r="A313" s="18" t="s">
         <v>312</v>
       </c>
@@ -28292,7 +28293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="314" spans="1:24" hidden="1">
+    <row r="314" spans="1:24">
       <c r="A314" s="18" t="s">
         <v>313</v>
       </c>
@@ -28320,7 +28321,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="315" spans="1:24" hidden="1">
+    <row r="315" spans="1:24">
       <c r="A315" s="18" t="s">
         <v>314</v>
       </c>
@@ -28348,7 +28349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="316" spans="1:24" hidden="1">
+    <row r="316" spans="1:24">
       <c r="A316" s="18" t="s">
         <v>315</v>
       </c>
@@ -28376,7 +28377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="317" spans="1:24" hidden="1">
+    <row r="317" spans="1:24">
       <c r="A317" s="18" t="s">
         <v>316</v>
       </c>
@@ -28404,7 +28405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="318" spans="1:24" hidden="1">
+    <row r="318" spans="1:24">
       <c r="A318" s="18" t="s">
         <v>317</v>
       </c>
@@ -28432,7 +28433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="319" spans="1:24" hidden="1">
+    <row r="319" spans="1:24">
       <c r="A319" s="18" t="s">
         <v>318</v>
       </c>
@@ -28460,7 +28461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="320" spans="1:24" hidden="1">
+    <row r="320" spans="1:24">
       <c r="A320" s="18" t="s">
         <v>319</v>
       </c>
@@ -28488,7 +28489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="321" spans="1:24" hidden="1">
+    <row r="321" spans="1:24">
       <c r="A321" s="18" t="s">
         <v>320</v>
       </c>
@@ -28516,7 +28517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="322" spans="1:24" hidden="1">
+    <row r="322" spans="1:24">
       <c r="A322" s="21" t="s">
         <v>321</v>
       </c>
@@ -28546,7 +28547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="323" spans="1:24" hidden="1">
+    <row r="323" spans="1:24">
       <c r="A323" s="21" t="s">
         <v>322</v>
       </c>
@@ -28574,7 +28575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="324" spans="1:24" hidden="1">
+    <row r="324" spans="1:24">
       <c r="A324" s="21" t="s">
         <v>323</v>
       </c>
@@ -28602,7 +28603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="325" spans="1:24" hidden="1">
+    <row r="325" spans="1:24">
       <c r="A325" s="21" t="s">
         <v>324</v>
       </c>
@@ -28640,7 +28641,7 @@
         <v>-24.5</v>
       </c>
     </row>
-    <row r="326" spans="1:24" hidden="1">
+    <row r="326" spans="1:24">
       <c r="A326" s="21" t="s">
         <v>325</v>
       </c>
@@ -28668,7 +28669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="327" spans="1:24" hidden="1">
+    <row r="327" spans="1:24">
       <c r="A327" s="21" t="s">
         <v>326</v>
       </c>
@@ -28696,7 +28697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="328" spans="1:24" hidden="1">
+    <row r="328" spans="1:24">
       <c r="A328" s="21" t="s">
         <v>327</v>
       </c>
@@ -28724,7 +28725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="329" spans="1:24" hidden="1">
+    <row r="329" spans="1:24">
       <c r="A329" s="21" t="s">
         <v>328</v>
       </c>
@@ -28752,7 +28753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="330" spans="1:24" hidden="1">
+    <row r="330" spans="1:24">
       <c r="A330" s="21" t="s">
         <v>329</v>
       </c>
@@ -28780,7 +28781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="331" spans="1:24" hidden="1">
+    <row r="331" spans="1:24">
       <c r="A331" s="21" t="s">
         <v>330</v>
       </c>
@@ -28808,7 +28809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="332" spans="1:24" hidden="1">
+    <row r="332" spans="1:24">
       <c r="A332" s="21" t="s">
         <v>331</v>
       </c>
@@ -28836,7 +28837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="333" spans="1:24" hidden="1">
+    <row r="333" spans="1:24">
       <c r="A333" s="21" t="s">
         <v>332</v>
       </c>
@@ -28864,7 +28865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="334" spans="1:24" hidden="1">
+    <row r="334" spans="1:24">
       <c r="A334" s="21" t="s">
         <v>333</v>
       </c>
@@ -28892,7 +28893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="335" spans="1:24" hidden="1">
+    <row r="335" spans="1:24">
       <c r="A335" s="21" t="s">
         <v>334</v>
       </c>
@@ -28928,7 +28929,7 @@
         <v>-15.9</v>
       </c>
     </row>
-    <row r="336" spans="1:24" hidden="1">
+    <row r="336" spans="1:24">
       <c r="A336" s="21" t="s">
         <v>335</v>
       </c>
@@ -28956,7 +28957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="337" spans="1:40" hidden="1">
+    <row r="337" spans="1:40">
       <c r="A337" s="21" t="s">
         <v>336</v>
       </c>

</xml_diff>